<commit_message>
Code updated 23-01-03 12:02:20
</commit_message>
<xml_diff>
--- a/Season_Attack/81.xlsx
+++ b/Season_Attack/81.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G150"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -418,10 +418,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>01-01_A</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>01-01_0</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>01-02_A</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>01-02_0</t>
         </is>
@@ -452,9 +462,15 @@
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2487</t>
+      <c r="G2" t="n">
+        <v>2487</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2767</t>
         </is>
       </c>
     </row>
@@ -483,9 +499,15 @@
       <c r="F3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2820</t>
+      <c r="G3" t="n">
+        <v>2820</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>3109</t>
         </is>
       </c>
     </row>
@@ -514,9 +536,15 @@
       <c r="F4" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2999</t>
+      <c r="G4" t="n">
+        <v>2999</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>3318</t>
         </is>
       </c>
     </row>
@@ -545,9 +573,15 @@
       <c r="F5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2812</t>
+      <c r="G5" t="n">
+        <v>2812</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>3131</t>
         </is>
       </c>
     </row>
@@ -576,9 +610,15 @@
       <c r="F6" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2918</t>
+      <c r="G6" t="n">
+        <v>2918</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>3218</t>
         </is>
       </c>
     </row>
@@ -607,9 +647,15 @@
       <c r="F7" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>2846</t>
+      <c r="G7" t="n">
+        <v>2846</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>3311</t>
         </is>
       </c>
     </row>
@@ -638,9 +684,15 @@
       <c r="F8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2761</t>
+      <c r="G8" t="n">
+        <v>2761</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>3138</t>
         </is>
       </c>
     </row>
@@ -669,9 +721,15 @@
       <c r="F9" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2877</t>
+      <c r="G9" t="n">
+        <v>2877</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>3223</t>
         </is>
       </c>
     </row>
@@ -700,9 +758,15 @@
       <c r="F10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2852</t>
+      <c r="G10" t="n">
+        <v>2852</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>3050</t>
         </is>
       </c>
     </row>
@@ -731,9 +795,15 @@
       <c r="F11" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2967</t>
+      <c r="G11" t="n">
+        <v>2967</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2824</t>
         </is>
       </c>
     </row>
@@ -762,9 +832,15 @@
       <c r="F12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2810</t>
+      <c r="G12" t="n">
+        <v>2810</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>3096</t>
         </is>
       </c>
     </row>
@@ -793,7 +869,13 @@
       <c r="F13" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" t="n">
+        <v>2586</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>2586</t>
         </is>
@@ -824,9 +906,15 @@
       <c r="F14" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2996</t>
+      <c r="G14" t="n">
+        <v>2996</v>
+      </c>
+      <c r="H14" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>3434</t>
         </is>
       </c>
     </row>
@@ -855,9 +943,15 @@
       <c r="F15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2862</t>
+      <c r="G15" t="n">
+        <v>2862</v>
+      </c>
+      <c r="H15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>3199</t>
         </is>
       </c>
     </row>
@@ -886,9 +980,15 @@
       <c r="F16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>2953</t>
+      <c r="G16" t="n">
+        <v>2953</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>3341</t>
         </is>
       </c>
     </row>
@@ -917,9 +1017,15 @@
       <c r="F17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>2887</t>
+      <c r="G17" t="n">
+        <v>2887</v>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>3320</t>
         </is>
       </c>
     </row>
@@ -948,9 +1054,15 @@
       <c r="F18" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>2962</t>
+      <c r="G18" t="n">
+        <v>2962</v>
+      </c>
+      <c r="H18" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>3197</t>
         </is>
       </c>
     </row>
@@ -979,9 +1091,15 @@
       <c r="F19" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2941</t>
+      <c r="G19" t="n">
+        <v>2941</v>
+      </c>
+      <c r="H19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>3308</t>
         </is>
       </c>
     </row>
@@ -1010,9 +1128,15 @@
       <c r="F20" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>2965</t>
+      <c r="G20" t="n">
+        <v>2965</v>
+      </c>
+      <c r="H20" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>3271</t>
         </is>
       </c>
     </row>
@@ -1041,9 +1165,15 @@
       <c r="F21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2825</t>
         </is>
       </c>
     </row>
@@ -1072,9 +1202,15 @@
       <c r="F22" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2749</t>
+      <c r="G22" t="n">
+        <v>2749</v>
+      </c>
+      <c r="H22" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>3203</t>
         </is>
       </c>
     </row>
@@ -1103,9 +1239,15 @@
       <c r="F23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2579</t>
+      <c r="G23" t="n">
+        <v>2579</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2606</t>
         </is>
       </c>
     </row>
@@ -1134,9 +1276,15 @@
       <c r="F24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>2951</t>
+      <c r="G24" t="n">
+        <v>2951</v>
+      </c>
+      <c r="H24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>3307</t>
         </is>
       </c>
     </row>
@@ -1165,9 +1313,15 @@
       <c r="F25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -1196,9 +1350,15 @@
       <c r="F26" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>2909</t>
+      <c r="G26" t="n">
+        <v>2909</v>
+      </c>
+      <c r="H26" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>3254</t>
         </is>
       </c>
     </row>
@@ -1227,9 +1387,15 @@
       <c r="F27" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>2999</t>
+      <c r="G27" t="n">
+        <v>2999</v>
+      </c>
+      <c r="H27" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>3350</t>
         </is>
       </c>
     </row>
@@ -1258,9 +1424,15 @@
       <c r="F28" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>2745</t>
+      <c r="G28" t="n">
+        <v>2745</v>
+      </c>
+      <c r="H28" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2984</t>
         </is>
       </c>
     </row>
@@ -1289,9 +1461,15 @@
       <c r="F29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>2838</t>
+      <c r="G29" t="n">
+        <v>2838</v>
+      </c>
+      <c r="H29" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>3011</t>
         </is>
       </c>
     </row>
@@ -1320,9 +1498,15 @@
       <c r="F30" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>3055</t>
+      <c r="G30" t="n">
+        <v>3055</v>
+      </c>
+      <c r="H30" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1351,9 +1535,15 @@
       <c r="F31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>2865</t>
+      <c r="G31" t="n">
+        <v>2865</v>
+      </c>
+      <c r="H31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>3020</t>
         </is>
       </c>
     </row>
@@ -1382,9 +1572,15 @@
       <c r="F32" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>3066</t>
+      <c r="G32" t="n">
+        <v>3066</v>
+      </c>
+      <c r="H32" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>3436</t>
         </is>
       </c>
     </row>
@@ -1413,9 +1609,15 @@
       <c r="F33" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>2978</t>
+      <c r="G33" t="n">
+        <v>2978</v>
+      </c>
+      <c r="H33" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>3250</t>
         </is>
       </c>
     </row>
@@ -1444,9 +1646,15 @@
       <c r="F34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2506</t>
         </is>
       </c>
     </row>
@@ -1475,9 +1683,15 @@
       <c r="F35" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>2995</t>
+      <c r="G35" t="n">
+        <v>2995</v>
+      </c>
+      <c r="H35" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>3352</t>
         </is>
       </c>
     </row>
@@ -1506,9 +1720,15 @@
       <c r="F36" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>2576</t>
+      <c r="G36" t="n">
+        <v>2576</v>
+      </c>
+      <c r="H36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2935</t>
         </is>
       </c>
     </row>
@@ -1537,9 +1757,15 @@
       <c r="F37" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>2820</t>
+      <c r="G37" t="n">
+        <v>2820</v>
+      </c>
+      <c r="H37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>3164</t>
         </is>
       </c>
     </row>
@@ -1568,9 +1794,15 @@
       <c r="F38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>3000</t>
+      <c r="G38" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H38" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>3366</t>
         </is>
       </c>
     </row>
@@ -1599,9 +1831,15 @@
       <c r="F39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>2941</t>
+      <c r="G39" t="n">
+        <v>2941</v>
+      </c>
+      <c r="H39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>3254</t>
         </is>
       </c>
     </row>
@@ -1630,9 +1868,15 @@
       <c r="F40" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>2922</t>
+      <c r="G40" t="n">
+        <v>2922</v>
+      </c>
+      <c r="H40" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>3214</t>
         </is>
       </c>
     </row>
@@ -1661,9 +1905,15 @@
       <c r="F41" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>2882</t>
+      <c r="G41" t="n">
+        <v>2882</v>
+      </c>
+      <c r="H41" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>3136</t>
         </is>
       </c>
     </row>
@@ -1692,9 +1942,15 @@
       <c r="F42" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>3006</t>
+      <c r="G42" t="n">
+        <v>3006</v>
+      </c>
+      <c r="H42" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>3461</t>
         </is>
       </c>
     </row>
@@ -1723,9 +1979,15 @@
       <c r="F43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>2938</t>
+      <c r="G43" t="n">
+        <v>2938</v>
+      </c>
+      <c r="H43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>3314</t>
         </is>
       </c>
     </row>
@@ -1754,9 +2016,15 @@
       <c r="F44" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>2676</t>
+      <c r="G44" t="n">
+        <v>2676</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>2749</t>
         </is>
       </c>
     </row>
@@ -1785,9 +2053,15 @@
       <c r="F45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>2825</t>
+      <c r="G45" t="n">
+        <v>2825</v>
+      </c>
+      <c r="H45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>3147</t>
         </is>
       </c>
     </row>
@@ -1816,9 +2090,15 @@
       <c r="F46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>2888</t>
+      <c r="G46" t="n">
+        <v>2888</v>
+      </c>
+      <c r="H46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>3132</t>
         </is>
       </c>
     </row>
@@ -1847,9 +2127,15 @@
       <c r="F47" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>2897</t>
+      <c r="G47" t="n">
+        <v>2897</v>
+      </c>
+      <c r="H47" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>3192</t>
         </is>
       </c>
     </row>
@@ -1878,9 +2164,15 @@
       <c r="F48" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>2902</t>
+      <c r="G48" t="n">
+        <v>2902</v>
+      </c>
+      <c r="H48" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>3157</t>
         </is>
       </c>
     </row>
@@ -1909,9 +2201,15 @@
       <c r="F49" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>2876</t>
+      <c r="G49" t="n">
+        <v>2876</v>
+      </c>
+      <c r="H49" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>3048</t>
         </is>
       </c>
     </row>
@@ -1940,9 +2238,15 @@
       <c r="F50" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>2944</t>
+      <c r="G50" t="n">
+        <v>2944</v>
+      </c>
+      <c r="H50" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>3216</t>
         </is>
       </c>
     </row>
@@ -1971,9 +2275,15 @@
       <c r="F51" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>2879</t>
+      <c r="G51" t="n">
+        <v>2879</v>
+      </c>
+      <c r="H51" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>3110</t>
         </is>
       </c>
     </row>
@@ -2002,7 +2312,13 @@
       <c r="F52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2033,7 +2349,13 @@
       <c r="F53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G53" t="inlineStr">
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2064,9 +2386,15 @@
       <c r="F54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>2539</t>
         </is>
       </c>
     </row>
@@ -2095,9 +2423,15 @@
       <c r="F55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>2676</t>
+      <c r="G55" t="n">
+        <v>2676</v>
+      </c>
+      <c r="H55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>2808</t>
         </is>
       </c>
     </row>
@@ -2126,9 +2460,15 @@
       <c r="F56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>2722</t>
+      <c r="G56" t="n">
+        <v>2722</v>
+      </c>
+      <c r="H56" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>2929</t>
         </is>
       </c>
     </row>
@@ -2157,9 +2497,15 @@
       <c r="F57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>2869</t>
+      <c r="G57" t="n">
+        <v>2869</v>
+      </c>
+      <c r="H57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>3109</t>
         </is>
       </c>
     </row>
@@ -2188,9 +2534,15 @@
       <c r="F58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>2738</t>
+      <c r="G58" t="n">
+        <v>2738</v>
+      </c>
+      <c r="H58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>2880</t>
         </is>
       </c>
     </row>
@@ -2219,9 +2571,15 @@
       <c r="F59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>2800</t>
+      <c r="G59" t="n">
+        <v>2800</v>
+      </c>
+      <c r="H59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>3035</t>
         </is>
       </c>
     </row>
@@ -2250,9 +2608,15 @@
       <c r="F60" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>2679</t>
+      <c r="G60" t="n">
+        <v>2679</v>
+      </c>
+      <c r="H60" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>3092</t>
         </is>
       </c>
     </row>
@@ -2281,9 +2645,15 @@
       <c r="F61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>2774</t>
+      <c r="G61" t="n">
+        <v>2774</v>
+      </c>
+      <c r="H61" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>3001</t>
         </is>
       </c>
     </row>
@@ -2312,9 +2682,15 @@
       <c r="F62" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>2841</t>
+      <c r="G62" t="n">
+        <v>2841</v>
+      </c>
+      <c r="H62" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>3098</t>
         </is>
       </c>
     </row>
@@ -2343,9 +2719,15 @@
       <c r="F63" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>2799</t>
+      <c r="G63" t="n">
+        <v>2799</v>
+      </c>
+      <c r="H63" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>2953</t>
         </is>
       </c>
     </row>
@@ -2374,9 +2756,15 @@
       <c r="F64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>2514</t>
         </is>
       </c>
     </row>
@@ -2405,9 +2793,15 @@
       <c r="F65" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="G65" t="n">
+        <v>2671</v>
+      </c>
+      <c r="H65" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>2931</t>
         </is>
       </c>
     </row>
@@ -2436,7 +2830,13 @@
       <c r="F66" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="G66" t="inlineStr">
+      <c r="G66" t="n">
+        <v>2671</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr">
         <is>
           <t>2671</t>
         </is>
@@ -2467,9 +2867,15 @@
       <c r="F67" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>2955</t>
+      <c r="G67" t="n">
+        <v>2955</v>
+      </c>
+      <c r="H67" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>3307</t>
         </is>
       </c>
     </row>
@@ -2498,9 +2904,15 @@
       <c r="F68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>2742</t>
+      <c r="G68" t="n">
+        <v>2742</v>
+      </c>
+      <c r="H68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>2986</t>
         </is>
       </c>
     </row>
@@ -2529,9 +2941,15 @@
       <c r="F69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="G69" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>2536</t>
         </is>
       </c>
     </row>
@@ -2560,9 +2978,15 @@
       <c r="F70" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>2664</t>
+      <c r="G70" t="n">
+        <v>2664</v>
+      </c>
+      <c r="H70" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>2781</t>
         </is>
       </c>
     </row>
@@ -2591,9 +3015,15 @@
       <c r="F71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>2837</t>
+      <c r="G71" t="n">
+        <v>2837</v>
+      </c>
+      <c r="H71" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>3144</t>
         </is>
       </c>
     </row>
@@ -2622,9 +3052,15 @@
       <c r="F72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>2802</t>
+      <c r="G72" t="n">
+        <v>2802</v>
+      </c>
+      <c r="H72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>2973</t>
         </is>
       </c>
     </row>
@@ -2653,9 +3089,15 @@
       <c r="F73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>2921</t>
+      <c r="G73" t="n">
+        <v>2921</v>
+      </c>
+      <c r="H73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>3081</t>
         </is>
       </c>
     </row>
@@ -2684,9 +3126,15 @@
       <c r="F74" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>2770</t>
+      <c r="G74" t="n">
+        <v>2770</v>
+      </c>
+      <c r="H74" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>2970</t>
         </is>
       </c>
     </row>
@@ -2715,9 +3163,15 @@
       <c r="F75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>2911</t>
+      <c r="G75" t="n">
+        <v>2911</v>
+      </c>
+      <c r="H75" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>3073</t>
         </is>
       </c>
     </row>
@@ -2746,9 +3200,15 @@
       <c r="F76" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>2858</t>
+      <c r="G76" t="n">
+        <v>2858</v>
+      </c>
+      <c r="H76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>2909</t>
         </is>
       </c>
     </row>
@@ -2777,9 +3237,15 @@
       <c r="F77" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>2557</t>
+      <c r="G77" t="n">
+        <v>2557</v>
+      </c>
+      <c r="H77" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>2604</t>
         </is>
       </c>
     </row>
@@ -2808,9 +3274,15 @@
       <c r="F78" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>2799</t>
+      <c r="G78" t="n">
+        <v>2799</v>
+      </c>
+      <c r="H78" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>2946</t>
         </is>
       </c>
     </row>
@@ -2839,9 +3311,15 @@
       <c r="F79" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>2765</t>
+      <c r="G79" t="n">
+        <v>2765</v>
+      </c>
+      <c r="H79" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>2856</t>
         </is>
       </c>
     </row>
@@ -2870,9 +3348,15 @@
       <c r="F80" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>2674</t>
+      <c r="G80" t="n">
+        <v>2674</v>
+      </c>
+      <c r="H80" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>2801</t>
         </is>
       </c>
     </row>
@@ -2901,9 +3385,15 @@
       <c r="F81" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>2546</t>
+      <c r="G81" t="n">
+        <v>2546</v>
+      </c>
+      <c r="H81" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>2562</t>
         </is>
       </c>
     </row>
@@ -2932,9 +3422,15 @@
       <c r="F82" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>2872</t>
+      <c r="G82" t="n">
+        <v>2872</v>
+      </c>
+      <c r="H82" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>3065</t>
         </is>
       </c>
     </row>
@@ -2963,9 +3459,15 @@
       <c r="F83" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>2458</t>
+      <c r="G83" t="n">
+        <v>2458</v>
+      </c>
+      <c r="H83" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>2598</t>
         </is>
       </c>
     </row>
@@ -2994,9 +3496,15 @@
       <c r="F84" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>2611</t>
+      <c r="G84" t="n">
+        <v>2611</v>
+      </c>
+      <c r="H84" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>2690</t>
         </is>
       </c>
     </row>
@@ -3025,9 +3533,15 @@
       <c r="F85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>1997</t>
         </is>
       </c>
     </row>
@@ -3056,9 +3570,15 @@
       <c r="F86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>2447</t>
+      <c r="G86" t="n">
+        <v>2447</v>
+      </c>
+      <c r="H86" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>2492</t>
         </is>
       </c>
     </row>
@@ -3087,9 +3607,15 @@
       <c r="F87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>2494</t>
+      <c r="G87" t="n">
+        <v>2494</v>
+      </c>
+      <c r="H87" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>2566</t>
         </is>
       </c>
     </row>
@@ -3118,7 +3644,13 @@
       <c r="F88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G88" t="inlineStr">
+      <c r="G88" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3149,7 +3681,13 @@
       <c r="F89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G89" t="inlineStr">
+      <c r="G89" t="n">
+        <v>0</v>
+      </c>
+      <c r="H89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3180,7 +3718,13 @@
       <c r="F90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G90" t="inlineStr">
+      <c r="G90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3211,9 +3755,15 @@
       <c r="F91" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>2502</t>
+      <c r="G91" t="n">
+        <v>2502</v>
+      </c>
+      <c r="H91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>2462</t>
         </is>
       </c>
     </row>
@@ -3242,9 +3792,15 @@
       <c r="F92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>2501</t>
+      <c r="G92" t="n">
+        <v>2501</v>
+      </c>
+      <c r="H92" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>2729</t>
         </is>
       </c>
     </row>
@@ -3273,9 +3829,15 @@
       <c r="F93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>2474</t>
+      <c r="G93" t="n">
+        <v>2474</v>
+      </c>
+      <c r="H93" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>2497</t>
         </is>
       </c>
     </row>
@@ -3304,9 +3866,15 @@
       <c r="F94" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>2786</t>
+      <c r="G94" t="n">
+        <v>2786</v>
+      </c>
+      <c r="H94" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>2997</t>
         </is>
       </c>
     </row>
@@ -3335,9 +3903,15 @@
       <c r="F95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>2646</t>
+      <c r="G95" t="n">
+        <v>2646</v>
+      </c>
+      <c r="H95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>2844</t>
         </is>
       </c>
     </row>
@@ -3366,9 +3940,15 @@
       <c r="F96" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>2592</t>
+      <c r="G96" t="n">
+        <v>2592</v>
+      </c>
+      <c r="H96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>2583</t>
         </is>
       </c>
     </row>
@@ -3397,9 +3977,15 @@
       <c r="F97" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>2765</t>
+      <c r="G97" t="n">
+        <v>2765</v>
+      </c>
+      <c r="H97" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>3026</t>
         </is>
       </c>
     </row>
@@ -3428,9 +4014,15 @@
       <c r="F98" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>2694</t>
+      <c r="G98" t="n">
+        <v>2694</v>
+      </c>
+      <c r="H98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>2780</t>
         </is>
       </c>
     </row>
@@ -3459,7 +4051,13 @@
       <c r="F99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G99" t="inlineStr">
+      <c r="G99" t="n">
+        <v>0</v>
+      </c>
+      <c r="H99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3490,9 +4088,15 @@
       <c r="F100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>2453</t>
+      <c r="G100" t="n">
+        <v>2453</v>
+      </c>
+      <c r="H100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>2471</t>
         </is>
       </c>
     </row>
@@ -3521,9 +4125,15 @@
       <c r="F101" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>2818</t>
+      <c r="G101" t="n">
+        <v>2818</v>
+      </c>
+      <c r="H101" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>3013</t>
         </is>
       </c>
     </row>
@@ -3552,9 +4162,15 @@
       <c r="F102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G102" t="n">
+        <v>0</v>
+      </c>
+      <c r="H102" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>2641</t>
         </is>
       </c>
     </row>
@@ -3583,9 +4199,15 @@
       <c r="F103" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>2501</t>
+      <c r="G103" t="n">
+        <v>2501</v>
+      </c>
+      <c r="H103" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>2673</t>
         </is>
       </c>
     </row>
@@ -3614,9 +4236,15 @@
       <c r="F104" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>2518</t>
+      <c r="G104" t="n">
+        <v>2518</v>
+      </c>
+      <c r="H104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -3645,9 +4273,15 @@
       <c r="F105" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="G105" t="n">
+        <v>2671</v>
+      </c>
+      <c r="H105" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>2792</t>
         </is>
       </c>
     </row>
@@ -3676,9 +4310,15 @@
       <c r="F106" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>2535</t>
+      <c r="G106" t="n">
+        <v>2535</v>
+      </c>
+      <c r="H106" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>2680</t>
         </is>
       </c>
     </row>
@@ -3707,9 +4347,15 @@
       <c r="F107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>2513</t>
+      <c r="G107" t="n">
+        <v>2513</v>
+      </c>
+      <c r="H107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>2597</t>
         </is>
       </c>
     </row>
@@ -3738,9 +4384,15 @@
       <c r="F108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>2472</t>
+      <c r="G108" t="n">
+        <v>2472</v>
+      </c>
+      <c r="H108" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>2466</t>
         </is>
       </c>
     </row>
@@ -3769,9 +4421,15 @@
       <c r="F109" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>2466</t>
+      <c r="G109" t="n">
+        <v>2466</v>
+      </c>
+      <c r="H109" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>2475</t>
         </is>
       </c>
     </row>
@@ -3800,9 +4458,15 @@
       <c r="F110" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>2776</t>
+      <c r="G110" t="n">
+        <v>2776</v>
+      </c>
+      <c r="H110" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>2754</t>
         </is>
       </c>
     </row>
@@ -3831,7 +4495,13 @@
       <c r="F111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G111" t="inlineStr">
+      <c r="G111" t="n">
+        <v>0</v>
+      </c>
+      <c r="H111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3862,9 +4532,15 @@
       <c r="F112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="G112" t="n">
+        <v>2499</v>
+      </c>
+      <c r="H112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>2671</t>
         </is>
       </c>
     </row>
@@ -3893,9 +4569,15 @@
       <c r="F113" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>2508</t>
+      <c r="G113" t="n">
+        <v>2508</v>
+      </c>
+      <c r="H113" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>2603</t>
         </is>
       </c>
     </row>
@@ -3924,9 +4606,15 @@
       <c r="F114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>2522</t>
+      <c r="G114" t="n">
+        <v>2522</v>
+      </c>
+      <c r="H114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>2540</t>
         </is>
       </c>
     </row>
@@ -3955,9 +4643,15 @@
       <c r="F115" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>2555</t>
+      <c r="G115" t="n">
+        <v>2555</v>
+      </c>
+      <c r="H115" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>2485</t>
         </is>
       </c>
     </row>
@@ -3986,9 +4680,15 @@
       <c r="F116" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>2534</t>
+      <c r="G116" t="n">
+        <v>2534</v>
+      </c>
+      <c r="H116" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>2607</t>
         </is>
       </c>
     </row>
@@ -4017,9 +4717,15 @@
       <c r="F117" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>2512</t>
+      <c r="G117" t="n">
+        <v>2512</v>
+      </c>
+      <c r="H117" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>2621</t>
         </is>
       </c>
     </row>
@@ -4048,7 +4754,13 @@
       <c r="F118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G118" t="inlineStr">
+      <c r="G118" t="n">
+        <v>0</v>
+      </c>
+      <c r="H118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4079,9 +4791,15 @@
       <c r="F119" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>2524</t>
+      <c r="G119" t="n">
+        <v>2524</v>
+      </c>
+      <c r="H119" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>2681</t>
         </is>
       </c>
     </row>
@@ -4110,7 +4828,13 @@
       <c r="F120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G120" t="inlineStr">
+      <c r="G120" t="n">
+        <v>0</v>
+      </c>
+      <c r="H120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4141,9 +4865,15 @@
       <c r="F121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>1993</t>
+      <c r="G121" t="n">
+        <v>1993</v>
+      </c>
+      <c r="H121" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>2053</t>
         </is>
       </c>
     </row>
@@ -4172,7 +4902,13 @@
       <c r="F122" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G122" t="inlineStr">
+      <c r="G122" t="n">
+        <v>2488</v>
+      </c>
+      <c r="H122" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I122" t="inlineStr">
         <is>
           <t>2488</t>
         </is>
@@ -4203,9 +4939,15 @@
       <c r="F123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>2512</t>
+      <c r="G123" t="n">
+        <v>2512</v>
+      </c>
+      <c r="H123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>2514</t>
         </is>
       </c>
     </row>
@@ -4234,9 +4976,15 @@
       <c r="F124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>2595</t>
+      <c r="G124" t="n">
+        <v>2595</v>
+      </c>
+      <c r="H124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>2648</t>
         </is>
       </c>
     </row>
@@ -4265,7 +5013,13 @@
       <c r="F125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G125" t="inlineStr">
+      <c r="G125" t="n">
+        <v>0</v>
+      </c>
+      <c r="H125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4296,9 +5050,15 @@
       <c r="F126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>2507</t>
+      <c r="G126" t="n">
+        <v>2507</v>
+      </c>
+      <c r="H126" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>2488</t>
         </is>
       </c>
     </row>
@@ -4327,7 +5087,13 @@
       <c r="F127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G127" t="inlineStr">
+      <c r="G127" t="n">
+        <v>0</v>
+      </c>
+      <c r="H127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I127" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4358,9 +5124,15 @@
       <c r="F128" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G128" t="inlineStr">
-        <is>
-          <t>2508</t>
+      <c r="G128" t="n">
+        <v>2508</v>
+      </c>
+      <c r="H128" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>2466</t>
         </is>
       </c>
     </row>
@@ -4389,9 +5161,15 @@
       <c r="F129" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G129" t="inlineStr">
-        <is>
-          <t>2066</t>
+      <c r="G129" t="n">
+        <v>2066</v>
+      </c>
+      <c r="H129" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>2073</t>
         </is>
       </c>
     </row>
@@ -4420,7 +5198,13 @@
       <c r="F130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G130" t="inlineStr">
+      <c r="G130" t="n">
+        <v>0</v>
+      </c>
+      <c r="H130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4451,7 +5235,13 @@
       <c r="F131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G131" t="inlineStr">
+      <c r="G131" t="n">
+        <v>0</v>
+      </c>
+      <c r="H131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4482,9 +5272,15 @@
       <c r="F132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G132" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G132" t="n">
+        <v>0</v>
+      </c>
+      <c r="H132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>1498</t>
         </is>
       </c>
     </row>
@@ -4513,7 +5309,13 @@
       <c r="F133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G133" t="inlineStr">
+      <c r="G133" t="n">
+        <v>0</v>
+      </c>
+      <c r="H133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4544,9 +5346,15 @@
       <c r="F134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G134" t="inlineStr">
-        <is>
-          <t>1997</t>
+      <c r="G134" t="n">
+        <v>1997</v>
+      </c>
+      <c r="H134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>1988</t>
         </is>
       </c>
     </row>
@@ -4575,9 +5383,15 @@
       <c r="F135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>1994</t>
+      <c r="G135" t="n">
+        <v>1994</v>
+      </c>
+      <c r="H135" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>2062</t>
         </is>
       </c>
     </row>
@@ -4606,9 +5420,15 @@
       <c r="F136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G136" t="n">
+        <v>0</v>
+      </c>
+      <c r="H136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>1500</t>
         </is>
       </c>
     </row>
@@ -4637,7 +5457,13 @@
       <c r="F137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G137" t="inlineStr">
+      <c r="G137" t="n">
+        <v>0</v>
+      </c>
+      <c r="H137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4668,7 +5494,13 @@
       <c r="F138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G138" t="inlineStr">
+      <c r="G138" t="n">
+        <v>0</v>
+      </c>
+      <c r="H138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4699,7 +5531,13 @@
       <c r="F139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G139" t="inlineStr">
+      <c r="G139" t="n">
+        <v>0</v>
+      </c>
+      <c r="H139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4730,9 +5568,15 @@
       <c r="F140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G140" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G140" t="n">
+        <v>0</v>
+      </c>
+      <c r="H140" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>2542</t>
         </is>
       </c>
     </row>
@@ -4761,7 +5605,13 @@
       <c r="F141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G141" t="inlineStr">
+      <c r="G141" t="n">
+        <v>0</v>
+      </c>
+      <c r="H141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4792,7 +5642,13 @@
       <c r="F142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G142" t="inlineStr">
+      <c r="G142" t="n">
+        <v>0</v>
+      </c>
+      <c r="H142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4823,9 +5679,15 @@
       <c r="F143" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G143" t="inlineStr">
-        <is>
-          <t>2944</t>
+      <c r="G143" t="n">
+        <v>2944</v>
+      </c>
+      <c r="H143" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>3062</t>
         </is>
       </c>
     </row>
@@ -4854,7 +5716,13 @@
       <c r="F144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G144" t="inlineStr">
+      <c r="G144" t="n">
+        <v>0</v>
+      </c>
+      <c r="H144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4885,9 +5753,15 @@
       <c r="F145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G145" t="inlineStr">
-        <is>
-          <t>2477</t>
+      <c r="G145" t="n">
+        <v>2477</v>
+      </c>
+      <c r="H145" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>2507</t>
         </is>
       </c>
     </row>
@@ -4916,7 +5790,13 @@
       <c r="F146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G146" t="inlineStr">
+      <c r="G146" t="n">
+        <v>0</v>
+      </c>
+      <c r="H146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4947,17 +5827,21 @@
       <c r="F147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G147" t="inlineStr">
+      <c r="G147" t="n">
+        <v>0</v>
+      </c>
+      <c r="H147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>35384730</t>
-        </is>
+      <c r="A148" t="n">
+        <v>35384730</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
@@ -4974,17 +5858,21 @@
       <c r="F148" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G148" t="inlineStr">
-        <is>
-          <t>2456</t>
+      <c r="G148" t="n">
+        <v>2456</v>
+      </c>
+      <c r="H148" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>2519</t>
         </is>
       </c>
     </row>
     <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>58386875</t>
-        </is>
+      <c r="A149" t="n">
+        <v>58386875</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
@@ -5001,17 +5889,21 @@
       <c r="F149" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G149" t="inlineStr">
-        <is>
-          <t>1330</t>
+      <c r="G149" t="n">
+        <v>1330</v>
+      </c>
+      <c r="H149" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>1329</t>
         </is>
       </c>
     </row>
     <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>58425274</t>
-        </is>
+      <c r="A150" t="n">
+        <v>58425274</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
@@ -5028,9 +5920,15 @@
       <c r="F150" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="G150" t="inlineStr">
-        <is>
-          <t>1390</t>
+      <c r="G150" t="n">
+        <v>1390</v>
+      </c>
+      <c r="H150" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>1379</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-04 11:31:30
</commit_message>
<xml_diff>
--- a/Season_Attack/81.xlsx
+++ b/Season_Attack/81.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I150"/>
+  <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,16 @@
           <t>01-02_0</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>01-03_A</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>01-03_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -468,9 +478,15 @@
       <c r="H2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2767</t>
+      <c r="I2" t="n">
+        <v>2767</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2999</t>
         </is>
       </c>
     </row>
@@ -505,9 +521,15 @@
       <c r="H3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>3109</t>
+      <c r="I3" t="n">
+        <v>3109</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>3368</t>
         </is>
       </c>
     </row>
@@ -542,9 +564,15 @@
       <c r="H4" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>3318</t>
+      <c r="I4" t="n">
+        <v>3318</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>3597</t>
         </is>
       </c>
     </row>
@@ -579,9 +607,15 @@
       <c r="H5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>3131</t>
+      <c r="I5" t="n">
+        <v>3131</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>3439</t>
         </is>
       </c>
     </row>
@@ -616,9 +650,15 @@
       <c r="H6" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>3218</t>
+      <c r="I6" t="n">
+        <v>3218</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>3537</t>
         </is>
       </c>
     </row>
@@ -653,9 +693,15 @@
       <c r="H7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>3311</t>
+      <c r="I7" t="n">
+        <v>3311</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>3729</t>
         </is>
       </c>
     </row>
@@ -690,9 +736,15 @@
       <c r="H8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>3138</t>
+      <c r="I8" t="n">
+        <v>3138</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>3390</t>
         </is>
       </c>
     </row>
@@ -727,9 +779,15 @@
       <c r="H9" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>3223</t>
+      <c r="I9" t="n">
+        <v>3223</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>3523</t>
         </is>
       </c>
     </row>
@@ -764,9 +822,15 @@
       <c r="H10" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>3050</t>
+      <c r="I10" t="n">
+        <v>3050</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>3309</t>
         </is>
       </c>
     </row>
@@ -801,9 +865,15 @@
       <c r="H11" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>2824</t>
+      <c r="I11" t="n">
+        <v>2824</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>3025</t>
         </is>
       </c>
     </row>
@@ -838,9 +908,15 @@
       <c r="H12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>3096</t>
+      <c r="I12" t="n">
+        <v>3096</v>
+      </c>
+      <c r="J12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>3318</t>
         </is>
       </c>
     </row>
@@ -875,7 +951,13 @@
       <c r="H13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I13" t="n">
+        <v>2586</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>2586</t>
         </is>
@@ -912,9 +994,15 @@
       <c r="H14" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>3434</t>
+      <c r="I14" t="n">
+        <v>3434</v>
+      </c>
+      <c r="J14" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>3811</t>
         </is>
       </c>
     </row>
@@ -949,9 +1037,15 @@
       <c r="H15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>3199</t>
+      <c r="I15" t="n">
+        <v>3199</v>
+      </c>
+      <c r="J15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>3476</t>
         </is>
       </c>
     </row>
@@ -986,9 +1080,15 @@
       <c r="H16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>3341</t>
+      <c r="I16" t="n">
+        <v>3341</v>
+      </c>
+      <c r="J16" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>3571</t>
         </is>
       </c>
     </row>
@@ -1023,9 +1123,15 @@
       <c r="H17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>3320</t>
+      <c r="I17" t="n">
+        <v>3320</v>
+      </c>
+      <c r="J17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>3585</t>
         </is>
       </c>
     </row>
@@ -1060,9 +1166,15 @@
       <c r="H18" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>3197</t>
+      <c r="I18" t="n">
+        <v>3197</v>
+      </c>
+      <c r="J18" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>3401</t>
         </is>
       </c>
     </row>
@@ -1085,7 +1197,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F19" s="4" t="n">
@@ -1097,9 +1209,15 @@
       <c r="H19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>3308</t>
+      <c r="I19" t="n">
+        <v>3308</v>
+      </c>
+      <c r="J19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>3644</t>
         </is>
       </c>
     </row>
@@ -1134,9 +1252,15 @@
       <c r="H20" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>3271</t>
+      <c r="I20" t="n">
+        <v>3271</v>
+      </c>
+      <c r="J20" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>3623</t>
         </is>
       </c>
     </row>
@@ -1171,9 +1295,15 @@
       <c r="H21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>2825</t>
+      <c r="I21" t="n">
+        <v>2825</v>
+      </c>
+      <c r="J21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>3073</t>
         </is>
       </c>
     </row>
@@ -1208,9 +1338,15 @@
       <c r="H22" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>3203</t>
+      <c r="I22" t="n">
+        <v>3203</v>
+      </c>
+      <c r="J22" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>3520</t>
         </is>
       </c>
     </row>
@@ -1245,9 +1381,15 @@
       <c r="H23" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>2606</t>
+      <c r="I23" t="n">
+        <v>2606</v>
+      </c>
+      <c r="J23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>2785</t>
         </is>
       </c>
     </row>
@@ -1282,9 +1424,15 @@
       <c r="H24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>3307</t>
+      <c r="I24" t="n">
+        <v>3307</v>
+      </c>
+      <c r="J24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>3587</t>
         </is>
       </c>
     </row>
@@ -1319,7 +1467,13 @@
       <c r="H25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="I25" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1356,9 +1510,15 @@
       <c r="H26" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>3254</t>
+      <c r="I26" t="n">
+        <v>3254</v>
+      </c>
+      <c r="J26" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>3621</t>
         </is>
       </c>
     </row>
@@ -1393,9 +1553,15 @@
       <c r="H27" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>3350</t>
+      <c r="I27" t="n">
+        <v>3350</v>
+      </c>
+      <c r="J27" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>3750</t>
         </is>
       </c>
     </row>
@@ -1430,9 +1596,15 @@
       <c r="H28" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>2984</t>
+      <c r="I28" t="n">
+        <v>2984</v>
+      </c>
+      <c r="J28" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>3173</t>
         </is>
       </c>
     </row>
@@ -1467,9 +1639,15 @@
       <c r="H29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>3011</t>
+      <c r="I29" t="n">
+        <v>3011</v>
+      </c>
+      <c r="J29" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>3236</t>
         </is>
       </c>
     </row>
@@ -1504,9 +1682,15 @@
       <c r="H30" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>3536</t>
+      <c r="I30" t="n">
+        <v>3536</v>
+      </c>
+      <c r="J30" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>3758</t>
         </is>
       </c>
     </row>
@@ -1541,9 +1725,15 @@
       <c r="H31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>3020</t>
+      <c r="I31" t="n">
+        <v>3020</v>
+      </c>
+      <c r="J31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>3406</t>
         </is>
       </c>
     </row>
@@ -1578,9 +1768,15 @@
       <c r="H32" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>3436</t>
+      <c r="I32" t="n">
+        <v>3436</v>
+      </c>
+      <c r="J32" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>3800</t>
         </is>
       </c>
     </row>
@@ -1615,9 +1811,15 @@
       <c r="H33" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>3250</t>
+      <c r="I33" t="n">
+        <v>3250</v>
+      </c>
+      <c r="J33" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>3623</t>
         </is>
       </c>
     </row>
@@ -1652,7 +1854,13 @@
       <c r="H34" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="I34" t="n">
+        <v>2506</v>
+      </c>
+      <c r="J34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>2506</t>
         </is>
@@ -1689,9 +1897,15 @@
       <c r="H35" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>3352</t>
+      <c r="I35" t="n">
+        <v>3352</v>
+      </c>
+      <c r="J35" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>3553</t>
         </is>
       </c>
     </row>
@@ -1726,9 +1940,15 @@
       <c r="H36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>2935</t>
+      <c r="I36" t="n">
+        <v>2935</v>
+      </c>
+      <c r="J36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>3251</t>
         </is>
       </c>
     </row>
@@ -1763,9 +1983,15 @@
       <c r="H37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>3164</t>
+      <c r="I37" t="n">
+        <v>3164</v>
+      </c>
+      <c r="J37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>3455</t>
         </is>
       </c>
     </row>
@@ -1800,9 +2026,15 @@
       <c r="H38" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>3366</t>
+      <c r="I38" t="n">
+        <v>3366</v>
+      </c>
+      <c r="J38" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>3701</t>
         </is>
       </c>
     </row>
@@ -1837,9 +2069,15 @@
       <c r="H39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>3254</t>
+      <c r="I39" t="n">
+        <v>3254</v>
+      </c>
+      <c r="J39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>3649</t>
         </is>
       </c>
     </row>
@@ -1874,9 +2112,15 @@
       <c r="H40" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>3214</t>
+      <c r="I40" t="n">
+        <v>3214</v>
+      </c>
+      <c r="J40" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>3562</t>
         </is>
       </c>
     </row>
@@ -1911,9 +2155,15 @@
       <c r="H41" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>3136</t>
+      <c r="I41" t="n">
+        <v>3136</v>
+      </c>
+      <c r="J41" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>3477</t>
         </is>
       </c>
     </row>
@@ -1948,9 +2198,15 @@
       <c r="H42" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>3461</t>
+      <c r="I42" t="n">
+        <v>3461</v>
+      </c>
+      <c r="J42" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>3724</t>
         </is>
       </c>
     </row>
@@ -1985,9 +2241,15 @@
       <c r="H43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>3314</t>
+      <c r="I43" t="n">
+        <v>3314</v>
+      </c>
+      <c r="J43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>3677</t>
         </is>
       </c>
     </row>
@@ -2022,9 +2284,15 @@
       <c r="H44" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>2749</t>
+      <c r="I44" t="n">
+        <v>2749</v>
+      </c>
+      <c r="J44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>2833</t>
         </is>
       </c>
     </row>
@@ -2059,9 +2327,15 @@
       <c r="H45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>3147</t>
+      <c r="I45" t="n">
+        <v>3147</v>
+      </c>
+      <c r="J45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>3428</t>
         </is>
       </c>
     </row>
@@ -2096,9 +2370,15 @@
       <c r="H46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>3132</t>
+      <c r="I46" t="n">
+        <v>3132</v>
+      </c>
+      <c r="J46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>3398</t>
         </is>
       </c>
     </row>
@@ -2133,9 +2413,15 @@
       <c r="H47" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>3192</t>
+      <c r="I47" t="n">
+        <v>3192</v>
+      </c>
+      <c r="J47" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>3473</t>
         </is>
       </c>
     </row>
@@ -2170,9 +2456,15 @@
       <c r="H48" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>3157</t>
+      <c r="I48" t="n">
+        <v>3157</v>
+      </c>
+      <c r="J48" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>3524</t>
         </is>
       </c>
     </row>
@@ -2207,9 +2499,15 @@
       <c r="H49" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>3048</t>
+      <c r="I49" t="n">
+        <v>3048</v>
+      </c>
+      <c r="J49" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>3087</t>
         </is>
       </c>
     </row>
@@ -2244,9 +2542,15 @@
       <c r="H50" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>3216</t>
+      <c r="I50" t="n">
+        <v>3216</v>
+      </c>
+      <c r="J50" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>3481</t>
         </is>
       </c>
     </row>
@@ -2281,9 +2585,15 @@
       <c r="H51" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>3110</t>
+      <c r="I51" t="n">
+        <v>3110</v>
+      </c>
+      <c r="J51" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>3464</t>
         </is>
       </c>
     </row>
@@ -2318,9 +2628,15 @@
       <c r="H52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>2513</t>
         </is>
       </c>
     </row>
@@ -2355,9 +2671,15 @@
       <c r="H53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>2839</t>
         </is>
       </c>
     </row>
@@ -2392,9 +2714,15 @@
       <c r="H54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>2539</t>
+      <c r="I54" t="n">
+        <v>2539</v>
+      </c>
+      <c r="J54" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>2571</t>
         </is>
       </c>
     </row>
@@ -2429,9 +2757,15 @@
       <c r="H55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>2808</t>
+      <c r="I55" t="n">
+        <v>2808</v>
+      </c>
+      <c r="J55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>2976</t>
         </is>
       </c>
     </row>
@@ -2466,9 +2800,15 @@
       <c r="H56" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>2929</t>
+      <c r="I56" t="n">
+        <v>2929</v>
+      </c>
+      <c r="J56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>3103</t>
         </is>
       </c>
     </row>
@@ -2503,9 +2843,15 @@
       <c r="H57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>3109</t>
+      <c r="I57" t="n">
+        <v>3109</v>
+      </c>
+      <c r="J57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>3360</t>
         </is>
       </c>
     </row>
@@ -2540,9 +2886,15 @@
       <c r="H58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>2880</t>
+      <c r="I58" t="n">
+        <v>2880</v>
+      </c>
+      <c r="J58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>2982</t>
         </is>
       </c>
     </row>
@@ -2577,9 +2929,15 @@
       <c r="H59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>3035</t>
+      <c r="I59" t="n">
+        <v>3035</v>
+      </c>
+      <c r="J59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>3332</t>
         </is>
       </c>
     </row>
@@ -2614,9 +2972,15 @@
       <c r="H60" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>3092</t>
+      <c r="I60" t="n">
+        <v>3092</v>
+      </c>
+      <c r="J60" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>3425</t>
         </is>
       </c>
     </row>
@@ -2651,9 +3015,15 @@
       <c r="H61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>3001</t>
+      <c r="I61" t="n">
+        <v>3001</v>
+      </c>
+      <c r="J61" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>3302</t>
         </is>
       </c>
     </row>
@@ -2688,9 +3058,15 @@
       <c r="H62" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>3098</t>
+      <c r="I62" t="n">
+        <v>3098</v>
+      </c>
+      <c r="J62" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>3331</t>
         </is>
       </c>
     </row>
@@ -2725,9 +3101,15 @@
       <c r="H63" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>2953</t>
+      <c r="I63" t="n">
+        <v>2953</v>
+      </c>
+      <c r="J63" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>3124</t>
         </is>
       </c>
     </row>
@@ -2762,7 +3144,13 @@
       <c r="H64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I64" t="inlineStr">
+      <c r="I64" t="n">
+        <v>2514</v>
+      </c>
+      <c r="J64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K64" t="inlineStr">
         <is>
           <t>2514</t>
         </is>
@@ -2799,9 +3187,15 @@
       <c r="H65" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>2931</t>
+      <c r="I65" t="n">
+        <v>2931</v>
+      </c>
+      <c r="J65" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>3068</t>
         </is>
       </c>
     </row>
@@ -2836,9 +3230,15 @@
       <c r="H66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="I66" t="n">
+        <v>2671</v>
+      </c>
+      <c r="J66" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>2897</t>
         </is>
       </c>
     </row>
@@ -2873,9 +3273,15 @@
       <c r="H67" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>3307</t>
+      <c r="I67" t="n">
+        <v>3307</v>
+      </c>
+      <c r="J67" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>3622</t>
         </is>
       </c>
     </row>
@@ -2910,9 +3316,15 @@
       <c r="H68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>2986</t>
+      <c r="I68" t="n">
+        <v>2986</v>
+      </c>
+      <c r="J68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>3128</t>
         </is>
       </c>
     </row>
@@ -2947,9 +3359,15 @@
       <c r="H69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>2536</t>
+      <c r="I69" t="n">
+        <v>2536</v>
+      </c>
+      <c r="J69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>2591</t>
         </is>
       </c>
     </row>
@@ -2984,9 +3402,15 @@
       <c r="H70" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>2781</t>
+      <c r="I70" t="n">
+        <v>2781</v>
+      </c>
+      <c r="J70" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>2830</t>
         </is>
       </c>
     </row>
@@ -3021,9 +3445,15 @@
       <c r="H71" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>3144</t>
+      <c r="I71" t="n">
+        <v>3144</v>
+      </c>
+      <c r="J71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>3492</t>
         </is>
       </c>
     </row>
@@ -3058,9 +3488,15 @@
       <c r="H72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>2973</t>
+      <c r="I72" t="n">
+        <v>2973</v>
+      </c>
+      <c r="J72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>3183</t>
         </is>
       </c>
     </row>
@@ -3095,9 +3531,15 @@
       <c r="H73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>3081</t>
+      <c r="I73" t="n">
+        <v>3081</v>
+      </c>
+      <c r="J73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>3345</t>
         </is>
       </c>
     </row>
@@ -3132,9 +3574,15 @@
       <c r="H74" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>2970</t>
+      <c r="I74" t="n">
+        <v>2970</v>
+      </c>
+      <c r="J74" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>3195</t>
         </is>
       </c>
     </row>
@@ -3169,9 +3617,15 @@
       <c r="H75" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>3073</t>
+      <c r="I75" t="n">
+        <v>3073</v>
+      </c>
+      <c r="J75" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>3306</t>
         </is>
       </c>
     </row>
@@ -3206,9 +3660,15 @@
       <c r="H76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>2909</t>
+      <c r="I76" t="n">
+        <v>2909</v>
+      </c>
+      <c r="J76" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>3153</t>
         </is>
       </c>
     </row>
@@ -3243,9 +3703,15 @@
       <c r="H77" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>2604</t>
+      <c r="I77" t="n">
+        <v>2604</v>
+      </c>
+      <c r="J77" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>2665</t>
         </is>
       </c>
     </row>
@@ -3280,9 +3746,15 @@
       <c r="H78" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>2946</t>
+      <c r="I78" t="n">
+        <v>2946</v>
+      </c>
+      <c r="J78" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>3125</t>
         </is>
       </c>
     </row>
@@ -3317,9 +3789,15 @@
       <c r="H79" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>2856</t>
+      <c r="I79" t="n">
+        <v>2856</v>
+      </c>
+      <c r="J79" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>3076</t>
         </is>
       </c>
     </row>
@@ -3354,9 +3832,15 @@
       <c r="H80" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>2801</t>
+      <c r="I80" t="n">
+        <v>2801</v>
+      </c>
+      <c r="J80" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>2939</t>
         </is>
       </c>
     </row>
@@ -3391,9 +3875,15 @@
       <c r="H81" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>2562</t>
+      <c r="I81" t="n">
+        <v>2562</v>
+      </c>
+      <c r="J81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>2606</t>
         </is>
       </c>
     </row>
@@ -3428,9 +3918,15 @@
       <c r="H82" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>3065</t>
+      <c r="I82" t="n">
+        <v>3065</v>
+      </c>
+      <c r="J82" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>3321</t>
         </is>
       </c>
     </row>
@@ -3465,9 +3961,15 @@
       <c r="H83" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>2598</t>
+      <c r="I83" t="n">
+        <v>2598</v>
+      </c>
+      <c r="J83" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>2641</t>
         </is>
       </c>
     </row>
@@ -3502,9 +4004,15 @@
       <c r="H84" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>2690</t>
+      <c r="I84" t="n">
+        <v>2690</v>
+      </c>
+      <c r="J84" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>2796</t>
         </is>
       </c>
     </row>
@@ -3539,9 +4047,15 @@
       <c r="H85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>1997</t>
+      <c r="I85" t="n">
+        <v>1997</v>
+      </c>
+      <c r="J85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>1993</t>
         </is>
       </c>
     </row>
@@ -3576,9 +4090,15 @@
       <c r="H86" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>2492</t>
+      <c r="I86" t="n">
+        <v>2492</v>
+      </c>
+      <c r="J86" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>2512</t>
         </is>
       </c>
     </row>
@@ -3613,9 +4133,15 @@
       <c r="H87" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>2566</t>
+      <c r="I87" t="n">
+        <v>2566</v>
+      </c>
+      <c r="J87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>2731</t>
         </is>
       </c>
     </row>
@@ -3650,9 +4176,15 @@
       <c r="H88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
+      <c r="J88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>1993</t>
         </is>
       </c>
     </row>
@@ -3687,7 +4219,13 @@
       <c r="H89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I89" t="inlineStr">
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
+      <c r="J89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3724,7 +4262,13 @@
       <c r="H90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I90" t="inlineStr">
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3761,9 +4305,15 @@
       <c r="H91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>2462</t>
+      <c r="I91" t="n">
+        <v>2462</v>
+      </c>
+      <c r="J91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>2470</t>
         </is>
       </c>
     </row>
@@ -3798,9 +4348,15 @@
       <c r="H92" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>2729</t>
+      <c r="I92" t="n">
+        <v>2729</v>
+      </c>
+      <c r="J92" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>2857</t>
         </is>
       </c>
     </row>
@@ -3835,9 +4391,15 @@
       <c r="H93" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>2497</t>
+      <c r="I93" t="n">
+        <v>2497</v>
+      </c>
+      <c r="J93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -3872,9 +4434,15 @@
       <c r="H94" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>2997</t>
+      <c r="I94" t="n">
+        <v>2997</v>
+      </c>
+      <c r="J94" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>3272</t>
         </is>
       </c>
     </row>
@@ -3909,9 +4477,15 @@
       <c r="H95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>2844</t>
+      <c r="I95" t="n">
+        <v>2844</v>
+      </c>
+      <c r="J95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>3020</t>
         </is>
       </c>
     </row>
@@ -3946,9 +4520,15 @@
       <c r="H96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>2583</t>
+      <c r="I96" t="n">
+        <v>2583</v>
+      </c>
+      <c r="J96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>2561</t>
         </is>
       </c>
     </row>
@@ -3983,9 +4563,15 @@
       <c r="H97" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>3026</t>
+      <c r="I97" t="n">
+        <v>3026</v>
+      </c>
+      <c r="J97" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>3219</t>
         </is>
       </c>
     </row>
@@ -4020,9 +4606,15 @@
       <c r="H98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>2780</t>
+      <c r="I98" t="n">
+        <v>2780</v>
+      </c>
+      <c r="J98" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>3008</t>
         </is>
       </c>
     </row>
@@ -4057,9 +4649,15 @@
       <c r="H99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>2488</t>
         </is>
       </c>
     </row>
@@ -4094,9 +4692,15 @@
       <c r="H100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>2471</t>
+      <c r="I100" t="n">
+        <v>2471</v>
+      </c>
+      <c r="J100" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>2591</t>
         </is>
       </c>
     </row>
@@ -4131,9 +4735,15 @@
       <c r="H101" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>3013</t>
+      <c r="I101" t="n">
+        <v>3013</v>
+      </c>
+      <c r="J101" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>3298</t>
         </is>
       </c>
     </row>
@@ -4168,9 +4778,15 @@
       <c r="H102" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>2641</t>
+      <c r="I102" t="n">
+        <v>2641</v>
+      </c>
+      <c r="J102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>2795</t>
         </is>
       </c>
     </row>
@@ -4205,9 +4821,15 @@
       <c r="H103" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>2673</t>
+      <c r="I103" t="n">
+        <v>2673</v>
+      </c>
+      <c r="J103" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>2815</t>
         </is>
       </c>
     </row>
@@ -4242,9 +4864,15 @@
       <c r="H104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>2493</t>
+      <c r="I104" t="n">
+        <v>2493</v>
+      </c>
+      <c r="J104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>2470</t>
         </is>
       </c>
     </row>
@@ -4279,9 +4907,15 @@
       <c r="H105" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>2792</t>
+      <c r="I105" t="n">
+        <v>2792</v>
+      </c>
+      <c r="J105" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>2844</t>
         </is>
       </c>
     </row>
@@ -4316,9 +4950,15 @@
       <c r="H106" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>2680</t>
+      <c r="I106" t="n">
+        <v>2680</v>
+      </c>
+      <c r="J106" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>2810</t>
         </is>
       </c>
     </row>
@@ -4353,9 +4993,15 @@
       <c r="H107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>2597</t>
+      <c r="I107" t="n">
+        <v>2597</v>
+      </c>
+      <c r="J107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>2671</t>
         </is>
       </c>
     </row>
@@ -4390,9 +5036,15 @@
       <c r="H108" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>2466</t>
+      <c r="I108" t="n">
+        <v>2466</v>
+      </c>
+      <c r="J108" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>2443</t>
         </is>
       </c>
     </row>
@@ -4427,9 +5079,15 @@
       <c r="H109" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>2475</t>
+      <c r="I109" t="n">
+        <v>2475</v>
+      </c>
+      <c r="J109" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>2490</t>
         </is>
       </c>
     </row>
@@ -4464,9 +5122,15 @@
       <c r="H110" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="I110" t="inlineStr">
-        <is>
-          <t>2754</t>
+      <c r="I110" t="n">
+        <v>2754</v>
+      </c>
+      <c r="J110" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>2890</t>
         </is>
       </c>
     </row>
@@ -4501,9 +5165,15 @@
       <c r="H111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I111" t="n">
+        <v>0</v>
+      </c>
+      <c r="J111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>2631</t>
         </is>
       </c>
     </row>
@@ -4538,9 +5208,15 @@
       <c r="H112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="I112" t="n">
+        <v>2671</v>
+      </c>
+      <c r="J112" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>2728</t>
         </is>
       </c>
     </row>
@@ -4575,9 +5251,15 @@
       <c r="H113" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>2603</t>
+      <c r="I113" t="n">
+        <v>2603</v>
+      </c>
+      <c r="J113" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>2639</t>
         </is>
       </c>
     </row>
@@ -4612,9 +5294,15 @@
       <c r="H114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I114" t="inlineStr">
-        <is>
-          <t>2540</t>
+      <c r="I114" t="n">
+        <v>2540</v>
+      </c>
+      <c r="J114" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>2804</t>
         </is>
       </c>
     </row>
@@ -4649,9 +5337,15 @@
       <c r="H115" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>2485</t>
+      <c r="I115" t="n">
+        <v>2485</v>
+      </c>
+      <c r="J115" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>2542</t>
         </is>
       </c>
     </row>
@@ -4686,9 +5380,15 @@
       <c r="H116" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>2607</t>
+      <c r="I116" t="n">
+        <v>2607</v>
+      </c>
+      <c r="J116" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>2670</t>
         </is>
       </c>
     </row>
@@ -4723,9 +5423,15 @@
       <c r="H117" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>2621</t>
+      <c r="I117" t="n">
+        <v>2621</v>
+      </c>
+      <c r="J117" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>2677</t>
         </is>
       </c>
     </row>
@@ -4760,7 +5466,13 @@
       <c r="H118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I118" t="inlineStr">
+      <c r="I118" t="n">
+        <v>0</v>
+      </c>
+      <c r="J118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4797,9 +5509,15 @@
       <c r="H119" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I119" t="inlineStr">
-        <is>
-          <t>2681</t>
+      <c r="I119" t="n">
+        <v>2681</v>
+      </c>
+      <c r="J119" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>2748</t>
         </is>
       </c>
     </row>
@@ -4834,9 +5552,15 @@
       <c r="H120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I120" t="n">
+        <v>0</v>
+      </c>
+      <c r="J120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>2713</t>
         </is>
       </c>
     </row>
@@ -4871,9 +5595,15 @@
       <c r="H121" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>2053</t>
+      <c r="I121" t="n">
+        <v>2053</v>
+      </c>
+      <c r="J121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>2046</t>
         </is>
       </c>
     </row>
@@ -4908,9 +5638,15 @@
       <c r="H122" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="I122" t="inlineStr">
-        <is>
-          <t>2488</t>
+      <c r="I122" t="n">
+        <v>2488</v>
+      </c>
+      <c r="J122" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>2436</t>
         </is>
       </c>
     </row>
@@ -4945,9 +5681,15 @@
       <c r="H123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>2514</t>
+      <c r="I123" t="n">
+        <v>2514</v>
+      </c>
+      <c r="J123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>2487</t>
         </is>
       </c>
     </row>
@@ -4982,9 +5724,15 @@
       <c r="H124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>2648</t>
+      <c r="I124" t="n">
+        <v>2648</v>
+      </c>
+      <c r="J124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>2803</t>
         </is>
       </c>
     </row>
@@ -5019,7 +5767,13 @@
       <c r="H125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I125" t="inlineStr">
+      <c r="I125" t="n">
+        <v>0</v>
+      </c>
+      <c r="J125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5056,9 +5810,15 @@
       <c r="H126" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="I126" t="inlineStr">
-        <is>
-          <t>2488</t>
+      <c r="I126" t="n">
+        <v>2488</v>
+      </c>
+      <c r="J126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>2630</t>
         </is>
       </c>
     </row>
@@ -5093,9 +5853,15 @@
       <c r="H127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I127" t="n">
+        <v>0</v>
+      </c>
+      <c r="J127" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -5130,9 +5896,15 @@
       <c r="H128" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="I128" t="inlineStr">
-        <is>
-          <t>2466</t>
+      <c r="I128" t="n">
+        <v>2466</v>
+      </c>
+      <c r="J128" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>2463</t>
         </is>
       </c>
     </row>
@@ -5167,9 +5939,15 @@
       <c r="H129" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I129" t="inlineStr">
-        <is>
-          <t>2073</t>
+      <c r="I129" t="n">
+        <v>2073</v>
+      </c>
+      <c r="J129" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>2117</t>
         </is>
       </c>
     </row>
@@ -5204,7 +5982,13 @@
       <c r="H130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I130" t="inlineStr">
+      <c r="I130" t="n">
+        <v>0</v>
+      </c>
+      <c r="J130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5241,7 +6025,13 @@
       <c r="H131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I131" t="inlineStr">
+      <c r="I131" t="n">
+        <v>0</v>
+      </c>
+      <c r="J131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5278,9 +6068,15 @@
       <c r="H132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I132" t="inlineStr">
-        <is>
-          <t>1498</t>
+      <c r="I132" t="n">
+        <v>1498</v>
+      </c>
+      <c r="J132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5315,7 +6111,13 @@
       <c r="H133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I133" t="inlineStr">
+      <c r="I133" t="n">
+        <v>0</v>
+      </c>
+      <c r="J133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5352,9 +6154,15 @@
       <c r="H134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I134" t="inlineStr">
-        <is>
-          <t>1988</t>
+      <c r="I134" t="n">
+        <v>1988</v>
+      </c>
+      <c r="J134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>1958</t>
         </is>
       </c>
     </row>
@@ -5389,9 +6197,15 @@
       <c r="H135" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I135" t="inlineStr">
-        <is>
-          <t>2062</t>
+      <c r="I135" t="n">
+        <v>2062</v>
+      </c>
+      <c r="J135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>2042</t>
         </is>
       </c>
     </row>
@@ -5426,9 +6240,15 @@
       <c r="H136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I136" t="inlineStr">
-        <is>
-          <t>1500</t>
+      <c r="I136" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5463,7 +6283,13 @@
       <c r="H137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I137" t="inlineStr">
+      <c r="I137" t="n">
+        <v>0</v>
+      </c>
+      <c r="J137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5500,7 +6326,13 @@
       <c r="H138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I138" t="inlineStr">
+      <c r="I138" t="n">
+        <v>0</v>
+      </c>
+      <c r="J138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5537,7 +6369,13 @@
       <c r="H139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I139" t="inlineStr">
+      <c r="I139" t="n">
+        <v>0</v>
+      </c>
+      <c r="J139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5574,9 +6412,15 @@
       <c r="H140" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I140" t="inlineStr">
-        <is>
-          <t>2542</t>
+      <c r="I140" t="n">
+        <v>2542</v>
+      </c>
+      <c r="J140" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>3003</t>
         </is>
       </c>
     </row>
@@ -5611,7 +6455,13 @@
       <c r="H141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I141" t="inlineStr">
+      <c r="I141" t="n">
+        <v>0</v>
+      </c>
+      <c r="J141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5648,7 +6498,13 @@
       <c r="H142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I142" t="inlineStr">
+      <c r="I142" t="n">
+        <v>0</v>
+      </c>
+      <c r="J142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5685,9 +6541,15 @@
       <c r="H143" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I143" t="inlineStr">
-        <is>
-          <t>3062</t>
+      <c r="I143" t="n">
+        <v>3062</v>
+      </c>
+      <c r="J143" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>3323</t>
         </is>
       </c>
     </row>
@@ -5722,7 +6584,13 @@
       <c r="H144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I144" t="inlineStr">
+      <c r="I144" t="n">
+        <v>0</v>
+      </c>
+      <c r="J144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5759,9 +6627,15 @@
       <c r="H145" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="I145" t="inlineStr">
-        <is>
-          <t>2507</t>
+      <c r="I145" t="n">
+        <v>2507</v>
+      </c>
+      <c r="J145" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>2618</t>
         </is>
       </c>
     </row>
@@ -5796,7 +6670,13 @@
       <c r="H146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I146" t="inlineStr">
+      <c r="I146" t="n">
+        <v>0</v>
+      </c>
+      <c r="J146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5833,7 +6713,13 @@
       <c r="H147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I147" t="inlineStr">
+      <c r="I147" t="n">
+        <v>0</v>
+      </c>
+      <c r="J147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5864,11 +6750,11 @@
       <c r="H148" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I148" t="inlineStr">
-        <is>
-          <t>2519</t>
-        </is>
-      </c>
+      <c r="I148" t="n">
+        <v>2519</v>
+      </c>
+      <c r="J148" s="3" t="inlineStr"/>
+      <c r="K148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -5895,9 +6781,15 @@
       <c r="H149" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I149" t="inlineStr">
-        <is>
-          <t>1329</t>
+      <c r="I149" t="n">
+        <v>1329</v>
+      </c>
+      <c r="J149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>1321</t>
         </is>
       </c>
     </row>
@@ -5926,9 +6818,15 @@
       <c r="H150" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I150" t="inlineStr">
-        <is>
-          <t>1379</t>
+      <c r="I150" t="n">
+        <v>1379</v>
+      </c>
+      <c r="J150" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>1384</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-06 09:42:06
</commit_message>
<xml_diff>
--- a/Season_Attack/81.xlsx
+++ b/Season_Attack/81.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K150"/>
+  <dimension ref="A1:M152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,16 @@
           <t>01-03_0</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>01-05_A</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>01-05_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -484,9 +494,15 @@
       <c r="J2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2999</t>
+      <c r="K2" t="n">
+        <v>2999</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>3198</t>
         </is>
       </c>
     </row>
@@ -527,9 +543,15 @@
       <c r="J3" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>3368</t>
+      <c r="K3" t="n">
+        <v>3368</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>3575</t>
         </is>
       </c>
     </row>
@@ -570,9 +592,15 @@
       <c r="J4" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>3597</t>
+      <c r="K4" t="n">
+        <v>3597</v>
+      </c>
+      <c r="L4" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>3906</t>
         </is>
       </c>
     </row>
@@ -613,9 +641,15 @@
       <c r="J5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>3439</t>
+      <c r="K5" t="n">
+        <v>3439</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>3734</t>
         </is>
       </c>
     </row>
@@ -656,9 +690,15 @@
       <c r="J6" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>3537</t>
+      <c r="K6" t="n">
+        <v>3537</v>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>3803</t>
         </is>
       </c>
     </row>
@@ -681,7 +721,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F7" s="3" t="n">
@@ -699,9 +739,15 @@
       <c r="J7" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>3729</t>
+      <c r="K7" t="n">
+        <v>3729</v>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>4086</t>
         </is>
       </c>
     </row>
@@ -742,9 +788,15 @@
       <c r="J8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>3390</t>
+      <c r="K8" t="n">
+        <v>3390</v>
+      </c>
+      <c r="L8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>3626</t>
         </is>
       </c>
     </row>
@@ -785,9 +837,15 @@
       <c r="J9" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>3523</t>
+      <c r="K9" t="n">
+        <v>3523</v>
+      </c>
+      <c r="L9" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>3859</t>
         </is>
       </c>
     </row>
@@ -810,7 +868,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F10" s="3" t="n">
@@ -828,9 +886,15 @@
       <c r="J10" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>3309</t>
+      <c r="K10" t="n">
+        <v>3309</v>
+      </c>
+      <c r="L10" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>3507</t>
         </is>
       </c>
     </row>
@@ -853,7 +917,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F11" s="3" t="n">
@@ -871,9 +935,15 @@
       <c r="J11" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>3025</t>
+      <c r="K11" t="n">
+        <v>3025</v>
+      </c>
+      <c r="L11" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>3098</t>
         </is>
       </c>
     </row>
@@ -896,7 +966,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F12" s="3" t="n">
@@ -914,9 +984,15 @@
       <c r="J12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>3318</t>
+      <c r="K12" t="n">
+        <v>3318</v>
+      </c>
+      <c r="L12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>3531</t>
         </is>
       </c>
     </row>
@@ -957,9 +1033,15 @@
       <c r="J13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>2586</t>
+      <c r="K13" t="n">
+        <v>2586</v>
+      </c>
+      <c r="L13" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>2684</t>
         </is>
       </c>
     </row>
@@ -982,7 +1064,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F14" s="4" t="n">
@@ -1000,9 +1082,15 @@
       <c r="J14" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>3811</t>
+      <c r="K14" t="n">
+        <v>3811</v>
+      </c>
+      <c r="L14" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>3993</t>
         </is>
       </c>
     </row>
@@ -1043,9 +1131,15 @@
       <c r="J15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>3476</t>
+      <c r="K15" t="n">
+        <v>3476</v>
+      </c>
+      <c r="L15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>3750</t>
         </is>
       </c>
     </row>
@@ -1086,9 +1180,15 @@
       <c r="J16" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>3571</t>
+      <c r="K16" t="n">
+        <v>3571</v>
+      </c>
+      <c r="L16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>3783</t>
         </is>
       </c>
     </row>
@@ -1129,9 +1229,15 @@
       <c r="J17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>3585</t>
+      <c r="K17" t="n">
+        <v>3585</v>
+      </c>
+      <c r="L17" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>3817</t>
         </is>
       </c>
     </row>
@@ -1154,7 +1260,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F18" s="3" t="n">
@@ -1172,9 +1278,15 @@
       <c r="J18" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>3401</t>
+      <c r="K18" t="n">
+        <v>3401</v>
+      </c>
+      <c r="L18" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>3639</t>
         </is>
       </c>
     </row>
@@ -1215,9 +1327,15 @@
       <c r="J19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>3644</t>
+      <c r="K19" t="n">
+        <v>3644</v>
+      </c>
+      <c r="L19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>3889</t>
         </is>
       </c>
     </row>
@@ -1240,7 +1358,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F20" s="4" t="n">
@@ -1258,9 +1376,15 @@
       <c r="J20" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>3623</t>
+      <c r="K20" t="n">
+        <v>3623</v>
+      </c>
+      <c r="L20" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>3945</t>
         </is>
       </c>
     </row>
@@ -1283,7 +1407,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F21" s="2" t="n">
@@ -1301,7 +1425,13 @@
       <c r="J21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K21" t="inlineStr">
+      <c r="K21" t="n">
+        <v>3073</v>
+      </c>
+      <c r="L21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="inlineStr">
         <is>
           <t>3073</t>
         </is>
@@ -1326,7 +1456,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F22" s="4" t="n">
@@ -1344,9 +1474,15 @@
       <c r="J22" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>3520</t>
+      <c r="K22" t="n">
+        <v>3520</v>
+      </c>
+      <c r="L22" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>3839</t>
         </is>
       </c>
     </row>
@@ -1387,9 +1523,15 @@
       <c r="J23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>2785</t>
+      <c r="K23" t="n">
+        <v>2785</v>
+      </c>
+      <c r="L23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>2873</t>
         </is>
       </c>
     </row>
@@ -1412,7 +1554,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F24" s="4" t="n">
@@ -1430,9 +1572,15 @@
       <c r="J24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>3587</t>
+      <c r="K24" t="n">
+        <v>3587</v>
+      </c>
+      <c r="L24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>3816</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1621,13 @@
       <c r="J25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="K25" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1498,7 +1652,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F26" s="3" t="n">
@@ -1516,9 +1670,15 @@
       <c r="J26" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>3621</t>
+      <c r="K26" t="n">
+        <v>3621</v>
+      </c>
+      <c r="L26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>3900</t>
         </is>
       </c>
     </row>
@@ -1559,9 +1719,15 @@
       <c r="J27" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>3750</t>
+      <c r="K27" t="n">
+        <v>3750</v>
+      </c>
+      <c r="L27" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>3868</t>
         </is>
       </c>
     </row>
@@ -1602,9 +1768,15 @@
       <c r="J28" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>3173</t>
+      <c r="K28" t="n">
+        <v>3173</v>
+      </c>
+      <c r="L28" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>3374</t>
         </is>
       </c>
     </row>
@@ -1645,9 +1817,15 @@
       <c r="J29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>3236</t>
+      <c r="K29" t="n">
+        <v>3236</v>
+      </c>
+      <c r="L29" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>3389</t>
         </is>
       </c>
     </row>
@@ -1670,7 +1848,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F30" s="4" t="n">
@@ -1688,9 +1866,15 @@
       <c r="J30" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>3758</t>
+      <c r="K30" t="n">
+        <v>3758</v>
+      </c>
+      <c r="L30" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>4002</t>
         </is>
       </c>
     </row>
@@ -1731,9 +1915,15 @@
       <c r="J31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>3406</t>
+      <c r="K31" t="n">
+        <v>3406</v>
+      </c>
+      <c r="L31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>3646</t>
         </is>
       </c>
     </row>
@@ -1774,9 +1964,15 @@
       <c r="J32" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>3800</t>
+      <c r="K32" t="n">
+        <v>3800</v>
+      </c>
+      <c r="L32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>4024</t>
         </is>
       </c>
     </row>
@@ -1817,9 +2013,15 @@
       <c r="J33" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>3623</t>
+      <c r="K33" t="n">
+        <v>3623</v>
+      </c>
+      <c r="L33" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>4134</t>
         </is>
       </c>
     </row>
@@ -1860,9 +2062,15 @@
       <c r="J34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>2506</t>
+      <c r="K34" t="n">
+        <v>2506</v>
+      </c>
+      <c r="L34" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>2765</t>
         </is>
       </c>
     </row>
@@ -1885,7 +2093,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F35" s="3" t="n">
@@ -1903,9 +2111,15 @@
       <c r="J35" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>3553</t>
+      <c r="K35" t="n">
+        <v>3553</v>
+      </c>
+      <c r="L35" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>4011</t>
         </is>
       </c>
     </row>
@@ -1946,9 +2160,15 @@
       <c r="J36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>3251</t>
+      <c r="K36" t="n">
+        <v>3251</v>
+      </c>
+      <c r="L36" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>3388</t>
         </is>
       </c>
     </row>
@@ -1971,7 +2191,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F37" s="3" t="n">
@@ -1989,9 +2209,15 @@
       <c r="J37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>3455</t>
+      <c r="K37" t="n">
+        <v>3455</v>
+      </c>
+      <c r="L37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>3696</t>
         </is>
       </c>
     </row>
@@ -2014,7 +2240,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F38" s="3" t="n">
@@ -2032,9 +2258,15 @@
       <c r="J38" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>3701</t>
+      <c r="K38" t="n">
+        <v>3701</v>
+      </c>
+      <c r="L38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>3966</t>
         </is>
       </c>
     </row>
@@ -2075,9 +2307,15 @@
       <c r="J39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>3649</t>
+      <c r="K39" t="n">
+        <v>3649</v>
+      </c>
+      <c r="L39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>3860</t>
         </is>
       </c>
     </row>
@@ -2118,9 +2356,15 @@
       <c r="J40" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>3562</t>
+      <c r="K40" t="n">
+        <v>3562</v>
+      </c>
+      <c r="L40" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>3871</t>
         </is>
       </c>
     </row>
@@ -2161,9 +2405,15 @@
       <c r="J41" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>3477</t>
+      <c r="K41" t="n">
+        <v>3477</v>
+      </c>
+      <c r="L41" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>3900</t>
         </is>
       </c>
     </row>
@@ -2186,7 +2436,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F42" s="4" t="n">
@@ -2204,9 +2454,15 @@
       <c r="J42" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>3724</t>
+      <c r="K42" t="n">
+        <v>3724</v>
+      </c>
+      <c r="L42" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>4149</t>
         </is>
       </c>
     </row>
@@ -2229,7 +2485,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F43" s="4" t="n">
@@ -2247,9 +2503,15 @@
       <c r="J43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>3677</t>
+      <c r="K43" t="n">
+        <v>3677</v>
+      </c>
+      <c r="L43" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>3722</t>
         </is>
       </c>
     </row>
@@ -2290,9 +2552,15 @@
       <c r="J44" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>2833</t>
+      <c r="K44" t="n">
+        <v>2833</v>
+      </c>
+      <c r="L44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>2844</t>
         </is>
       </c>
     </row>
@@ -2315,7 +2583,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F45" s="4" t="n">
@@ -2333,9 +2601,15 @@
       <c r="J45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>3428</t>
+      <c r="K45" t="n">
+        <v>3428</v>
+      </c>
+      <c r="L45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>3680</t>
         </is>
       </c>
     </row>
@@ -2358,7 +2632,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F46" s="3" t="n">
@@ -2376,9 +2650,15 @@
       <c r="J46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>3398</t>
+      <c r="K46" t="n">
+        <v>3398</v>
+      </c>
+      <c r="L46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>3597</t>
         </is>
       </c>
     </row>
@@ -2419,9 +2699,15 @@
       <c r="J47" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>3473</t>
+      <c r="K47" t="n">
+        <v>3473</v>
+      </c>
+      <c r="L47" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>3734</t>
         </is>
       </c>
     </row>
@@ -2462,9 +2748,15 @@
       <c r="J48" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>3524</t>
+      <c r="K48" t="n">
+        <v>3524</v>
+      </c>
+      <c r="L48" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>3754</t>
         </is>
       </c>
     </row>
@@ -2487,7 +2779,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F49" s="4" t="n">
@@ -2505,9 +2797,15 @@
       <c r="J49" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>3087</t>
+      <c r="K49" t="n">
+        <v>3087</v>
+      </c>
+      <c r="L49" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>3270</t>
         </is>
       </c>
     </row>
@@ -2548,9 +2846,15 @@
       <c r="J50" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>3481</t>
+      <c r="K50" t="n">
+        <v>3481</v>
+      </c>
+      <c r="L50" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>3744</t>
         </is>
       </c>
     </row>
@@ -2591,9 +2895,15 @@
       <c r="J51" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>3464</t>
+      <c r="K51" t="n">
+        <v>3464</v>
+      </c>
+      <c r="L51" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>3667</t>
         </is>
       </c>
     </row>
@@ -2634,9 +2944,15 @@
       <c r="J52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>2513</t>
+      <c r="K52" t="n">
+        <v>2513</v>
+      </c>
+      <c r="L52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>2550</t>
         </is>
       </c>
     </row>
@@ -2677,9 +2993,15 @@
       <c r="J53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>2839</t>
+      <c r="K53" t="n">
+        <v>2839</v>
+      </c>
+      <c r="L53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>2852</t>
         </is>
       </c>
     </row>
@@ -2720,9 +3042,15 @@
       <c r="J54" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>2571</t>
+      <c r="K54" t="n">
+        <v>2571</v>
+      </c>
+      <c r="L54" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>2660</t>
         </is>
       </c>
     </row>
@@ -2763,9 +3091,15 @@
       <c r="J55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>2976</t>
+      <c r="K55" t="n">
+        <v>2976</v>
+      </c>
+      <c r="L55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>3156</t>
         </is>
       </c>
     </row>
@@ -2806,9 +3140,15 @@
       <c r="J56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>3103</t>
+      <c r="K56" t="n">
+        <v>3103</v>
+      </c>
+      <c r="L56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>3371</t>
         </is>
       </c>
     </row>
@@ -2849,9 +3189,15 @@
       <c r="J57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>3360</t>
+      <c r="K57" t="n">
+        <v>3360</v>
+      </c>
+      <c r="L57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>3643</t>
         </is>
       </c>
     </row>
@@ -2892,9 +3238,15 @@
       <c r="J58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>2982</t>
+      <c r="K58" t="n">
+        <v>2982</v>
+      </c>
+      <c r="L58" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>3205</t>
         </is>
       </c>
     </row>
@@ -2935,9 +3287,15 @@
       <c r="J59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>3332</t>
+      <c r="K59" t="n">
+        <v>3332</v>
+      </c>
+      <c r="L59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>3551</t>
         </is>
       </c>
     </row>
@@ -2978,9 +3336,15 @@
       <c r="J60" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>3425</t>
+      <c r="K60" t="n">
+        <v>3425</v>
+      </c>
+      <c r="L60" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>3755</t>
         </is>
       </c>
     </row>
@@ -3021,9 +3385,15 @@
       <c r="J61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>3302</t>
+      <c r="K61" t="n">
+        <v>3302</v>
+      </c>
+      <c r="L61" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>3569</t>
         </is>
       </c>
     </row>
@@ -3064,9 +3434,15 @@
       <c r="J62" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>3331</t>
+      <c r="K62" t="n">
+        <v>3331</v>
+      </c>
+      <c r="L62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>3700</t>
         </is>
       </c>
     </row>
@@ -3107,9 +3483,15 @@
       <c r="J63" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>3124</t>
+      <c r="K63" t="n">
+        <v>3124</v>
+      </c>
+      <c r="L63" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>3253</t>
         </is>
       </c>
     </row>
@@ -3150,7 +3532,13 @@
       <c r="J64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K64" t="inlineStr">
+      <c r="K64" t="n">
+        <v>2514</v>
+      </c>
+      <c r="L64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M64" t="inlineStr">
         <is>
           <t>2514</t>
         </is>
@@ -3193,9 +3581,15 @@
       <c r="J65" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>3068</t>
+      <c r="K65" t="n">
+        <v>3068</v>
+      </c>
+      <c r="L65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>3144</t>
         </is>
       </c>
     </row>
@@ -3236,9 +3630,15 @@
       <c r="J66" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>2897</t>
+      <c r="K66" t="n">
+        <v>2897</v>
+      </c>
+      <c r="L66" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>3138</t>
         </is>
       </c>
     </row>
@@ -3279,9 +3679,15 @@
       <c r="J67" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>3622</t>
+      <c r="K67" t="n">
+        <v>3622</v>
+      </c>
+      <c r="L67" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>3753</t>
         </is>
       </c>
     </row>
@@ -3322,9 +3728,15 @@
       <c r="J68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>3128</t>
+      <c r="K68" t="n">
+        <v>3128</v>
+      </c>
+      <c r="L68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>3322</t>
         </is>
       </c>
     </row>
@@ -3365,9 +3777,15 @@
       <c r="J69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>2591</t>
+      <c r="K69" t="n">
+        <v>2591</v>
+      </c>
+      <c r="L69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>2585</t>
         </is>
       </c>
     </row>
@@ -3408,9 +3826,15 @@
       <c r="J70" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>2830</t>
+      <c r="K70" t="n">
+        <v>2830</v>
+      </c>
+      <c r="L70" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>2927</t>
         </is>
       </c>
     </row>
@@ -3451,9 +3875,15 @@
       <c r="J71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>3492</t>
+      <c r="K71" t="n">
+        <v>3492</v>
+      </c>
+      <c r="L71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>3923</t>
         </is>
       </c>
     </row>
@@ -3494,9 +3924,15 @@
       <c r="J72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>3183</t>
+      <c r="K72" t="n">
+        <v>3183</v>
+      </c>
+      <c r="L72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>3357</t>
         </is>
       </c>
     </row>
@@ -3537,9 +3973,15 @@
       <c r="J73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>3345</t>
+      <c r="K73" t="n">
+        <v>3345</v>
+      </c>
+      <c r="L73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>3607</t>
         </is>
       </c>
     </row>
@@ -3580,9 +4022,15 @@
       <c r="J74" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>3195</t>
+      <c r="K74" t="n">
+        <v>3195</v>
+      </c>
+      <c r="L74" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>3290</t>
         </is>
       </c>
     </row>
@@ -3623,9 +4071,15 @@
       <c r="J75" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>3306</t>
+      <c r="K75" t="n">
+        <v>3306</v>
+      </c>
+      <c r="L75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>3593</t>
         </is>
       </c>
     </row>
@@ -3666,9 +4120,15 @@
       <c r="J76" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>3153</t>
+      <c r="K76" t="n">
+        <v>3153</v>
+      </c>
+      <c r="L76" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>3369</t>
         </is>
       </c>
     </row>
@@ -3709,9 +4169,15 @@
       <c r="J77" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>2665</t>
+      <c r="K77" t="n">
+        <v>2665</v>
+      </c>
+      <c r="L77" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>2783</t>
         </is>
       </c>
     </row>
@@ -3752,9 +4218,15 @@
       <c r="J78" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>3125</t>
+      <c r="K78" t="n">
+        <v>3125</v>
+      </c>
+      <c r="L78" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>3285</t>
         </is>
       </c>
     </row>
@@ -3795,9 +4267,15 @@
       <c r="J79" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>3076</t>
+      <c r="K79" t="n">
+        <v>3076</v>
+      </c>
+      <c r="L79" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>3315</t>
         </is>
       </c>
     </row>
@@ -3838,9 +4316,15 @@
       <c r="J80" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>2939</t>
+      <c r="K80" t="n">
+        <v>2939</v>
+      </c>
+      <c r="L80" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>3002</t>
         </is>
       </c>
     </row>
@@ -3881,9 +4365,15 @@
       <c r="J81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>2606</t>
+      <c r="K81" t="n">
+        <v>2606</v>
+      </c>
+      <c r="L81" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>2666</t>
         </is>
       </c>
     </row>
@@ -3924,9 +4414,15 @@
       <c r="J82" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>3321</t>
+      <c r="K82" t="n">
+        <v>3321</v>
+      </c>
+      <c r="L82" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>3451</t>
         </is>
       </c>
     </row>
@@ -3967,9 +4463,15 @@
       <c r="J83" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>2641</t>
+      <c r="K83" t="n">
+        <v>2641</v>
+      </c>
+      <c r="L83" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>2712</t>
         </is>
       </c>
     </row>
@@ -4010,9 +4512,15 @@
       <c r="J84" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>2796</t>
+      <c r="K84" t="n">
+        <v>2796</v>
+      </c>
+      <c r="L84" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>2912</t>
         </is>
       </c>
     </row>
@@ -4053,9 +4561,15 @@
       <c r="J85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>1993</t>
+      <c r="K85" t="n">
+        <v>1993</v>
+      </c>
+      <c r="L85" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>2016</t>
         </is>
       </c>
     </row>
@@ -4096,9 +4610,15 @@
       <c r="J86" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>2512</t>
+      <c r="K86" t="n">
+        <v>2512</v>
+      </c>
+      <c r="L86" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>2629</t>
         </is>
       </c>
     </row>
@@ -4139,9 +4659,15 @@
       <c r="J87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>2731</t>
+      <c r="K87" t="n">
+        <v>2731</v>
+      </c>
+      <c r="L87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>2868</t>
         </is>
       </c>
     </row>
@@ -4182,9 +4708,15 @@
       <c r="J88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>1993</t>
+      <c r="K88" t="n">
+        <v>1993</v>
+      </c>
+      <c r="L88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>2002</t>
         </is>
       </c>
     </row>
@@ -4225,7 +4757,13 @@
       <c r="J89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K89" t="inlineStr">
+      <c r="K89" t="n">
+        <v>0</v>
+      </c>
+      <c r="L89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4268,7 +4806,13 @@
       <c r="J90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K90" t="inlineStr">
+      <c r="K90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4311,9 +4855,15 @@
       <c r="J91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>2470</t>
+      <c r="K91" t="n">
+        <v>2470</v>
+      </c>
+      <c r="L91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>2453</t>
         </is>
       </c>
     </row>
@@ -4354,9 +4904,15 @@
       <c r="J92" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>2857</t>
+      <c r="K92" t="n">
+        <v>2857</v>
+      </c>
+      <c r="L92" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>2903</t>
         </is>
       </c>
     </row>
@@ -4397,9 +4953,15 @@
       <c r="J93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="K93" t="n">
+        <v>2498</v>
+      </c>
+      <c r="L93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>2490</t>
         </is>
       </c>
     </row>
@@ -4440,9 +5002,15 @@
       <c r="J94" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K94" t="inlineStr">
-        <is>
-          <t>3272</t>
+      <c r="K94" t="n">
+        <v>3272</v>
+      </c>
+      <c r="L94" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>3426</t>
         </is>
       </c>
     </row>
@@ -4483,9 +5051,15 @@
       <c r="J95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>3020</t>
+      <c r="K95" t="n">
+        <v>3020</v>
+      </c>
+      <c r="L95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>3177</t>
         </is>
       </c>
     </row>
@@ -4526,9 +5100,15 @@
       <c r="J96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>2561</t>
+      <c r="K96" t="n">
+        <v>2561</v>
+      </c>
+      <c r="L96" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>2902</t>
         </is>
       </c>
     </row>
@@ -4569,9 +5149,15 @@
       <c r="J97" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K97" t="inlineStr">
-        <is>
-          <t>3219</t>
+      <c r="K97" t="n">
+        <v>3219</v>
+      </c>
+      <c r="L97" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>3365</t>
         </is>
       </c>
     </row>
@@ -4612,9 +5198,15 @@
       <c r="J98" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="K98" t="inlineStr">
-        <is>
-          <t>3008</t>
+      <c r="K98" t="n">
+        <v>3008</v>
+      </c>
+      <c r="L98" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>3163</t>
         </is>
       </c>
     </row>
@@ -4655,9 +5247,15 @@
       <c r="J99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K99" t="inlineStr">
-        <is>
-          <t>2488</t>
+      <c r="K99" t="n">
+        <v>2488</v>
+      </c>
+      <c r="L99" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>2691</t>
         </is>
       </c>
     </row>
@@ -4698,9 +5296,15 @@
       <c r="J100" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="K100" t="inlineStr">
-        <is>
-          <t>2591</t>
+      <c r="K100" t="n">
+        <v>2591</v>
+      </c>
+      <c r="L100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>2587</t>
         </is>
       </c>
     </row>
@@ -4741,9 +5345,15 @@
       <c r="J101" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>3298</t>
+      <c r="K101" t="n">
+        <v>3298</v>
+      </c>
+      <c r="L101" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>3482</t>
         </is>
       </c>
     </row>
@@ -4784,9 +5394,15 @@
       <c r="J102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K102" t="inlineStr">
-        <is>
-          <t>2795</t>
+      <c r="K102" t="n">
+        <v>2795</v>
+      </c>
+      <c r="L102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>2938</t>
         </is>
       </c>
     </row>
@@ -4827,9 +5443,15 @@
       <c r="J103" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K103" t="inlineStr">
-        <is>
-          <t>2815</t>
+      <c r="K103" t="n">
+        <v>2815</v>
+      </c>
+      <c r="L103" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>2893</t>
         </is>
       </c>
     </row>
@@ -4870,9 +5492,15 @@
       <c r="J104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>2470</t>
+      <c r="K104" t="n">
+        <v>2470</v>
+      </c>
+      <c r="L104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>2451</t>
         </is>
       </c>
     </row>
@@ -4913,9 +5541,15 @@
       <c r="J105" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="K105" t="inlineStr">
-        <is>
-          <t>2844</t>
+      <c r="K105" t="n">
+        <v>2844</v>
+      </c>
+      <c r="L105" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>3094</t>
         </is>
       </c>
     </row>
@@ -4956,9 +5590,15 @@
       <c r="J106" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="K106" t="inlineStr">
-        <is>
-          <t>2810</t>
+      <c r="K106" t="n">
+        <v>2810</v>
+      </c>
+      <c r="L106" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>2795</t>
         </is>
       </c>
     </row>
@@ -4999,9 +5639,15 @@
       <c r="J107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K107" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="K107" t="n">
+        <v>2671</v>
+      </c>
+      <c r="L107" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>2877</t>
         </is>
       </c>
     </row>
@@ -5042,9 +5688,15 @@
       <c r="J108" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="K108" t="inlineStr">
-        <is>
-          <t>2443</t>
+      <c r="K108" t="n">
+        <v>2443</v>
+      </c>
+      <c r="L108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>2416</t>
         </is>
       </c>
     </row>
@@ -5085,9 +5737,15 @@
       <c r="J109" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="K109" t="inlineStr">
-        <is>
-          <t>2490</t>
+      <c r="K109" t="n">
+        <v>2490</v>
+      </c>
+      <c r="L109" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>2511</t>
         </is>
       </c>
     </row>
@@ -5128,9 +5786,15 @@
       <c r="J110" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="K110" t="inlineStr">
-        <is>
-          <t>2890</t>
+      <c r="K110" t="n">
+        <v>2890</v>
+      </c>
+      <c r="L110" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>2977</t>
         </is>
       </c>
     </row>
@@ -5171,9 +5835,15 @@
       <c r="J111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K111" t="inlineStr">
-        <is>
-          <t>2631</t>
+      <c r="K111" t="n">
+        <v>2631</v>
+      </c>
+      <c r="L111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>2695</t>
         </is>
       </c>
     </row>
@@ -5214,9 +5884,15 @@
       <c r="J112" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>2728</t>
+      <c r="K112" t="n">
+        <v>2728</v>
+      </c>
+      <c r="L112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>2869</t>
         </is>
       </c>
     </row>
@@ -5257,9 +5933,15 @@
       <c r="J113" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K113" t="inlineStr">
-        <is>
-          <t>2639</t>
+      <c r="K113" t="n">
+        <v>2639</v>
+      </c>
+      <c r="L113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>2594</t>
         </is>
       </c>
     </row>
@@ -5300,9 +5982,15 @@
       <c r="J114" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="K114" t="inlineStr">
-        <is>
-          <t>2804</t>
+      <c r="K114" t="n">
+        <v>2804</v>
+      </c>
+      <c r="L114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>2939</t>
         </is>
       </c>
     </row>
@@ -5343,9 +6031,15 @@
       <c r="J115" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K115" t="inlineStr">
-        <is>
-          <t>2542</t>
+      <c r="K115" t="n">
+        <v>2542</v>
+      </c>
+      <c r="L115" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>2619</t>
         </is>
       </c>
     </row>
@@ -5386,9 +6080,15 @@
       <c r="J116" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K116" t="inlineStr">
-        <is>
-          <t>2670</t>
+      <c r="K116" t="n">
+        <v>2670</v>
+      </c>
+      <c r="L116" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>2760</t>
         </is>
       </c>
     </row>
@@ -5429,9 +6129,15 @@
       <c r="J117" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K117" t="inlineStr">
-        <is>
-          <t>2677</t>
+      <c r="K117" t="n">
+        <v>2677</v>
+      </c>
+      <c r="L117" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>2744</t>
         </is>
       </c>
     </row>
@@ -5472,7 +6178,13 @@
       <c r="J118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K118" t="inlineStr">
+      <c r="K118" t="n">
+        <v>0</v>
+      </c>
+      <c r="L118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5515,9 +6227,15 @@
       <c r="J119" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K119" t="inlineStr">
-        <is>
-          <t>2748</t>
+      <c r="K119" t="n">
+        <v>2748</v>
+      </c>
+      <c r="L119" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>2830</t>
         </is>
       </c>
     </row>
@@ -5558,9 +6276,15 @@
       <c r="J120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K120" t="inlineStr">
-        <is>
-          <t>2713</t>
+      <c r="K120" t="n">
+        <v>2713</v>
+      </c>
+      <c r="L120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>2817</t>
         </is>
       </c>
     </row>
@@ -5601,9 +6325,15 @@
       <c r="J121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K121" t="inlineStr">
-        <is>
-          <t>2046</t>
+      <c r="K121" t="n">
+        <v>2046</v>
+      </c>
+      <c r="L121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>2039</t>
         </is>
       </c>
     </row>
@@ -5644,9 +6374,15 @@
       <c r="J122" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="K122" t="inlineStr">
-        <is>
-          <t>2436</t>
+      <c r="K122" t="n">
+        <v>2436</v>
+      </c>
+      <c r="L122" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>2422</t>
         </is>
       </c>
     </row>
@@ -5687,9 +6423,15 @@
       <c r="J123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K123" t="inlineStr">
-        <is>
-          <t>2487</t>
+      <c r="K123" t="n">
+        <v>2487</v>
+      </c>
+      <c r="L123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>2458</t>
         </is>
       </c>
     </row>
@@ -5730,9 +6472,15 @@
       <c r="J124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K124" t="inlineStr">
-        <is>
-          <t>2803</t>
+      <c r="K124" t="n">
+        <v>2803</v>
+      </c>
+      <c r="L124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>2878</t>
         </is>
       </c>
     </row>
@@ -5773,7 +6521,13 @@
       <c r="J125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K125" t="inlineStr">
+      <c r="K125" t="n">
+        <v>0</v>
+      </c>
+      <c r="L125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5816,9 +6570,15 @@
       <c r="J126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K126" t="inlineStr">
-        <is>
-          <t>2630</t>
+      <c r="K126" t="n">
+        <v>2630</v>
+      </c>
+      <c r="L126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>2743</t>
         </is>
       </c>
     </row>
@@ -5859,9 +6619,15 @@
       <c r="J127" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K127" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="K127" t="n">
+        <v>2530</v>
+      </c>
+      <c r="L127" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>2535</t>
         </is>
       </c>
     </row>
@@ -5902,9 +6668,15 @@
       <c r="J128" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="K128" t="inlineStr">
-        <is>
-          <t>2463</t>
+      <c r="K128" t="n">
+        <v>2463</v>
+      </c>
+      <c r="L128" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M128" t="inlineStr">
+        <is>
+          <t>2470</t>
         </is>
       </c>
     </row>
@@ -5945,9 +6717,15 @@
       <c r="J129" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="K129" t="inlineStr">
-        <is>
-          <t>2117</t>
+      <c r="K129" t="n">
+        <v>2117</v>
+      </c>
+      <c r="L129" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="M129" t="inlineStr">
+        <is>
+          <t>2300</t>
         </is>
       </c>
     </row>
@@ -5988,7 +6766,13 @@
       <c r="J130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K130" t="inlineStr">
+      <c r="K130" t="n">
+        <v>0</v>
+      </c>
+      <c r="L130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6031,7 +6815,13 @@
       <c r="J131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K131" t="inlineStr">
+      <c r="K131" t="n">
+        <v>0</v>
+      </c>
+      <c r="L131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6074,7 +6864,13 @@
       <c r="J132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K132" t="inlineStr">
+      <c r="K132" t="n">
+        <v>0</v>
+      </c>
+      <c r="L132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6117,7 +6913,13 @@
       <c r="J133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K133" t="inlineStr">
+      <c r="K133" t="n">
+        <v>0</v>
+      </c>
+      <c r="L133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6160,9 +6962,15 @@
       <c r="J134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K134" t="inlineStr">
-        <is>
-          <t>1958</t>
+      <c r="K134" t="n">
+        <v>1958</v>
+      </c>
+      <c r="L134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>1955</t>
         </is>
       </c>
     </row>
@@ -6203,9 +7011,15 @@
       <c r="J135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K135" t="inlineStr">
-        <is>
-          <t>2042</t>
+      <c r="K135" t="n">
+        <v>2042</v>
+      </c>
+      <c r="L135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t>2032</t>
         </is>
       </c>
     </row>
@@ -6246,9 +7060,15 @@
       <c r="J136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K136" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K136" t="n">
+        <v>0</v>
+      </c>
+      <c r="L136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>1496</t>
         </is>
       </c>
     </row>
@@ -6289,7 +7109,13 @@
       <c r="J137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K137" t="inlineStr">
+      <c r="K137" t="n">
+        <v>0</v>
+      </c>
+      <c r="L137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6332,7 +7158,13 @@
       <c r="J138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K138" t="inlineStr">
+      <c r="K138" t="n">
+        <v>0</v>
+      </c>
+      <c r="L138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6375,7 +7207,13 @@
       <c r="J139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K139" t="inlineStr">
+      <c r="K139" t="n">
+        <v>0</v>
+      </c>
+      <c r="L139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6418,9 +7256,15 @@
       <c r="J140" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="K140" t="inlineStr">
-        <is>
-          <t>3003</t>
+      <c r="K140" t="n">
+        <v>3003</v>
+      </c>
+      <c r="L140" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>3408</t>
         </is>
       </c>
     </row>
@@ -6461,7 +7305,13 @@
       <c r="J141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K141" t="inlineStr">
+      <c r="K141" t="n">
+        <v>0</v>
+      </c>
+      <c r="L141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6504,7 +7354,13 @@
       <c r="J142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K142" t="inlineStr">
+      <c r="K142" t="n">
+        <v>0</v>
+      </c>
+      <c r="L142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6547,9 +7403,15 @@
       <c r="J143" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="K143" t="inlineStr">
-        <is>
-          <t>3323</t>
+      <c r="K143" t="n">
+        <v>3323</v>
+      </c>
+      <c r="L143" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>3551</t>
         </is>
       </c>
     </row>
@@ -6590,7 +7452,13 @@
       <c r="J144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K144" t="inlineStr">
+      <c r="K144" t="n">
+        <v>0</v>
+      </c>
+      <c r="L144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6633,9 +7501,15 @@
       <c r="J145" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="K145" t="inlineStr">
-        <is>
-          <t>2618</t>
+      <c r="K145" t="n">
+        <v>2618</v>
+      </c>
+      <c r="L145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M145" t="inlineStr">
+        <is>
+          <t>2560</t>
         </is>
       </c>
     </row>
@@ -6676,7 +7550,13 @@
       <c r="J146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K146" t="inlineStr">
+      <c r="K146" t="n">
+        <v>0</v>
+      </c>
+      <c r="L146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6719,7 +7599,13 @@
       <c r="J147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K147" t="inlineStr">
+      <c r="K147" t="n">
+        <v>0</v>
+      </c>
+      <c r="L147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6755,6 +7641,8 @@
       </c>
       <c r="J148" s="3" t="inlineStr"/>
       <c r="K148" t="inlineStr"/>
+      <c r="L148" s="3" t="inlineStr"/>
+      <c r="M148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -6787,9 +7675,15 @@
       <c r="J149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K149" t="inlineStr">
-        <is>
-          <t>1321</t>
+      <c r="K149" t="n">
+        <v>1321</v>
+      </c>
+      <c r="L149" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>1343</t>
         </is>
       </c>
     </row>
@@ -6824,9 +7718,81 @@
       <c r="J150" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="K150" t="inlineStr">
-        <is>
-          <t>1384</t>
+      <c r="K150" t="n">
+        <v>1384</v>
+      </c>
+      <c r="L150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>1396</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>58340439</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Player-58340439</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr"/>
+      <c r="D151" t="inlineStr"/>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F151" s="3" t="inlineStr"/>
+      <c r="G151" t="inlineStr"/>
+      <c r="H151" s="3" t="inlineStr"/>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" s="3" t="inlineStr"/>
+      <c r="K151" t="inlineStr"/>
+      <c r="L151" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t>2167</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>57908454</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Player-57908454</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr"/>
+      <c r="D152" t="inlineStr"/>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F152" s="3" t="inlineStr"/>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" s="3" t="inlineStr"/>
+      <c r="I152" t="inlineStr"/>
+      <c r="J152" s="3" t="inlineStr"/>
+      <c r="K152" t="inlineStr"/>
+      <c r="L152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-06 11:30:48
</commit_message>
<xml_diff>
--- a/Season_Attack/81.xlsx
+++ b/Season_Attack/81.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M152"/>
+  <dimension ref="A1:O152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,10 +448,20 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>01-04_A</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>01-04_0</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>01-05_A</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>01-05_0</t>
         </is>
@@ -500,9 +510,15 @@
       <c r="L2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>3198</t>
+      <c r="M2" t="n">
+        <v>3198</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>3201</t>
         </is>
       </c>
     </row>
@@ -549,9 +565,15 @@
       <c r="L3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>3575</t>
+      <c r="M3" t="n">
+        <v>3575</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>3801</t>
         </is>
       </c>
     </row>
@@ -598,9 +620,15 @@
       <c r="L4" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>3906</t>
+      <c r="M4" t="n">
+        <v>3906</v>
+      </c>
+      <c r="N4" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>4068</t>
         </is>
       </c>
     </row>
@@ -623,7 +651,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F5" s="3" t="n">
@@ -647,9 +675,15 @@
       <c r="L5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>3734</t>
+      <c r="M5" t="n">
+        <v>3734</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>4048</t>
         </is>
       </c>
     </row>
@@ -672,7 +706,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F6" s="3" t="n">
@@ -696,9 +730,15 @@
       <c r="L6" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>3803</t>
+      <c r="M6" t="n">
+        <v>3803</v>
+      </c>
+      <c r="N6" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>4093</t>
         </is>
       </c>
     </row>
@@ -745,9 +785,15 @@
       <c r="L7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>4086</t>
+      <c r="M7" t="n">
+        <v>4086</v>
+      </c>
+      <c r="N7" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>4371</t>
         </is>
       </c>
     </row>
@@ -794,9 +840,15 @@
       <c r="L8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>3626</t>
+      <c r="M8" t="n">
+        <v>3626</v>
+      </c>
+      <c r="N8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>3889</t>
         </is>
       </c>
     </row>
@@ -843,9 +895,15 @@
       <c r="L9" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>3859</t>
+      <c r="M9" t="n">
+        <v>3859</v>
+      </c>
+      <c r="N9" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>4076</t>
         </is>
       </c>
     </row>
@@ -892,9 +950,15 @@
       <c r="L10" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>3507</t>
+      <c r="M10" t="n">
+        <v>3507</v>
+      </c>
+      <c r="N10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>3723</t>
         </is>
       </c>
     </row>
@@ -941,9 +1005,15 @@
       <c r="L11" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>3098</t>
+      <c r="M11" t="n">
+        <v>3098</v>
+      </c>
+      <c r="N11" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>3151</t>
         </is>
       </c>
     </row>
@@ -990,9 +1060,15 @@
       <c r="L12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>3531</t>
+      <c r="M12" t="n">
+        <v>3531</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>3709</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1115,13 @@
       <c r="L13" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="M13" t="n">
+        <v>2684</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="inlineStr">
         <is>
           <t>2684</t>
         </is>
@@ -1088,9 +1170,15 @@
       <c r="L14" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>3993</t>
+      <c r="M14" t="n">
+        <v>3993</v>
+      </c>
+      <c r="N14" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>4421</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1201,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F15" s="3" t="n">
@@ -1137,9 +1225,15 @@
       <c r="L15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>3750</t>
+      <c r="M15" t="n">
+        <v>3750</v>
+      </c>
+      <c r="N15" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>4046</t>
         </is>
       </c>
     </row>
@@ -1162,7 +1256,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F16" s="3" t="n">
@@ -1186,9 +1280,15 @@
       <c r="L16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>3783</t>
+      <c r="M16" t="n">
+        <v>3783</v>
+      </c>
+      <c r="N16" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>4046</t>
         </is>
       </c>
     </row>
@@ -1235,9 +1335,15 @@
       <c r="L17" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>3817</t>
+      <c r="M17" t="n">
+        <v>3817</v>
+      </c>
+      <c r="N17" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>4063</t>
         </is>
       </c>
     </row>
@@ -1284,9 +1390,15 @@
       <c r="L18" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>3639</t>
+      <c r="M18" t="n">
+        <v>3639</v>
+      </c>
+      <c r="N18" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>3872</t>
         </is>
       </c>
     </row>
@@ -1333,9 +1445,15 @@
       <c r="L19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>3889</t>
+      <c r="M19" t="n">
+        <v>3889</v>
+      </c>
+      <c r="N19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>4213</t>
         </is>
       </c>
     </row>
@@ -1382,9 +1500,15 @@
       <c r="L20" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>3945</t>
+      <c r="M20" t="n">
+        <v>3945</v>
+      </c>
+      <c r="N20" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>4119</t>
         </is>
       </c>
     </row>
@@ -1431,9 +1555,15 @@
       <c r="L21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>3073</t>
+      <c r="M21" t="n">
+        <v>3073</v>
+      </c>
+      <c r="N21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>3386</t>
         </is>
       </c>
     </row>
@@ -1456,7 +1586,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F22" s="4" t="n">
@@ -1480,9 +1610,15 @@
       <c r="L22" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>3839</t>
+      <c r="M22" t="n">
+        <v>3839</v>
+      </c>
+      <c r="N22" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>4162</t>
         </is>
       </c>
     </row>
@@ -1505,7 +1641,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F23" s="4" t="n">
@@ -1529,9 +1665,15 @@
       <c r="L23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>2873</t>
+      <c r="M23" t="n">
+        <v>2873</v>
+      </c>
+      <c r="N23" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>2923</t>
         </is>
       </c>
     </row>
@@ -1578,9 +1720,15 @@
       <c r="L24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>3816</t>
+      <c r="M24" t="n">
+        <v>3816</v>
+      </c>
+      <c r="N24" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>3797</t>
         </is>
       </c>
     </row>
@@ -1627,7 +1775,13 @@
       <c r="L25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M25" t="inlineStr">
+      <c r="M25" t="n">
+        <v>2500</v>
+      </c>
+      <c r="N25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1676,9 +1830,15 @@
       <c r="L26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>3900</t>
+      <c r="M26" t="n">
+        <v>3900</v>
+      </c>
+      <c r="N26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>4179</t>
         </is>
       </c>
     </row>
@@ -1725,9 +1885,15 @@
       <c r="L27" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>3868</t>
+      <c r="M27" t="n">
+        <v>3868</v>
+      </c>
+      <c r="N27" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>4188</t>
         </is>
       </c>
     </row>
@@ -1750,7 +1916,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F28" s="3" t="n">
@@ -1774,9 +1940,15 @@
       <c r="L28" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>3374</t>
+      <c r="M28" t="n">
+        <v>3374</v>
+      </c>
+      <c r="N28" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>3617</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1971,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F29" s="3" t="n">
@@ -1823,9 +1995,15 @@
       <c r="L29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>3389</t>
+      <c r="M29" t="n">
+        <v>3389</v>
+      </c>
+      <c r="N29" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>3634</t>
         </is>
       </c>
     </row>
@@ -1872,9 +2050,15 @@
       <c r="L30" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>4002</t>
+      <c r="M30" t="n">
+        <v>4002</v>
+      </c>
+      <c r="N30" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>4346</t>
         </is>
       </c>
     </row>
@@ -1921,9 +2105,15 @@
       <c r="L31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>3646</t>
+      <c r="M31" t="n">
+        <v>3646</v>
+      </c>
+      <c r="N31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>4008</t>
         </is>
       </c>
     </row>
@@ -1946,7 +2136,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F32" s="4" t="n">
@@ -1970,9 +2160,15 @@
       <c r="L32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>4024</t>
+      <c r="M32" t="n">
+        <v>4024</v>
+      </c>
+      <c r="N32" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>4325</t>
         </is>
       </c>
     </row>
@@ -2019,9 +2215,15 @@
       <c r="L33" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>4134</t>
+      <c r="M33" t="n">
+        <v>4134</v>
+      </c>
+      <c r="N33" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>4758</t>
         </is>
       </c>
     </row>
@@ -2068,9 +2270,15 @@
       <c r="L34" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>2765</t>
+      <c r="M34" t="n">
+        <v>2765</v>
+      </c>
+      <c r="N34" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>2763</t>
         </is>
       </c>
     </row>
@@ -2117,9 +2325,15 @@
       <c r="L35" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>4011</t>
+      <c r="M35" t="n">
+        <v>4011</v>
+      </c>
+      <c r="N35" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>4224</t>
         </is>
       </c>
     </row>
@@ -2166,9 +2380,15 @@
       <c r="L36" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>3388</t>
+      <c r="M36" t="n">
+        <v>3388</v>
+      </c>
+      <c r="N36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>3665</t>
         </is>
       </c>
     </row>
@@ -2215,9 +2435,15 @@
       <c r="L37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>3696</t>
+      <c r="M37" t="n">
+        <v>3696</v>
+      </c>
+      <c r="N37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>3880</t>
         </is>
       </c>
     </row>
@@ -2264,9 +2490,15 @@
       <c r="L38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>3966</t>
+      <c r="M38" t="n">
+        <v>3966</v>
+      </c>
+      <c r="N38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>4256</t>
         </is>
       </c>
     </row>
@@ -2313,9 +2545,15 @@
       <c r="L39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>3860</t>
+      <c r="M39" t="n">
+        <v>3860</v>
+      </c>
+      <c r="N39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>4045</t>
         </is>
       </c>
     </row>
@@ -2338,7 +2576,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F40" s="3" t="n">
@@ -2362,9 +2600,15 @@
       <c r="L40" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>3871</t>
+      <c r="M40" t="n">
+        <v>3871</v>
+      </c>
+      <c r="N40" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>4148</t>
         </is>
       </c>
     </row>
@@ -2411,9 +2655,15 @@
       <c r="L41" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>3900</t>
+      <c r="M41" t="n">
+        <v>3900</v>
+      </c>
+      <c r="N41" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>4241</t>
         </is>
       </c>
     </row>
@@ -2460,9 +2710,15 @@
       <c r="L42" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>4149</t>
+      <c r="M42" t="n">
+        <v>4149</v>
+      </c>
+      <c r="N42" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>4525</t>
         </is>
       </c>
     </row>
@@ -2509,9 +2765,15 @@
       <c r="L43" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>3722</t>
+      <c r="M43" t="n">
+        <v>3722</v>
+      </c>
+      <c r="N43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>4037</t>
         </is>
       </c>
     </row>
@@ -2534,7 +2796,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F44" s="5" t="n">
@@ -2558,9 +2820,15 @@
       <c r="L44" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>2844</t>
+      <c r="M44" t="n">
+        <v>2844</v>
+      </c>
+      <c r="N44" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>3260</t>
         </is>
       </c>
     </row>
@@ -2583,7 +2851,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F45" s="4" t="n">
@@ -2607,9 +2875,15 @@
       <c r="L45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>3680</t>
+      <c r="M45" t="n">
+        <v>3680</v>
+      </c>
+      <c r="N45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>3776</t>
         </is>
       </c>
     </row>
@@ -2656,9 +2930,15 @@
       <c r="L46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>3597</t>
+      <c r="M46" t="n">
+        <v>3597</v>
+      </c>
+      <c r="N46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>3853</t>
         </is>
       </c>
     </row>
@@ -2705,9 +2985,15 @@
       <c r="L47" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>3734</t>
+      <c r="M47" t="n">
+        <v>3734</v>
+      </c>
+      <c r="N47" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>3948</t>
         </is>
       </c>
     </row>
@@ -2754,9 +3040,15 @@
       <c r="L48" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>3754</t>
+      <c r="M48" t="n">
+        <v>3754</v>
+      </c>
+      <c r="N48" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>4000</t>
         </is>
       </c>
     </row>
@@ -2803,9 +3095,15 @@
       <c r="L49" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>3270</t>
+      <c r="M49" t="n">
+        <v>3270</v>
+      </c>
+      <c r="N49" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>3547</t>
         </is>
       </c>
     </row>
@@ -2828,7 +3126,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F50" s="4" t="n">
@@ -2852,9 +3150,15 @@
       <c r="L50" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>3744</t>
+      <c r="M50" t="n">
+        <v>3744</v>
+      </c>
+      <c r="N50" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>3922</t>
         </is>
       </c>
     </row>
@@ -2901,9 +3205,15 @@
       <c r="L51" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>3667</t>
+      <c r="M51" t="n">
+        <v>3667</v>
+      </c>
+      <c r="N51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>3682</t>
         </is>
       </c>
     </row>
@@ -2950,9 +3260,15 @@
       <c r="L52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>2550</t>
+      <c r="M52" t="n">
+        <v>2550</v>
+      </c>
+      <c r="N52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>2574</t>
         </is>
       </c>
     </row>
@@ -2999,9 +3315,15 @@
       <c r="L53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>2852</t>
+      <c r="M53" t="n">
+        <v>2852</v>
+      </c>
+      <c r="N53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>2917</t>
         </is>
       </c>
     </row>
@@ -3048,9 +3370,15 @@
       <c r="L54" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>2660</t>
+      <c r="M54" t="n">
+        <v>2660</v>
+      </c>
+      <c r="N54" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>2834</t>
         </is>
       </c>
     </row>
@@ -3097,9 +3425,15 @@
       <c r="L55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>3156</t>
+      <c r="M55" t="n">
+        <v>3156</v>
+      </c>
+      <c r="N55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>3316</t>
         </is>
       </c>
     </row>
@@ -3146,9 +3480,15 @@
       <c r="L56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>3371</t>
+      <c r="M56" t="n">
+        <v>3371</v>
+      </c>
+      <c r="N56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>3587</t>
         </is>
       </c>
     </row>
@@ -3195,9 +3535,15 @@
       <c r="L57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>3643</t>
+      <c r="M57" t="n">
+        <v>3643</v>
+      </c>
+      <c r="N57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>3815</t>
         </is>
       </c>
     </row>
@@ -3244,9 +3590,15 @@
       <c r="L58" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>3205</t>
+      <c r="M58" t="n">
+        <v>3205</v>
+      </c>
+      <c r="N58" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>3343</t>
         </is>
       </c>
     </row>
@@ -3293,9 +3645,15 @@
       <c r="L59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>3551</t>
+      <c r="M59" t="n">
+        <v>3551</v>
+      </c>
+      <c r="N59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>3790</t>
         </is>
       </c>
     </row>
@@ -3342,9 +3700,15 @@
       <c r="L60" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>3755</t>
+      <c r="M60" t="n">
+        <v>3755</v>
+      </c>
+      <c r="N60" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -3391,9 +3755,15 @@
       <c r="L61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>3569</t>
+      <c r="M61" t="n">
+        <v>3569</v>
+      </c>
+      <c r="N61" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>3894</t>
         </is>
       </c>
     </row>
@@ -3440,9 +3810,15 @@
       <c r="L62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>3700</t>
+      <c r="M62" t="n">
+        <v>3700</v>
+      </c>
+      <c r="N62" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>3868</t>
         </is>
       </c>
     </row>
@@ -3489,9 +3865,15 @@
       <c r="L63" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>3253</t>
+      <c r="M63" t="n">
+        <v>3253</v>
+      </c>
+      <c r="N63" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>3414</t>
         </is>
       </c>
     </row>
@@ -3538,7 +3920,13 @@
       <c r="L64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M64" t="inlineStr">
+      <c r="M64" t="n">
+        <v>2514</v>
+      </c>
+      <c r="N64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O64" t="inlineStr">
         <is>
           <t>2514</t>
         </is>
@@ -3587,9 +3975,15 @@
       <c r="L65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>3144</t>
+      <c r="M65" t="n">
+        <v>3144</v>
+      </c>
+      <c r="N65" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>3377</t>
         </is>
       </c>
     </row>
@@ -3636,9 +4030,15 @@
       <c r="L66" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>3138</t>
+      <c r="M66" t="n">
+        <v>3138</v>
+      </c>
+      <c r="N66" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>3204</t>
         </is>
       </c>
     </row>
@@ -3685,9 +4085,15 @@
       <c r="L67" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>3753</t>
+      <c r="M67" t="n">
+        <v>3753</v>
+      </c>
+      <c r="N67" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>4007</t>
         </is>
       </c>
     </row>
@@ -3734,9 +4140,15 @@
       <c r="L68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>3322</t>
+      <c r="M68" t="n">
+        <v>3322</v>
+      </c>
+      <c r="N68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>3432</t>
         </is>
       </c>
     </row>
@@ -3783,9 +4195,15 @@
       <c r="L69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M69" t="inlineStr">
-        <is>
-          <t>2585</t>
+      <c r="M69" t="n">
+        <v>2585</v>
+      </c>
+      <c r="N69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>2636</t>
         </is>
       </c>
     </row>
@@ -3832,9 +4250,15 @@
       <c r="L70" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="M70" t="inlineStr">
-        <is>
-          <t>2927</t>
+      <c r="M70" t="n">
+        <v>2927</v>
+      </c>
+      <c r="N70" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>3097</t>
         </is>
       </c>
     </row>
@@ -3881,9 +4305,15 @@
       <c r="L71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>3923</t>
+      <c r="M71" t="n">
+        <v>3923</v>
+      </c>
+      <c r="N71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>4093</t>
         </is>
       </c>
     </row>
@@ -3930,9 +4360,15 @@
       <c r="L72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>3357</t>
+      <c r="M72" t="n">
+        <v>3357</v>
+      </c>
+      <c r="N72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>3493</t>
         </is>
       </c>
     </row>
@@ -3979,9 +4415,15 @@
       <c r="L73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>3607</t>
+      <c r="M73" t="n">
+        <v>3607</v>
+      </c>
+      <c r="N73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>3803</t>
         </is>
       </c>
     </row>
@@ -4028,9 +4470,15 @@
       <c r="L74" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>3290</t>
+      <c r="M74" t="n">
+        <v>3290</v>
+      </c>
+      <c r="N74" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>3547</t>
         </is>
       </c>
     </row>
@@ -4077,9 +4525,15 @@
       <c r="L75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M75" t="inlineStr">
-        <is>
-          <t>3593</t>
+      <c r="M75" t="n">
+        <v>3593</v>
+      </c>
+      <c r="N75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>3727</t>
         </is>
       </c>
     </row>
@@ -4126,9 +4580,15 @@
       <c r="L76" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>3369</t>
+      <c r="M76" t="n">
+        <v>3369</v>
+      </c>
+      <c r="N76" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>3585</t>
         </is>
       </c>
     </row>
@@ -4175,9 +4635,15 @@
       <c r="L77" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>2783</t>
+      <c r="M77" t="n">
+        <v>2783</v>
+      </c>
+      <c r="N77" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>2822</t>
         </is>
       </c>
     </row>
@@ -4224,9 +4690,15 @@
       <c r="L78" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M78" t="inlineStr">
-        <is>
-          <t>3285</t>
+      <c r="M78" t="n">
+        <v>3285</v>
+      </c>
+      <c r="N78" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>3497</t>
         </is>
       </c>
     </row>
@@ -4273,9 +4745,15 @@
       <c r="L79" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>3315</t>
+      <c r="M79" t="n">
+        <v>3315</v>
+      </c>
+      <c r="N79" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>3465</t>
         </is>
       </c>
     </row>
@@ -4322,9 +4800,15 @@
       <c r="L80" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M80" t="inlineStr">
-        <is>
-          <t>3002</t>
+      <c r="M80" t="n">
+        <v>3002</v>
+      </c>
+      <c r="N80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>3015</t>
         </is>
       </c>
     </row>
@@ -4371,9 +4855,15 @@
       <c r="L81" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>2666</t>
+      <c r="M81" t="n">
+        <v>2666</v>
+      </c>
+      <c r="N81" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>2773</t>
         </is>
       </c>
     </row>
@@ -4420,9 +4910,15 @@
       <c r="L82" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>3451</t>
+      <c r="M82" t="n">
+        <v>3451</v>
+      </c>
+      <c r="N82" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>3606</t>
         </is>
       </c>
     </row>
@@ -4469,9 +4965,15 @@
       <c r="L83" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M83" t="inlineStr">
-        <is>
-          <t>2712</t>
+      <c r="M83" t="n">
+        <v>2712</v>
+      </c>
+      <c r="N83" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>2735</t>
         </is>
       </c>
     </row>
@@ -4518,9 +5020,15 @@
       <c r="L84" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M84" t="inlineStr">
-        <is>
-          <t>2912</t>
+      <c r="M84" t="n">
+        <v>2912</v>
+      </c>
+      <c r="N84" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>2984</t>
         </is>
       </c>
     </row>
@@ -4567,7 +5075,13 @@
       <c r="L85" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="M85" t="inlineStr">
+      <c r="M85" t="n">
+        <v>2016</v>
+      </c>
+      <c r="N85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O85" t="inlineStr">
         <is>
           <t>2016</t>
         </is>
@@ -4616,9 +5130,15 @@
       <c r="L86" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M86" t="inlineStr">
-        <is>
-          <t>2629</t>
+      <c r="M86" t="n">
+        <v>2629</v>
+      </c>
+      <c r="N86" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>2566</t>
         </is>
       </c>
     </row>
@@ -4665,9 +5185,15 @@
       <c r="L87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M87" t="inlineStr">
-        <is>
-          <t>2868</t>
+      <c r="M87" t="n">
+        <v>2868</v>
+      </c>
+      <c r="N87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>2908</t>
         </is>
       </c>
     </row>
@@ -4714,9 +5240,15 @@
       <c r="L88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M88" t="inlineStr">
-        <is>
-          <t>2002</t>
+      <c r="M88" t="n">
+        <v>2002</v>
+      </c>
+      <c r="N88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>2017</t>
         </is>
       </c>
     </row>
@@ -4763,11 +5295,11 @@
       <c r="L89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M89" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="M89" t="n">
+        <v>0</v>
+      </c>
+      <c r="N89" s="3" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -4812,11 +5344,11 @@
       <c r="L90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="M90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N90" s="3" t="inlineStr"/>
+      <c r="O90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -4861,9 +5393,15 @@
       <c r="L91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>2453</t>
+      <c r="M91" t="n">
+        <v>2453</v>
+      </c>
+      <c r="N91" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>2536</t>
         </is>
       </c>
     </row>
@@ -4910,9 +5448,15 @@
       <c r="L92" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="M92" t="inlineStr">
-        <is>
-          <t>2903</t>
+      <c r="M92" t="n">
+        <v>2903</v>
+      </c>
+      <c r="N92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>2923</t>
         </is>
       </c>
     </row>
@@ -4959,9 +5503,15 @@
       <c r="L93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M93" t="inlineStr">
-        <is>
-          <t>2490</t>
+      <c r="M93" t="n">
+        <v>2490</v>
+      </c>
+      <c r="N93" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>2777</t>
         </is>
       </c>
     </row>
@@ -5008,9 +5558,15 @@
       <c r="L94" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M94" t="inlineStr">
-        <is>
-          <t>3426</t>
+      <c r="M94" t="n">
+        <v>3426</v>
+      </c>
+      <c r="N94" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>3575</t>
         </is>
       </c>
     </row>
@@ -5057,9 +5613,15 @@
       <c r="L95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M95" t="inlineStr">
-        <is>
-          <t>3177</t>
+      <c r="M95" t="n">
+        <v>3177</v>
+      </c>
+      <c r="N95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>3376</t>
         </is>
       </c>
     </row>
@@ -5106,9 +5668,15 @@
       <c r="L96" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>2902</t>
+      <c r="M96" t="n">
+        <v>2902</v>
+      </c>
+      <c r="N96" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>3159</t>
         </is>
       </c>
     </row>
@@ -5155,9 +5723,15 @@
       <c r="L97" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M97" t="inlineStr">
-        <is>
-          <t>3365</t>
+      <c r="M97" t="n">
+        <v>3365</v>
+      </c>
+      <c r="N97" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>3537</t>
         </is>
       </c>
     </row>
@@ -5204,9 +5778,15 @@
       <c r="L98" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="M98" t="inlineStr">
-        <is>
-          <t>3163</t>
+      <c r="M98" t="n">
+        <v>3163</v>
+      </c>
+      <c r="N98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>3266</t>
         </is>
       </c>
     </row>
@@ -5253,9 +5833,15 @@
       <c r="L99" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>2691</t>
+      <c r="M99" t="n">
+        <v>2691</v>
+      </c>
+      <c r="N99" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>2721</t>
         </is>
       </c>
     </row>
@@ -5302,9 +5888,15 @@
       <c r="L100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M100" t="inlineStr">
-        <is>
-          <t>2587</t>
+      <c r="M100" t="n">
+        <v>2587</v>
+      </c>
+      <c r="N100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>2599</t>
         </is>
       </c>
     </row>
@@ -5351,9 +5943,15 @@
       <c r="L101" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>3482</t>
+      <c r="M101" t="n">
+        <v>3482</v>
+      </c>
+      <c r="N101" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>3677</t>
         </is>
       </c>
     </row>
@@ -5400,9 +5998,15 @@
       <c r="L102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M102" t="inlineStr">
-        <is>
-          <t>2938</t>
+      <c r="M102" t="n">
+        <v>2938</v>
+      </c>
+      <c r="N102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>3074</t>
         </is>
       </c>
     </row>
@@ -5449,9 +6053,15 @@
       <c r="L103" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="M103" t="inlineStr">
-        <is>
-          <t>2893</t>
+      <c r="M103" t="n">
+        <v>2893</v>
+      </c>
+      <c r="N103" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>2997</t>
         </is>
       </c>
     </row>
@@ -5498,9 +6108,15 @@
       <c r="L104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M104" t="inlineStr">
-        <is>
-          <t>2451</t>
+      <c r="M104" t="n">
+        <v>2451</v>
+      </c>
+      <c r="N104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -5547,9 +6163,15 @@
       <c r="L105" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M105" t="inlineStr">
-        <is>
-          <t>3094</t>
+      <c r="M105" t="n">
+        <v>3094</v>
+      </c>
+      <c r="N105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>3069</t>
         </is>
       </c>
     </row>
@@ -5596,9 +6218,15 @@
       <c r="L106" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M106" t="inlineStr">
-        <is>
-          <t>2795</t>
+      <c r="M106" t="n">
+        <v>2795</v>
+      </c>
+      <c r="N106" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>2857</t>
         </is>
       </c>
     </row>
@@ -5645,9 +6273,15 @@
       <c r="L107" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="M107" t="inlineStr">
-        <is>
-          <t>2877</t>
+      <c r="M107" t="n">
+        <v>2877</v>
+      </c>
+      <c r="N107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>3016</t>
         </is>
       </c>
     </row>
@@ -5694,9 +6328,15 @@
       <c r="L108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M108" t="inlineStr">
-        <is>
-          <t>2416</t>
+      <c r="M108" t="n">
+        <v>2416</v>
+      </c>
+      <c r="N108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>2390</t>
         </is>
       </c>
     </row>
@@ -5743,9 +6383,15 @@
       <c r="L109" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="M109" t="inlineStr">
-        <is>
-          <t>2511</t>
+      <c r="M109" t="n">
+        <v>2511</v>
+      </c>
+      <c r="N109" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>2535</t>
         </is>
       </c>
     </row>
@@ -5792,9 +6438,15 @@
       <c r="L110" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="M110" t="inlineStr">
-        <is>
-          <t>2977</t>
+      <c r="M110" t="n">
+        <v>2977</v>
+      </c>
+      <c r="N110" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>3039</t>
         </is>
       </c>
     </row>
@@ -5841,9 +6493,15 @@
       <c r="L111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M111" t="inlineStr">
-        <is>
-          <t>2695</t>
+      <c r="M111" t="n">
+        <v>2695</v>
+      </c>
+      <c r="N111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>2743</t>
         </is>
       </c>
     </row>
@@ -5890,9 +6548,15 @@
       <c r="L112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M112" t="inlineStr">
-        <is>
-          <t>2869</t>
+      <c r="M112" t="n">
+        <v>2869</v>
+      </c>
+      <c r="N112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>2960</t>
         </is>
       </c>
     </row>
@@ -5939,9 +6603,15 @@
       <c r="L113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M113" t="inlineStr">
-        <is>
-          <t>2594</t>
+      <c r="M113" t="n">
+        <v>2594</v>
+      </c>
+      <c r="N113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>2568</t>
         </is>
       </c>
     </row>
@@ -5988,9 +6658,15 @@
       <c r="L114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M114" t="inlineStr">
-        <is>
-          <t>2939</t>
+      <c r="M114" t="n">
+        <v>2939</v>
+      </c>
+      <c r="N114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>2968</t>
         </is>
       </c>
     </row>
@@ -6037,9 +6713,15 @@
       <c r="L115" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M115" t="inlineStr">
-        <is>
-          <t>2619</t>
+      <c r="M115" t="n">
+        <v>2619</v>
+      </c>
+      <c r="N115" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>2705</t>
         </is>
       </c>
     </row>
@@ -6086,9 +6768,15 @@
       <c r="L116" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="M116" t="inlineStr">
-        <is>
-          <t>2760</t>
+      <c r="M116" t="n">
+        <v>2760</v>
+      </c>
+      <c r="N116" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>2717</t>
         </is>
       </c>
     </row>
@@ -6135,9 +6823,15 @@
       <c r="L117" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M117" t="inlineStr">
-        <is>
-          <t>2744</t>
+      <c r="M117" t="n">
+        <v>2744</v>
+      </c>
+      <c r="N117" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>2864</t>
         </is>
       </c>
     </row>
@@ -6184,7 +6878,13 @@
       <c r="L118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M118" t="inlineStr">
+      <c r="M118" t="n">
+        <v>0</v>
+      </c>
+      <c r="N118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6233,9 +6933,15 @@
       <c r="L119" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M119" t="inlineStr">
-        <is>
-          <t>2830</t>
+      <c r="M119" t="n">
+        <v>2830</v>
+      </c>
+      <c r="N119" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>2979</t>
         </is>
       </c>
     </row>
@@ -6282,9 +6988,15 @@
       <c r="L120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M120" t="inlineStr">
-        <is>
-          <t>2817</t>
+      <c r="M120" t="n">
+        <v>2817</v>
+      </c>
+      <c r="N120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>2890</t>
         </is>
       </c>
     </row>
@@ -6331,9 +7043,15 @@
       <c r="L121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M121" t="inlineStr">
-        <is>
-          <t>2039</t>
+      <c r="M121" t="n">
+        <v>2039</v>
+      </c>
+      <c r="N121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>2053</t>
         </is>
       </c>
     </row>
@@ -6380,9 +7098,15 @@
       <c r="L122" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="M122" t="inlineStr">
-        <is>
-          <t>2422</t>
+      <c r="M122" t="n">
+        <v>2422</v>
+      </c>
+      <c r="N122" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>2445</t>
         </is>
       </c>
     </row>
@@ -6429,9 +7153,15 @@
       <c r="L123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M123" t="inlineStr">
-        <is>
-          <t>2458</t>
+      <c r="M123" t="n">
+        <v>2458</v>
+      </c>
+      <c r="N123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O123" t="inlineStr">
+        <is>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -6478,9 +7208,15 @@
       <c r="L124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M124" t="inlineStr">
-        <is>
-          <t>2878</t>
+      <c r="M124" t="n">
+        <v>2878</v>
+      </c>
+      <c r="N124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>2993</t>
         </is>
       </c>
     </row>
@@ -6527,7 +7263,13 @@
       <c r="L125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M125" t="inlineStr">
+      <c r="M125" t="n">
+        <v>0</v>
+      </c>
+      <c r="N125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6576,9 +7318,15 @@
       <c r="L126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M126" t="inlineStr">
-        <is>
-          <t>2743</t>
+      <c r="M126" t="n">
+        <v>2743</v>
+      </c>
+      <c r="N126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>2699</t>
         </is>
       </c>
     </row>
@@ -6625,9 +7373,15 @@
       <c r="L127" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="M127" t="inlineStr">
-        <is>
-          <t>2535</t>
+      <c r="M127" t="n">
+        <v>2535</v>
+      </c>
+      <c r="N127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>2514</t>
         </is>
       </c>
     </row>
@@ -6674,9 +7428,15 @@
       <c r="L128" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M128" t="inlineStr">
-        <is>
-          <t>2470</t>
+      <c r="M128" t="n">
+        <v>2470</v>
+      </c>
+      <c r="N128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O128" t="inlineStr">
+        <is>
+          <t>2456</t>
         </is>
       </c>
     </row>
@@ -6723,9 +7483,15 @@
       <c r="L129" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="M129" t="inlineStr">
-        <is>
-          <t>2300</t>
+      <c r="M129" t="n">
+        <v>2300</v>
+      </c>
+      <c r="N129" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O129" t="inlineStr">
+        <is>
+          <t>2353</t>
         </is>
       </c>
     </row>
@@ -6772,9 +7538,15 @@
       <c r="L130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M130" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M130" t="n">
+        <v>0</v>
+      </c>
+      <c r="N130" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="O130" t="inlineStr">
+        <is>
+          <t>1708</t>
         </is>
       </c>
     </row>
@@ -6821,7 +7593,13 @@
       <c r="L131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M131" t="inlineStr">
+      <c r="M131" t="n">
+        <v>0</v>
+      </c>
+      <c r="N131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6870,9 +7648,15 @@
       <c r="L132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M132" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M132" t="n">
+        <v>0</v>
+      </c>
+      <c r="N132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O132" t="inlineStr">
+        <is>
+          <t>1494</t>
         </is>
       </c>
     </row>
@@ -6919,7 +7703,13 @@
       <c r="L133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M133" t="inlineStr">
+      <c r="M133" t="n">
+        <v>0</v>
+      </c>
+      <c r="N133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6968,9 +7758,15 @@
       <c r="L134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M134" t="inlineStr">
-        <is>
-          <t>1955</t>
+      <c r="M134" t="n">
+        <v>1955</v>
+      </c>
+      <c r="N134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>1944</t>
         </is>
       </c>
     </row>
@@ -7017,7 +7813,13 @@
       <c r="L135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M135" t="inlineStr">
+      <c r="M135" t="n">
+        <v>2032</v>
+      </c>
+      <c r="N135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O135" t="inlineStr">
         <is>
           <t>2032</t>
         </is>
@@ -7066,9 +7868,15 @@
       <c r="L136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M136" t="inlineStr">
-        <is>
-          <t>1496</t>
+      <c r="M136" t="n">
+        <v>1496</v>
+      </c>
+      <c r="N136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>1512</t>
         </is>
       </c>
     </row>
@@ -7115,7 +7923,13 @@
       <c r="L137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M137" t="inlineStr">
+      <c r="M137" t="n">
+        <v>0</v>
+      </c>
+      <c r="N137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7164,7 +7978,13 @@
       <c r="L138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M138" t="inlineStr">
+      <c r="M138" t="n">
+        <v>0</v>
+      </c>
+      <c r="N138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7213,7 +8033,13 @@
       <c r="L139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M139" t="inlineStr">
+      <c r="M139" t="n">
+        <v>0</v>
+      </c>
+      <c r="N139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7262,9 +8088,15 @@
       <c r="L140" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="M140" t="inlineStr">
-        <is>
-          <t>3408</t>
+      <c r="M140" t="n">
+        <v>3408</v>
+      </c>
+      <c r="N140" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>3530</t>
         </is>
       </c>
     </row>
@@ -7311,7 +8143,13 @@
       <c r="L141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M141" t="inlineStr">
+      <c r="M141" t="n">
+        <v>0</v>
+      </c>
+      <c r="N141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7360,7 +8198,13 @@
       <c r="L142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M142" t="inlineStr">
+      <c r="M142" t="n">
+        <v>0</v>
+      </c>
+      <c r="N142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7409,9 +8253,15 @@
       <c r="L143" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M143" t="inlineStr">
-        <is>
-          <t>3551</t>
+      <c r="M143" t="n">
+        <v>3551</v>
+      </c>
+      <c r="N143" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O143" t="inlineStr">
+        <is>
+          <t>3757</t>
         </is>
       </c>
     </row>
@@ -7458,7 +8308,13 @@
       <c r="L144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M144" t="inlineStr">
+      <c r="M144" t="n">
+        <v>0</v>
+      </c>
+      <c r="N144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7507,9 +8363,15 @@
       <c r="L145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M145" t="inlineStr">
-        <is>
-          <t>2560</t>
+      <c r="M145" t="n">
+        <v>2560</v>
+      </c>
+      <c r="N145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O145" t="inlineStr">
+        <is>
+          <t>2601</t>
         </is>
       </c>
     </row>
@@ -7556,7 +8418,13 @@
       <c r="L146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M146" t="inlineStr">
+      <c r="M146" t="n">
+        <v>0</v>
+      </c>
+      <c r="N146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7605,9 +8473,15 @@
       <c r="L147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M147" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M147" t="n">
+        <v>0</v>
+      </c>
+      <c r="N147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O147" t="inlineStr">
+        <is>
+          <t>2513</t>
         </is>
       </c>
     </row>
@@ -7624,7 +8498,7 @@
       <c r="D148" t="inlineStr"/>
       <c r="E148" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F148" s="3" t="n">
@@ -7643,6 +8517,14 @@
       <c r="K148" t="inlineStr"/>
       <c r="L148" s="3" t="inlineStr"/>
       <c r="M148" t="inlineStr"/>
+      <c r="N148" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="O148" t="inlineStr">
+        <is>
+          <t>2759</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -7681,9 +8563,15 @@
       <c r="L149" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="M149" t="inlineStr">
-        <is>
-          <t>1343</t>
+      <c r="M149" t="n">
+        <v>1343</v>
+      </c>
+      <c r="N149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O149" t="inlineStr">
+        <is>
+          <t>1336</t>
         </is>
       </c>
     </row>
@@ -7724,17 +8612,21 @@
       <c r="L150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M150" t="inlineStr">
-        <is>
-          <t>1396</t>
+      <c r="M150" t="n">
+        <v>1396</v>
+      </c>
+      <c r="N150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O150" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>58340439</t>
-        </is>
+      <c r="A151" t="n">
+        <v>58340439</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
@@ -7757,17 +8649,21 @@
       <c r="L151" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M151" t="inlineStr">
-        <is>
-          <t>2167</t>
+      <c r="M151" t="n">
+        <v>2167</v>
+      </c>
+      <c r="N151" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O151" t="inlineStr">
+        <is>
+          <t>2256</t>
         </is>
       </c>
     </row>
     <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>57908454</t>
-        </is>
+      <c r="A152" t="n">
+        <v>57908454</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
@@ -7790,7 +8686,13 @@
       <c r="L152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M152" t="inlineStr">
+      <c r="M152" t="n">
+        <v>0</v>
+      </c>
+      <c r="N152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O152" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-01-07 11:31:31
</commit_message>
<xml_diff>
--- a/Season_Attack/81.xlsx
+++ b/Season_Attack/81.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O152"/>
+  <dimension ref="A1:Q154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,16 @@
           <t>01-05_0</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>01-06_A</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>01-06_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -516,9 +526,15 @@
       <c r="N2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>3201</t>
+      <c r="O2" t="n">
+        <v>3201</v>
+      </c>
+      <c r="P2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>3433</t>
         </is>
       </c>
     </row>
@@ -571,9 +587,15 @@
       <c r="N3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>3801</t>
+      <c r="O3" t="n">
+        <v>3801</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>3994</t>
         </is>
       </c>
     </row>
@@ -626,9 +648,15 @@
       <c r="N4" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>4068</t>
+      <c r="O4" t="n">
+        <v>4068</v>
+      </c>
+      <c r="P4" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>4297</t>
         </is>
       </c>
     </row>
@@ -681,9 +709,15 @@
       <c r="N5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>4048</t>
+      <c r="O5" t="n">
+        <v>4048</v>
+      </c>
+      <c r="P5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>4355</t>
         </is>
       </c>
     </row>
@@ -736,9 +770,15 @@
       <c r="N6" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>4093</t>
+      <c r="O6" t="n">
+        <v>4093</v>
+      </c>
+      <c r="P6" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>4412</t>
         </is>
       </c>
     </row>
@@ -791,9 +831,15 @@
       <c r="N7" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>4371</t>
+      <c r="O7" t="n">
+        <v>4371</v>
+      </c>
+      <c r="P7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>4700</t>
         </is>
       </c>
     </row>
@@ -846,9 +892,15 @@
       <c r="N8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>3889</t>
+      <c r="O8" t="n">
+        <v>3889</v>
+      </c>
+      <c r="P8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>4174</t>
         </is>
       </c>
     </row>
@@ -901,9 +953,15 @@
       <c r="N9" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>4076</t>
+      <c r="O9" t="n">
+        <v>4076</v>
+      </c>
+      <c r="P9" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>4320</t>
         </is>
       </c>
     </row>
@@ -956,9 +1014,15 @@
       <c r="N10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>3723</t>
+      <c r="O10" t="n">
+        <v>3723</v>
+      </c>
+      <c r="P10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>3971</t>
         </is>
       </c>
     </row>
@@ -1011,9 +1075,15 @@
       <c r="N11" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>3151</t>
+      <c r="O11" t="n">
+        <v>3151</v>
+      </c>
+      <c r="P11" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>3428</t>
         </is>
       </c>
     </row>
@@ -1066,9 +1136,15 @@
       <c r="N12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>3709</t>
+      <c r="O12" t="n">
+        <v>3709</v>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>3904</t>
         </is>
       </c>
     </row>
@@ -1121,9 +1197,15 @@
       <c r="N13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>2684</t>
+      <c r="O13" t="n">
+        <v>2684</v>
+      </c>
+      <c r="P13" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>2770</t>
         </is>
       </c>
     </row>
@@ -1176,9 +1258,15 @@
       <c r="N14" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>4421</t>
+      <c r="O14" t="n">
+        <v>4421</v>
+      </c>
+      <c r="P14" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>4753</t>
         </is>
       </c>
     </row>
@@ -1231,9 +1319,15 @@
       <c r="N15" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>4046</t>
+      <c r="O15" t="n">
+        <v>4046</v>
+      </c>
+      <c r="P15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>4290</t>
         </is>
       </c>
     </row>
@@ -1286,9 +1380,15 @@
       <c r="N16" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>4046</t>
+      <c r="O16" t="n">
+        <v>4046</v>
+      </c>
+      <c r="P16" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>4363</t>
         </is>
       </c>
     </row>
@@ -1341,9 +1441,15 @@
       <c r="N17" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>4063</t>
+      <c r="O17" t="n">
+        <v>4063</v>
+      </c>
+      <c r="P17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>4265</t>
         </is>
       </c>
     </row>
@@ -1396,9 +1502,15 @@
       <c r="N18" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>3872</t>
+      <c r="O18" t="n">
+        <v>3872</v>
+      </c>
+      <c r="P18" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>4086</t>
         </is>
       </c>
     </row>
@@ -1451,9 +1563,15 @@
       <c r="N19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>4213</t>
+      <c r="O19" t="n">
+        <v>4213</v>
+      </c>
+      <c r="P19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>4510</t>
         </is>
       </c>
     </row>
@@ -1506,9 +1624,15 @@
       <c r="N20" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>4119</t>
+      <c r="O20" t="n">
+        <v>4119</v>
+      </c>
+      <c r="P20" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>4315</t>
         </is>
       </c>
     </row>
@@ -1561,9 +1685,15 @@
       <c r="N21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>3386</t>
+      <c r="O21" t="n">
+        <v>3386</v>
+      </c>
+      <c r="P21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>3692</t>
         </is>
       </c>
     </row>
@@ -1616,9 +1746,15 @@
       <c r="N22" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>4162</t>
+      <c r="O22" t="n">
+        <v>4162</v>
+      </c>
+      <c r="P22" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>4413</t>
         </is>
       </c>
     </row>
@@ -1671,9 +1807,15 @@
       <c r="N23" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>2923</t>
+      <c r="O23" t="n">
+        <v>2923</v>
+      </c>
+      <c r="P23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>3315</t>
         </is>
       </c>
     </row>
@@ -1726,9 +1868,15 @@
       <c r="N24" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>3797</t>
+      <c r="O24" t="n">
+        <v>3797</v>
+      </c>
+      <c r="P24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>4114</t>
         </is>
       </c>
     </row>
@@ -1781,7 +1929,13 @@
       <c r="N25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O25" t="inlineStr">
+      <c r="O25" t="n">
+        <v>2500</v>
+      </c>
+      <c r="P25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1836,9 +1990,15 @@
       <c r="N26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>4179</t>
+      <c r="O26" t="n">
+        <v>4179</v>
+      </c>
+      <c r="P26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>4411</t>
         </is>
       </c>
     </row>
@@ -1891,9 +2051,15 @@
       <c r="N27" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>4188</t>
+      <c r="O27" t="n">
+        <v>4188</v>
+      </c>
+      <c r="P27" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>4578</t>
         </is>
       </c>
     </row>
@@ -1946,9 +2112,15 @@
       <c r="N28" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>3617</t>
+      <c r="O28" t="n">
+        <v>3617</v>
+      </c>
+      <c r="P28" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>3751</t>
         </is>
       </c>
     </row>
@@ -2001,9 +2173,15 @@
       <c r="N29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>3634</t>
+      <c r="O29" t="n">
+        <v>3634</v>
+      </c>
+      <c r="P29" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>3788</t>
         </is>
       </c>
     </row>
@@ -2056,9 +2234,15 @@
       <c r="N30" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>4346</t>
+      <c r="O30" t="n">
+        <v>4346</v>
+      </c>
+      <c r="P30" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>4516</t>
         </is>
       </c>
     </row>
@@ -2111,9 +2295,15 @@
       <c r="N31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>4008</t>
+      <c r="O31" t="n">
+        <v>4008</v>
+      </c>
+      <c r="P31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>4282</t>
         </is>
       </c>
     </row>
@@ -2166,9 +2356,15 @@
       <c r="N32" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>4325</t>
+      <c r="O32" t="n">
+        <v>4325</v>
+      </c>
+      <c r="P32" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>4737</t>
         </is>
       </c>
     </row>
@@ -2191,7 +2387,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F33" s="4" t="n">
@@ -2221,9 +2417,15 @@
       <c r="N33" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>4758</t>
+      <c r="O33" t="n">
+        <v>4758</v>
+      </c>
+      <c r="P33" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>4918</t>
         </is>
       </c>
     </row>
@@ -2276,7 +2478,13 @@
       <c r="N34" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="O34" t="inlineStr">
+      <c r="O34" t="n">
+        <v>2763</v>
+      </c>
+      <c r="P34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="inlineStr">
         <is>
           <t>2763</t>
         </is>
@@ -2331,9 +2539,15 @@
       <c r="N35" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>4224</t>
+      <c r="O35" t="n">
+        <v>4224</v>
+      </c>
+      <c r="P35" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>4544</t>
         </is>
       </c>
     </row>
@@ -2386,9 +2600,15 @@
       <c r="N36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>3665</t>
+      <c r="O36" t="n">
+        <v>3665</v>
+      </c>
+      <c r="P36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>3978</t>
         </is>
       </c>
     </row>
@@ -2441,9 +2661,15 @@
       <c r="N37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>3880</t>
+      <c r="O37" t="n">
+        <v>3880</v>
+      </c>
+      <c r="P37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>4040</t>
         </is>
       </c>
     </row>
@@ -2496,9 +2722,15 @@
       <c r="N38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>4256</t>
+      <c r="O38" t="n">
+        <v>4256</v>
+      </c>
+      <c r="P38" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>4531</t>
         </is>
       </c>
     </row>
@@ -2551,9 +2783,15 @@
       <c r="N39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>4045</t>
+      <c r="O39" t="n">
+        <v>4045</v>
+      </c>
+      <c r="P39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>4200</t>
         </is>
       </c>
     </row>
@@ -2606,9 +2844,15 @@
       <c r="N40" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>4148</t>
+      <c r="O40" t="n">
+        <v>4148</v>
+      </c>
+      <c r="P40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>4638</t>
         </is>
       </c>
     </row>
@@ -2661,9 +2905,15 @@
       <c r="N41" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>4241</t>
+      <c r="O41" t="n">
+        <v>4241</v>
+      </c>
+      <c r="P41" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>4614</t>
         </is>
       </c>
     </row>
@@ -2716,9 +2966,15 @@
       <c r="N42" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>4525</t>
+      <c r="O42" t="n">
+        <v>4525</v>
+      </c>
+      <c r="P42" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>4706</t>
         </is>
       </c>
     </row>
@@ -2771,9 +3027,15 @@
       <c r="N43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>4037</t>
+      <c r="O43" t="n">
+        <v>4037</v>
+      </c>
+      <c r="P43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>4349</t>
         </is>
       </c>
     </row>
@@ -2826,9 +3088,15 @@
       <c r="N44" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>3260</t>
+      <c r="O44" t="n">
+        <v>3260</v>
+      </c>
+      <c r="P44" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>3325</t>
         </is>
       </c>
     </row>
@@ -2881,9 +3149,15 @@
       <c r="N45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>3776</t>
+      <c r="O45" t="n">
+        <v>3776</v>
+      </c>
+      <c r="P45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>3951</t>
         </is>
       </c>
     </row>
@@ -2936,9 +3210,15 @@
       <c r="N46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>3853</t>
+      <c r="O46" t="n">
+        <v>3853</v>
+      </c>
+      <c r="P46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>4030</t>
         </is>
       </c>
     </row>
@@ -2991,9 +3271,15 @@
       <c r="N47" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>3948</t>
+      <c r="O47" t="n">
+        <v>3948</v>
+      </c>
+      <c r="P47" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>4141</t>
         </is>
       </c>
     </row>
@@ -3046,9 +3332,15 @@
       <c r="N48" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>4000</t>
+      <c r="O48" t="n">
+        <v>4000</v>
+      </c>
+      <c r="P48" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>4280</t>
         </is>
       </c>
     </row>
@@ -3101,9 +3393,15 @@
       <c r="N49" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>3547</t>
+      <c r="O49" t="n">
+        <v>3547</v>
+      </c>
+      <c r="P49" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>3809</t>
         </is>
       </c>
     </row>
@@ -3156,9 +3454,15 @@
       <c r="N50" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>3922</t>
+      <c r="O50" t="n">
+        <v>3922</v>
+      </c>
+      <c r="P50" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>4167</t>
         </is>
       </c>
     </row>
@@ -3181,7 +3485,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F51" s="3" t="n">
@@ -3211,9 +3515,15 @@
       <c r="N51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>3682</t>
+      <c r="O51" t="n">
+        <v>3682</v>
+      </c>
+      <c r="P51" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>3949</t>
         </is>
       </c>
     </row>
@@ -3266,7 +3576,13 @@
       <c r="N52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O52" t="inlineStr">
+      <c r="O52" t="n">
+        <v>2574</v>
+      </c>
+      <c r="P52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="inlineStr">
         <is>
           <t>2574</t>
         </is>
@@ -3321,9 +3637,15 @@
       <c r="N53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>2917</t>
+      <c r="O53" t="n">
+        <v>2917</v>
+      </c>
+      <c r="P53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>2993</t>
         </is>
       </c>
     </row>
@@ -3376,9 +3698,15 @@
       <c r="N54" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>2834</t>
+      <c r="O54" t="n">
+        <v>2834</v>
+      </c>
+      <c r="P54" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>2910</t>
         </is>
       </c>
     </row>
@@ -3431,9 +3759,15 @@
       <c r="N55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>3316</t>
+      <c r="O55" t="n">
+        <v>3316</v>
+      </c>
+      <c r="P55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>3525</t>
         </is>
       </c>
     </row>
@@ -3486,9 +3820,15 @@
       <c r="N56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>3587</t>
+      <c r="O56" t="n">
+        <v>3587</v>
+      </c>
+      <c r="P56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>3721</t>
         </is>
       </c>
     </row>
@@ -3541,9 +3881,15 @@
       <c r="N57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>3815</t>
+      <c r="O57" t="n">
+        <v>3815</v>
+      </c>
+      <c r="P57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>4067</t>
         </is>
       </c>
     </row>
@@ -3596,9 +3942,15 @@
       <c r="N58" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>3343</t>
+      <c r="O58" t="n">
+        <v>3343</v>
+      </c>
+      <c r="P58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>3557</t>
         </is>
       </c>
     </row>
@@ -3651,9 +4003,15 @@
       <c r="N59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>3790</t>
+      <c r="O59" t="n">
+        <v>3790</v>
+      </c>
+      <c r="P59" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>3981</t>
         </is>
       </c>
     </row>
@@ -3706,9 +4064,15 @@
       <c r="N60" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>3988</t>
+      <c r="O60" t="n">
+        <v>3988</v>
+      </c>
+      <c r="P60" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>4209</t>
         </is>
       </c>
     </row>
@@ -3761,9 +4125,15 @@
       <c r="N61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>3894</t>
+      <c r="O61" t="n">
+        <v>3894</v>
+      </c>
+      <c r="P61" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>4094</t>
         </is>
       </c>
     </row>
@@ -3816,9 +4186,15 @@
       <c r="N62" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>3868</t>
+      <c r="O62" t="n">
+        <v>3868</v>
+      </c>
+      <c r="P62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>4037</t>
         </is>
       </c>
     </row>
@@ -3871,9 +4247,15 @@
       <c r="N63" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>3414</t>
+      <c r="O63" t="n">
+        <v>3414</v>
+      </c>
+      <c r="P63" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>3630</t>
         </is>
       </c>
     </row>
@@ -3926,9 +4308,15 @@
       <c r="N64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>2514</t>
+      <c r="O64" t="n">
+        <v>2514</v>
+      </c>
+      <c r="P64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>2544</t>
         </is>
       </c>
     </row>
@@ -3981,9 +4369,15 @@
       <c r="N65" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>3377</t>
+      <c r="O65" t="n">
+        <v>3377</v>
+      </c>
+      <c r="P65" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>3528</t>
         </is>
       </c>
     </row>
@@ -4036,9 +4430,15 @@
       <c r="N66" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>3204</t>
+      <c r="O66" t="n">
+        <v>3204</v>
+      </c>
+      <c r="P66" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>3463</t>
         </is>
       </c>
     </row>
@@ -4091,9 +4491,15 @@
       <c r="N67" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>4007</t>
+      <c r="O67" t="n">
+        <v>4007</v>
+      </c>
+      <c r="P67" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>4242</t>
         </is>
       </c>
     </row>
@@ -4146,9 +4552,15 @@
       <c r="N68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O68" t="inlineStr">
-        <is>
-          <t>3432</t>
+      <c r="O68" t="n">
+        <v>3432</v>
+      </c>
+      <c r="P68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>3561</t>
         </is>
       </c>
     </row>
@@ -4201,9 +4613,15 @@
       <c r="N69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>2636</t>
+      <c r="O69" t="n">
+        <v>2636</v>
+      </c>
+      <c r="P69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>2665</t>
         </is>
       </c>
     </row>
@@ -4256,9 +4674,15 @@
       <c r="N70" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>3097</t>
+      <c r="O70" t="n">
+        <v>3097</v>
+      </c>
+      <c r="P70" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>3214</t>
         </is>
       </c>
     </row>
@@ -4311,9 +4735,15 @@
       <c r="N71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O71" t="inlineStr">
-        <is>
-          <t>4093</t>
+      <c r="O71" t="n">
+        <v>4093</v>
+      </c>
+      <c r="P71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>4303</t>
         </is>
       </c>
     </row>
@@ -4366,9 +4796,15 @@
       <c r="N72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>3493</t>
+      <c r="O72" t="n">
+        <v>3493</v>
+      </c>
+      <c r="P72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>3469</t>
         </is>
       </c>
     </row>
@@ -4421,9 +4857,15 @@
       <c r="N73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>3803</t>
+      <c r="O73" t="n">
+        <v>3803</v>
+      </c>
+      <c r="P73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>4036</t>
         </is>
       </c>
     </row>
@@ -4476,9 +4918,15 @@
       <c r="N74" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>3547</t>
+      <c r="O74" t="n">
+        <v>3547</v>
+      </c>
+      <c r="P74" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>3704</t>
         </is>
       </c>
     </row>
@@ -4531,9 +4979,15 @@
       <c r="N75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>3727</t>
+      <c r="O75" t="n">
+        <v>3727</v>
+      </c>
+      <c r="P75" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>3885</t>
         </is>
       </c>
     </row>
@@ -4586,9 +5040,15 @@
       <c r="N76" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>3585</t>
+      <c r="O76" t="n">
+        <v>3585</v>
+      </c>
+      <c r="P76" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>3770</t>
         </is>
       </c>
     </row>
@@ -4641,9 +5101,15 @@
       <c r="N77" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>2822</t>
+      <c r="O77" t="n">
+        <v>2822</v>
+      </c>
+      <c r="P77" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>2850</t>
         </is>
       </c>
     </row>
@@ -4696,9 +5162,15 @@
       <c r="N78" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>3497</t>
+      <c r="O78" t="n">
+        <v>3497</v>
+      </c>
+      <c r="P78" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>3740</t>
         </is>
       </c>
     </row>
@@ -4751,9 +5223,15 @@
       <c r="N79" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>3465</t>
+      <c r="O79" t="n">
+        <v>3465</v>
+      </c>
+      <c r="P79" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>3721</t>
         </is>
       </c>
     </row>
@@ -4806,9 +5284,15 @@
       <c r="N80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>3015</t>
+      <c r="O80" t="n">
+        <v>3015</v>
+      </c>
+      <c r="P80" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>3174</t>
         </is>
       </c>
     </row>
@@ -4861,9 +5345,15 @@
       <c r="N81" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>2773</t>
+      <c r="O81" t="n">
+        <v>2773</v>
+      </c>
+      <c r="P81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>2823</t>
         </is>
       </c>
     </row>
@@ -4916,9 +5406,15 @@
       <c r="N82" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>3606</t>
+      <c r="O82" t="n">
+        <v>3606</v>
+      </c>
+      <c r="P82" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>3956</t>
         </is>
       </c>
     </row>
@@ -4971,9 +5467,15 @@
       <c r="N83" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>2735</t>
+      <c r="O83" t="n">
+        <v>2735</v>
+      </c>
+      <c r="P83" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>2761</t>
         </is>
       </c>
     </row>
@@ -5026,9 +5528,15 @@
       <c r="N84" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>2984</t>
+      <c r="O84" t="n">
+        <v>2984</v>
+      </c>
+      <c r="P84" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>3009</t>
         </is>
       </c>
     </row>
@@ -5081,9 +5589,15 @@
       <c r="N85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>2016</t>
+      <c r="O85" t="n">
+        <v>2016</v>
+      </c>
+      <c r="P85" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>2050</t>
         </is>
       </c>
     </row>
@@ -5136,9 +5650,15 @@
       <c r="N86" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>2566</t>
+      <c r="O86" t="n">
+        <v>2566</v>
+      </c>
+      <c r="P86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>2535</t>
         </is>
       </c>
     </row>
@@ -5191,9 +5711,15 @@
       <c r="N87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>2908</t>
+      <c r="O87" t="n">
+        <v>2908</v>
+      </c>
+      <c r="P87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>2911</t>
         </is>
       </c>
     </row>
@@ -5246,9 +5772,15 @@
       <c r="N88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>2017</t>
+      <c r="O88" t="n">
+        <v>2017</v>
+      </c>
+      <c r="P88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>2026</t>
         </is>
       </c>
     </row>
@@ -5300,6 +5832,8 @@
       </c>
       <c r="N89" s="3" t="inlineStr"/>
       <c r="O89" t="inlineStr"/>
+      <c r="P89" s="3" t="inlineStr"/>
+      <c r="Q89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -5349,6 +5883,8 @@
       </c>
       <c r="N90" s="3" t="inlineStr"/>
       <c r="O90" t="inlineStr"/>
+      <c r="P90" s="3" t="inlineStr"/>
+      <c r="Q90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -5399,9 +5935,15 @@
       <c r="N91" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>2536</t>
+      <c r="O91" t="n">
+        <v>2536</v>
+      </c>
+      <c r="P91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>2520</t>
         </is>
       </c>
     </row>
@@ -5454,9 +5996,15 @@
       <c r="N92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>2923</t>
+      <c r="O92" t="n">
+        <v>2923</v>
+      </c>
+      <c r="P92" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>3000</t>
         </is>
       </c>
     </row>
@@ -5509,9 +6057,15 @@
       <c r="N93" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>2777</t>
+      <c r="O93" t="n">
+        <v>2777</v>
+      </c>
+      <c r="P93" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>2779</t>
         </is>
       </c>
     </row>
@@ -5564,9 +6118,15 @@
       <c r="N94" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O94" t="inlineStr">
-        <is>
-          <t>3575</t>
+      <c r="O94" t="n">
+        <v>3575</v>
+      </c>
+      <c r="P94" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>3699</t>
         </is>
       </c>
     </row>
@@ -5619,9 +6179,15 @@
       <c r="N95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>3376</t>
+      <c r="O95" t="n">
+        <v>3376</v>
+      </c>
+      <c r="P95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>3499</t>
         </is>
       </c>
     </row>
@@ -5674,9 +6240,15 @@
       <c r="N96" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>3159</t>
+      <c r="O96" t="n">
+        <v>3159</v>
+      </c>
+      <c r="P96" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>3313</t>
         </is>
       </c>
     </row>
@@ -5729,9 +6301,15 @@
       <c r="N97" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>3537</t>
+      <c r="O97" t="n">
+        <v>3537</v>
+      </c>
+      <c r="P97" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>3717</t>
         </is>
       </c>
     </row>
@@ -5784,9 +6362,15 @@
       <c r="N98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O98" t="inlineStr">
-        <is>
-          <t>3266</t>
+      <c r="O98" t="n">
+        <v>3266</v>
+      </c>
+      <c r="P98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>3285</t>
         </is>
       </c>
     </row>
@@ -5839,9 +6423,15 @@
       <c r="N99" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O99" t="inlineStr">
-        <is>
-          <t>2721</t>
+      <c r="O99" t="n">
+        <v>2721</v>
+      </c>
+      <c r="P99" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>2732</t>
         </is>
       </c>
     </row>
@@ -5894,9 +6484,15 @@
       <c r="N100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O100" t="inlineStr">
-        <is>
-          <t>2599</t>
+      <c r="O100" t="n">
+        <v>2599</v>
+      </c>
+      <c r="P100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>2583</t>
         </is>
       </c>
     </row>
@@ -5949,9 +6545,15 @@
       <c r="N101" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O101" t="inlineStr">
-        <is>
-          <t>3677</t>
+      <c r="O101" t="n">
+        <v>3677</v>
+      </c>
+      <c r="P101" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q101" t="inlineStr">
+        <is>
+          <t>3821</t>
         </is>
       </c>
     </row>
@@ -6004,9 +6606,15 @@
       <c r="N102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O102" t="inlineStr">
-        <is>
-          <t>3074</t>
+      <c r="O102" t="n">
+        <v>3074</v>
+      </c>
+      <c r="P102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>3254</t>
         </is>
       </c>
     </row>
@@ -6059,9 +6667,15 @@
       <c r="N103" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="O103" t="inlineStr">
-        <is>
-          <t>2997</t>
+      <c r="O103" t="n">
+        <v>2997</v>
+      </c>
+      <c r="P103" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>3176</t>
         </is>
       </c>
     </row>
@@ -6114,9 +6728,15 @@
       <c r="N104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O104" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="O104" t="n">
+        <v>2498</v>
+      </c>
+      <c r="P104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>2558</t>
         </is>
       </c>
     </row>
@@ -6169,9 +6789,15 @@
       <c r="N105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O105" t="inlineStr">
-        <is>
-          <t>3069</t>
+      <c r="O105" t="n">
+        <v>3069</v>
+      </c>
+      <c r="P105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>3059</t>
         </is>
       </c>
     </row>
@@ -6224,9 +6850,15 @@
       <c r="N106" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O106" t="inlineStr">
-        <is>
-          <t>2857</t>
+      <c r="O106" t="n">
+        <v>2857</v>
+      </c>
+      <c r="P106" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>2808</t>
         </is>
       </c>
     </row>
@@ -6279,9 +6911,15 @@
       <c r="N107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O107" t="inlineStr">
-        <is>
-          <t>3016</t>
+      <c r="O107" t="n">
+        <v>3016</v>
+      </c>
+      <c r="P107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>3155</t>
         </is>
       </c>
     </row>
@@ -6334,9 +6972,15 @@
       <c r="N108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O108" t="inlineStr">
-        <is>
-          <t>2390</t>
+      <c r="O108" t="n">
+        <v>2390</v>
+      </c>
+      <c r="P108" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>2453</t>
         </is>
       </c>
     </row>
@@ -6389,9 +7033,15 @@
       <c r="N109" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="O109" t="inlineStr">
-        <is>
-          <t>2535</t>
+      <c r="O109" t="n">
+        <v>2535</v>
+      </c>
+      <c r="P109" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>2587</t>
         </is>
       </c>
     </row>
@@ -6444,9 +7094,15 @@
       <c r="N110" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="O110" t="inlineStr">
-        <is>
-          <t>3039</t>
+      <c r="O110" t="n">
+        <v>3039</v>
+      </c>
+      <c r="P110" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>3119</t>
         </is>
       </c>
     </row>
@@ -6499,9 +7155,15 @@
       <c r="N111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O111" t="inlineStr">
-        <is>
-          <t>2743</t>
+      <c r="O111" t="n">
+        <v>2743</v>
+      </c>
+      <c r="P111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>2787</t>
         </is>
       </c>
     </row>
@@ -6554,9 +7216,15 @@
       <c r="N112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O112" t="inlineStr">
-        <is>
-          <t>2960</t>
+      <c r="O112" t="n">
+        <v>2960</v>
+      </c>
+      <c r="P112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>3065</t>
         </is>
       </c>
     </row>
@@ -6609,9 +7277,15 @@
       <c r="N113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O113" t="inlineStr">
-        <is>
-          <t>2568</t>
+      <c r="O113" t="n">
+        <v>2568</v>
+      </c>
+      <c r="P113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>2534</t>
         </is>
       </c>
     </row>
@@ -6664,9 +7338,15 @@
       <c r="N114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O114" t="inlineStr">
-        <is>
-          <t>2968</t>
+      <c r="O114" t="n">
+        <v>2968</v>
+      </c>
+      <c r="P114" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>3108</t>
         </is>
       </c>
     </row>
@@ -6719,9 +7399,15 @@
       <c r="N115" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O115" t="inlineStr">
-        <is>
-          <t>2705</t>
+      <c r="O115" t="n">
+        <v>2705</v>
+      </c>
+      <c r="P115" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>2634</t>
         </is>
       </c>
     </row>
@@ -6774,9 +7460,15 @@
       <c r="N116" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="O116" t="inlineStr">
-        <is>
-          <t>2717</t>
+      <c r="O116" t="n">
+        <v>2717</v>
+      </c>
+      <c r="P116" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>2862</t>
         </is>
       </c>
     </row>
@@ -6829,9 +7521,15 @@
       <c r="N117" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O117" t="inlineStr">
-        <is>
-          <t>2864</t>
+      <c r="O117" t="n">
+        <v>2864</v>
+      </c>
+      <c r="P117" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>2917</t>
         </is>
       </c>
     </row>
@@ -6884,7 +7582,13 @@
       <c r="N118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O118" t="inlineStr">
+      <c r="O118" t="n">
+        <v>0</v>
+      </c>
+      <c r="P118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6939,9 +7643,15 @@
       <c r="N119" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O119" t="inlineStr">
-        <is>
-          <t>2979</t>
+      <c r="O119" t="n">
+        <v>2979</v>
+      </c>
+      <c r="P119" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>3027</t>
         </is>
       </c>
     </row>
@@ -6994,9 +7704,15 @@
       <c r="N120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O120" t="inlineStr">
-        <is>
-          <t>2890</t>
+      <c r="O120" t="n">
+        <v>2890</v>
+      </c>
+      <c r="P120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>2982</t>
         </is>
       </c>
     </row>
@@ -7049,9 +7765,15 @@
       <c r="N121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O121" t="inlineStr">
-        <is>
-          <t>2053</t>
+      <c r="O121" t="n">
+        <v>2053</v>
+      </c>
+      <c r="P121" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>2218</t>
         </is>
       </c>
     </row>
@@ -7104,9 +7826,15 @@
       <c r="N122" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="O122" t="inlineStr">
-        <is>
-          <t>2445</t>
+      <c r="O122" t="n">
+        <v>2445</v>
+      </c>
+      <c r="P122" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -7159,9 +7887,15 @@
       <c r="N123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O123" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="O123" t="n">
+        <v>2498</v>
+      </c>
+      <c r="P123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q123" t="inlineStr">
+        <is>
+          <t>2505</t>
         </is>
       </c>
     </row>
@@ -7214,9 +7948,15 @@
       <c r="N124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O124" t="inlineStr">
-        <is>
-          <t>2993</t>
+      <c r="O124" t="n">
+        <v>2993</v>
+      </c>
+      <c r="P124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>3060</t>
         </is>
       </c>
     </row>
@@ -7269,7 +8009,13 @@
       <c r="N125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O125" t="inlineStr">
+      <c r="O125" t="n">
+        <v>0</v>
+      </c>
+      <c r="P125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7324,9 +8070,15 @@
       <c r="N126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O126" t="inlineStr">
-        <is>
-          <t>2699</t>
+      <c r="O126" t="n">
+        <v>2699</v>
+      </c>
+      <c r="P126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>2899</t>
         </is>
       </c>
     </row>
@@ -7379,9 +8131,15 @@
       <c r="N127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O127" t="inlineStr">
-        <is>
-          <t>2514</t>
+      <c r="O127" t="n">
+        <v>2514</v>
+      </c>
+      <c r="P127" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>2667</t>
         </is>
       </c>
     </row>
@@ -7434,9 +8192,15 @@
       <c r="N128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O128" t="inlineStr">
-        <is>
-          <t>2456</t>
+      <c r="O128" t="n">
+        <v>2456</v>
+      </c>
+      <c r="P128" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q128" t="inlineStr">
+        <is>
+          <t>2458</t>
         </is>
       </c>
     </row>
@@ -7489,9 +8253,15 @@
       <c r="N129" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="O129" t="inlineStr">
-        <is>
-          <t>2353</t>
+      <c r="O129" t="n">
+        <v>2353</v>
+      </c>
+      <c r="P129" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q129" t="inlineStr">
+        <is>
+          <t>2419</t>
         </is>
       </c>
     </row>
@@ -7544,9 +8314,15 @@
       <c r="N130" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="O130" t="inlineStr">
-        <is>
-          <t>1708</t>
+      <c r="O130" t="n">
+        <v>1708</v>
+      </c>
+      <c r="P130" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q130" t="inlineStr">
+        <is>
+          <t>1942</t>
         </is>
       </c>
     </row>
@@ -7599,7 +8375,13 @@
       <c r="N131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O131" t="inlineStr">
+      <c r="O131" t="n">
+        <v>0</v>
+      </c>
+      <c r="P131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7654,9 +8436,15 @@
       <c r="N132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O132" t="inlineStr">
-        <is>
-          <t>1494</t>
+      <c r="O132" t="n">
+        <v>1494</v>
+      </c>
+      <c r="P132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q132" t="inlineStr">
+        <is>
+          <t>1511</t>
         </is>
       </c>
     </row>
@@ -7709,7 +8497,13 @@
       <c r="N133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O133" t="inlineStr">
+      <c r="O133" t="n">
+        <v>0</v>
+      </c>
+      <c r="P133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7764,9 +8558,15 @@
       <c r="N134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O134" t="inlineStr">
-        <is>
-          <t>1944</t>
+      <c r="O134" t="n">
+        <v>1944</v>
+      </c>
+      <c r="P134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>1950</t>
         </is>
       </c>
     </row>
@@ -7819,9 +8619,15 @@
       <c r="N135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O135" t="inlineStr">
-        <is>
-          <t>2032</t>
+      <c r="O135" t="n">
+        <v>2032</v>
+      </c>
+      <c r="P135" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q135" t="inlineStr">
+        <is>
+          <t>2272</t>
         </is>
       </c>
     </row>
@@ -7874,9 +8680,15 @@
       <c r="N136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O136" t="inlineStr">
-        <is>
-          <t>1512</t>
+      <c r="O136" t="n">
+        <v>1512</v>
+      </c>
+      <c r="P136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>1528</t>
         </is>
       </c>
     </row>
@@ -7929,7 +8741,13 @@
       <c r="N137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O137" t="inlineStr">
+      <c r="O137" t="n">
+        <v>0</v>
+      </c>
+      <c r="P137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7984,7 +8802,13 @@
       <c r="N138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O138" t="inlineStr">
+      <c r="O138" t="n">
+        <v>0</v>
+      </c>
+      <c r="P138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8039,7 +8863,13 @@
       <c r="N139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O139" t="inlineStr">
+      <c r="O139" t="n">
+        <v>0</v>
+      </c>
+      <c r="P139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8094,9 +8924,15 @@
       <c r="N140" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="O140" t="inlineStr">
-        <is>
-          <t>3530</t>
+      <c r="O140" t="n">
+        <v>3530</v>
+      </c>
+      <c r="P140" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -8149,7 +8985,13 @@
       <c r="N141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O141" t="inlineStr">
+      <c r="O141" t="n">
+        <v>0</v>
+      </c>
+      <c r="P141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8204,7 +9046,13 @@
       <c r="N142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O142" t="inlineStr">
+      <c r="O142" t="n">
+        <v>0</v>
+      </c>
+      <c r="P142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8259,9 +9107,15 @@
       <c r="N143" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O143" t="inlineStr">
-        <is>
-          <t>3757</t>
+      <c r="O143" t="n">
+        <v>3757</v>
+      </c>
+      <c r="P143" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q143" t="inlineStr">
+        <is>
+          <t>4101</t>
         </is>
       </c>
     </row>
@@ -8314,7 +9168,13 @@
       <c r="N144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O144" t="inlineStr">
+      <c r="O144" t="n">
+        <v>0</v>
+      </c>
+      <c r="P144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8369,9 +9229,15 @@
       <c r="N145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O145" t="inlineStr">
-        <is>
-          <t>2601</t>
+      <c r="O145" t="n">
+        <v>2601</v>
+      </c>
+      <c r="P145" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q145" t="inlineStr">
+        <is>
+          <t>2804</t>
         </is>
       </c>
     </row>
@@ -8424,7 +9290,13 @@
       <c r="N146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O146" t="inlineStr">
+      <c r="O146" t="n">
+        <v>0</v>
+      </c>
+      <c r="P146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8479,9 +9351,15 @@
       <c r="N147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O147" t="inlineStr">
-        <is>
-          <t>2513</t>
+      <c r="O147" t="n">
+        <v>2513</v>
+      </c>
+      <c r="P147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>2578</t>
         </is>
       </c>
     </row>
@@ -8520,11 +9398,11 @@
       <c r="N148" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="O148" t="inlineStr">
-        <is>
-          <t>2759</t>
-        </is>
-      </c>
+      <c r="O148" t="n">
+        <v>2759</v>
+      </c>
+      <c r="P148" s="3" t="inlineStr"/>
+      <c r="Q148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -8569,9 +9447,15 @@
       <c r="N149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O149" t="inlineStr">
-        <is>
-          <t>1336</t>
+      <c r="O149" t="n">
+        <v>1336</v>
+      </c>
+      <c r="P149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q149" t="inlineStr">
+        <is>
+          <t>1328</t>
         </is>
       </c>
     </row>
@@ -8618,9 +9502,15 @@
       <c r="N150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O150" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="O150" t="n">
+        <v>0</v>
+      </c>
+      <c r="P150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q150" t="inlineStr">
+        <is>
+          <t>1411</t>
         </is>
       </c>
     </row>
@@ -8655,9 +9545,15 @@
       <c r="N151" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O151" t="inlineStr">
-        <is>
-          <t>2256</t>
+      <c r="O151" t="n">
+        <v>2256</v>
+      </c>
+      <c r="P151" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q151" t="inlineStr">
+        <is>
+          <t>2310</t>
         </is>
       </c>
     </row>
@@ -8692,9 +9588,89 @@
       <c r="N152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O152" t="inlineStr">
+      <c r="O152" t="n">
+        <v>0</v>
+      </c>
+      <c r="P152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q152" t="inlineStr">
         <is>
           <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>51841127</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>"Muhammad Shox"</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr"/>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F153" s="3" t="inlineStr"/>
+      <c r="G153" t="inlineStr"/>
+      <c r="H153" s="3" t="inlineStr"/>
+      <c r="I153" t="inlineStr"/>
+      <c r="J153" s="3" t="inlineStr"/>
+      <c r="K153" t="inlineStr"/>
+      <c r="L153" s="3" t="inlineStr"/>
+      <c r="M153" t="inlineStr"/>
+      <c r="N153" s="3" t="inlineStr"/>
+      <c r="O153" t="inlineStr"/>
+      <c r="P153" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q153" t="inlineStr">
+        <is>
+          <t>3492</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>58437456</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>中国人不骗中国人</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr"/>
+      <c r="D154" t="inlineStr"/>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F154" s="3" t="inlineStr"/>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" s="3" t="inlineStr"/>
+      <c r="I154" t="inlineStr"/>
+      <c r="J154" s="3" t="inlineStr"/>
+      <c r="K154" t="inlineStr"/>
+      <c r="L154" s="3" t="inlineStr"/>
+      <c r="M154" t="inlineStr"/>
+      <c r="N154" s="3" t="inlineStr"/>
+      <c r="O154" t="inlineStr"/>
+      <c r="P154" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q154" t="inlineStr">
+        <is>
+          <t>1671</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-08 11:30:49
</commit_message>
<xml_diff>
--- a/Season_Attack/81.xlsx
+++ b/Season_Attack/81.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q154"/>
+  <dimension ref="A1:S155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,16 @@
           <t>01-06_0</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>01-07_A</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>01-07_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -532,9 +542,15 @@
       <c r="P2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>3433</t>
+      <c r="Q2" t="n">
+        <v>3433</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>3475</t>
         </is>
       </c>
     </row>
@@ -593,9 +609,15 @@
       <c r="P3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>3994</t>
+      <c r="Q3" t="n">
+        <v>3994</v>
+      </c>
+      <c r="R3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>4183</t>
         </is>
       </c>
     </row>
@@ -654,9 +676,15 @@
       <c r="P4" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>4297</t>
+      <c r="Q4" t="n">
+        <v>4297</v>
+      </c>
+      <c r="R4" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>4504</t>
         </is>
       </c>
     </row>
@@ -679,7 +707,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F5" s="3" t="n">
@@ -715,9 +743,15 @@
       <c r="P5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>4355</t>
+      <c r="Q5" t="n">
+        <v>4355</v>
+      </c>
+      <c r="R5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>4673</t>
         </is>
       </c>
     </row>
@@ -776,9 +810,15 @@
       <c r="P6" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>4412</t>
+      <c r="Q6" t="n">
+        <v>4412</v>
+      </c>
+      <c r="R6" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>4705</t>
         </is>
       </c>
     </row>
@@ -837,9 +877,15 @@
       <c r="P7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>4700</t>
+      <c r="Q7" t="n">
+        <v>4700</v>
+      </c>
+      <c r="R7" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>4933</t>
         </is>
       </c>
     </row>
@@ -898,9 +944,15 @@
       <c r="P8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>4174</t>
+      <c r="Q8" t="n">
+        <v>4174</v>
+      </c>
+      <c r="R8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>4364</t>
         </is>
       </c>
     </row>
@@ -959,9 +1011,15 @@
       <c r="P9" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>4320</t>
+      <c r="Q9" t="n">
+        <v>4320</v>
+      </c>
+      <c r="R9" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>4591</t>
         </is>
       </c>
     </row>
@@ -1020,9 +1078,15 @@
       <c r="P10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>3971</t>
+      <c r="Q10" t="n">
+        <v>3971</v>
+      </c>
+      <c r="R10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>4048</t>
         </is>
       </c>
     </row>
@@ -1081,9 +1145,15 @@
       <c r="P11" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>3428</t>
+      <c r="Q11" t="n">
+        <v>3428</v>
+      </c>
+      <c r="R11" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>4201</t>
         </is>
       </c>
     </row>
@@ -1142,9 +1212,15 @@
       <c r="P12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>3904</t>
+      <c r="Q12" t="n">
+        <v>3904</v>
+      </c>
+      <c r="R12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>4119</t>
         </is>
       </c>
     </row>
@@ -1203,7 +1279,13 @@
       <c r="P13" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="Q13" t="inlineStr">
+      <c r="Q13" t="n">
+        <v>2770</v>
+      </c>
+      <c r="R13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="inlineStr">
         <is>
           <t>2770</t>
         </is>
@@ -1264,9 +1346,15 @@
       <c r="P14" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>4753</t>
+      <c r="Q14" t="n">
+        <v>4753</v>
+      </c>
+      <c r="R14" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>5104</t>
         </is>
       </c>
     </row>
@@ -1325,9 +1413,15 @@
       <c r="P15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>4290</t>
+      <c r="Q15" t="n">
+        <v>4290</v>
+      </c>
+      <c r="R15" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>4513</t>
         </is>
       </c>
     </row>
@@ -1386,9 +1480,15 @@
       <c r="P16" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>4363</t>
+      <c r="Q16" t="n">
+        <v>4363</v>
+      </c>
+      <c r="R16" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>4523</t>
         </is>
       </c>
     </row>
@@ -1447,9 +1547,15 @@
       <c r="P17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>4265</t>
+      <c r="Q17" t="n">
+        <v>4265</v>
+      </c>
+      <c r="R17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>4451</t>
         </is>
       </c>
     </row>
@@ -1508,9 +1614,15 @@
       <c r="P18" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>4086</t>
+      <c r="Q18" t="n">
+        <v>4086</v>
+      </c>
+      <c r="R18" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>4228</t>
         </is>
       </c>
     </row>
@@ -1569,9 +1681,15 @@
       <c r="P19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>4510</t>
+      <c r="Q19" t="n">
+        <v>4510</v>
+      </c>
+      <c r="R19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>4813</t>
         </is>
       </c>
     </row>
@@ -1630,9 +1748,15 @@
       <c r="P20" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>4315</t>
+      <c r="Q20" t="n">
+        <v>4315</v>
+      </c>
+      <c r="R20" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>4608</t>
         </is>
       </c>
     </row>
@@ -1691,9 +1815,15 @@
       <c r="P21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>3692</t>
+      <c r="Q21" t="n">
+        <v>3692</v>
+      </c>
+      <c r="R21" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>4119</t>
         </is>
       </c>
     </row>
@@ -1752,9 +1882,15 @@
       <c r="P22" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>4413</t>
+      <c r="Q22" t="n">
+        <v>4413</v>
+      </c>
+      <c r="R22" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>4646</t>
         </is>
       </c>
     </row>
@@ -1813,9 +1949,15 @@
       <c r="P23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>3315</t>
+      <c r="Q23" t="n">
+        <v>3315</v>
+      </c>
+      <c r="R23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>4029</t>
         </is>
       </c>
     </row>
@@ -1874,9 +2016,15 @@
       <c r="P24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>4114</t>
+      <c r="Q24" t="n">
+        <v>4114</v>
+      </c>
+      <c r="R24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>4354</t>
         </is>
       </c>
     </row>
@@ -1935,7 +2083,13 @@
       <c r="P25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q25" t="inlineStr">
+      <c r="Q25" t="n">
+        <v>2500</v>
+      </c>
+      <c r="R25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1996,9 +2150,15 @@
       <c r="P26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>4411</t>
+      <c r="Q26" t="n">
+        <v>4411</v>
+      </c>
+      <c r="R26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>4593</t>
         </is>
       </c>
     </row>
@@ -2057,9 +2217,15 @@
       <c r="P27" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>4578</t>
+      <c r="Q27" t="n">
+        <v>4578</v>
+      </c>
+      <c r="R27" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>4825</t>
         </is>
       </c>
     </row>
@@ -2118,9 +2284,15 @@
       <c r="P28" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>3751</t>
+      <c r="Q28" t="n">
+        <v>3751</v>
+      </c>
+      <c r="R28" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>3924</t>
         </is>
       </c>
     </row>
@@ -2179,9 +2351,15 @@
       <c r="P29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>3788</t>
+      <c r="Q29" t="n">
+        <v>3788</v>
+      </c>
+      <c r="R29" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>3949</t>
         </is>
       </c>
     </row>
@@ -2240,9 +2418,15 @@
       <c r="P30" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>4516</t>
+      <c r="Q30" t="n">
+        <v>4516</v>
+      </c>
+      <c r="R30" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>4988</t>
         </is>
       </c>
     </row>
@@ -2301,9 +2485,15 @@
       <c r="P31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>4282</t>
+      <c r="Q31" t="n">
+        <v>4282</v>
+      </c>
+      <c r="R31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>4471</t>
         </is>
       </c>
     </row>
@@ -2362,9 +2552,15 @@
       <c r="P32" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>4737</t>
+      <c r="Q32" t="n">
+        <v>4737</v>
+      </c>
+      <c r="R32" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>4990</t>
         </is>
       </c>
     </row>
@@ -2423,9 +2619,15 @@
       <c r="P33" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>4918</t>
+      <c r="Q33" t="n">
+        <v>4918</v>
+      </c>
+      <c r="R33" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>5076</t>
         </is>
       </c>
     </row>
@@ -2484,9 +2686,15 @@
       <c r="P34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>2763</t>
+      <c r="Q34" t="n">
+        <v>2763</v>
+      </c>
+      <c r="R34" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>3134</t>
         </is>
       </c>
     </row>
@@ -2545,9 +2753,15 @@
       <c r="P35" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>4544</t>
+      <c r="Q35" t="n">
+        <v>4544</v>
+      </c>
+      <c r="R35" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>4888</t>
         </is>
       </c>
     </row>
@@ -2606,9 +2820,15 @@
       <c r="P36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>3978</t>
+      <c r="Q36" t="n">
+        <v>3978</v>
+      </c>
+      <c r="R36" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>4197</t>
         </is>
       </c>
     </row>
@@ -2667,9 +2887,15 @@
       <c r="P37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>4040</t>
+      <c r="Q37" t="n">
+        <v>4040</v>
+      </c>
+      <c r="R37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>4295</t>
         </is>
       </c>
     </row>
@@ -2728,9 +2954,15 @@
       <c r="P38" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>4531</t>
+      <c r="Q38" t="n">
+        <v>4531</v>
+      </c>
+      <c r="R38" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>4715</t>
         </is>
       </c>
     </row>
@@ -2789,9 +3021,15 @@
       <c r="P39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>4200</t>
+      <c r="Q39" t="n">
+        <v>4200</v>
+      </c>
+      <c r="R39" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>4368</t>
         </is>
       </c>
     </row>
@@ -2850,9 +3088,15 @@
       <c r="P40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>4638</t>
+      <c r="Q40" t="n">
+        <v>4638</v>
+      </c>
+      <c r="R40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>4999</t>
         </is>
       </c>
     </row>
@@ -2911,9 +3155,15 @@
       <c r="P41" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>4614</t>
+      <c r="Q41" t="n">
+        <v>4614</v>
+      </c>
+      <c r="R41" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>4815</t>
         </is>
       </c>
     </row>
@@ -2972,9 +3222,15 @@
       <c r="P42" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>4706</t>
+      <c r="Q42" t="n">
+        <v>4706</v>
+      </c>
+      <c r="R42" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>5000</t>
         </is>
       </c>
     </row>
@@ -3033,9 +3289,15 @@
       <c r="P43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>4349</t>
+      <c r="Q43" t="n">
+        <v>4349</v>
+      </c>
+      <c r="R43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>4600</t>
         </is>
       </c>
     </row>
@@ -3094,9 +3356,15 @@
       <c r="P44" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>3325</t>
+      <c r="Q44" t="n">
+        <v>3325</v>
+      </c>
+      <c r="R44" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>3735</t>
         </is>
       </c>
     </row>
@@ -3155,9 +3423,15 @@
       <c r="P45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>3951</t>
+      <c r="Q45" t="n">
+        <v>3951</v>
+      </c>
+      <c r="R45" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>4356</t>
         </is>
       </c>
     </row>
@@ -3180,7 +3454,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F46" s="3" t="n">
@@ -3216,9 +3490,15 @@
       <c r="P46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>4030</t>
+      <c r="Q46" t="n">
+        <v>4030</v>
+      </c>
+      <c r="R46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>4210</t>
         </is>
       </c>
     </row>
@@ -3277,9 +3557,15 @@
       <c r="P47" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>4141</t>
+      <c r="Q47" t="n">
+        <v>4141</v>
+      </c>
+      <c r="R47" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>4386</t>
         </is>
       </c>
     </row>
@@ -3338,9 +3624,15 @@
       <c r="P48" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>4280</t>
+      <c r="Q48" t="n">
+        <v>4280</v>
+      </c>
+      <c r="R48" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>4488</t>
         </is>
       </c>
     </row>
@@ -3399,9 +3691,15 @@
       <c r="P49" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>3809</t>
+      <c r="Q49" t="n">
+        <v>3809</v>
+      </c>
+      <c r="R49" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>3683</t>
         </is>
       </c>
     </row>
@@ -3460,9 +3758,15 @@
       <c r="P50" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>4167</t>
+      <c r="Q50" t="n">
+        <v>4167</v>
+      </c>
+      <c r="R50" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>4401</t>
         </is>
       </c>
     </row>
@@ -3521,9 +3825,15 @@
       <c r="P51" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>3949</t>
+      <c r="Q51" t="n">
+        <v>3949</v>
+      </c>
+      <c r="R51" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>4352</t>
         </is>
       </c>
     </row>
@@ -3582,9 +3892,15 @@
       <c r="P52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>2574</t>
+      <c r="Q52" t="n">
+        <v>2574</v>
+      </c>
+      <c r="R52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>2573</t>
         </is>
       </c>
     </row>
@@ -3643,9 +3959,15 @@
       <c r="P53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>2993</t>
+      <c r="Q53" t="n">
+        <v>2993</v>
+      </c>
+      <c r="R53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>3018</t>
         </is>
       </c>
     </row>
@@ -3704,9 +4026,15 @@
       <c r="P54" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>2910</t>
+      <c r="Q54" t="n">
+        <v>2910</v>
+      </c>
+      <c r="R54" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>2990</t>
         </is>
       </c>
     </row>
@@ -3765,9 +4093,15 @@
       <c r="P55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>3525</t>
+      <c r="Q55" t="n">
+        <v>3525</v>
+      </c>
+      <c r="R55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>3542</t>
         </is>
       </c>
     </row>
@@ -3826,9 +4160,15 @@
       <c r="P56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>3721</t>
+      <c r="Q56" t="n">
+        <v>3721</v>
+      </c>
+      <c r="R56" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>3871</t>
         </is>
       </c>
     </row>
@@ -3887,9 +4227,15 @@
       <c r="P57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>4067</t>
+      <c r="Q57" t="n">
+        <v>4067</v>
+      </c>
+      <c r="R57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>4295</t>
         </is>
       </c>
     </row>
@@ -3948,9 +4294,15 @@
       <c r="P58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t>3557</t>
+      <c r="Q58" t="n">
+        <v>3557</v>
+      </c>
+      <c r="R58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>3685</t>
         </is>
       </c>
     </row>
@@ -4009,9 +4361,15 @@
       <c r="P59" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="Q59" t="inlineStr">
-        <is>
-          <t>3981</t>
+      <c r="Q59" t="n">
+        <v>3981</v>
+      </c>
+      <c r="R59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>4211</t>
         </is>
       </c>
     </row>
@@ -4070,9 +4428,15 @@
       <c r="P60" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="Q60" t="inlineStr">
-        <is>
-          <t>4209</t>
+      <c r="Q60" t="n">
+        <v>4209</v>
+      </c>
+      <c r="R60" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>4464</t>
         </is>
       </c>
     </row>
@@ -4131,9 +4495,15 @@
       <c r="P61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q61" t="inlineStr">
-        <is>
-          <t>4094</t>
+      <c r="Q61" t="n">
+        <v>4094</v>
+      </c>
+      <c r="R61" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>4270</t>
         </is>
       </c>
     </row>
@@ -4192,9 +4562,15 @@
       <c r="P62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q62" t="inlineStr">
-        <is>
-          <t>4037</t>
+      <c r="Q62" t="n">
+        <v>4037</v>
+      </c>
+      <c r="R62" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>4274</t>
         </is>
       </c>
     </row>
@@ -4253,9 +4629,15 @@
       <c r="P63" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>3630</t>
+      <c r="Q63" t="n">
+        <v>3630</v>
+      </c>
+      <c r="R63" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>3755</t>
         </is>
       </c>
     </row>
@@ -4314,9 +4696,15 @@
       <c r="P64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q64" t="inlineStr">
-        <is>
-          <t>2544</t>
+      <c r="Q64" t="n">
+        <v>2544</v>
+      </c>
+      <c r="R64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>2575</t>
         </is>
       </c>
     </row>
@@ -4375,9 +4763,15 @@
       <c r="P65" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q65" t="inlineStr">
-        <is>
-          <t>3528</t>
+      <c r="Q65" t="n">
+        <v>3528</v>
+      </c>
+      <c r="R65" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>3610</t>
         </is>
       </c>
     </row>
@@ -4436,9 +4830,15 @@
       <c r="P66" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>3463</t>
+      <c r="Q66" t="n">
+        <v>3463</v>
+      </c>
+      <c r="R66" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>3457</t>
         </is>
       </c>
     </row>
@@ -4497,9 +4897,15 @@
       <c r="P67" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>4242</t>
+      <c r="Q67" t="n">
+        <v>4242</v>
+      </c>
+      <c r="R67" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>4435</t>
         </is>
       </c>
     </row>
@@ -4558,9 +4964,15 @@
       <c r="P68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q68" t="inlineStr">
-        <is>
-          <t>3561</t>
+      <c r="Q68" t="n">
+        <v>3561</v>
+      </c>
+      <c r="R68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S68" t="inlineStr">
+        <is>
+          <t>3779</t>
         </is>
       </c>
     </row>
@@ -4619,9 +5031,15 @@
       <c r="P69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q69" t="inlineStr">
-        <is>
-          <t>2665</t>
+      <c r="Q69" t="n">
+        <v>2665</v>
+      </c>
+      <c r="R69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>2691</t>
         </is>
       </c>
     </row>
@@ -4680,9 +5098,15 @@
       <c r="P70" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="Q70" t="inlineStr">
-        <is>
-          <t>3214</t>
+      <c r="Q70" t="n">
+        <v>3214</v>
+      </c>
+      <c r="R70" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>3357</t>
         </is>
       </c>
     </row>
@@ -4741,9 +5165,15 @@
       <c r="P71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q71" t="inlineStr">
-        <is>
-          <t>4303</t>
+      <c r="Q71" t="n">
+        <v>4303</v>
+      </c>
+      <c r="R71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>4643</t>
         </is>
       </c>
     </row>
@@ -4802,9 +5232,15 @@
       <c r="P72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q72" t="inlineStr">
-        <is>
-          <t>3469</t>
+      <c r="Q72" t="n">
+        <v>3469</v>
+      </c>
+      <c r="R72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>3525</t>
         </is>
       </c>
     </row>
@@ -4863,9 +5299,15 @@
       <c r="P73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q73" t="inlineStr">
-        <is>
-          <t>4036</t>
+      <c r="Q73" t="n">
+        <v>4036</v>
+      </c>
+      <c r="R73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>4285</t>
         </is>
       </c>
     </row>
@@ -4924,9 +5366,15 @@
       <c r="P74" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Q74" t="inlineStr">
-        <is>
-          <t>3704</t>
+      <c r="Q74" t="n">
+        <v>3704</v>
+      </c>
+      <c r="R74" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>3914</t>
         </is>
       </c>
     </row>
@@ -4985,9 +5433,15 @@
       <c r="P75" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Q75" t="inlineStr">
-        <is>
-          <t>3885</t>
+      <c r="Q75" t="n">
+        <v>3885</v>
+      </c>
+      <c r="R75" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>4070</t>
         </is>
       </c>
     </row>
@@ -5046,9 +5500,15 @@
       <c r="P76" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q76" t="inlineStr">
-        <is>
-          <t>3770</t>
+      <c r="Q76" t="n">
+        <v>3770</v>
+      </c>
+      <c r="R76" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>4081</t>
         </is>
       </c>
     </row>
@@ -5107,9 +5567,15 @@
       <c r="P77" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="Q77" t="inlineStr">
-        <is>
-          <t>2850</t>
+      <c r="Q77" t="n">
+        <v>2850</v>
+      </c>
+      <c r="R77" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>2848</t>
         </is>
       </c>
     </row>
@@ -5168,9 +5634,15 @@
       <c r="P78" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q78" t="inlineStr">
-        <is>
-          <t>3740</t>
+      <c r="Q78" t="n">
+        <v>3740</v>
+      </c>
+      <c r="R78" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S78" t="inlineStr">
+        <is>
+          <t>3845</t>
         </is>
       </c>
     </row>
@@ -5229,9 +5701,15 @@
       <c r="P79" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q79" t="inlineStr">
-        <is>
-          <t>3721</t>
+      <c r="Q79" t="n">
+        <v>3721</v>
+      </c>
+      <c r="R79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>3684</t>
         </is>
       </c>
     </row>
@@ -5290,9 +5768,15 @@
       <c r="P80" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q80" t="inlineStr">
-        <is>
-          <t>3174</t>
+      <c r="Q80" t="n">
+        <v>3174</v>
+      </c>
+      <c r="R80" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S80" t="inlineStr">
+        <is>
+          <t>3316</t>
         </is>
       </c>
     </row>
@@ -5351,9 +5835,15 @@
       <c r="P81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q81" t="inlineStr">
-        <is>
-          <t>2823</t>
+      <c r="Q81" t="n">
+        <v>2823</v>
+      </c>
+      <c r="R81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>2828</t>
         </is>
       </c>
     </row>
@@ -5412,9 +5902,15 @@
       <c r="P82" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="Q82" t="inlineStr">
-        <is>
-          <t>3956</t>
+      <c r="Q82" t="n">
+        <v>3956</v>
+      </c>
+      <c r="R82" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>4122</t>
         </is>
       </c>
     </row>
@@ -5473,9 +5969,15 @@
       <c r="P83" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="Q83" t="inlineStr">
-        <is>
-          <t>2761</t>
+      <c r="Q83" t="n">
+        <v>2761</v>
+      </c>
+      <c r="R83" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>2780</t>
         </is>
       </c>
     </row>
@@ -5534,9 +6036,15 @@
       <c r="P84" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q84" t="inlineStr">
-        <is>
-          <t>3009</t>
+      <c r="Q84" t="n">
+        <v>3009</v>
+      </c>
+      <c r="R84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>2943</t>
         </is>
       </c>
     </row>
@@ -5595,9 +6103,15 @@
       <c r="P85" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="Q85" t="inlineStr">
-        <is>
-          <t>2050</t>
+      <c r="Q85" t="n">
+        <v>2050</v>
+      </c>
+      <c r="R85" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="S85" t="inlineStr">
+        <is>
+          <t>2106</t>
         </is>
       </c>
     </row>
@@ -5656,9 +6170,15 @@
       <c r="P86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q86" t="inlineStr">
-        <is>
-          <t>2535</t>
+      <c r="Q86" t="n">
+        <v>2535</v>
+      </c>
+      <c r="R86" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S86" t="inlineStr">
+        <is>
+          <t>2655</t>
         </is>
       </c>
     </row>
@@ -5717,9 +6237,15 @@
       <c r="P87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q87" t="inlineStr">
-        <is>
-          <t>2911</t>
+      <c r="Q87" t="n">
+        <v>2911</v>
+      </c>
+      <c r="R87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S87" t="inlineStr">
+        <is>
+          <t>2912</t>
         </is>
       </c>
     </row>
@@ -5778,9 +6304,15 @@
       <c r="P88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q88" t="inlineStr">
-        <is>
-          <t>2026</t>
+      <c r="Q88" t="n">
+        <v>2026</v>
+      </c>
+      <c r="R88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>2013</t>
         </is>
       </c>
     </row>
@@ -5834,6 +6366,8 @@
       <c r="O89" t="inlineStr"/>
       <c r="P89" s="3" t="inlineStr"/>
       <c r="Q89" t="inlineStr"/>
+      <c r="R89" s="3" t="inlineStr"/>
+      <c r="S89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -5885,6 +6419,8 @@
       <c r="O90" t="inlineStr"/>
       <c r="P90" s="3" t="inlineStr"/>
       <c r="Q90" t="inlineStr"/>
+      <c r="R90" s="3" t="inlineStr"/>
+      <c r="S90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -5941,9 +6477,15 @@
       <c r="P91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q91" t="inlineStr">
-        <is>
-          <t>2520</t>
+      <c r="Q91" t="n">
+        <v>2520</v>
+      </c>
+      <c r="R91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S91" t="inlineStr">
+        <is>
+          <t>2523</t>
         </is>
       </c>
     </row>
@@ -6002,9 +6544,15 @@
       <c r="P92" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Q92" t="inlineStr">
-        <is>
-          <t>3000</t>
+      <c r="Q92" t="n">
+        <v>3000</v>
+      </c>
+      <c r="R92" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="S92" t="inlineStr">
+        <is>
+          <t>3267</t>
         </is>
       </c>
     </row>
@@ -6063,9 +6611,15 @@
       <c r="P93" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Q93" t="inlineStr">
-        <is>
-          <t>2779</t>
+      <c r="Q93" t="n">
+        <v>2779</v>
+      </c>
+      <c r="R93" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="S93" t="inlineStr">
+        <is>
+          <t>2821</t>
         </is>
       </c>
     </row>
@@ -6124,9 +6678,15 @@
       <c r="P94" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q94" t="inlineStr">
-        <is>
-          <t>3699</t>
+      <c r="Q94" t="n">
+        <v>3699</v>
+      </c>
+      <c r="R94" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S94" t="inlineStr">
+        <is>
+          <t>3841</t>
         </is>
       </c>
     </row>
@@ -6185,9 +6745,15 @@
       <c r="P95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q95" t="inlineStr">
-        <is>
-          <t>3499</t>
+      <c r="Q95" t="n">
+        <v>3499</v>
+      </c>
+      <c r="R95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>3602</t>
         </is>
       </c>
     </row>
@@ -6246,9 +6812,15 @@
       <c r="P96" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="Q96" t="inlineStr">
-        <is>
-          <t>3313</t>
+      <c r="Q96" t="n">
+        <v>3313</v>
+      </c>
+      <c r="R96" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>3433</t>
         </is>
       </c>
     </row>
@@ -6307,9 +6879,15 @@
       <c r="P97" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Q97" t="inlineStr">
-        <is>
-          <t>3717</t>
+      <c r="Q97" t="n">
+        <v>3717</v>
+      </c>
+      <c r="R97" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>3902</t>
         </is>
       </c>
     </row>
@@ -6368,9 +6946,15 @@
       <c r="P98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q98" t="inlineStr">
-        <is>
-          <t>3285</t>
+      <c r="Q98" t="n">
+        <v>3285</v>
+      </c>
+      <c r="R98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S98" t="inlineStr">
+        <is>
+          <t>3300</t>
         </is>
       </c>
     </row>
@@ -6429,9 +7013,15 @@
       <c r="P99" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q99" t="inlineStr">
-        <is>
-          <t>2732</t>
+      <c r="Q99" t="n">
+        <v>2732</v>
+      </c>
+      <c r="R99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S99" t="inlineStr">
+        <is>
+          <t>2656</t>
         </is>
       </c>
     </row>
@@ -6490,9 +7080,15 @@
       <c r="P100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q100" t="inlineStr">
-        <is>
-          <t>2583</t>
+      <c r="Q100" t="n">
+        <v>2583</v>
+      </c>
+      <c r="R100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S100" t="inlineStr">
+        <is>
+          <t>2600</t>
         </is>
       </c>
     </row>
@@ -6551,9 +7147,15 @@
       <c r="P101" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q101" t="inlineStr">
-        <is>
-          <t>3821</t>
+      <c r="Q101" t="n">
+        <v>3821</v>
+      </c>
+      <c r="R101" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S101" t="inlineStr">
+        <is>
+          <t>3946</t>
         </is>
       </c>
     </row>
@@ -6612,9 +7214,15 @@
       <c r="P102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q102" t="inlineStr">
-        <is>
-          <t>3254</t>
+      <c r="Q102" t="n">
+        <v>3254</v>
+      </c>
+      <c r="R102" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="S102" t="inlineStr">
+        <is>
+          <t>3499</t>
         </is>
       </c>
     </row>
@@ -6673,9 +7281,15 @@
       <c r="P103" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="Q103" t="inlineStr">
-        <is>
-          <t>3176</t>
+      <c r="Q103" t="n">
+        <v>3176</v>
+      </c>
+      <c r="R103" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S103" t="inlineStr">
+        <is>
+          <t>3233</t>
         </is>
       </c>
     </row>
@@ -6734,9 +7348,15 @@
       <c r="P104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q104" t="inlineStr">
-        <is>
-          <t>2558</t>
+      <c r="Q104" t="n">
+        <v>2558</v>
+      </c>
+      <c r="R104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t>2566</t>
         </is>
       </c>
     </row>
@@ -6795,9 +7415,15 @@
       <c r="P105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q105" t="inlineStr">
-        <is>
-          <t>3059</t>
+      <c r="Q105" t="n">
+        <v>3059</v>
+      </c>
+      <c r="R105" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S105" t="inlineStr">
+        <is>
+          <t>3269</t>
         </is>
       </c>
     </row>
@@ -6856,9 +7482,15 @@
       <c r="P106" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="Q106" t="inlineStr">
-        <is>
-          <t>2808</t>
+      <c r="Q106" t="n">
+        <v>2808</v>
+      </c>
+      <c r="R106" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="S106" t="inlineStr">
+        <is>
+          <t>2826</t>
         </is>
       </c>
     </row>
@@ -6917,9 +7549,15 @@
       <c r="P107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q107" t="inlineStr">
-        <is>
-          <t>3155</t>
+      <c r="Q107" t="n">
+        <v>3155</v>
+      </c>
+      <c r="R107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S107" t="inlineStr">
+        <is>
+          <t>3298</t>
         </is>
       </c>
     </row>
@@ -6978,9 +7616,15 @@
       <c r="P108" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Q108" t="inlineStr">
-        <is>
-          <t>2453</t>
+      <c r="Q108" t="n">
+        <v>2453</v>
+      </c>
+      <c r="R108" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="S108" t="inlineStr">
+        <is>
+          <t>2532</t>
         </is>
       </c>
     </row>
@@ -7039,9 +7683,15 @@
       <c r="P109" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="Q109" t="inlineStr">
-        <is>
-          <t>2587</t>
+      <c r="Q109" t="n">
+        <v>2587</v>
+      </c>
+      <c r="R109" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="S109" t="inlineStr">
+        <is>
+          <t>2624</t>
         </is>
       </c>
     </row>
@@ -7100,9 +7750,15 @@
       <c r="P110" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q110" t="inlineStr">
-        <is>
-          <t>3119</t>
+      <c r="Q110" t="n">
+        <v>3119</v>
+      </c>
+      <c r="R110" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="S110" t="inlineStr">
+        <is>
+          <t>3118</t>
         </is>
       </c>
     </row>
@@ -7161,9 +7817,15 @@
       <c r="P111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q111" t="inlineStr">
-        <is>
-          <t>2787</t>
+      <c r="Q111" t="n">
+        <v>2787</v>
+      </c>
+      <c r="R111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S111" t="inlineStr">
+        <is>
+          <t>2832</t>
         </is>
       </c>
     </row>
@@ -7222,9 +7884,15 @@
       <c r="P112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q112" t="inlineStr">
-        <is>
-          <t>3065</t>
+      <c r="Q112" t="n">
+        <v>3065</v>
+      </c>
+      <c r="R112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S112" t="inlineStr">
+        <is>
+          <t>3193</t>
         </is>
       </c>
     </row>
@@ -7283,9 +7951,15 @@
       <c r="P113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q113" t="inlineStr">
-        <is>
-          <t>2534</t>
+      <c r="Q113" t="n">
+        <v>2534</v>
+      </c>
+      <c r="R113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>2542</t>
         </is>
       </c>
     </row>
@@ -7344,9 +8018,15 @@
       <c r="P114" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q114" t="inlineStr">
-        <is>
-          <t>3108</t>
+      <c r="Q114" t="n">
+        <v>3108</v>
+      </c>
+      <c r="R114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S114" t="inlineStr">
+        <is>
+          <t>3165</t>
         </is>
       </c>
     </row>
@@ -7405,9 +8085,15 @@
       <c r="P115" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Q115" t="inlineStr">
-        <is>
-          <t>2634</t>
+      <c r="Q115" t="n">
+        <v>2634</v>
+      </c>
+      <c r="R115" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S115" t="inlineStr">
+        <is>
+          <t>2625</t>
         </is>
       </c>
     </row>
@@ -7466,9 +8152,15 @@
       <c r="P116" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="Q116" t="inlineStr">
-        <is>
-          <t>2862</t>
+      <c r="Q116" t="n">
+        <v>2862</v>
+      </c>
+      <c r="R116" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S116" t="inlineStr">
+        <is>
+          <t>2968</t>
         </is>
       </c>
     </row>
@@ -7527,9 +8219,15 @@
       <c r="P117" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q117" t="inlineStr">
-        <is>
-          <t>2917</t>
+      <c r="Q117" t="n">
+        <v>2917</v>
+      </c>
+      <c r="R117" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="S117" t="inlineStr">
+        <is>
+          <t>2982</t>
         </is>
       </c>
     </row>
@@ -7588,7 +8286,13 @@
       <c r="P118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q118" t="inlineStr">
+      <c r="Q118" t="n">
+        <v>0</v>
+      </c>
+      <c r="R118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7649,9 +8353,15 @@
       <c r="P119" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="Q119" t="inlineStr">
-        <is>
-          <t>3027</t>
+      <c r="Q119" t="n">
+        <v>3027</v>
+      </c>
+      <c r="R119" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S119" t="inlineStr">
+        <is>
+          <t>3134</t>
         </is>
       </c>
     </row>
@@ -7710,9 +8420,15 @@
       <c r="P120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q120" t="inlineStr">
-        <is>
-          <t>2982</t>
+      <c r="Q120" t="n">
+        <v>2982</v>
+      </c>
+      <c r="R120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S120" t="inlineStr">
+        <is>
+          <t>3020</t>
         </is>
       </c>
     </row>
@@ -7771,9 +8487,15 @@
       <c r="P121" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="Q121" t="inlineStr">
-        <is>
-          <t>2218</t>
+      <c r="Q121" t="n">
+        <v>2218</v>
+      </c>
+      <c r="R121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S121" t="inlineStr">
+        <is>
+          <t>2190</t>
         </is>
       </c>
     </row>
@@ -7832,9 +8554,15 @@
       <c r="P122" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="Q122" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="Q122" t="n">
+        <v>2500</v>
+      </c>
+      <c r="R122" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="S122" t="inlineStr">
+        <is>
+          <t>2537</t>
         </is>
       </c>
     </row>
@@ -7893,9 +8621,15 @@
       <c r="P123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q123" t="inlineStr">
-        <is>
-          <t>2505</t>
+      <c r="Q123" t="n">
+        <v>2505</v>
+      </c>
+      <c r="R123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S123" t="inlineStr">
+        <is>
+          <t>2504</t>
         </is>
       </c>
     </row>
@@ -7954,9 +8688,15 @@
       <c r="P124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q124" t="inlineStr">
-        <is>
-          <t>3060</t>
+      <c r="Q124" t="n">
+        <v>3060</v>
+      </c>
+      <c r="R124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S124" t="inlineStr">
+        <is>
+          <t>3234</t>
         </is>
       </c>
     </row>
@@ -8015,7 +8755,13 @@
       <c r="P125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q125" t="inlineStr">
+      <c r="Q125" t="n">
+        <v>0</v>
+      </c>
+      <c r="R125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8076,9 +8822,15 @@
       <c r="P126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q126" t="inlineStr">
-        <is>
-          <t>2899</t>
+      <c r="Q126" t="n">
+        <v>2899</v>
+      </c>
+      <c r="R126" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="S126" t="inlineStr">
+        <is>
+          <t>2897</t>
         </is>
       </c>
     </row>
@@ -8137,9 +8889,15 @@
       <c r="P127" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q127" t="inlineStr">
-        <is>
-          <t>2667</t>
+      <c r="Q127" t="n">
+        <v>2667</v>
+      </c>
+      <c r="R127" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S127" t="inlineStr">
+        <is>
+          <t>2653</t>
         </is>
       </c>
     </row>
@@ -8198,9 +8956,15 @@
       <c r="P128" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="Q128" t="inlineStr">
-        <is>
-          <t>2458</t>
+      <c r="Q128" t="n">
+        <v>2458</v>
+      </c>
+      <c r="R128" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S128" t="inlineStr">
+        <is>
+          <t>2633</t>
         </is>
       </c>
     </row>
@@ -8259,9 +9023,15 @@
       <c r="P129" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Q129" t="inlineStr">
-        <is>
-          <t>2419</t>
+      <c r="Q129" t="n">
+        <v>2419</v>
+      </c>
+      <c r="R129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S129" t="inlineStr">
+        <is>
+          <t>2403</t>
         </is>
       </c>
     </row>
@@ -8320,9 +9090,15 @@
       <c r="P130" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="Q130" t="inlineStr">
-        <is>
-          <t>1942</t>
+      <c r="Q130" t="n">
+        <v>1942</v>
+      </c>
+      <c r="R130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S130" t="inlineStr">
+        <is>
+          <t>1928</t>
         </is>
       </c>
     </row>
@@ -8381,7 +9157,13 @@
       <c r="P131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q131" t="inlineStr">
+      <c r="Q131" t="n">
+        <v>0</v>
+      </c>
+      <c r="R131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8442,9 +9224,15 @@
       <c r="P132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q132" t="inlineStr">
-        <is>
-          <t>1511</t>
+      <c r="Q132" t="n">
+        <v>1511</v>
+      </c>
+      <c r="R132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S132" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -8503,7 +9291,13 @@
       <c r="P133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q133" t="inlineStr">
+      <c r="Q133" t="n">
+        <v>0</v>
+      </c>
+      <c r="R133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8564,9 +9358,15 @@
       <c r="P134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q134" t="inlineStr">
-        <is>
-          <t>1950</t>
+      <c r="Q134" t="n">
+        <v>1950</v>
+      </c>
+      <c r="R134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S134" t="inlineStr">
+        <is>
+          <t>1958</t>
         </is>
       </c>
     </row>
@@ -8625,9 +9425,15 @@
       <c r="P135" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Q135" t="inlineStr">
-        <is>
-          <t>2272</t>
+      <c r="Q135" t="n">
+        <v>2272</v>
+      </c>
+      <c r="R135" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S135" t="inlineStr">
+        <is>
+          <t>2280</t>
         </is>
       </c>
     </row>
@@ -8686,9 +9492,15 @@
       <c r="P136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q136" t="inlineStr">
-        <is>
-          <t>1528</t>
+      <c r="Q136" t="n">
+        <v>1528</v>
+      </c>
+      <c r="R136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -8747,7 +9559,13 @@
       <c r="P137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q137" t="inlineStr">
+      <c r="Q137" t="n">
+        <v>0</v>
+      </c>
+      <c r="R137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8808,7 +9626,13 @@
       <c r="P138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q138" t="inlineStr">
+      <c r="Q138" t="n">
+        <v>0</v>
+      </c>
+      <c r="R138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8869,7 +9693,13 @@
       <c r="P139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q139" t="inlineStr">
+      <c r="Q139" t="n">
+        <v>0</v>
+      </c>
+      <c r="R139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8930,9 +9760,15 @@
       <c r="P140" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Q140" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="Q140" t="n">
+        <v>3991</v>
+      </c>
+      <c r="R140" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="S140" t="inlineStr">
+        <is>
+          <t>4109</t>
         </is>
       </c>
     </row>
@@ -8991,7 +9827,13 @@
       <c r="P141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q141" t="inlineStr">
+      <c r="Q141" t="n">
+        <v>0</v>
+      </c>
+      <c r="R141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9052,7 +9894,13 @@
       <c r="P142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q142" t="inlineStr">
+      <c r="Q142" t="n">
+        <v>0</v>
+      </c>
+      <c r="R142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9113,9 +9961,15 @@
       <c r="P143" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q143" t="inlineStr">
-        <is>
-          <t>4101</t>
+      <c r="Q143" t="n">
+        <v>4101</v>
+      </c>
+      <c r="R143" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="S143" t="inlineStr">
+        <is>
+          <t>4397</t>
         </is>
       </c>
     </row>
@@ -9174,7 +10028,13 @@
       <c r="P144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q144" t="inlineStr">
+      <c r="Q144" t="n">
+        <v>0</v>
+      </c>
+      <c r="R144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9235,9 +10095,15 @@
       <c r="P145" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Q145" t="inlineStr">
-        <is>
-          <t>2804</t>
+      <c r="Q145" t="n">
+        <v>2804</v>
+      </c>
+      <c r="R145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S145" t="inlineStr">
+        <is>
+          <t>2795</t>
         </is>
       </c>
     </row>
@@ -9296,7 +10162,13 @@
       <c r="P146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q146" t="inlineStr">
+      <c r="Q146" t="n">
+        <v>0</v>
+      </c>
+      <c r="R146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9357,9 +10229,15 @@
       <c r="P147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q147" t="inlineStr">
-        <is>
-          <t>2578</t>
+      <c r="Q147" t="n">
+        <v>2578</v>
+      </c>
+      <c r="R147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S147" t="inlineStr">
+        <is>
+          <t>2633</t>
         </is>
       </c>
     </row>
@@ -9403,6 +10281,8 @@
       </c>
       <c r="P148" s="3" t="inlineStr"/>
       <c r="Q148" t="inlineStr"/>
+      <c r="R148" s="3" t="inlineStr"/>
+      <c r="S148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -9453,9 +10333,15 @@
       <c r="P149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q149" t="inlineStr">
-        <is>
-          <t>1328</t>
+      <c r="Q149" t="n">
+        <v>1328</v>
+      </c>
+      <c r="R149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S149" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -9508,9 +10394,15 @@
       <c r="P150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q150" t="inlineStr">
-        <is>
-          <t>1411</t>
+      <c r="Q150" t="n">
+        <v>1411</v>
+      </c>
+      <c r="R150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S150" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -9551,9 +10443,15 @@
       <c r="P151" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q151" t="inlineStr">
-        <is>
-          <t>2310</t>
+      <c r="Q151" t="n">
+        <v>2310</v>
+      </c>
+      <c r="R151" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S151" t="inlineStr">
+        <is>
+          <t>2361</t>
         </is>
       </c>
     </row>
@@ -9594,17 +10492,21 @@
       <c r="P152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q152" t="inlineStr">
+      <c r="Q152" t="n">
+        <v>0</v>
+      </c>
+      <c r="R152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>51841127</t>
-        </is>
+      <c r="A153" t="n">
+        <v>51841127</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
@@ -9631,17 +10533,21 @@
       <c r="P153" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q153" t="inlineStr">
-        <is>
-          <t>3492</t>
+      <c r="Q153" t="n">
+        <v>3492</v>
+      </c>
+      <c r="R153" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="S153" t="inlineStr">
+        <is>
+          <t>3553</t>
         </is>
       </c>
     </row>
     <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>58437456</t>
-        </is>
+      <c r="A154" t="n">
+        <v>58437456</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
@@ -9668,9 +10574,54 @@
       <c r="P154" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="Q154" t="inlineStr">
-        <is>
-          <t>1671</t>
+      <c r="Q154" t="n">
+        <v>1671</v>
+      </c>
+      <c r="R154" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S154" t="inlineStr">
+        <is>
+          <t>1648</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>58415620</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>"el pepe"</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr"/>
+      <c r="D155" t="inlineStr"/>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F155" s="3" t="inlineStr"/>
+      <c r="G155" t="inlineStr"/>
+      <c r="H155" s="3" t="inlineStr"/>
+      <c r="I155" t="inlineStr"/>
+      <c r="J155" s="3" t="inlineStr"/>
+      <c r="K155" t="inlineStr"/>
+      <c r="L155" s="3" t="inlineStr"/>
+      <c r="M155" t="inlineStr"/>
+      <c r="N155" s="3" t="inlineStr"/>
+      <c r="O155" t="inlineStr"/>
+      <c r="P155" s="3" t="inlineStr"/>
+      <c r="Q155" t="inlineStr"/>
+      <c r="R155" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="S155" t="inlineStr">
+        <is>
+          <t>1441</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-09 11:31:02
</commit_message>
<xml_diff>
--- a/Season_Attack/81.xlsx
+++ b/Season_Attack/81.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S155"/>
+  <dimension ref="A1:U158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,16 @@
           <t>01-07_0</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>01-08_A</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>01-08_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -548,9 +558,15 @@
       <c r="R2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>3475</t>
+      <c r="S2" t="n">
+        <v>3475</v>
+      </c>
+      <c r="T2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>3729</t>
         </is>
       </c>
     </row>
@@ -573,7 +589,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F3" s="3" t="n">
@@ -615,9 +631,15 @@
       <c r="R3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>4183</t>
+      <c r="S3" t="n">
+        <v>4183</v>
+      </c>
+      <c r="T3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>4348</t>
         </is>
       </c>
     </row>
@@ -640,7 +662,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F4" s="4" t="n">
@@ -682,9 +704,15 @@
       <c r="R4" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>4504</t>
+      <c r="S4" t="n">
+        <v>4504</v>
+      </c>
+      <c r="T4" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>4689</t>
         </is>
       </c>
     </row>
@@ -749,9 +777,15 @@
       <c r="R5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>4673</t>
+      <c r="S5" t="n">
+        <v>4673</v>
+      </c>
+      <c r="T5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>5016</t>
         </is>
       </c>
     </row>
@@ -816,9 +850,15 @@
       <c r="R6" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>4705</t>
+      <c r="S6" t="n">
+        <v>4705</v>
+      </c>
+      <c r="T6" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>5004</t>
         </is>
       </c>
     </row>
@@ -883,9 +923,15 @@
       <c r="R7" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>4933</t>
+      <c r="S7" t="n">
+        <v>4933</v>
+      </c>
+      <c r="T7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>5314</t>
         </is>
       </c>
     </row>
@@ -950,9 +996,15 @@
       <c r="R8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>4364</t>
+      <c r="S8" t="n">
+        <v>4364</v>
+      </c>
+      <c r="T8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>4572</t>
         </is>
       </c>
     </row>
@@ -975,7 +1027,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F9" s="3" t="n">
@@ -1017,9 +1069,15 @@
       <c r="R9" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>4591</t>
+      <c r="S9" t="n">
+        <v>4591</v>
+      </c>
+      <c r="T9" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>4713</t>
         </is>
       </c>
     </row>
@@ -1084,9 +1142,15 @@
       <c r="R10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>4048</t>
+      <c r="S10" t="n">
+        <v>4048</v>
+      </c>
+      <c r="T10" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>4274</t>
         </is>
       </c>
     </row>
@@ -1151,9 +1215,15 @@
       <c r="R11" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>4201</t>
+      <c r="S11" t="n">
+        <v>4201</v>
+      </c>
+      <c r="T11" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>4866</t>
         </is>
       </c>
     </row>
@@ -1218,9 +1288,15 @@
       <c r="R12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>4119</t>
+      <c r="S12" t="n">
+        <v>4119</v>
+      </c>
+      <c r="T12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>4249</t>
         </is>
       </c>
     </row>
@@ -1285,9 +1361,15 @@
       <c r="R13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>2770</t>
+      <c r="S13" t="n">
+        <v>2770</v>
+      </c>
+      <c r="T13" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>2831</t>
         </is>
       </c>
     </row>
@@ -1352,9 +1434,15 @@
       <c r="R14" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>5104</t>
+      <c r="S14" t="n">
+        <v>5104</v>
+      </c>
+      <c r="T14" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>5486</t>
         </is>
       </c>
     </row>
@@ -1419,9 +1507,15 @@
       <c r="R15" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>4513</t>
+      <c r="S15" t="n">
+        <v>4513</v>
+      </c>
+      <c r="T15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>4720</t>
         </is>
       </c>
     </row>
@@ -1486,9 +1580,15 @@
       <c r="R16" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>4523</t>
+      <c r="S16" t="n">
+        <v>4523</v>
+      </c>
+      <c r="T16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>4754</t>
         </is>
       </c>
     </row>
@@ -1511,7 +1611,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F17" s="3" t="n">
@@ -1553,9 +1653,15 @@
       <c r="R17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>4451</t>
+      <c r="S17" t="n">
+        <v>4451</v>
+      </c>
+      <c r="T17" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>4695</t>
         </is>
       </c>
     </row>
@@ -1578,7 +1684,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F18" s="3" t="n">
@@ -1620,9 +1726,15 @@
       <c r="R18" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>4228</t>
+      <c r="S18" t="n">
+        <v>4228</v>
+      </c>
+      <c r="T18" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>4604</t>
         </is>
       </c>
     </row>
@@ -1687,9 +1799,15 @@
       <c r="R19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>4813</t>
+      <c r="S19" t="n">
+        <v>4813</v>
+      </c>
+      <c r="T19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>5078</t>
         </is>
       </c>
     </row>
@@ -1754,9 +1872,15 @@
       <c r="R20" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>4608</t>
+      <c r="S20" t="n">
+        <v>4608</v>
+      </c>
+      <c r="T20" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>4998</t>
         </is>
       </c>
     </row>
@@ -1779,7 +1903,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F21" s="2" t="n">
@@ -1821,9 +1945,15 @@
       <c r="R21" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>4119</t>
+      <c r="S21" t="n">
+        <v>4119</v>
+      </c>
+      <c r="T21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>4385</t>
         </is>
       </c>
     </row>
@@ -1888,9 +2018,15 @@
       <c r="R22" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>4646</t>
+      <c r="S22" t="n">
+        <v>4646</v>
+      </c>
+      <c r="T22" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>4991</t>
         </is>
       </c>
     </row>
@@ -1955,9 +2091,15 @@
       <c r="R23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>4029</t>
+      <c r="S23" t="n">
+        <v>4029</v>
+      </c>
+      <c r="T23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>4426</t>
         </is>
       </c>
     </row>
@@ -2022,9 +2164,15 @@
       <c r="R24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>4354</t>
+      <c r="S24" t="n">
+        <v>4354</v>
+      </c>
+      <c r="T24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>4602</t>
         </is>
       </c>
     </row>
@@ -2089,7 +2237,13 @@
       <c r="R25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S25" t="inlineStr">
+      <c r="S25" t="n">
+        <v>2500</v>
+      </c>
+      <c r="T25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2156,9 +2310,15 @@
       <c r="R26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>4593</t>
+      <c r="S26" t="n">
+        <v>4593</v>
+      </c>
+      <c r="T26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>4853</t>
         </is>
       </c>
     </row>
@@ -2223,9 +2383,15 @@
       <c r="R27" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>4825</t>
+      <c r="S27" t="n">
+        <v>4825</v>
+      </c>
+      <c r="T27" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>5213</t>
         </is>
       </c>
     </row>
@@ -2290,9 +2456,15 @@
       <c r="R28" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>3924</t>
+      <c r="S28" t="n">
+        <v>3924</v>
+      </c>
+      <c r="T28" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>4132</t>
         </is>
       </c>
     </row>
@@ -2357,9 +2529,15 @@
       <c r="R29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>3949</t>
+      <c r="S29" t="n">
+        <v>3949</v>
+      </c>
+      <c r="T29" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>4016</t>
         </is>
       </c>
     </row>
@@ -2424,9 +2602,15 @@
       <c r="R30" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>4988</t>
+      <c r="S30" t="n">
+        <v>4988</v>
+      </c>
+      <c r="T30" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>5258</t>
         </is>
       </c>
     </row>
@@ -2491,9 +2675,15 @@
       <c r="R31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>4471</t>
+      <c r="S31" t="n">
+        <v>4471</v>
+      </c>
+      <c r="T31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>4763</t>
         </is>
       </c>
     </row>
@@ -2558,9 +2748,15 @@
       <c r="R32" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>4990</t>
+      <c r="S32" t="n">
+        <v>4990</v>
+      </c>
+      <c r="T32" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>5234</t>
         </is>
       </c>
     </row>
@@ -2625,9 +2821,15 @@
       <c r="R33" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>5076</t>
+      <c r="S33" t="n">
+        <v>5076</v>
+      </c>
+      <c r="T33" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>5352</t>
         </is>
       </c>
     </row>
@@ -2650,7 +2852,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F34" s="2" t="n">
@@ -2692,9 +2894,15 @@
       <c r="R34" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>3134</t>
+      <c r="S34" t="n">
+        <v>3134</v>
+      </c>
+      <c r="T34" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>3476</t>
         </is>
       </c>
     </row>
@@ -2759,9 +2967,15 @@
       <c r="R35" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>4888</t>
+      <c r="S35" t="n">
+        <v>4888</v>
+      </c>
+      <c r="T35" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>5030</t>
         </is>
       </c>
     </row>
@@ -2784,7 +2998,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F36" s="5" t="n">
@@ -2826,9 +3040,15 @@
       <c r="R36" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="S36" t="inlineStr">
-        <is>
-          <t>4197</t>
+      <c r="S36" t="n">
+        <v>4197</v>
+      </c>
+      <c r="T36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>4443</t>
         </is>
       </c>
     </row>
@@ -2893,9 +3113,15 @@
       <c r="R37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>4295</t>
+      <c r="S37" t="n">
+        <v>4295</v>
+      </c>
+      <c r="T37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>4466</t>
         </is>
       </c>
     </row>
@@ -2960,9 +3186,15 @@
       <c r="R38" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S38" t="inlineStr">
-        <is>
-          <t>4715</t>
+      <c r="S38" t="n">
+        <v>4715</v>
+      </c>
+      <c r="T38" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>4936</t>
         </is>
       </c>
     </row>
@@ -3027,9 +3259,15 @@
       <c r="R39" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="S39" t="inlineStr">
-        <is>
-          <t>4368</t>
+      <c r="S39" t="n">
+        <v>4368</v>
+      </c>
+      <c r="T39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>4616</t>
         </is>
       </c>
     </row>
@@ -3094,9 +3332,15 @@
       <c r="R40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S40" t="inlineStr">
-        <is>
-          <t>4999</t>
+      <c r="S40" t="n">
+        <v>4999</v>
+      </c>
+      <c r="T40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>5310</t>
         </is>
       </c>
     </row>
@@ -3119,7 +3363,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F41" s="3" t="n">
@@ -3161,9 +3405,15 @@
       <c r="R41" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>4815</t>
+      <c r="S41" t="n">
+        <v>4815</v>
+      </c>
+      <c r="T41" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>5076</t>
         </is>
       </c>
     </row>
@@ -3228,9 +3478,15 @@
       <c r="R42" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>5000</t>
+      <c r="S42" t="n">
+        <v>5000</v>
+      </c>
+      <c r="T42" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>5382</t>
         </is>
       </c>
     </row>
@@ -3295,9 +3551,15 @@
       <c r="R43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S43" t="inlineStr">
-        <is>
-          <t>4600</t>
+      <c r="S43" t="n">
+        <v>4600</v>
+      </c>
+      <c r="T43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>4851</t>
         </is>
       </c>
     </row>
@@ -3362,9 +3624,15 @@
       <c r="R44" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S44" t="inlineStr">
-        <is>
-          <t>3735</t>
+      <c r="S44" t="n">
+        <v>3735</v>
+      </c>
+      <c r="T44" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>3910</t>
         </is>
       </c>
     </row>
@@ -3429,9 +3697,15 @@
       <c r="R45" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="S45" t="inlineStr">
-        <is>
-          <t>4356</t>
+      <c r="S45" t="n">
+        <v>4356</v>
+      </c>
+      <c r="T45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>4506</t>
         </is>
       </c>
     </row>
@@ -3496,9 +3770,15 @@
       <c r="R46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>4210</t>
+      <c r="S46" t="n">
+        <v>4210</v>
+      </c>
+      <c r="T46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>4331</t>
         </is>
       </c>
     </row>
@@ -3521,7 +3801,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F47" s="4" t="n">
@@ -3563,9 +3843,15 @@
       <c r="R47" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S47" t="inlineStr">
-        <is>
-          <t>4386</t>
+      <c r="S47" t="n">
+        <v>4386</v>
+      </c>
+      <c r="T47" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>4561</t>
         </is>
       </c>
     </row>
@@ -3588,7 +3874,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F48" s="4" t="n">
@@ -3630,9 +3916,15 @@
       <c r="R48" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S48" t="inlineStr">
-        <is>
-          <t>4488</t>
+      <c r="S48" t="n">
+        <v>4488</v>
+      </c>
+      <c r="T48" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>4742</t>
         </is>
       </c>
     </row>
@@ -3697,9 +3989,15 @@
       <c r="R49" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="S49" t="inlineStr">
-        <is>
-          <t>3683</t>
+      <c r="S49" t="n">
+        <v>3683</v>
+      </c>
+      <c r="T49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>3604</t>
         </is>
       </c>
     </row>
@@ -3764,9 +4062,15 @@
       <c r="R50" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S50" t="inlineStr">
-        <is>
-          <t>4401</t>
+      <c r="S50" t="n">
+        <v>4401</v>
+      </c>
+      <c r="T50" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>4470</t>
         </is>
       </c>
     </row>
@@ -3831,9 +4135,15 @@
       <c r="R51" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="S51" t="inlineStr">
-        <is>
-          <t>4352</t>
+      <c r="S51" t="n">
+        <v>4352</v>
+      </c>
+      <c r="T51" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>4809</t>
         </is>
       </c>
     </row>
@@ -3898,9 +4208,15 @@
       <c r="R52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S52" t="inlineStr">
-        <is>
-          <t>2573</t>
+      <c r="S52" t="n">
+        <v>2573</v>
+      </c>
+      <c r="T52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>2584</t>
         </is>
       </c>
     </row>
@@ -3965,9 +4281,15 @@
       <c r="R53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S53" t="inlineStr">
-        <is>
-          <t>3018</t>
+      <c r="S53" t="n">
+        <v>3018</v>
+      </c>
+      <c r="T53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>3091</t>
         </is>
       </c>
     </row>
@@ -4032,7 +4354,13 @@
       <c r="R54" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="S54" t="inlineStr">
+      <c r="S54" t="n">
+        <v>2990</v>
+      </c>
+      <c r="T54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U54" t="inlineStr">
         <is>
           <t>2990</t>
         </is>
@@ -4099,9 +4427,15 @@
       <c r="R55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>3542</t>
+      <c r="S55" t="n">
+        <v>3542</v>
+      </c>
+      <c r="T55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>3752</t>
         </is>
       </c>
     </row>
@@ -4166,9 +4500,15 @@
       <c r="R56" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="S56" t="inlineStr">
-        <is>
-          <t>3871</t>
+      <c r="S56" t="n">
+        <v>3871</v>
+      </c>
+      <c r="T56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>3978</t>
         </is>
       </c>
     </row>
@@ -4233,9 +4573,15 @@
       <c r="R57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>4295</t>
+      <c r="S57" t="n">
+        <v>4295</v>
+      </c>
+      <c r="T57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>4512</t>
         </is>
       </c>
     </row>
@@ -4300,9 +4646,15 @@
       <c r="R58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S58" t="inlineStr">
-        <is>
-          <t>3685</t>
+      <c r="S58" t="n">
+        <v>3685</v>
+      </c>
+      <c r="T58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>3843</t>
         </is>
       </c>
     </row>
@@ -4367,9 +4719,15 @@
       <c r="R59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S59" t="inlineStr">
-        <is>
-          <t>4211</t>
+      <c r="S59" t="n">
+        <v>4211</v>
+      </c>
+      <c r="T59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>4371</t>
         </is>
       </c>
     </row>
@@ -4434,9 +4792,15 @@
       <c r="R60" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="S60" t="inlineStr">
-        <is>
-          <t>4464</t>
+      <c r="S60" t="n">
+        <v>4464</v>
+      </c>
+      <c r="T60" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>4673</t>
         </is>
       </c>
     </row>
@@ -4501,9 +4865,15 @@
       <c r="R61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S61" t="inlineStr">
-        <is>
-          <t>4270</t>
+      <c r="S61" t="n">
+        <v>4270</v>
+      </c>
+      <c r="T61" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>4406</t>
         </is>
       </c>
     </row>
@@ -4568,9 +4938,15 @@
       <c r="R62" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="S62" t="inlineStr">
-        <is>
-          <t>4274</t>
+      <c r="S62" t="n">
+        <v>4274</v>
+      </c>
+      <c r="T62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>4430</t>
         </is>
       </c>
     </row>
@@ -4635,9 +5011,15 @@
       <c r="R63" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>3755</t>
+      <c r="S63" t="n">
+        <v>3755</v>
+      </c>
+      <c r="T63" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>3937</t>
         </is>
       </c>
     </row>
@@ -4702,7 +5084,13 @@
       <c r="R64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S64" t="inlineStr">
+      <c r="S64" t="n">
+        <v>2575</v>
+      </c>
+      <c r="T64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U64" t="inlineStr">
         <is>
           <t>2575</t>
         </is>
@@ -4769,9 +5157,15 @@
       <c r="R65" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="S65" t="inlineStr">
-        <is>
-          <t>3610</t>
+      <c r="S65" t="n">
+        <v>3610</v>
+      </c>
+      <c r="T65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>3628</t>
         </is>
       </c>
     </row>
@@ -4836,9 +5230,15 @@
       <c r="R66" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="S66" t="inlineStr">
-        <is>
-          <t>3457</t>
+      <c r="S66" t="n">
+        <v>3457</v>
+      </c>
+      <c r="T66" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>3753</t>
         </is>
       </c>
     </row>
@@ -4903,9 +5303,15 @@
       <c r="R67" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S67" t="inlineStr">
-        <is>
-          <t>4435</t>
+      <c r="S67" t="n">
+        <v>4435</v>
+      </c>
+      <c r="T67" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>4613</t>
         </is>
       </c>
     </row>
@@ -4970,9 +5376,15 @@
       <c r="R68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S68" t="inlineStr">
-        <is>
-          <t>3779</t>
+      <c r="S68" t="n">
+        <v>3779</v>
+      </c>
+      <c r="T68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>3851</t>
         </is>
       </c>
     </row>
@@ -5037,9 +5449,15 @@
       <c r="R69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S69" t="inlineStr">
-        <is>
-          <t>2691</t>
+      <c r="S69" t="n">
+        <v>2691</v>
+      </c>
+      <c r="T69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>2712</t>
         </is>
       </c>
     </row>
@@ -5104,9 +5522,15 @@
       <c r="R70" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="S70" t="inlineStr">
-        <is>
-          <t>3357</t>
+      <c r="S70" t="n">
+        <v>3357</v>
+      </c>
+      <c r="T70" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>3480</t>
         </is>
       </c>
     </row>
@@ -5171,9 +5595,15 @@
       <c r="R71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S71" t="inlineStr">
-        <is>
-          <t>4643</t>
+      <c r="S71" t="n">
+        <v>4643</v>
+      </c>
+      <c r="T71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>4740</t>
         </is>
       </c>
     </row>
@@ -5238,9 +5668,15 @@
       <c r="R72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S72" t="inlineStr">
-        <is>
-          <t>3525</t>
+      <c r="S72" t="n">
+        <v>3525</v>
+      </c>
+      <c r="T72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>3522</t>
         </is>
       </c>
     </row>
@@ -5305,9 +5741,15 @@
       <c r="R73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S73" t="inlineStr">
-        <is>
-          <t>4285</t>
+      <c r="S73" t="n">
+        <v>4285</v>
+      </c>
+      <c r="T73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>4487</t>
         </is>
       </c>
     </row>
@@ -5372,9 +5814,15 @@
       <c r="R74" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="S74" t="inlineStr">
-        <is>
-          <t>3914</t>
+      <c r="S74" t="n">
+        <v>3914</v>
+      </c>
+      <c r="T74" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U74" t="inlineStr">
+        <is>
+          <t>4118</t>
         </is>
       </c>
     </row>
@@ -5439,9 +5887,15 @@
       <c r="R75" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="S75" t="inlineStr">
-        <is>
-          <t>4070</t>
+      <c r="S75" t="n">
+        <v>4070</v>
+      </c>
+      <c r="T75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>4287</t>
         </is>
       </c>
     </row>
@@ -5506,9 +5960,15 @@
       <c r="R76" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S76" t="inlineStr">
-        <is>
-          <t>4081</t>
+      <c r="S76" t="n">
+        <v>4081</v>
+      </c>
+      <c r="T76" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>4251</t>
         </is>
       </c>
     </row>
@@ -5573,11 +6033,11 @@
       <c r="R77" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="S77" t="inlineStr">
-        <is>
-          <t>2848</t>
-        </is>
-      </c>
+      <c r="S77" t="n">
+        <v>2848</v>
+      </c>
+      <c r="T77" s="3" t="inlineStr"/>
+      <c r="U77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -5640,9 +6100,15 @@
       <c r="R78" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S78" t="inlineStr">
-        <is>
-          <t>3845</t>
+      <c r="S78" t="n">
+        <v>3845</v>
+      </c>
+      <c r="T78" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t>4027</t>
         </is>
       </c>
     </row>
@@ -5707,9 +6173,15 @@
       <c r="R79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S79" t="inlineStr">
-        <is>
-          <t>3684</t>
+      <c r="S79" t="n">
+        <v>3684</v>
+      </c>
+      <c r="T79" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>3875</t>
         </is>
       </c>
     </row>
@@ -5774,9 +6246,15 @@
       <c r="R80" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S80" t="inlineStr">
-        <is>
-          <t>3316</t>
+      <c r="S80" t="n">
+        <v>3316</v>
+      </c>
+      <c r="T80" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U80" t="inlineStr">
+        <is>
+          <t>3352</t>
         </is>
       </c>
     </row>
@@ -5841,9 +6319,15 @@
       <c r="R81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S81" t="inlineStr">
-        <is>
-          <t>2828</t>
+      <c r="S81" t="n">
+        <v>2828</v>
+      </c>
+      <c r="T81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U81" t="inlineStr">
+        <is>
+          <t>2807</t>
         </is>
       </c>
     </row>
@@ -5908,9 +6392,15 @@
       <c r="R82" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S82" t="inlineStr">
-        <is>
-          <t>4122</t>
+      <c r="S82" t="n">
+        <v>4122</v>
+      </c>
+      <c r="T82" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U82" t="inlineStr">
+        <is>
+          <t>4300</t>
         </is>
       </c>
     </row>
@@ -5975,9 +6465,15 @@
       <c r="R83" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S83" t="inlineStr">
-        <is>
-          <t>2780</t>
+      <c r="S83" t="n">
+        <v>2780</v>
+      </c>
+      <c r="T83" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="U83" t="inlineStr">
+        <is>
+          <t>2758</t>
         </is>
       </c>
     </row>
@@ -6042,9 +6538,15 @@
       <c r="R84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S84" t="inlineStr">
-        <is>
-          <t>2943</t>
+      <c r="S84" t="n">
+        <v>2943</v>
+      </c>
+      <c r="T84" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="U84" t="inlineStr">
+        <is>
+          <t>3022</t>
         </is>
       </c>
     </row>
@@ -6109,9 +6611,15 @@
       <c r="R85" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="S85" t="inlineStr">
-        <is>
-          <t>2106</t>
+      <c r="S85" t="n">
+        <v>2106</v>
+      </c>
+      <c r="T85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U85" t="inlineStr">
+        <is>
+          <t>2089</t>
         </is>
       </c>
     </row>
@@ -6176,9 +6684,15 @@
       <c r="R86" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S86" t="inlineStr">
-        <is>
-          <t>2655</t>
+      <c r="S86" t="n">
+        <v>2655</v>
+      </c>
+      <c r="T86" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U86" t="inlineStr">
+        <is>
+          <t>2707</t>
         </is>
       </c>
     </row>
@@ -6243,9 +6757,15 @@
       <c r="R87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S87" t="inlineStr">
-        <is>
-          <t>2912</t>
+      <c r="S87" t="n">
+        <v>2912</v>
+      </c>
+      <c r="T87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U87" t="inlineStr">
+        <is>
+          <t>3015</t>
         </is>
       </c>
     </row>
@@ -6310,9 +6830,15 @@
       <c r="R88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S88" t="inlineStr">
-        <is>
-          <t>2013</t>
+      <c r="S88" t="n">
+        <v>2013</v>
+      </c>
+      <c r="T88" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="U88" t="inlineStr">
+        <is>
+          <t>2413</t>
         </is>
       </c>
     </row>
@@ -6368,6 +6894,8 @@
       <c r="Q89" t="inlineStr"/>
       <c r="R89" s="3" t="inlineStr"/>
       <c r="S89" t="inlineStr"/>
+      <c r="T89" s="3" t="inlineStr"/>
+      <c r="U89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -6421,6 +6949,8 @@
       <c r="Q90" t="inlineStr"/>
       <c r="R90" s="3" t="inlineStr"/>
       <c r="S90" t="inlineStr"/>
+      <c r="T90" s="3" t="inlineStr"/>
+      <c r="U90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -6483,9 +7013,15 @@
       <c r="R91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S91" t="inlineStr">
-        <is>
-          <t>2523</t>
+      <c r="S91" t="n">
+        <v>2523</v>
+      </c>
+      <c r="T91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U91" t="inlineStr">
+        <is>
+          <t>2532</t>
         </is>
       </c>
     </row>
@@ -6550,7 +7086,13 @@
       <c r="R92" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="S92" t="inlineStr">
+      <c r="S92" t="n">
+        <v>3267</v>
+      </c>
+      <c r="T92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U92" t="inlineStr">
         <is>
           <t>3267</t>
         </is>
@@ -6617,9 +7159,15 @@
       <c r="R93" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="S93" t="inlineStr">
-        <is>
-          <t>2821</t>
+      <c r="S93" t="n">
+        <v>2821</v>
+      </c>
+      <c r="T93" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="U93" t="inlineStr">
+        <is>
+          <t>2907</t>
         </is>
       </c>
     </row>
@@ -6684,9 +7232,15 @@
       <c r="R94" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S94" t="inlineStr">
-        <is>
-          <t>3841</t>
+      <c r="S94" t="n">
+        <v>3841</v>
+      </c>
+      <c r="T94" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U94" t="inlineStr">
+        <is>
+          <t>3938</t>
         </is>
       </c>
     </row>
@@ -6751,9 +7305,15 @@
       <c r="R95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S95" t="inlineStr">
-        <is>
-          <t>3602</t>
+      <c r="S95" t="n">
+        <v>3602</v>
+      </c>
+      <c r="T95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U95" t="inlineStr">
+        <is>
+          <t>3750</t>
         </is>
       </c>
     </row>
@@ -6818,9 +7378,15 @@
       <c r="R96" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="S96" t="inlineStr">
-        <is>
-          <t>3433</t>
+      <c r="S96" t="n">
+        <v>3433</v>
+      </c>
+      <c r="T96" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="U96" t="inlineStr">
+        <is>
+          <t>3535</t>
         </is>
       </c>
     </row>
@@ -6885,9 +7451,15 @@
       <c r="R97" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="S97" t="inlineStr">
-        <is>
-          <t>3902</t>
+      <c r="S97" t="n">
+        <v>3902</v>
+      </c>
+      <c r="T97" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="U97" t="inlineStr">
+        <is>
+          <t>4037</t>
         </is>
       </c>
     </row>
@@ -6952,9 +7524,15 @@
       <c r="R98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S98" t="inlineStr">
-        <is>
-          <t>3300</t>
+      <c r="S98" t="n">
+        <v>3300</v>
+      </c>
+      <c r="T98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U98" t="inlineStr">
+        <is>
+          <t>3325</t>
         </is>
       </c>
     </row>
@@ -7019,9 +7597,15 @@
       <c r="R99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S99" t="inlineStr">
-        <is>
-          <t>2656</t>
+      <c r="S99" t="n">
+        <v>2656</v>
+      </c>
+      <c r="T99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U99" t="inlineStr">
+        <is>
+          <t>2605</t>
         </is>
       </c>
     </row>
@@ -7044,7 +7628,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F100" s="2" t="n">
@@ -7086,9 +7670,15 @@
       <c r="R100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S100" t="inlineStr">
-        <is>
-          <t>2600</t>
+      <c r="S100" t="n">
+        <v>2600</v>
+      </c>
+      <c r="T100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U100" t="inlineStr">
+        <is>
+          <t>2604</t>
         </is>
       </c>
     </row>
@@ -7153,9 +7743,15 @@
       <c r="R101" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S101" t="inlineStr">
-        <is>
-          <t>3946</t>
+      <c r="S101" t="n">
+        <v>3946</v>
+      </c>
+      <c r="T101" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="U101" t="inlineStr">
+        <is>
+          <t>4128</t>
         </is>
       </c>
     </row>
@@ -7220,9 +7816,15 @@
       <c r="R102" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="S102" t="inlineStr">
-        <is>
-          <t>3499</t>
+      <c r="S102" t="n">
+        <v>3499</v>
+      </c>
+      <c r="T102" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="U102" t="inlineStr">
+        <is>
+          <t>3554</t>
         </is>
       </c>
     </row>
@@ -7287,9 +7889,15 @@
       <c r="R103" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="S103" t="inlineStr">
-        <is>
-          <t>3233</t>
+      <c r="S103" t="n">
+        <v>3233</v>
+      </c>
+      <c r="T103" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="U103" t="inlineStr">
+        <is>
+          <t>3354</t>
         </is>
       </c>
     </row>
@@ -7354,9 +7962,15 @@
       <c r="R104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S104" t="inlineStr">
-        <is>
-          <t>2566</t>
+      <c r="S104" t="n">
+        <v>2566</v>
+      </c>
+      <c r="T104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U104" t="inlineStr">
+        <is>
+          <t>2561</t>
         </is>
       </c>
     </row>
@@ -7421,9 +8035,15 @@
       <c r="R105" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S105" t="inlineStr">
-        <is>
-          <t>3269</t>
+      <c r="S105" t="n">
+        <v>3269</v>
+      </c>
+      <c r="T105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U105" t="inlineStr">
+        <is>
+          <t>3238</t>
         </is>
       </c>
     </row>
@@ -7488,9 +8108,15 @@
       <c r="R106" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="S106" t="inlineStr">
-        <is>
-          <t>2826</t>
+      <c r="S106" t="n">
+        <v>2826</v>
+      </c>
+      <c r="T106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U106" t="inlineStr">
+        <is>
+          <t>2906</t>
         </is>
       </c>
     </row>
@@ -7555,9 +8181,15 @@
       <c r="R107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S107" t="inlineStr">
-        <is>
-          <t>3298</t>
+      <c r="S107" t="n">
+        <v>3298</v>
+      </c>
+      <c r="T107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U107" t="inlineStr">
+        <is>
+          <t>3431</t>
         </is>
       </c>
     </row>
@@ -7622,9 +8254,15 @@
       <c r="R108" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="S108" t="inlineStr">
-        <is>
-          <t>2532</t>
+      <c r="S108" t="n">
+        <v>2532</v>
+      </c>
+      <c r="T108" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="U108" t="inlineStr">
+        <is>
+          <t>2647</t>
         </is>
       </c>
     </row>
@@ -7689,9 +8327,15 @@
       <c r="R109" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="S109" t="inlineStr">
-        <is>
-          <t>2624</t>
+      <c r="S109" t="n">
+        <v>2624</v>
+      </c>
+      <c r="T109" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="U109" t="inlineStr">
+        <is>
+          <t>2709</t>
         </is>
       </c>
     </row>
@@ -7756,9 +8400,15 @@
       <c r="R110" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="S110" t="inlineStr">
-        <is>
-          <t>3118</t>
+      <c r="S110" t="n">
+        <v>3118</v>
+      </c>
+      <c r="T110" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="U110" t="inlineStr">
+        <is>
+          <t>3200</t>
         </is>
       </c>
     </row>
@@ -7823,9 +8473,15 @@
       <c r="R111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S111" t="inlineStr">
-        <is>
-          <t>2832</t>
+      <c r="S111" t="n">
+        <v>2832</v>
+      </c>
+      <c r="T111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U111" t="inlineStr">
+        <is>
+          <t>2836</t>
         </is>
       </c>
     </row>
@@ -7890,9 +8546,15 @@
       <c r="R112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S112" t="inlineStr">
-        <is>
-          <t>3193</t>
+      <c r="S112" t="n">
+        <v>3193</v>
+      </c>
+      <c r="T112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U112" t="inlineStr">
+        <is>
+          <t>3312</t>
         </is>
       </c>
     </row>
@@ -7957,9 +8619,15 @@
       <c r="R113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S113" t="inlineStr">
-        <is>
-          <t>2542</t>
+      <c r="S113" t="n">
+        <v>2542</v>
+      </c>
+      <c r="T113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U113" t="inlineStr">
+        <is>
+          <t>2525</t>
         </is>
       </c>
     </row>
@@ -8024,9 +8692,15 @@
       <c r="R114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S114" t="inlineStr">
-        <is>
-          <t>3165</t>
+      <c r="S114" t="n">
+        <v>3165</v>
+      </c>
+      <c r="T114" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U114" t="inlineStr">
+        <is>
+          <t>3465</t>
         </is>
       </c>
     </row>
@@ -8091,9 +8765,15 @@
       <c r="R115" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S115" t="inlineStr">
-        <is>
-          <t>2625</t>
+      <c r="S115" t="n">
+        <v>2625</v>
+      </c>
+      <c r="T115" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="U115" t="inlineStr">
+        <is>
+          <t>2622</t>
         </is>
       </c>
     </row>
@@ -8158,9 +8838,15 @@
       <c r="R116" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S116" t="inlineStr">
-        <is>
-          <t>2968</t>
+      <c r="S116" t="n">
+        <v>2968</v>
+      </c>
+      <c r="T116" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U116" t="inlineStr">
+        <is>
+          <t>3009</t>
         </is>
       </c>
     </row>
@@ -8225,9 +8911,15 @@
       <c r="R117" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="S117" t="inlineStr">
-        <is>
-          <t>2982</t>
+      <c r="S117" t="n">
+        <v>2982</v>
+      </c>
+      <c r="T117" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U117" t="inlineStr">
+        <is>
+          <t>3121</t>
         </is>
       </c>
     </row>
@@ -8292,11 +8984,11 @@
       <c r="R118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S118" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="S118" t="n">
+        <v>0</v>
+      </c>
+      <c r="T118" s="3" t="inlineStr"/>
+      <c r="U118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -8359,9 +9051,15 @@
       <c r="R119" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S119" t="inlineStr">
-        <is>
-          <t>3134</t>
+      <c r="S119" t="n">
+        <v>3134</v>
+      </c>
+      <c r="T119" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U119" t="inlineStr">
+        <is>
+          <t>3327</t>
         </is>
       </c>
     </row>
@@ -8426,9 +9124,15 @@
       <c r="R120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S120" t="inlineStr">
-        <is>
-          <t>3020</t>
+      <c r="S120" t="n">
+        <v>3020</v>
+      </c>
+      <c r="T120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U120" t="inlineStr">
+        <is>
+          <t>3088</t>
         </is>
       </c>
     </row>
@@ -8493,9 +9197,15 @@
       <c r="R121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S121" t="inlineStr">
-        <is>
-          <t>2190</t>
+      <c r="S121" t="n">
+        <v>2190</v>
+      </c>
+      <c r="T121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U121" t="inlineStr">
+        <is>
+          <t>2183</t>
         </is>
       </c>
     </row>
@@ -8560,9 +9270,15 @@
       <c r="R122" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="S122" t="inlineStr">
-        <is>
-          <t>2537</t>
+      <c r="S122" t="n">
+        <v>2537</v>
+      </c>
+      <c r="T122" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="U122" t="inlineStr">
+        <is>
+          <t>2566</t>
         </is>
       </c>
     </row>
@@ -8627,9 +9343,15 @@
       <c r="R123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S123" t="inlineStr">
-        <is>
-          <t>2504</t>
+      <c r="S123" t="n">
+        <v>2504</v>
+      </c>
+      <c r="T123" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="U123" t="inlineStr">
+        <is>
+          <t>2667</t>
         </is>
       </c>
     </row>
@@ -8694,9 +9416,15 @@
       <c r="R124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S124" t="inlineStr">
-        <is>
-          <t>3234</t>
+      <c r="S124" t="n">
+        <v>3234</v>
+      </c>
+      <c r="T124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U124" t="inlineStr">
+        <is>
+          <t>3336</t>
         </is>
       </c>
     </row>
@@ -8761,7 +9489,13 @@
       <c r="R125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S125" t="inlineStr">
+      <c r="S125" t="n">
+        <v>0</v>
+      </c>
+      <c r="T125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8828,9 +9562,15 @@
       <c r="R126" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="S126" t="inlineStr">
-        <is>
-          <t>2897</t>
+      <c r="S126" t="n">
+        <v>2897</v>
+      </c>
+      <c r="T126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U126" t="inlineStr">
+        <is>
+          <t>2918</t>
         </is>
       </c>
     </row>
@@ -8895,9 +9635,15 @@
       <c r="R127" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="S127" t="inlineStr">
-        <is>
-          <t>2653</t>
+      <c r="S127" t="n">
+        <v>2653</v>
+      </c>
+      <c r="T127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U127" t="inlineStr">
+        <is>
+          <t>2606</t>
         </is>
       </c>
     </row>
@@ -8962,9 +9708,15 @@
       <c r="R128" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S128" t="inlineStr">
-        <is>
-          <t>2633</t>
+      <c r="S128" t="n">
+        <v>2633</v>
+      </c>
+      <c r="T128" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="U128" t="inlineStr">
+        <is>
+          <t>2638</t>
         </is>
       </c>
     </row>
@@ -9029,9 +9781,15 @@
       <c r="R129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S129" t="inlineStr">
-        <is>
-          <t>2403</t>
+      <c r="S129" t="n">
+        <v>2403</v>
+      </c>
+      <c r="T129" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="U129" t="inlineStr">
+        <is>
+          <t>2504</t>
         </is>
       </c>
     </row>
@@ -9096,9 +9854,15 @@
       <c r="R130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S130" t="inlineStr">
-        <is>
-          <t>1928</t>
+      <c r="S130" t="n">
+        <v>1928</v>
+      </c>
+      <c r="T130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U130" t="inlineStr">
+        <is>
+          <t>1915</t>
         </is>
       </c>
     </row>
@@ -9163,7 +9927,13 @@
       <c r="R131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S131" t="inlineStr">
+      <c r="S131" t="n">
+        <v>0</v>
+      </c>
+      <c r="T131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9230,7 +10000,13 @@
       <c r="R132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S132" t="inlineStr">
+      <c r="S132" t="n">
+        <v>0</v>
+      </c>
+      <c r="T132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9297,11 +10073,11 @@
       <c r="R133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S133" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="S133" t="n">
+        <v>0</v>
+      </c>
+      <c r="T133" s="3" t="inlineStr"/>
+      <c r="U133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -9364,9 +10140,15 @@
       <c r="R134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S134" t="inlineStr">
-        <is>
-          <t>1958</t>
+      <c r="S134" t="n">
+        <v>1958</v>
+      </c>
+      <c r="T134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U134" t="inlineStr">
+        <is>
+          <t>1988</t>
         </is>
       </c>
     </row>
@@ -9431,9 +10213,15 @@
       <c r="R135" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="S135" t="inlineStr">
-        <is>
-          <t>2280</t>
+      <c r="S135" t="n">
+        <v>2280</v>
+      </c>
+      <c r="T135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U135" t="inlineStr">
+        <is>
+          <t>2237</t>
         </is>
       </c>
     </row>
@@ -9498,9 +10286,15 @@
       <c r="R136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S136" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="S136" t="n">
+        <v>0</v>
+      </c>
+      <c r="T136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U136" t="inlineStr">
+        <is>
+          <t>1520</t>
         </is>
       </c>
     </row>
@@ -9565,11 +10359,11 @@
       <c r="R137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S137" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="S137" t="n">
+        <v>0</v>
+      </c>
+      <c r="T137" s="3" t="inlineStr"/>
+      <c r="U137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -9632,7 +10426,13 @@
       <c r="R138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S138" t="inlineStr">
+      <c r="S138" t="n">
+        <v>0</v>
+      </c>
+      <c r="T138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9699,11 +10499,11 @@
       <c r="R139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S139" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="S139" t="n">
+        <v>0</v>
+      </c>
+      <c r="T139" s="3" t="inlineStr"/>
+      <c r="U139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -9766,9 +10566,15 @@
       <c r="R140" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="S140" t="inlineStr">
-        <is>
-          <t>4109</t>
+      <c r="S140" t="n">
+        <v>4109</v>
+      </c>
+      <c r="T140" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="U140" t="inlineStr">
+        <is>
+          <t>4322</t>
         </is>
       </c>
     </row>
@@ -9833,7 +10639,13 @@
       <c r="R141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S141" t="inlineStr">
+      <c r="S141" t="n">
+        <v>0</v>
+      </c>
+      <c r="T141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9900,7 +10712,13 @@
       <c r="R142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S142" t="inlineStr">
+      <c r="S142" t="n">
+        <v>0</v>
+      </c>
+      <c r="T142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9967,9 +10785,15 @@
       <c r="R143" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="S143" t="inlineStr">
-        <is>
-          <t>4397</t>
+      <c r="S143" t="n">
+        <v>4397</v>
+      </c>
+      <c r="T143" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="U143" t="inlineStr">
+        <is>
+          <t>4650</t>
         </is>
       </c>
     </row>
@@ -10034,7 +10858,13 @@
       <c r="R144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S144" t="inlineStr">
+      <c r="S144" t="n">
+        <v>0</v>
+      </c>
+      <c r="T144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10101,9 +10931,15 @@
       <c r="R145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S145" t="inlineStr">
-        <is>
-          <t>2795</t>
+      <c r="S145" t="n">
+        <v>2795</v>
+      </c>
+      <c r="T145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U145" t="inlineStr">
+        <is>
+          <t>2751</t>
         </is>
       </c>
     </row>
@@ -10168,7 +11004,13 @@
       <c r="R146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S146" t="inlineStr">
+      <c r="S146" t="n">
+        <v>0</v>
+      </c>
+      <c r="T146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10235,9 +11077,15 @@
       <c r="R147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S147" t="inlineStr">
-        <is>
-          <t>2633</t>
+      <c r="S147" t="n">
+        <v>2633</v>
+      </c>
+      <c r="T147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U147" t="inlineStr">
+        <is>
+          <t>2659</t>
         </is>
       </c>
     </row>
@@ -10247,7 +11095,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>"Cool dude"</t>
+          <t>"king of war £"</t>
         </is>
       </c>
       <c r="C148" t="inlineStr"/>
@@ -10283,6 +11131,14 @@
       <c r="Q148" t="inlineStr"/>
       <c r="R148" s="3" t="inlineStr"/>
       <c r="S148" t="inlineStr"/>
+      <c r="T148" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="U148" t="inlineStr">
+        <is>
+          <t>2943</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -10339,7 +11195,13 @@
       <c r="R149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S149" t="inlineStr">
+      <c r="S149" t="n">
+        <v>0</v>
+      </c>
+      <c r="T149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10400,7 +11262,13 @@
       <c r="R150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S150" t="inlineStr">
+      <c r="S150" t="n">
+        <v>0</v>
+      </c>
+      <c r="T150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10449,9 +11317,15 @@
       <c r="R151" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S151" t="inlineStr">
-        <is>
-          <t>2361</t>
+      <c r="S151" t="n">
+        <v>2361</v>
+      </c>
+      <c r="T151" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="U151" t="inlineStr">
+        <is>
+          <t>2262</t>
         </is>
       </c>
     </row>
@@ -10498,7 +11372,13 @@
       <c r="R152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S152" t="inlineStr">
+      <c r="S152" t="n">
+        <v>0</v>
+      </c>
+      <c r="T152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10539,9 +11419,15 @@
       <c r="R153" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="S153" t="inlineStr">
-        <is>
-          <t>3553</t>
+      <c r="S153" t="n">
+        <v>3553</v>
+      </c>
+      <c r="T153" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U153" t="inlineStr">
+        <is>
+          <t>3795</t>
         </is>
       </c>
     </row>
@@ -10580,17 +11466,21 @@
       <c r="R154" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="S154" t="inlineStr">
-        <is>
-          <t>1648</t>
+      <c r="S154" t="n">
+        <v>1648</v>
+      </c>
+      <c r="T154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U154" t="inlineStr">
+        <is>
+          <t>1700</t>
         </is>
       </c>
     </row>
     <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>58415620</t>
-        </is>
+      <c r="A155" t="n">
+        <v>58415620</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
@@ -10619,9 +11509,138 @@
       <c r="R155" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="S155" t="inlineStr">
-        <is>
-          <t>1441</t>
+      <c r="S155" t="n">
+        <v>1441</v>
+      </c>
+      <c r="T155" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="U155" t="inlineStr">
+        <is>
+          <t>1509</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>14110169</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>"Pasiony CANQ"</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr"/>
+      <c r="D156" t="inlineStr"/>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F156" s="3" t="inlineStr"/>
+      <c r="G156" t="inlineStr"/>
+      <c r="H156" s="3" t="inlineStr"/>
+      <c r="I156" t="inlineStr"/>
+      <c r="J156" s="3" t="inlineStr"/>
+      <c r="K156" t="inlineStr"/>
+      <c r="L156" s="3" t="inlineStr"/>
+      <c r="M156" t="inlineStr"/>
+      <c r="N156" s="3" t="inlineStr"/>
+      <c r="O156" t="inlineStr"/>
+      <c r="P156" s="3" t="inlineStr"/>
+      <c r="Q156" t="inlineStr"/>
+      <c r="R156" s="3" t="inlineStr"/>
+      <c r="S156" t="inlineStr"/>
+      <c r="T156" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="U156" t="inlineStr">
+        <is>
+          <t>3065</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>47928278</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>㊥JOSE</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr"/>
+      <c r="D157" t="inlineStr"/>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F157" s="3" t="inlineStr"/>
+      <c r="G157" t="inlineStr"/>
+      <c r="H157" s="3" t="inlineStr"/>
+      <c r="I157" t="inlineStr"/>
+      <c r="J157" s="3" t="inlineStr"/>
+      <c r="K157" t="inlineStr"/>
+      <c r="L157" s="3" t="inlineStr"/>
+      <c r="M157" t="inlineStr"/>
+      <c r="N157" s="3" t="inlineStr"/>
+      <c r="O157" t="inlineStr"/>
+      <c r="P157" s="3" t="inlineStr"/>
+      <c r="Q157" t="inlineStr"/>
+      <c r="R157" s="3" t="inlineStr"/>
+      <c r="S157" t="inlineStr"/>
+      <c r="T157" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="U157" t="inlineStr">
+        <is>
+          <t>5535</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>8031795</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>復仇者聯盟</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr"/>
+      <c r="D158" t="inlineStr"/>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F158" s="3" t="inlineStr"/>
+      <c r="G158" t="inlineStr"/>
+      <c r="H158" s="3" t="inlineStr"/>
+      <c r="I158" t="inlineStr"/>
+      <c r="J158" s="3" t="inlineStr"/>
+      <c r="K158" t="inlineStr"/>
+      <c r="L158" s="3" t="inlineStr"/>
+      <c r="M158" t="inlineStr"/>
+      <c r="N158" s="3" t="inlineStr"/>
+      <c r="O158" t="inlineStr"/>
+      <c r="P158" s="3" t="inlineStr"/>
+      <c r="Q158" t="inlineStr"/>
+      <c r="R158" s="3" t="inlineStr"/>
+      <c r="S158" t="inlineStr"/>
+      <c r="T158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U158" t="inlineStr">
+        <is>
+          <t>1926</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-10 11:30:51
</commit_message>
<xml_diff>
--- a/Season_Attack/81.xlsx
+++ b/Season_Attack/81.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U158"/>
+  <dimension ref="A1:W162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,6 +496,16 @@
           <t>01-08_0</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>01-09_A</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>01-09_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -564,9 +574,15 @@
       <c r="T2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>3729</t>
+      <c r="U2" t="n">
+        <v>3729</v>
+      </c>
+      <c r="V2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>4069</t>
         </is>
       </c>
     </row>
@@ -589,7 +605,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F3" s="3" t="n">
@@ -637,9 +653,15 @@
       <c r="T3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>4348</t>
+      <c r="U3" t="n">
+        <v>4348</v>
+      </c>
+      <c r="V3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>4523</t>
         </is>
       </c>
     </row>
@@ -710,9 +732,15 @@
       <c r="T4" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>4689</t>
+      <c r="U4" t="n">
+        <v>4689</v>
+      </c>
+      <c r="V4" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>5068</t>
         </is>
       </c>
     </row>
@@ -783,9 +811,15 @@
       <c r="T5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>5016</t>
+      <c r="U5" t="n">
+        <v>5016</v>
+      </c>
+      <c r="V5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>5364</t>
         </is>
       </c>
     </row>
@@ -856,9 +890,15 @@
       <c r="T6" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>5004</t>
+      <c r="U6" t="n">
+        <v>5004</v>
+      </c>
+      <c r="V6" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>5340</t>
         </is>
       </c>
     </row>
@@ -929,9 +969,15 @@
       <c r="T7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>5314</t>
+      <c r="U7" t="n">
+        <v>5314</v>
+      </c>
+      <c r="V7" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>5729</t>
         </is>
       </c>
     </row>
@@ -1002,9 +1048,15 @@
       <c r="T8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>4572</t>
+      <c r="U8" t="n">
+        <v>4572</v>
+      </c>
+      <c r="V8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>4768</t>
         </is>
       </c>
     </row>
@@ -1075,9 +1127,15 @@
       <c r="T9" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>4713</t>
+      <c r="U9" t="n">
+        <v>4713</v>
+      </c>
+      <c r="V9" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>4856</t>
         </is>
       </c>
     </row>
@@ -1148,9 +1206,15 @@
       <c r="T10" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>4274</t>
+      <c r="U10" t="n">
+        <v>4274</v>
+      </c>
+      <c r="V10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>4414</t>
         </is>
       </c>
     </row>
@@ -1221,9 +1285,15 @@
       <c r="T11" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>4866</t>
+      <c r="U11" t="n">
+        <v>4866</v>
+      </c>
+      <c r="V11" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>5377</t>
         </is>
       </c>
     </row>
@@ -1294,9 +1364,15 @@
       <c r="T12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U12" t="inlineStr">
-        <is>
-          <t>4249</t>
+      <c r="U12" t="n">
+        <v>4249</v>
+      </c>
+      <c r="V12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>4609</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1443,13 @@
       <c r="T13" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="U13" t="inlineStr">
+      <c r="U13" t="n">
+        <v>2831</v>
+      </c>
+      <c r="V13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="inlineStr">
         <is>
           <t>2831</t>
         </is>
@@ -1440,9 +1522,15 @@
       <c r="T14" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>5486</t>
+      <c r="U14" t="n">
+        <v>5486</v>
+      </c>
+      <c r="V14" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>5663</t>
         </is>
       </c>
     </row>
@@ -1513,9 +1601,15 @@
       <c r="T15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>4720</t>
+      <c r="U15" t="n">
+        <v>4720</v>
+      </c>
+      <c r="V15" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>5010</t>
         </is>
       </c>
     </row>
@@ -1586,9 +1680,15 @@
       <c r="T16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U16" t="inlineStr">
-        <is>
-          <t>4754</t>
+      <c r="U16" t="n">
+        <v>4754</v>
+      </c>
+      <c r="V16" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>5285</t>
         </is>
       </c>
     </row>
@@ -1659,9 +1759,15 @@
       <c r="T17" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>4695</t>
+      <c r="U17" t="n">
+        <v>4695</v>
+      </c>
+      <c r="V17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>4869</t>
         </is>
       </c>
     </row>
@@ -1732,9 +1838,15 @@
       <c r="T18" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>4604</t>
+      <c r="U18" t="n">
+        <v>4604</v>
+      </c>
+      <c r="V18" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>4786</t>
         </is>
       </c>
     </row>
@@ -1805,9 +1917,15 @@
       <c r="T19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>5078</t>
+      <c r="U19" t="n">
+        <v>5078</v>
+      </c>
+      <c r="V19" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>5357</t>
         </is>
       </c>
     </row>
@@ -1878,9 +1996,15 @@
       <c r="T20" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>4998</t>
+      <c r="U20" t="n">
+        <v>4998</v>
+      </c>
+      <c r="V20" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>5513</t>
         </is>
       </c>
     </row>
@@ -1951,9 +2075,15 @@
       <c r="T21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>4385</t>
+      <c r="U21" t="n">
+        <v>4385</v>
+      </c>
+      <c r="V21" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>4548</t>
         </is>
       </c>
     </row>
@@ -2024,9 +2154,15 @@
       <c r="T22" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>4991</t>
+      <c r="U22" t="n">
+        <v>4991</v>
+      </c>
+      <c r="V22" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>5428</t>
         </is>
       </c>
     </row>
@@ -2097,9 +2233,15 @@
       <c r="T23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>4426</t>
+      <c r="U23" t="n">
+        <v>4426</v>
+      </c>
+      <c r="V23" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>5002</t>
         </is>
       </c>
     </row>
@@ -2170,9 +2312,15 @@
       <c r="T24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>4602</t>
+      <c r="U24" t="n">
+        <v>4602</v>
+      </c>
+      <c r="V24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>4673</t>
         </is>
       </c>
     </row>
@@ -2243,7 +2391,13 @@
       <c r="T25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U25" t="inlineStr">
+      <c r="U25" t="n">
+        <v>2500</v>
+      </c>
+      <c r="V25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2316,9 +2470,15 @@
       <c r="T26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>4853</t>
+      <c r="U26" t="n">
+        <v>4853</v>
+      </c>
+      <c r="V26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>5188</t>
         </is>
       </c>
     </row>
@@ -2341,7 +2501,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F27" s="4" t="n">
@@ -2389,9 +2549,15 @@
       <c r="T27" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="U27" t="inlineStr">
-        <is>
-          <t>5213</t>
+      <c r="U27" t="n">
+        <v>5213</v>
+      </c>
+      <c r="V27" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>5350</t>
         </is>
       </c>
     </row>
@@ -2462,9 +2628,15 @@
       <c r="T28" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>4132</t>
+      <c r="U28" t="n">
+        <v>4132</v>
+      </c>
+      <c r="V28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>4238</t>
         </is>
       </c>
     </row>
@@ -2535,9 +2707,15 @@
       <c r="T29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>4016</t>
+      <c r="U29" t="n">
+        <v>4016</v>
+      </c>
+      <c r="V29" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>4156</t>
         </is>
       </c>
     </row>
@@ -2608,9 +2786,15 @@
       <c r="T30" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>5258</t>
+      <c r="U30" t="n">
+        <v>5258</v>
+      </c>
+      <c r="V30" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>5535</t>
         </is>
       </c>
     </row>
@@ -2633,7 +2817,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F31" s="4" t="n">
@@ -2681,9 +2865,15 @@
       <c r="T31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>4763</t>
+      <c r="U31" t="n">
+        <v>4763</v>
+      </c>
+      <c r="V31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>5084</t>
         </is>
       </c>
     </row>
@@ -2754,9 +2944,15 @@
       <c r="T32" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U32" t="inlineStr">
-        <is>
-          <t>5234</t>
+      <c r="U32" t="n">
+        <v>5234</v>
+      </c>
+      <c r="V32" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>5339</t>
         </is>
       </c>
     </row>
@@ -2827,9 +3023,15 @@
       <c r="T33" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U33" t="inlineStr">
-        <is>
-          <t>5352</t>
+      <c r="U33" t="n">
+        <v>5352</v>
+      </c>
+      <c r="V33" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>5702</t>
         </is>
       </c>
     </row>
@@ -2900,7 +3102,13 @@
       <c r="T34" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U34" t="inlineStr">
+      <c r="U34" t="n">
+        <v>3476</v>
+      </c>
+      <c r="V34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W34" t="inlineStr">
         <is>
           <t>3476</t>
         </is>
@@ -2973,9 +3181,15 @@
       <c r="T35" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="U35" t="inlineStr">
-        <is>
-          <t>5030</t>
+      <c r="U35" t="n">
+        <v>5030</v>
+      </c>
+      <c r="V35" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>5305</t>
         </is>
       </c>
     </row>
@@ -3046,9 +3260,15 @@
       <c r="T36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U36" t="inlineStr">
-        <is>
-          <t>4443</t>
+      <c r="U36" t="n">
+        <v>4443</v>
+      </c>
+      <c r="V36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>4494</t>
         </is>
       </c>
     </row>
@@ -3119,9 +3339,15 @@
       <c r="T37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>4466</t>
+      <c r="U37" t="n">
+        <v>4466</v>
+      </c>
+      <c r="V37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>4691</t>
         </is>
       </c>
     </row>
@@ -3192,9 +3418,15 @@
       <c r="T38" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>4936</t>
+      <c r="U38" t="n">
+        <v>4936</v>
+      </c>
+      <c r="V38" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>5130</t>
         </is>
       </c>
     </row>
@@ -3265,9 +3497,15 @@
       <c r="T39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>4616</t>
+      <c r="U39" t="n">
+        <v>4616</v>
+      </c>
+      <c r="V39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>4964</t>
         </is>
       </c>
     </row>
@@ -3338,9 +3576,15 @@
       <c r="T40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U40" t="inlineStr">
-        <is>
-          <t>5310</t>
+      <c r="U40" t="n">
+        <v>5310</v>
+      </c>
+      <c r="V40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>5589</t>
         </is>
       </c>
     </row>
@@ -3411,9 +3655,15 @@
       <c r="T41" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U41" t="inlineStr">
-        <is>
-          <t>5076</t>
+      <c r="U41" t="n">
+        <v>5076</v>
+      </c>
+      <c r="V41" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>5289</t>
         </is>
       </c>
     </row>
@@ -3484,9 +3734,15 @@
       <c r="T42" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="U42" t="inlineStr">
-        <is>
-          <t>5382</t>
+      <c r="U42" t="n">
+        <v>5382</v>
+      </c>
+      <c r="V42" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>5692</t>
         </is>
       </c>
     </row>
@@ -3557,9 +3813,15 @@
       <c r="T43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>4851</t>
+      <c r="U43" t="n">
+        <v>4851</v>
+      </c>
+      <c r="V43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>5006</t>
         </is>
       </c>
     </row>
@@ -3630,9 +3892,15 @@
       <c r="T44" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="U44" t="inlineStr">
-        <is>
-          <t>3910</t>
+      <c r="U44" t="n">
+        <v>3910</v>
+      </c>
+      <c r="V44" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="W44" t="inlineStr">
+        <is>
+          <t>3978</t>
         </is>
       </c>
     </row>
@@ -3703,9 +3971,15 @@
       <c r="T45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U45" t="inlineStr">
-        <is>
-          <t>4506</t>
+      <c r="U45" t="n">
+        <v>4506</v>
+      </c>
+      <c r="V45" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>4828</t>
         </is>
       </c>
     </row>
@@ -3776,9 +4050,15 @@
       <c r="T46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U46" t="inlineStr">
-        <is>
-          <t>4331</t>
+      <c r="U46" t="n">
+        <v>4331</v>
+      </c>
+      <c r="V46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>4523</t>
         </is>
       </c>
     </row>
@@ -3849,9 +4129,15 @@
       <c r="T47" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U47" t="inlineStr">
-        <is>
-          <t>4561</t>
+      <c r="U47" t="n">
+        <v>4561</v>
+      </c>
+      <c r="V47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>4687</t>
         </is>
       </c>
     </row>
@@ -3922,9 +4208,15 @@
       <c r="T48" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="U48" t="inlineStr">
-        <is>
-          <t>4742</t>
+      <c r="U48" t="n">
+        <v>4742</v>
+      </c>
+      <c r="V48" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="W48" t="inlineStr">
+        <is>
+          <t>5115</t>
         </is>
       </c>
     </row>
@@ -3995,9 +4287,15 @@
       <c r="T49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U49" t="inlineStr">
-        <is>
-          <t>3604</t>
+      <c r="U49" t="n">
+        <v>3604</v>
+      </c>
+      <c r="V49" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="W49" t="inlineStr">
+        <is>
+          <t>3637</t>
         </is>
       </c>
     </row>
@@ -4020,7 +4318,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F50" s="4" t="n">
@@ -4068,9 +4366,15 @@
       <c r="T50" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U50" t="inlineStr">
-        <is>
-          <t>4470</t>
+      <c r="U50" t="n">
+        <v>4470</v>
+      </c>
+      <c r="V50" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W50" t="inlineStr">
+        <is>
+          <t>4904</t>
         </is>
       </c>
     </row>
@@ -4141,9 +4445,15 @@
       <c r="T51" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="U51" t="inlineStr">
-        <is>
-          <t>4809</t>
+      <c r="U51" t="n">
+        <v>4809</v>
+      </c>
+      <c r="V51" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W51" t="inlineStr">
+        <is>
+          <t>5027</t>
         </is>
       </c>
     </row>
@@ -4214,9 +4524,15 @@
       <c r="T52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U52" t="inlineStr">
-        <is>
-          <t>2584</t>
+      <c r="U52" t="n">
+        <v>2584</v>
+      </c>
+      <c r="V52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W52" t="inlineStr">
+        <is>
+          <t>2610</t>
         </is>
       </c>
     </row>
@@ -4287,9 +4603,15 @@
       <c r="T53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U53" t="inlineStr">
-        <is>
-          <t>3091</t>
+      <c r="U53" t="n">
+        <v>3091</v>
+      </c>
+      <c r="V53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W53" t="inlineStr">
+        <is>
+          <t>3147</t>
         </is>
       </c>
     </row>
@@ -4360,9 +4682,15 @@
       <c r="T54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U54" t="inlineStr">
-        <is>
-          <t>2990</t>
+      <c r="U54" t="n">
+        <v>2990</v>
+      </c>
+      <c r="V54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W54" t="inlineStr">
+        <is>
+          <t>3050</t>
         </is>
       </c>
     </row>
@@ -4433,9 +4761,15 @@
       <c r="T55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U55" t="inlineStr">
-        <is>
-          <t>3752</t>
+      <c r="U55" t="n">
+        <v>3752</v>
+      </c>
+      <c r="V55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W55" t="inlineStr">
+        <is>
+          <t>3919</t>
         </is>
       </c>
     </row>
@@ -4506,9 +4840,15 @@
       <c r="T56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U56" t="inlineStr">
-        <is>
-          <t>3978</t>
+      <c r="U56" t="n">
+        <v>3978</v>
+      </c>
+      <c r="V56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W56" t="inlineStr">
+        <is>
+          <t>4191</t>
         </is>
       </c>
     </row>
@@ -4579,9 +4919,15 @@
       <c r="T57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U57" t="inlineStr">
-        <is>
-          <t>4512</t>
+      <c r="U57" t="n">
+        <v>4512</v>
+      </c>
+      <c r="V57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W57" t="inlineStr">
+        <is>
+          <t>4642</t>
         </is>
       </c>
     </row>
@@ -4652,9 +4998,15 @@
       <c r="T58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U58" t="inlineStr">
-        <is>
-          <t>3843</t>
+      <c r="U58" t="n">
+        <v>3843</v>
+      </c>
+      <c r="V58" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="W58" t="inlineStr">
+        <is>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -4725,9 +5077,15 @@
       <c r="T59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U59" t="inlineStr">
-        <is>
-          <t>4371</t>
+      <c r="U59" t="n">
+        <v>4371</v>
+      </c>
+      <c r="V59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W59" t="inlineStr">
+        <is>
+          <t>4551</t>
         </is>
       </c>
     </row>
@@ -4798,9 +5156,15 @@
       <c r="T60" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="U60" t="inlineStr">
-        <is>
-          <t>4673</t>
+      <c r="U60" t="n">
+        <v>4673</v>
+      </c>
+      <c r="V60" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="W60" t="inlineStr">
+        <is>
+          <t>4864</t>
         </is>
       </c>
     </row>
@@ -4871,9 +5235,15 @@
       <c r="T61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U61" t="inlineStr">
-        <is>
-          <t>4406</t>
+      <c r="U61" t="n">
+        <v>4406</v>
+      </c>
+      <c r="V61" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W61" t="inlineStr">
+        <is>
+          <t>4602</t>
         </is>
       </c>
     </row>
@@ -4944,9 +5314,15 @@
       <c r="T62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U62" t="inlineStr">
-        <is>
-          <t>4430</t>
+      <c r="U62" t="n">
+        <v>4430</v>
+      </c>
+      <c r="V62" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="W62" t="inlineStr">
+        <is>
+          <t>4751</t>
         </is>
       </c>
     </row>
@@ -5017,9 +5393,15 @@
       <c r="T63" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="U63" t="inlineStr">
-        <is>
-          <t>3937</t>
+      <c r="U63" t="n">
+        <v>3937</v>
+      </c>
+      <c r="V63" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="W63" t="inlineStr">
+        <is>
+          <t>4050</t>
         </is>
       </c>
     </row>
@@ -5090,9 +5472,15 @@
       <c r="T64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U64" t="inlineStr">
-        <is>
-          <t>2575</t>
+      <c r="U64" t="n">
+        <v>2575</v>
+      </c>
+      <c r="V64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W64" t="inlineStr">
+        <is>
+          <t>2606</t>
         </is>
       </c>
     </row>
@@ -5163,9 +5551,15 @@
       <c r="T65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U65" t="inlineStr">
-        <is>
-          <t>3628</t>
+      <c r="U65" t="n">
+        <v>3628</v>
+      </c>
+      <c r="V65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W65" t="inlineStr">
+        <is>
+          <t>3761</t>
         </is>
       </c>
     </row>
@@ -5236,9 +5630,15 @@
       <c r="T66" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="U66" t="inlineStr">
-        <is>
-          <t>3753</t>
+      <c r="U66" t="n">
+        <v>3753</v>
+      </c>
+      <c r="V66" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="W66" t="inlineStr">
+        <is>
+          <t>3862</t>
         </is>
       </c>
     </row>
@@ -5309,9 +5709,15 @@
       <c r="T67" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U67" t="inlineStr">
-        <is>
-          <t>4613</t>
+      <c r="U67" t="n">
+        <v>4613</v>
+      </c>
+      <c r="V67" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W67" t="inlineStr">
+        <is>
+          <t>4794</t>
         </is>
       </c>
     </row>
@@ -5382,9 +5788,15 @@
       <c r="T68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U68" t="inlineStr">
-        <is>
-          <t>3851</t>
+      <c r="U68" t="n">
+        <v>3851</v>
+      </c>
+      <c r="V68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W68" t="inlineStr">
+        <is>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -5455,9 +5867,15 @@
       <c r="T69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U69" t="inlineStr">
-        <is>
-          <t>2712</t>
+      <c r="U69" t="n">
+        <v>2712</v>
+      </c>
+      <c r="V69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W69" t="inlineStr">
+        <is>
+          <t>2711</t>
         </is>
       </c>
     </row>
@@ -5528,9 +5946,15 @@
       <c r="T70" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="U70" t="inlineStr">
-        <is>
-          <t>3480</t>
+      <c r="U70" t="n">
+        <v>3480</v>
+      </c>
+      <c r="V70" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="W70" t="inlineStr">
+        <is>
+          <t>3561</t>
         </is>
       </c>
     </row>
@@ -5601,9 +6025,15 @@
       <c r="T71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U71" t="inlineStr">
-        <is>
-          <t>4740</t>
+      <c r="U71" t="n">
+        <v>4740</v>
+      </c>
+      <c r="V71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W71" t="inlineStr">
+        <is>
+          <t>4930</t>
         </is>
       </c>
     </row>
@@ -5674,9 +6104,15 @@
       <c r="T72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U72" t="inlineStr">
-        <is>
-          <t>3522</t>
+      <c r="U72" t="n">
+        <v>3522</v>
+      </c>
+      <c r="V72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W72" t="inlineStr">
+        <is>
+          <t>3573</t>
         </is>
       </c>
     </row>
@@ -5747,9 +6183,15 @@
       <c r="T73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U73" t="inlineStr">
-        <is>
-          <t>4487</t>
+      <c r="U73" t="n">
+        <v>4487</v>
+      </c>
+      <c r="V73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W73" t="inlineStr">
+        <is>
+          <t>4719</t>
         </is>
       </c>
     </row>
@@ -5820,9 +6262,15 @@
       <c r="T74" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U74" t="inlineStr">
-        <is>
-          <t>4118</t>
+      <c r="U74" t="n">
+        <v>4118</v>
+      </c>
+      <c r="V74" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W74" t="inlineStr">
+        <is>
+          <t>4376</t>
         </is>
       </c>
     </row>
@@ -5893,9 +6341,15 @@
       <c r="T75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U75" t="inlineStr">
-        <is>
-          <t>4287</t>
+      <c r="U75" t="n">
+        <v>4287</v>
+      </c>
+      <c r="V75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W75" t="inlineStr">
+        <is>
+          <t>4527</t>
         </is>
       </c>
     </row>
@@ -5966,9 +6420,15 @@
       <c r="T76" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U76" t="inlineStr">
-        <is>
-          <t>4251</t>
+      <c r="U76" t="n">
+        <v>4251</v>
+      </c>
+      <c r="V76" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W76" t="inlineStr">
+        <is>
+          <t>4385</t>
         </is>
       </c>
     </row>
@@ -6038,6 +6498,8 @@
       </c>
       <c r="T77" s="3" t="inlineStr"/>
       <c r="U77" t="inlineStr"/>
+      <c r="V77" s="3" t="inlineStr"/>
+      <c r="W77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -6106,9 +6568,15 @@
       <c r="T78" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U78" t="inlineStr">
-        <is>
-          <t>4027</t>
+      <c r="U78" t="n">
+        <v>4027</v>
+      </c>
+      <c r="V78" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W78" t="inlineStr">
+        <is>
+          <t>4028</t>
         </is>
       </c>
     </row>
@@ -6179,9 +6647,15 @@
       <c r="T79" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U79" t="inlineStr">
-        <is>
-          <t>3875</t>
+      <c r="U79" t="n">
+        <v>3875</v>
+      </c>
+      <c r="V79" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W79" t="inlineStr">
+        <is>
+          <t>4070</t>
         </is>
       </c>
     </row>
@@ -6252,9 +6726,15 @@
       <c r="T80" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U80" t="inlineStr">
-        <is>
-          <t>3352</t>
+      <c r="U80" t="n">
+        <v>3352</v>
+      </c>
+      <c r="V80" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W80" t="inlineStr">
+        <is>
+          <t>3565</t>
         </is>
       </c>
     </row>
@@ -6325,9 +6805,15 @@
       <c r="T81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U81" t="inlineStr">
-        <is>
-          <t>2807</t>
+      <c r="U81" t="n">
+        <v>2807</v>
+      </c>
+      <c r="V81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W81" t="inlineStr">
+        <is>
+          <t>2931</t>
         </is>
       </c>
     </row>
@@ -6398,9 +6884,15 @@
       <c r="T82" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U82" t="inlineStr">
-        <is>
-          <t>4300</t>
+      <c r="U82" t="n">
+        <v>4300</v>
+      </c>
+      <c r="V82" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="W82" t="inlineStr">
+        <is>
+          <t>4297</t>
         </is>
       </c>
     </row>
@@ -6471,9 +6963,15 @@
       <c r="T83" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="U83" t="inlineStr">
-        <is>
-          <t>2758</t>
+      <c r="U83" t="n">
+        <v>2758</v>
+      </c>
+      <c r="V83" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W83" t="inlineStr">
+        <is>
+          <t>2823</t>
         </is>
       </c>
     </row>
@@ -6544,9 +7042,15 @@
       <c r="T84" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="U84" t="inlineStr">
-        <is>
-          <t>3022</t>
+      <c r="U84" t="n">
+        <v>3022</v>
+      </c>
+      <c r="V84" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W84" t="inlineStr">
+        <is>
+          <t>3141</t>
         </is>
       </c>
     </row>
@@ -6617,9 +7121,15 @@
       <c r="T85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U85" t="inlineStr">
-        <is>
-          <t>2089</t>
+      <c r="U85" t="n">
+        <v>2089</v>
+      </c>
+      <c r="V85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W85" t="inlineStr">
+        <is>
+          <t>2084</t>
         </is>
       </c>
     </row>
@@ -6690,9 +7200,15 @@
       <c r="T86" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U86" t="inlineStr">
-        <is>
-          <t>2707</t>
+      <c r="U86" t="n">
+        <v>2707</v>
+      </c>
+      <c r="V86" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W86" t="inlineStr">
+        <is>
+          <t>2704</t>
         </is>
       </c>
     </row>
@@ -6763,9 +7279,15 @@
       <c r="T87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U87" t="inlineStr">
-        <is>
-          <t>3015</t>
+      <c r="U87" t="n">
+        <v>3015</v>
+      </c>
+      <c r="V87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W87" t="inlineStr">
+        <is>
+          <t>3061</t>
         </is>
       </c>
     </row>
@@ -6836,9 +7358,15 @@
       <c r="T88" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="U88" t="inlineStr">
-        <is>
-          <t>2413</t>
+      <c r="U88" t="n">
+        <v>2413</v>
+      </c>
+      <c r="V88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W88" t="inlineStr">
+        <is>
+          <t>2408</t>
         </is>
       </c>
     </row>
@@ -6896,6 +7424,8 @@
       <c r="S89" t="inlineStr"/>
       <c r="T89" s="3" t="inlineStr"/>
       <c r="U89" t="inlineStr"/>
+      <c r="V89" s="3" t="inlineStr"/>
+      <c r="W89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -6951,6 +7481,8 @@
       <c r="S90" t="inlineStr"/>
       <c r="T90" s="3" t="inlineStr"/>
       <c r="U90" t="inlineStr"/>
+      <c r="V90" s="3" t="inlineStr"/>
+      <c r="W90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -7019,9 +7551,15 @@
       <c r="T91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U91" t="inlineStr">
-        <is>
-          <t>2532</t>
+      <c r="U91" t="n">
+        <v>2532</v>
+      </c>
+      <c r="V91" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="W91" t="inlineStr">
+        <is>
+          <t>2706</t>
         </is>
       </c>
     </row>
@@ -7092,9 +7630,15 @@
       <c r="T92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U92" t="inlineStr">
-        <is>
-          <t>3267</t>
+      <c r="U92" t="n">
+        <v>3267</v>
+      </c>
+      <c r="V92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W92" t="inlineStr">
+        <is>
+          <t>3279</t>
         </is>
       </c>
     </row>
@@ -7165,9 +7709,15 @@
       <c r="T93" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="U93" t="inlineStr">
-        <is>
-          <t>2907</t>
+      <c r="U93" t="n">
+        <v>2907</v>
+      </c>
+      <c r="V93" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="W93" t="inlineStr">
+        <is>
+          <t>2928</t>
         </is>
       </c>
     </row>
@@ -7238,9 +7788,15 @@
       <c r="T94" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U94" t="inlineStr">
-        <is>
-          <t>3938</t>
+      <c r="U94" t="n">
+        <v>3938</v>
+      </c>
+      <c r="V94" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W94" t="inlineStr">
+        <is>
+          <t>4088</t>
         </is>
       </c>
     </row>
@@ -7311,9 +7867,15 @@
       <c r="T95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U95" t="inlineStr">
-        <is>
-          <t>3750</t>
+      <c r="U95" t="n">
+        <v>3750</v>
+      </c>
+      <c r="V95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W95" t="inlineStr">
+        <is>
+          <t>3885</t>
         </is>
       </c>
     </row>
@@ -7384,9 +7946,15 @@
       <c r="T96" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="U96" t="inlineStr">
-        <is>
-          <t>3535</t>
+      <c r="U96" t="n">
+        <v>3535</v>
+      </c>
+      <c r="V96" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="W96" t="inlineStr">
+        <is>
+          <t>3679</t>
         </is>
       </c>
     </row>
@@ -7457,9 +8025,15 @@
       <c r="T97" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="U97" t="inlineStr">
-        <is>
-          <t>4037</t>
+      <c r="U97" t="n">
+        <v>4037</v>
+      </c>
+      <c r="V97" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="W97" t="inlineStr">
+        <is>
+          <t>4169</t>
         </is>
       </c>
     </row>
@@ -7530,9 +8104,15 @@
       <c r="T98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U98" t="inlineStr">
-        <is>
-          <t>3325</t>
+      <c r="U98" t="n">
+        <v>3325</v>
+      </c>
+      <c r="V98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W98" t="inlineStr">
+        <is>
+          <t>3400</t>
         </is>
       </c>
     </row>
@@ -7603,9 +8183,15 @@
       <c r="T99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U99" t="inlineStr">
-        <is>
-          <t>2605</t>
+      <c r="U99" t="n">
+        <v>2605</v>
+      </c>
+      <c r="V99" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W99" t="inlineStr">
+        <is>
+          <t>2868</t>
         </is>
       </c>
     </row>
@@ -7676,9 +8262,15 @@
       <c r="T100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U100" t="inlineStr">
-        <is>
-          <t>2604</t>
+      <c r="U100" t="n">
+        <v>2604</v>
+      </c>
+      <c r="V100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W100" t="inlineStr">
+        <is>
+          <t>2639</t>
         </is>
       </c>
     </row>
@@ -7749,9 +8341,15 @@
       <c r="T101" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="U101" t="inlineStr">
-        <is>
-          <t>4128</t>
+      <c r="U101" t="n">
+        <v>4128</v>
+      </c>
+      <c r="V101" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W101" t="inlineStr">
+        <is>
+          <t>4294</t>
         </is>
       </c>
     </row>
@@ -7822,9 +8420,15 @@
       <c r="T102" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="U102" t="inlineStr">
-        <is>
-          <t>3554</t>
+      <c r="U102" t="n">
+        <v>3554</v>
+      </c>
+      <c r="V102" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="W102" t="inlineStr">
+        <is>
+          <t>3690</t>
         </is>
       </c>
     </row>
@@ -7895,9 +8499,15 @@
       <c r="T103" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="U103" t="inlineStr">
-        <is>
-          <t>3354</t>
+      <c r="U103" t="n">
+        <v>3354</v>
+      </c>
+      <c r="V103" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W103" t="inlineStr">
+        <is>
+          <t>3389</t>
         </is>
       </c>
     </row>
@@ -7968,9 +8578,15 @@
       <c r="T104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U104" t="inlineStr">
-        <is>
-          <t>2561</t>
+      <c r="U104" t="n">
+        <v>2561</v>
+      </c>
+      <c r="V104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W104" t="inlineStr">
+        <is>
+          <t>2560</t>
         </is>
       </c>
     </row>
@@ -8041,9 +8657,15 @@
       <c r="T105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U105" t="inlineStr">
-        <is>
-          <t>3238</t>
+      <c r="U105" t="n">
+        <v>3238</v>
+      </c>
+      <c r="V105" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W105" t="inlineStr">
+        <is>
+          <t>3454</t>
         </is>
       </c>
     </row>
@@ -8114,9 +8736,15 @@
       <c r="T106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U106" t="inlineStr">
-        <is>
-          <t>2906</t>
+      <c r="U106" t="n">
+        <v>2906</v>
+      </c>
+      <c r="V106" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W106" t="inlineStr">
+        <is>
+          <t>3053</t>
         </is>
       </c>
     </row>
@@ -8187,9 +8815,15 @@
       <c r="T107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U107" t="inlineStr">
-        <is>
-          <t>3431</t>
+      <c r="U107" t="n">
+        <v>3431</v>
+      </c>
+      <c r="V107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W107" t="inlineStr">
+        <is>
+          <t>3545</t>
         </is>
       </c>
     </row>
@@ -8260,9 +8894,15 @@
       <c r="T108" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="U108" t="inlineStr">
-        <is>
-          <t>2647</t>
+      <c r="U108" t="n">
+        <v>2647</v>
+      </c>
+      <c r="V108" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="W108" t="inlineStr">
+        <is>
+          <t>2667</t>
         </is>
       </c>
     </row>
@@ -8333,9 +8973,15 @@
       <c r="T109" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="U109" t="inlineStr">
-        <is>
-          <t>2709</t>
+      <c r="U109" t="n">
+        <v>2709</v>
+      </c>
+      <c r="V109" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="W109" t="inlineStr">
+        <is>
+          <t>2742</t>
         </is>
       </c>
     </row>
@@ -8406,9 +9052,15 @@
       <c r="T110" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="U110" t="inlineStr">
-        <is>
-          <t>3200</t>
+      <c r="U110" t="n">
+        <v>3200</v>
+      </c>
+      <c r="V110" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="W110" t="inlineStr">
+        <is>
+          <t>3345</t>
         </is>
       </c>
     </row>
@@ -8479,9 +9131,15 @@
       <c r="T111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U111" t="inlineStr">
-        <is>
-          <t>2836</t>
+      <c r="U111" t="n">
+        <v>2836</v>
+      </c>
+      <c r="V111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W111" t="inlineStr">
+        <is>
+          <t>2864</t>
         </is>
       </c>
     </row>
@@ -8552,9 +9210,15 @@
       <c r="T112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U112" t="inlineStr">
-        <is>
-          <t>3312</t>
+      <c r="U112" t="n">
+        <v>3312</v>
+      </c>
+      <c r="V112" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="W112" t="inlineStr">
+        <is>
+          <t>3370</t>
         </is>
       </c>
     </row>
@@ -8625,9 +9289,15 @@
       <c r="T113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U113" t="inlineStr">
-        <is>
-          <t>2525</t>
+      <c r="U113" t="n">
+        <v>2525</v>
+      </c>
+      <c r="V113" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="W113" t="inlineStr">
+        <is>
+          <t>2524</t>
         </is>
       </c>
     </row>
@@ -8698,9 +9368,15 @@
       <c r="T114" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U114" t="inlineStr">
-        <is>
-          <t>3465</t>
+      <c r="U114" t="n">
+        <v>3465</v>
+      </c>
+      <c r="V114" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W114" t="inlineStr">
+        <is>
+          <t>3567</t>
         </is>
       </c>
     </row>
@@ -8771,9 +9447,15 @@
       <c r="T115" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="U115" t="inlineStr">
-        <is>
-          <t>2622</t>
+      <c r="U115" t="n">
+        <v>2622</v>
+      </c>
+      <c r="V115" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W115" t="inlineStr">
+        <is>
+          <t>2645</t>
         </is>
       </c>
     </row>
@@ -8844,9 +9526,15 @@
       <c r="T116" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U116" t="inlineStr">
-        <is>
-          <t>3009</t>
+      <c r="U116" t="n">
+        <v>3009</v>
+      </c>
+      <c r="V116" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="W116" t="inlineStr">
+        <is>
+          <t>3105</t>
         </is>
       </c>
     </row>
@@ -8917,9 +9605,15 @@
       <c r="T117" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U117" t="inlineStr">
-        <is>
-          <t>3121</t>
+      <c r="U117" t="n">
+        <v>3121</v>
+      </c>
+      <c r="V117" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W117" t="inlineStr">
+        <is>
+          <t>3215</t>
         </is>
       </c>
     </row>
@@ -8989,6 +9683,8 @@
       </c>
       <c r="T118" s="3" t="inlineStr"/>
       <c r="U118" t="inlineStr"/>
+      <c r="V118" s="3" t="inlineStr"/>
+      <c r="W118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -9057,9 +9753,15 @@
       <c r="T119" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U119" t="inlineStr">
-        <is>
-          <t>3327</t>
+      <c r="U119" t="n">
+        <v>3327</v>
+      </c>
+      <c r="V119" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W119" t="inlineStr">
+        <is>
+          <t>3432</t>
         </is>
       </c>
     </row>
@@ -9130,9 +9832,15 @@
       <c r="T120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U120" t="inlineStr">
-        <is>
-          <t>3088</t>
+      <c r="U120" t="n">
+        <v>3088</v>
+      </c>
+      <c r="V120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W120" t="inlineStr">
+        <is>
+          <t>3193</t>
         </is>
       </c>
     </row>
@@ -9203,9 +9911,15 @@
       <c r="T121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U121" t="inlineStr">
-        <is>
-          <t>2183</t>
+      <c r="U121" t="n">
+        <v>2183</v>
+      </c>
+      <c r="V121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W121" t="inlineStr">
+        <is>
+          <t>2173</t>
         </is>
       </c>
     </row>
@@ -9276,9 +9990,15 @@
       <c r="T122" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="U122" t="inlineStr">
-        <is>
-          <t>2566</t>
+      <c r="U122" t="n">
+        <v>2566</v>
+      </c>
+      <c r="V122" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="W122" t="inlineStr">
+        <is>
+          <t>2560</t>
         </is>
       </c>
     </row>
@@ -9349,9 +10069,15 @@
       <c r="T123" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="U123" t="inlineStr">
-        <is>
-          <t>2667</t>
+      <c r="U123" t="n">
+        <v>2667</v>
+      </c>
+      <c r="V123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W123" t="inlineStr">
+        <is>
+          <t>2675</t>
         </is>
       </c>
     </row>
@@ -9422,9 +10148,15 @@
       <c r="T124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U124" t="inlineStr">
-        <is>
-          <t>3336</t>
+      <c r="U124" t="n">
+        <v>3336</v>
+      </c>
+      <c r="V124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W124" t="inlineStr">
+        <is>
+          <t>3498</t>
         </is>
       </c>
     </row>
@@ -9495,7 +10227,13 @@
       <c r="T125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U125" t="inlineStr">
+      <c r="U125" t="n">
+        <v>0</v>
+      </c>
+      <c r="V125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9568,9 +10306,15 @@
       <c r="T126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U126" t="inlineStr">
-        <is>
-          <t>2918</t>
+      <c r="U126" t="n">
+        <v>2918</v>
+      </c>
+      <c r="V126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W126" t="inlineStr">
+        <is>
+          <t>2892</t>
         </is>
       </c>
     </row>
@@ -9641,9 +10385,15 @@
       <c r="T127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U127" t="inlineStr">
-        <is>
-          <t>2606</t>
+      <c r="U127" t="n">
+        <v>2606</v>
+      </c>
+      <c r="V127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W127" t="inlineStr">
+        <is>
+          <t>2566</t>
         </is>
       </c>
     </row>
@@ -9714,9 +10464,15 @@
       <c r="T128" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="U128" t="inlineStr">
-        <is>
-          <t>2638</t>
+      <c r="U128" t="n">
+        <v>2638</v>
+      </c>
+      <c r="V128" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W128" t="inlineStr">
+        <is>
+          <t>2736</t>
         </is>
       </c>
     </row>
@@ -9787,9 +10543,15 @@
       <c r="T129" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="U129" t="inlineStr">
-        <is>
-          <t>2504</t>
+      <c r="U129" t="n">
+        <v>2504</v>
+      </c>
+      <c r="V129" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="W129" t="inlineStr">
+        <is>
+          <t>2574</t>
         </is>
       </c>
     </row>
@@ -9860,9 +10622,15 @@
       <c r="T130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U130" t="inlineStr">
-        <is>
-          <t>1915</t>
+      <c r="U130" t="n">
+        <v>1915</v>
+      </c>
+      <c r="V130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W130" t="inlineStr">
+        <is>
+          <t>1914</t>
         </is>
       </c>
     </row>
@@ -9933,7 +10701,13 @@
       <c r="T131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U131" t="inlineStr">
+      <c r="U131" t="n">
+        <v>0</v>
+      </c>
+      <c r="V131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10006,9 +10780,15 @@
       <c r="T132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U132" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="U132" t="n">
+        <v>0</v>
+      </c>
+      <c r="V132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W132" t="inlineStr">
+        <is>
+          <t>1509</t>
         </is>
       </c>
     </row>
@@ -10078,6 +10858,8 @@
       </c>
       <c r="T133" s="3" t="inlineStr"/>
       <c r="U133" t="inlineStr"/>
+      <c r="V133" s="3" t="inlineStr"/>
+      <c r="W133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -10146,9 +10928,15 @@
       <c r="T134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U134" t="inlineStr">
-        <is>
-          <t>1988</t>
+      <c r="U134" t="n">
+        <v>1988</v>
+      </c>
+      <c r="V134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W134" t="inlineStr">
+        <is>
+          <t>2035</t>
         </is>
       </c>
     </row>
@@ -10219,9 +11007,15 @@
       <c r="T135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U135" t="inlineStr">
-        <is>
-          <t>2237</t>
+      <c r="U135" t="n">
+        <v>2237</v>
+      </c>
+      <c r="V135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W135" t="inlineStr">
+        <is>
+          <t>2218</t>
         </is>
       </c>
     </row>
@@ -10292,9 +11086,15 @@
       <c r="T136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U136" t="inlineStr">
-        <is>
-          <t>1520</t>
+      <c r="U136" t="n">
+        <v>1520</v>
+      </c>
+      <c r="V136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W136" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -10364,6 +11164,8 @@
       </c>
       <c r="T137" s="3" t="inlineStr"/>
       <c r="U137" t="inlineStr"/>
+      <c r="V137" s="3" t="inlineStr"/>
+      <c r="W137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -10432,7 +11234,13 @@
       <c r="T138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U138" t="inlineStr">
+      <c r="U138" t="n">
+        <v>0</v>
+      </c>
+      <c r="V138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10504,6 +11312,8 @@
       </c>
       <c r="T139" s="3" t="inlineStr"/>
       <c r="U139" t="inlineStr"/>
+      <c r="V139" s="3" t="inlineStr"/>
+      <c r="W139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -10572,9 +11382,15 @@
       <c r="T140" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="U140" t="inlineStr">
-        <is>
-          <t>4322</t>
+      <c r="U140" t="n">
+        <v>4322</v>
+      </c>
+      <c r="V140" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="W140" t="inlineStr">
+        <is>
+          <t>4402</t>
         </is>
       </c>
     </row>
@@ -10645,7 +11461,13 @@
       <c r="T141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U141" t="inlineStr">
+      <c r="U141" t="n">
+        <v>0</v>
+      </c>
+      <c r="V141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10718,7 +11540,13 @@
       <c r="T142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U142" t="inlineStr">
+      <c r="U142" t="n">
+        <v>0</v>
+      </c>
+      <c r="V142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10791,9 +11619,15 @@
       <c r="T143" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="U143" t="inlineStr">
-        <is>
-          <t>4650</t>
+      <c r="U143" t="n">
+        <v>4650</v>
+      </c>
+      <c r="V143" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="W143" t="inlineStr">
+        <is>
+          <t>4934</t>
         </is>
       </c>
     </row>
@@ -10864,7 +11698,13 @@
       <c r="T144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U144" t="inlineStr">
+      <c r="U144" t="n">
+        <v>0</v>
+      </c>
+      <c r="V144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10937,9 +11777,15 @@
       <c r="T145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U145" t="inlineStr">
-        <is>
-          <t>2751</t>
+      <c r="U145" t="n">
+        <v>2751</v>
+      </c>
+      <c r="V145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W145" t="inlineStr">
+        <is>
+          <t>2736</t>
         </is>
       </c>
     </row>
@@ -11010,7 +11856,13 @@
       <c r="T146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U146" t="inlineStr">
+      <c r="U146" t="n">
+        <v>0</v>
+      </c>
+      <c r="V146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11083,9 +11935,15 @@
       <c r="T147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U147" t="inlineStr">
-        <is>
-          <t>2659</t>
+      <c r="U147" t="n">
+        <v>2659</v>
+      </c>
+      <c r="V147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W147" t="inlineStr">
+        <is>
+          <t>2764</t>
         </is>
       </c>
     </row>
@@ -11134,9 +11992,15 @@
       <c r="T148" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="U148" t="inlineStr">
-        <is>
-          <t>2943</t>
+      <c r="U148" t="n">
+        <v>2943</v>
+      </c>
+      <c r="V148" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W148" t="inlineStr">
+        <is>
+          <t>2997</t>
         </is>
       </c>
     </row>
@@ -11201,7 +12065,13 @@
       <c r="T149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U149" t="inlineStr">
+      <c r="U149" t="n">
+        <v>0</v>
+      </c>
+      <c r="V149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11268,7 +12138,13 @@
       <c r="T150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U150" t="inlineStr">
+      <c r="U150" t="n">
+        <v>0</v>
+      </c>
+      <c r="V150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11323,9 +12199,15 @@
       <c r="T151" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="U151" t="inlineStr">
-        <is>
-          <t>2262</t>
+      <c r="U151" t="n">
+        <v>2262</v>
+      </c>
+      <c r="V151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W151" t="inlineStr">
+        <is>
+          <t>2249</t>
         </is>
       </c>
     </row>
@@ -11378,7 +12260,13 @@
       <c r="T152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U152" t="inlineStr">
+      <c r="U152" t="n">
+        <v>0</v>
+      </c>
+      <c r="V152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11425,9 +12313,15 @@
       <c r="T153" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U153" t="inlineStr">
-        <is>
-          <t>3795</t>
+      <c r="U153" t="n">
+        <v>3795</v>
+      </c>
+      <c r="V153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W153" t="inlineStr">
+        <is>
+          <t>3750</t>
         </is>
       </c>
     </row>
@@ -11472,9 +12366,15 @@
       <c r="T154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U154" t="inlineStr">
-        <is>
-          <t>1700</t>
+      <c r="U154" t="n">
+        <v>1700</v>
+      </c>
+      <c r="V154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W154" t="inlineStr">
+        <is>
+          <t>1665</t>
         </is>
       </c>
     </row>
@@ -11515,17 +12415,21 @@
       <c r="T155" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="U155" t="inlineStr">
-        <is>
-          <t>1509</t>
+      <c r="U155" t="n">
+        <v>1509</v>
+      </c>
+      <c r="V155" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="W155" t="inlineStr">
+        <is>
+          <t>1538</t>
         </is>
       </c>
     </row>
     <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>14110169</t>
-        </is>
+      <c r="A156" t="n">
+        <v>14110169</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -11556,17 +12460,21 @@
       <c r="T156" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="U156" t="inlineStr">
-        <is>
-          <t>3065</t>
+      <c r="U156" t="n">
+        <v>3065</v>
+      </c>
+      <c r="V156" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="W156" t="inlineStr">
+        <is>
+          <t>3476</t>
         </is>
       </c>
     </row>
     <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>47928278</t>
-        </is>
+      <c r="A157" t="n">
+        <v>47928278</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
@@ -11597,17 +12505,21 @@
       <c r="T157" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="U157" t="inlineStr">
-        <is>
-          <t>5535</t>
+      <c r="U157" t="n">
+        <v>5535</v>
+      </c>
+      <c r="V157" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W157" t="inlineStr">
+        <is>
+          <t>5772</t>
         </is>
       </c>
     </row>
     <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>8031795</t>
-        </is>
+      <c r="A158" t="n">
+        <v>8031795</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
@@ -11638,9 +12550,181 @@
       <c r="T158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U158" t="inlineStr">
-        <is>
-          <t>1926</t>
+      <c r="U158" t="n">
+        <v>1926</v>
+      </c>
+      <c r="V158" s="3" t="inlineStr"/>
+      <c r="W158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>7857221</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Rename</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr"/>
+      <c r="D159" t="inlineStr"/>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F159" s="3" t="inlineStr"/>
+      <c r="G159" t="inlineStr"/>
+      <c r="H159" s="3" t="inlineStr"/>
+      <c r="I159" t="inlineStr"/>
+      <c r="J159" s="3" t="inlineStr"/>
+      <c r="K159" t="inlineStr"/>
+      <c r="L159" s="3" t="inlineStr"/>
+      <c r="M159" t="inlineStr"/>
+      <c r="N159" s="3" t="inlineStr"/>
+      <c r="O159" t="inlineStr"/>
+      <c r="P159" s="3" t="inlineStr"/>
+      <c r="Q159" t="inlineStr"/>
+      <c r="R159" s="3" t="inlineStr"/>
+      <c r="S159" t="inlineStr"/>
+      <c r="T159" s="3" t="inlineStr"/>
+      <c r="U159" t="inlineStr"/>
+      <c r="V159" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W159" t="inlineStr">
+        <is>
+          <t>4733</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>57038133</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Player-57038133</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr"/>
+      <c r="D160" t="inlineStr"/>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F160" s="3" t="inlineStr"/>
+      <c r="G160" t="inlineStr"/>
+      <c r="H160" s="3" t="inlineStr"/>
+      <c r="I160" t="inlineStr"/>
+      <c r="J160" s="3" t="inlineStr"/>
+      <c r="K160" t="inlineStr"/>
+      <c r="L160" s="3" t="inlineStr"/>
+      <c r="M160" t="inlineStr"/>
+      <c r="N160" s="3" t="inlineStr"/>
+      <c r="O160" t="inlineStr"/>
+      <c r="P160" s="3" t="inlineStr"/>
+      <c r="Q160" t="inlineStr"/>
+      <c r="R160" s="3" t="inlineStr"/>
+      <c r="S160" t="inlineStr"/>
+      <c r="T160" s="3" t="inlineStr"/>
+      <c r="U160" t="inlineStr"/>
+      <c r="V160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W160" t="inlineStr">
+        <is>
+          <t>2628</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>58463042</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>DiamondSloth80</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr"/>
+      <c r="D161" t="inlineStr"/>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F161" s="3" t="inlineStr"/>
+      <c r="G161" t="inlineStr"/>
+      <c r="H161" s="3" t="inlineStr"/>
+      <c r="I161" t="inlineStr"/>
+      <c r="J161" s="3" t="inlineStr"/>
+      <c r="K161" t="inlineStr"/>
+      <c r="L161" s="3" t="inlineStr"/>
+      <c r="M161" t="inlineStr"/>
+      <c r="N161" s="3" t="inlineStr"/>
+      <c r="O161" t="inlineStr"/>
+      <c r="P161" s="3" t="inlineStr"/>
+      <c r="Q161" t="inlineStr"/>
+      <c r="R161" s="3" t="inlineStr"/>
+      <c r="S161" t="inlineStr"/>
+      <c r="T161" s="3" t="inlineStr"/>
+      <c r="U161" t="inlineStr"/>
+      <c r="V161" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="W161" t="inlineStr">
+        <is>
+          <t>1848</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>58526469</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>ItaloFlausino</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr"/>
+      <c r="D162" t="inlineStr"/>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F162" s="3" t="inlineStr"/>
+      <c r="G162" t="inlineStr"/>
+      <c r="H162" s="3" t="inlineStr"/>
+      <c r="I162" t="inlineStr"/>
+      <c r="J162" s="3" t="inlineStr"/>
+      <c r="K162" t="inlineStr"/>
+      <c r="L162" s="3" t="inlineStr"/>
+      <c r="M162" t="inlineStr"/>
+      <c r="N162" s="3" t="inlineStr"/>
+      <c r="O162" t="inlineStr"/>
+      <c r="P162" s="3" t="inlineStr"/>
+      <c r="Q162" t="inlineStr"/>
+      <c r="R162" s="3" t="inlineStr"/>
+      <c r="S162" t="inlineStr"/>
+      <c r="T162" s="3" t="inlineStr"/>
+      <c r="U162" t="inlineStr"/>
+      <c r="V162" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W162" t="inlineStr">
+        <is>
+          <t>1371</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-11 11:30:50
</commit_message>
<xml_diff>
--- a/Season_Attack/81.xlsx
+++ b/Season_Attack/81.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W162"/>
+  <dimension ref="A1:Y163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +506,16 @@
           <t>01-09_0</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>01-10_A</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>01-10_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -580,9 +590,15 @@
       <c r="V2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>4069</t>
+      <c r="W2" t="n">
+        <v>4069</v>
+      </c>
+      <c r="X2" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>4248</t>
         </is>
       </c>
     </row>
@@ -659,9 +675,15 @@
       <c r="V3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>4523</t>
+      <c r="W3" t="n">
+        <v>4523</v>
+      </c>
+      <c r="X3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>4753</t>
         </is>
       </c>
     </row>
@@ -738,9 +760,15 @@
       <c r="V4" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>5068</t>
+      <c r="W4" t="n">
+        <v>5068</v>
+      </c>
+      <c r="X4" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>5415</t>
         </is>
       </c>
     </row>
@@ -817,9 +845,15 @@
       <c r="V5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>5364</t>
+      <c r="W5" t="n">
+        <v>5364</v>
+      </c>
+      <c r="X5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>5724</t>
         </is>
       </c>
     </row>
@@ -896,9 +930,15 @@
       <c r="V6" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>5340</t>
+      <c r="W6" t="n">
+        <v>5340</v>
+      </c>
+      <c r="X6" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>5616</t>
         </is>
       </c>
     </row>
@@ -975,9 +1015,15 @@
       <c r="V7" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>5729</t>
+      <c r="W7" t="n">
+        <v>5729</v>
+      </c>
+      <c r="X7" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>5746</t>
         </is>
       </c>
     </row>
@@ -1054,9 +1100,15 @@
       <c r="V8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>4768</t>
+      <c r="W8" t="n">
+        <v>4768</v>
+      </c>
+      <c r="X8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>4930</t>
         </is>
       </c>
     </row>
@@ -1133,9 +1185,15 @@
       <c r="V9" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>4856</t>
+      <c r="W9" t="n">
+        <v>4856</v>
+      </c>
+      <c r="X9" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>5073</t>
         </is>
       </c>
     </row>
@@ -1212,9 +1270,15 @@
       <c r="V10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>4414</t>
+      <c r="W10" t="n">
+        <v>4414</v>
+      </c>
+      <c r="X10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>4529</t>
         </is>
       </c>
     </row>
@@ -1291,9 +1355,15 @@
       <c r="V11" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>5377</t>
+      <c r="W11" t="n">
+        <v>5377</v>
+      </c>
+      <c r="X11" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>5704</t>
         </is>
       </c>
     </row>
@@ -1370,9 +1440,15 @@
       <c r="V12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W12" t="inlineStr">
-        <is>
-          <t>4609</t>
+      <c r="W12" t="n">
+        <v>4609</v>
+      </c>
+      <c r="X12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>4998</t>
         </is>
       </c>
     </row>
@@ -1449,9 +1525,15 @@
       <c r="V13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>2831</t>
+      <c r="W13" t="n">
+        <v>2831</v>
+      </c>
+      <c r="X13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>2863</t>
         </is>
       </c>
     </row>
@@ -1528,9 +1610,15 @@
       <c r="V14" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>5663</t>
+      <c r="W14" t="n">
+        <v>5663</v>
+      </c>
+      <c r="X14" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>6065</t>
         </is>
       </c>
     </row>
@@ -1607,9 +1695,15 @@
       <c r="V15" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>5010</t>
+      <c r="W15" t="n">
+        <v>5010</v>
+      </c>
+      <c r="X15" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>5254</t>
         </is>
       </c>
     </row>
@@ -1686,9 +1780,15 @@
       <c r="V16" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W16" t="inlineStr">
-        <is>
-          <t>5285</t>
+      <c r="W16" t="n">
+        <v>5285</v>
+      </c>
+      <c r="X16" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>5710</t>
         </is>
       </c>
     </row>
@@ -1765,9 +1865,15 @@
       <c r="V17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W17" t="inlineStr">
-        <is>
-          <t>4869</t>
+      <c r="W17" t="n">
+        <v>4869</v>
+      </c>
+      <c r="X17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>5066</t>
         </is>
       </c>
     </row>
@@ -1844,9 +1950,15 @@
       <c r="V18" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="W18" t="inlineStr">
-        <is>
-          <t>4786</t>
+      <c r="W18" t="n">
+        <v>4786</v>
+      </c>
+      <c r="X18" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>4964</t>
         </is>
       </c>
     </row>
@@ -1923,9 +2035,15 @@
       <c r="V19" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="W19" t="inlineStr">
-        <is>
-          <t>5357</t>
+      <c r="W19" t="n">
+        <v>5357</v>
+      </c>
+      <c r="X19" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>5523</t>
         </is>
       </c>
     </row>
@@ -2002,9 +2120,15 @@
       <c r="V20" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="W20" t="inlineStr">
-        <is>
-          <t>5513</t>
+      <c r="W20" t="n">
+        <v>5513</v>
+      </c>
+      <c r="X20" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>5941</t>
         </is>
       </c>
     </row>
@@ -2081,9 +2205,15 @@
       <c r="V21" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="W21" t="inlineStr">
-        <is>
-          <t>4548</t>
+      <c r="W21" t="n">
+        <v>4548</v>
+      </c>
+      <c r="X21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>4818</t>
         </is>
       </c>
     </row>
@@ -2160,9 +2290,15 @@
       <c r="V22" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="W22" t="inlineStr">
-        <is>
-          <t>5428</t>
+      <c r="W22" t="n">
+        <v>5428</v>
+      </c>
+      <c r="X22" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>5560</t>
         </is>
       </c>
     </row>
@@ -2239,9 +2375,15 @@
       <c r="V23" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="W23" t="inlineStr">
-        <is>
-          <t>5002</t>
+      <c r="W23" t="n">
+        <v>5002</v>
+      </c>
+      <c r="X23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>5419</t>
         </is>
       </c>
     </row>
@@ -2318,9 +2460,15 @@
       <c r="V24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W24" t="inlineStr">
-        <is>
-          <t>4673</t>
+      <c r="W24" t="n">
+        <v>4673</v>
+      </c>
+      <c r="X24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>5211</t>
         </is>
       </c>
     </row>
@@ -2397,7 +2545,13 @@
       <c r="V25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W25" t="inlineStr">
+      <c r="W25" t="n">
+        <v>2500</v>
+      </c>
+      <c r="X25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y25" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2476,9 +2630,15 @@
       <c r="V26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="W26" t="inlineStr">
-        <is>
-          <t>5188</t>
+      <c r="W26" t="n">
+        <v>5188</v>
+      </c>
+      <c r="X26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>5419</t>
         </is>
       </c>
     </row>
@@ -2555,9 +2715,15 @@
       <c r="V27" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W27" t="inlineStr">
-        <is>
-          <t>5350</t>
+      <c r="W27" t="n">
+        <v>5350</v>
+      </c>
+      <c r="X27" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>5705</t>
         </is>
       </c>
     </row>
@@ -2634,9 +2800,15 @@
       <c r="V28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>4238</t>
+      <c r="W28" t="n">
+        <v>4238</v>
+      </c>
+      <c r="X28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>4267</t>
         </is>
       </c>
     </row>
@@ -2713,9 +2885,15 @@
       <c r="V29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="W29" t="inlineStr">
-        <is>
-          <t>4156</t>
+      <c r="W29" t="n">
+        <v>4156</v>
+      </c>
+      <c r="X29" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>4714</t>
         </is>
       </c>
     </row>
@@ -2792,9 +2970,15 @@
       <c r="V30" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>5535</t>
+      <c r="W30" t="n">
+        <v>5535</v>
+      </c>
+      <c r="X30" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>5768</t>
         </is>
       </c>
     </row>
@@ -2871,9 +3055,15 @@
       <c r="V31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>5084</t>
+      <c r="W31" t="n">
+        <v>5084</v>
+      </c>
+      <c r="X31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>5367</t>
         </is>
       </c>
     </row>
@@ -2950,9 +3140,15 @@
       <c r="V32" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="W32" t="inlineStr">
-        <is>
-          <t>5339</t>
+      <c r="W32" t="n">
+        <v>5339</v>
+      </c>
+      <c r="X32" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>5737</t>
         </is>
       </c>
     </row>
@@ -3029,9 +3225,15 @@
       <c r="V33" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="W33" t="inlineStr">
-        <is>
-          <t>5702</t>
+      <c r="W33" t="n">
+        <v>5702</v>
+      </c>
+      <c r="X33" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>5880</t>
         </is>
       </c>
     </row>
@@ -3108,7 +3310,13 @@
       <c r="V34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W34" t="inlineStr">
+      <c r="W34" t="n">
+        <v>3476</v>
+      </c>
+      <c r="X34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="inlineStr">
         <is>
           <t>3476</t>
         </is>
@@ -3187,9 +3395,15 @@
       <c r="V35" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="W35" t="inlineStr">
-        <is>
-          <t>5305</t>
+      <c r="W35" t="n">
+        <v>5305</v>
+      </c>
+      <c r="X35" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>5760</t>
         </is>
       </c>
     </row>
@@ -3266,9 +3480,15 @@
       <c r="V36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W36" t="inlineStr">
-        <is>
-          <t>4494</t>
+      <c r="W36" t="n">
+        <v>4494</v>
+      </c>
+      <c r="X36" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y36" t="inlineStr">
+        <is>
+          <t>4816</t>
         </is>
       </c>
     </row>
@@ -3345,9 +3565,15 @@
       <c r="V37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W37" t="inlineStr">
-        <is>
-          <t>4691</t>
+      <c r="W37" t="n">
+        <v>4691</v>
+      </c>
+      <c r="X37" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Y37" t="inlineStr">
+        <is>
+          <t>4767</t>
         </is>
       </c>
     </row>
@@ -3424,9 +3650,15 @@
       <c r="V38" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="W38" t="inlineStr">
-        <is>
-          <t>5130</t>
+      <c r="W38" t="n">
+        <v>5130</v>
+      </c>
+      <c r="X38" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y38" t="inlineStr">
+        <is>
+          <t>5307</t>
         </is>
       </c>
     </row>
@@ -3503,9 +3735,15 @@
       <c r="V39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="W39" t="inlineStr">
-        <is>
-          <t>4964</t>
+      <c r="W39" t="n">
+        <v>4964</v>
+      </c>
+      <c r="X39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>5113</t>
         </is>
       </c>
     </row>
@@ -3582,9 +3820,15 @@
       <c r="V40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W40" t="inlineStr">
-        <is>
-          <t>5589</t>
+      <c r="W40" t="n">
+        <v>5589</v>
+      </c>
+      <c r="X40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y40" t="inlineStr">
+        <is>
+          <t>5817</t>
         </is>
       </c>
     </row>
@@ -3661,9 +3905,15 @@
       <c r="V41" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W41" t="inlineStr">
-        <is>
-          <t>5289</t>
+      <c r="W41" t="n">
+        <v>5289</v>
+      </c>
+      <c r="X41" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y41" t="inlineStr">
+        <is>
+          <t>5556</t>
         </is>
       </c>
     </row>
@@ -3740,9 +3990,15 @@
       <c r="V42" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="W42" t="inlineStr">
-        <is>
-          <t>5692</t>
+      <c r="W42" t="n">
+        <v>5692</v>
+      </c>
+      <c r="X42" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t>5921</t>
         </is>
       </c>
     </row>
@@ -3819,9 +4075,15 @@
       <c r="V43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W43" t="inlineStr">
-        <is>
-          <t>5006</t>
+      <c r="W43" t="n">
+        <v>5006</v>
+      </c>
+      <c r="X43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y43" t="inlineStr">
+        <is>
+          <t>5298</t>
         </is>
       </c>
     </row>
@@ -3898,9 +4160,15 @@
       <c r="V44" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="W44" t="inlineStr">
-        <is>
-          <t>3978</t>
+      <c r="W44" t="n">
+        <v>3978</v>
+      </c>
+      <c r="X44" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y44" t="inlineStr">
+        <is>
+          <t>4428</t>
         </is>
       </c>
     </row>
@@ -3977,9 +4245,15 @@
       <c r="V45" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="W45" t="inlineStr">
-        <is>
-          <t>4828</t>
+      <c r="W45" t="n">
+        <v>4828</v>
+      </c>
+      <c r="X45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y45" t="inlineStr">
+        <is>
+          <t>4995</t>
         </is>
       </c>
     </row>
@@ -4056,9 +4330,15 @@
       <c r="V46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W46" t="inlineStr">
-        <is>
-          <t>4523</t>
+      <c r="W46" t="n">
+        <v>4523</v>
+      </c>
+      <c r="X46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>5019</t>
         </is>
       </c>
     </row>
@@ -4135,9 +4415,15 @@
       <c r="V47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W47" t="inlineStr">
-        <is>
-          <t>4687</t>
+      <c r="W47" t="n">
+        <v>4687</v>
+      </c>
+      <c r="X47" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y47" t="inlineStr">
+        <is>
+          <t>4702</t>
         </is>
       </c>
     </row>
@@ -4214,9 +4500,15 @@
       <c r="V48" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="W48" t="inlineStr">
-        <is>
-          <t>5115</t>
+      <c r="W48" t="n">
+        <v>5115</v>
+      </c>
+      <c r="X48" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="Y48" t="inlineStr">
+        <is>
+          <t>5300</t>
         </is>
       </c>
     </row>
@@ -4293,9 +4585,15 @@
       <c r="V49" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="W49" t="inlineStr">
-        <is>
-          <t>3637</t>
+      <c r="W49" t="n">
+        <v>3637</v>
+      </c>
+      <c r="X49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y49" t="inlineStr">
+        <is>
+          <t>3676</t>
         </is>
       </c>
     </row>
@@ -4372,9 +4670,15 @@
       <c r="V50" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="W50" t="inlineStr">
-        <is>
-          <t>4904</t>
+      <c r="W50" t="n">
+        <v>4904</v>
+      </c>
+      <c r="X50" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="Y50" t="inlineStr">
+        <is>
+          <t>5112</t>
         </is>
       </c>
     </row>
@@ -4451,9 +4755,15 @@
       <c r="V51" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="W51" t="inlineStr">
-        <is>
-          <t>5027</t>
+      <c r="W51" t="n">
+        <v>5027</v>
+      </c>
+      <c r="X51" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y51" t="inlineStr">
+        <is>
+          <t>5256</t>
         </is>
       </c>
     </row>
@@ -4530,9 +4840,15 @@
       <c r="V52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W52" t="inlineStr">
-        <is>
-          <t>2610</t>
+      <c r="W52" t="n">
+        <v>2610</v>
+      </c>
+      <c r="X52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y52" t="inlineStr">
+        <is>
+          <t>2647</t>
         </is>
       </c>
     </row>
@@ -4609,9 +4925,15 @@
       <c r="V53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W53" t="inlineStr">
-        <is>
-          <t>3147</t>
+      <c r="W53" t="n">
+        <v>3147</v>
+      </c>
+      <c r="X53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y53" t="inlineStr">
+        <is>
+          <t>3175</t>
         </is>
       </c>
     </row>
@@ -4688,9 +5010,15 @@
       <c r="V54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W54" t="inlineStr">
-        <is>
-          <t>3050</t>
+      <c r="W54" t="n">
+        <v>3050</v>
+      </c>
+      <c r="X54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y54" t="inlineStr">
+        <is>
+          <t>3079</t>
         </is>
       </c>
     </row>
@@ -4767,9 +5095,15 @@
       <c r="V55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="W55" t="inlineStr">
-        <is>
-          <t>3919</t>
+      <c r="W55" t="n">
+        <v>3919</v>
+      </c>
+      <c r="X55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y55" t="inlineStr">
+        <is>
+          <t>4111</t>
         </is>
       </c>
     </row>
@@ -4846,9 +5180,15 @@
       <c r="V56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W56" t="inlineStr">
-        <is>
-          <t>4191</t>
+      <c r="W56" t="n">
+        <v>4191</v>
+      </c>
+      <c r="X56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>4263</t>
         </is>
       </c>
     </row>
@@ -4925,9 +5265,15 @@
       <c r="V57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W57" t="inlineStr">
-        <is>
-          <t>4642</t>
+      <c r="W57" t="n">
+        <v>4642</v>
+      </c>
+      <c r="X57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y57" t="inlineStr">
+        <is>
+          <t>4778</t>
         </is>
       </c>
     </row>
@@ -5004,9 +5350,15 @@
       <c r="V58" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="W58" t="inlineStr">
-        <is>
-          <t>3988</t>
+      <c r="W58" t="n">
+        <v>3988</v>
+      </c>
+      <c r="X58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>4155</t>
         </is>
       </c>
     </row>
@@ -5083,9 +5435,15 @@
       <c r="V59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W59" t="inlineStr">
-        <is>
-          <t>4551</t>
+      <c r="W59" t="n">
+        <v>4551</v>
+      </c>
+      <c r="X59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y59" t="inlineStr">
+        <is>
+          <t>4689</t>
         </is>
       </c>
     </row>
@@ -5162,9 +5520,15 @@
       <c r="V60" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="W60" t="inlineStr">
-        <is>
-          <t>4864</t>
+      <c r="W60" t="n">
+        <v>4864</v>
+      </c>
+      <c r="X60" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y60" t="inlineStr">
+        <is>
+          <t>4990</t>
         </is>
       </c>
     </row>
@@ -5241,9 +5605,15 @@
       <c r="V61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W61" t="inlineStr">
-        <is>
-          <t>4602</t>
+      <c r="W61" t="n">
+        <v>4602</v>
+      </c>
+      <c r="X61" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y61" t="inlineStr">
+        <is>
+          <t>4785</t>
         </is>
       </c>
     </row>
@@ -5320,9 +5690,15 @@
       <c r="V62" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="W62" t="inlineStr">
-        <is>
-          <t>4751</t>
+      <c r="W62" t="n">
+        <v>4751</v>
+      </c>
+      <c r="X62" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="Y62" t="inlineStr">
+        <is>
+          <t>4870</t>
         </is>
       </c>
     </row>
@@ -5399,9 +5775,15 @@
       <c r="V63" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="W63" t="inlineStr">
-        <is>
-          <t>4050</t>
+      <c r="W63" t="n">
+        <v>4050</v>
+      </c>
+      <c r="X63" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y63" t="inlineStr">
+        <is>
+          <t>4166</t>
         </is>
       </c>
     </row>
@@ -5478,9 +5860,15 @@
       <c r="V64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W64" t="inlineStr">
-        <is>
-          <t>2606</t>
+      <c r="W64" t="n">
+        <v>2606</v>
+      </c>
+      <c r="X64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y64" t="inlineStr">
+        <is>
+          <t>2605</t>
         </is>
       </c>
     </row>
@@ -5557,9 +5945,15 @@
       <c r="V65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W65" t="inlineStr">
-        <is>
-          <t>3761</t>
+      <c r="W65" t="n">
+        <v>3761</v>
+      </c>
+      <c r="X65" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y65" t="inlineStr">
+        <is>
+          <t>4019</t>
         </is>
       </c>
     </row>
@@ -5636,9 +6030,15 @@
       <c r="V66" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="W66" t="inlineStr">
-        <is>
-          <t>3862</t>
+      <c r="W66" t="n">
+        <v>3862</v>
+      </c>
+      <c r="X66" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y66" t="inlineStr">
+        <is>
+          <t>3976</t>
         </is>
       </c>
     </row>
@@ -5715,9 +6115,15 @@
       <c r="V67" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="W67" t="inlineStr">
-        <is>
-          <t>4794</t>
+      <c r="W67" t="n">
+        <v>4794</v>
+      </c>
+      <c r="X67" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y67" t="inlineStr">
+        <is>
+          <t>5037</t>
         </is>
       </c>
     </row>
@@ -5794,9 +6200,15 @@
       <c r="V68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W68" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="W68" t="n">
+        <v>3996</v>
+      </c>
+      <c r="X68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y68" t="inlineStr">
+        <is>
+          <t>4153</t>
         </is>
       </c>
     </row>
@@ -5873,9 +6285,15 @@
       <c r="V69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W69" t="inlineStr">
-        <is>
-          <t>2711</t>
+      <c r="W69" t="n">
+        <v>2711</v>
+      </c>
+      <c r="X69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y69" t="inlineStr">
+        <is>
+          <t>2741</t>
         </is>
       </c>
     </row>
@@ -5952,9 +6370,15 @@
       <c r="V70" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="W70" t="inlineStr">
-        <is>
-          <t>3561</t>
+      <c r="W70" t="n">
+        <v>3561</v>
+      </c>
+      <c r="X70" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y70" t="inlineStr">
+        <is>
+          <t>3727</t>
         </is>
       </c>
     </row>
@@ -6031,9 +6455,15 @@
       <c r="V71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W71" t="inlineStr">
-        <is>
-          <t>4930</t>
+      <c r="W71" t="n">
+        <v>4930</v>
+      </c>
+      <c r="X71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y71" t="inlineStr">
+        <is>
+          <t>5126</t>
         </is>
       </c>
     </row>
@@ -6110,7 +6540,13 @@
       <c r="V72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W72" t="inlineStr">
+      <c r="W72" t="n">
+        <v>3573</v>
+      </c>
+      <c r="X72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y72" t="inlineStr">
         <is>
           <t>3573</t>
         </is>
@@ -6189,9 +6625,15 @@
       <c r="V73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W73" t="inlineStr">
-        <is>
-          <t>4719</t>
+      <c r="W73" t="n">
+        <v>4719</v>
+      </c>
+      <c r="X73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y73" t="inlineStr">
+        <is>
+          <t>4828</t>
         </is>
       </c>
     </row>
@@ -6268,9 +6710,15 @@
       <c r="V74" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W74" t="inlineStr">
-        <is>
-          <t>4376</t>
+      <c r="W74" t="n">
+        <v>4376</v>
+      </c>
+      <c r="X74" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Y74" t="inlineStr">
+        <is>
+          <t>4560</t>
         </is>
       </c>
     </row>
@@ -6347,9 +6795,15 @@
       <c r="V75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W75" t="inlineStr">
-        <is>
-          <t>4527</t>
+      <c r="W75" t="n">
+        <v>4527</v>
+      </c>
+      <c r="X75" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y75" t="inlineStr">
+        <is>
+          <t>4706</t>
         </is>
       </c>
     </row>
@@ -6426,9 +6880,15 @@
       <c r="V76" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W76" t="inlineStr">
-        <is>
-          <t>4385</t>
+      <c r="W76" t="n">
+        <v>4385</v>
+      </c>
+      <c r="X76" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y76" t="inlineStr">
+        <is>
+          <t>4497</t>
         </is>
       </c>
     </row>
@@ -6500,6 +6960,8 @@
       <c r="U77" t="inlineStr"/>
       <c r="V77" s="3" t="inlineStr"/>
       <c r="W77" t="inlineStr"/>
+      <c r="X77" s="3" t="inlineStr"/>
+      <c r="Y77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -6574,9 +7036,15 @@
       <c r="V78" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W78" t="inlineStr">
-        <is>
-          <t>4028</t>
+      <c r="W78" t="n">
+        <v>4028</v>
+      </c>
+      <c r="X78" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="Y78" t="inlineStr">
+        <is>
+          <t>4400</t>
         </is>
       </c>
     </row>
@@ -6653,9 +7121,15 @@
       <c r="V79" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W79" t="inlineStr">
-        <is>
-          <t>4070</t>
+      <c r="W79" t="n">
+        <v>4070</v>
+      </c>
+      <c r="X79" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y79" t="inlineStr">
+        <is>
+          <t>4267</t>
         </is>
       </c>
     </row>
@@ -6732,9 +7206,15 @@
       <c r="V80" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W80" t="inlineStr">
-        <is>
-          <t>3565</t>
+      <c r="W80" t="n">
+        <v>3565</v>
+      </c>
+      <c r="X80" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y80" t="inlineStr">
+        <is>
+          <t>3600</t>
         </is>
       </c>
     </row>
@@ -6811,9 +7291,15 @@
       <c r="V81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W81" t="inlineStr">
-        <is>
-          <t>2931</t>
+      <c r="W81" t="n">
+        <v>2931</v>
+      </c>
+      <c r="X81" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y81" t="inlineStr">
+        <is>
+          <t>3196</t>
         </is>
       </c>
     </row>
@@ -6890,9 +7376,15 @@
       <c r="V82" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="W82" t="inlineStr">
-        <is>
-          <t>4297</t>
+      <c r="W82" t="n">
+        <v>4297</v>
+      </c>
+      <c r="X82" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y82" t="inlineStr">
+        <is>
+          <t>4398</t>
         </is>
       </c>
     </row>
@@ -6969,9 +7461,15 @@
       <c r="V83" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W83" t="inlineStr">
-        <is>
-          <t>2823</t>
+      <c r="W83" t="n">
+        <v>2823</v>
+      </c>
+      <c r="X83" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y83" t="inlineStr">
+        <is>
+          <t>2913</t>
         </is>
       </c>
     </row>
@@ -7048,9 +7546,15 @@
       <c r="V84" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W84" t="inlineStr">
-        <is>
-          <t>3141</t>
+      <c r="W84" t="n">
+        <v>3141</v>
+      </c>
+      <c r="X84" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y84" t="inlineStr">
+        <is>
+          <t>3314</t>
         </is>
       </c>
     </row>
@@ -7127,9 +7631,15 @@
       <c r="V85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W85" t="inlineStr">
-        <is>
-          <t>2084</t>
+      <c r="W85" t="n">
+        <v>2084</v>
+      </c>
+      <c r="X85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y85" t="inlineStr">
+        <is>
+          <t>2116</t>
         </is>
       </c>
     </row>
@@ -7206,9 +7716,15 @@
       <c r="V86" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W86" t="inlineStr">
-        <is>
-          <t>2704</t>
+      <c r="W86" t="n">
+        <v>2704</v>
+      </c>
+      <c r="X86" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y86" t="inlineStr">
+        <is>
+          <t>2832</t>
         </is>
       </c>
     </row>
@@ -7285,9 +7801,15 @@
       <c r="V87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W87" t="inlineStr">
-        <is>
-          <t>3061</t>
+      <c r="W87" t="n">
+        <v>3061</v>
+      </c>
+      <c r="X87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y87" t="inlineStr">
+        <is>
+          <t>3084</t>
         </is>
       </c>
     </row>
@@ -7364,9 +7886,15 @@
       <c r="V88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W88" t="inlineStr">
-        <is>
-          <t>2408</t>
+      <c r="W88" t="n">
+        <v>2408</v>
+      </c>
+      <c r="X88" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y88" t="inlineStr">
+        <is>
+          <t>2436</t>
         </is>
       </c>
     </row>
@@ -7426,6 +7954,8 @@
       <c r="U89" t="inlineStr"/>
       <c r="V89" s="3" t="inlineStr"/>
       <c r="W89" t="inlineStr"/>
+      <c r="X89" s="3" t="inlineStr"/>
+      <c r="Y89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -7483,6 +8013,8 @@
       <c r="U90" t="inlineStr"/>
       <c r="V90" s="3" t="inlineStr"/>
       <c r="W90" t="inlineStr"/>
+      <c r="X90" s="3" t="inlineStr"/>
+      <c r="Y90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -7557,9 +8089,15 @@
       <c r="V91" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="W91" t="inlineStr">
-        <is>
-          <t>2706</t>
+      <c r="W91" t="n">
+        <v>2706</v>
+      </c>
+      <c r="X91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y91" t="inlineStr">
+        <is>
+          <t>2701</t>
         </is>
       </c>
     </row>
@@ -7636,9 +8174,15 @@
       <c r="V92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W92" t="inlineStr">
-        <is>
-          <t>3279</t>
+      <c r="W92" t="n">
+        <v>3279</v>
+      </c>
+      <c r="X92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y92" t="inlineStr">
+        <is>
+          <t>3307</t>
         </is>
       </c>
     </row>
@@ -7715,9 +8259,15 @@
       <c r="V93" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="W93" t="inlineStr">
-        <is>
-          <t>2928</t>
+      <c r="W93" t="n">
+        <v>2928</v>
+      </c>
+      <c r="X93" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y93" t="inlineStr">
+        <is>
+          <t>3086</t>
         </is>
       </c>
     </row>
@@ -7794,9 +8344,15 @@
       <c r="V94" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W94" t="inlineStr">
-        <is>
-          <t>4088</t>
+      <c r="W94" t="n">
+        <v>4088</v>
+      </c>
+      <c r="X94" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y94" t="inlineStr">
+        <is>
+          <t>4235</t>
         </is>
       </c>
     </row>
@@ -7873,9 +8429,15 @@
       <c r="V95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W95" t="inlineStr">
-        <is>
-          <t>3885</t>
+      <c r="W95" t="n">
+        <v>3885</v>
+      </c>
+      <c r="X95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y95" t="inlineStr">
+        <is>
+          <t>3932</t>
         </is>
       </c>
     </row>
@@ -7952,9 +8514,15 @@
       <c r="V96" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="W96" t="inlineStr">
-        <is>
-          <t>3679</t>
+      <c r="W96" t="n">
+        <v>3679</v>
+      </c>
+      <c r="X96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y96" t="inlineStr">
+        <is>
+          <t>3649</t>
         </is>
       </c>
     </row>
@@ -8031,9 +8599,15 @@
       <c r="V97" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="W97" t="inlineStr">
-        <is>
-          <t>4169</t>
+      <c r="W97" t="n">
+        <v>4169</v>
+      </c>
+      <c r="X97" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Y97" t="inlineStr">
+        <is>
+          <t>4288</t>
         </is>
       </c>
     </row>
@@ -8110,9 +8684,15 @@
       <c r="V98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W98" t="inlineStr">
-        <is>
-          <t>3400</t>
+      <c r="W98" t="n">
+        <v>3400</v>
+      </c>
+      <c r="X98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y98" t="inlineStr">
+        <is>
+          <t>3430</t>
         </is>
       </c>
     </row>
@@ -8189,9 +8769,15 @@
       <c r="V99" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W99" t="inlineStr">
-        <is>
-          <t>2868</t>
+      <c r="W99" t="n">
+        <v>2868</v>
+      </c>
+      <c r="X99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y99" t="inlineStr">
+        <is>
+          <t>2855</t>
         </is>
       </c>
     </row>
@@ -8268,9 +8854,15 @@
       <c r="V100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W100" t="inlineStr">
-        <is>
-          <t>2639</t>
+      <c r="W100" t="n">
+        <v>2639</v>
+      </c>
+      <c r="X100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y100" t="inlineStr">
+        <is>
+          <t>2628</t>
         </is>
       </c>
     </row>
@@ -8347,9 +8939,15 @@
       <c r="V101" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W101" t="inlineStr">
-        <is>
-          <t>4294</t>
+      <c r="W101" t="n">
+        <v>4294</v>
+      </c>
+      <c r="X101" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y101" t="inlineStr">
+        <is>
+          <t>4377</t>
         </is>
       </c>
     </row>
@@ -8426,9 +9024,15 @@
       <c r="V102" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="W102" t="inlineStr">
-        <is>
-          <t>3690</t>
+      <c r="W102" t="n">
+        <v>3690</v>
+      </c>
+      <c r="X102" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="Y102" t="inlineStr">
+        <is>
+          <t>3831</t>
         </is>
       </c>
     </row>
@@ -8505,9 +9109,15 @@
       <c r="V103" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W103" t="inlineStr">
-        <is>
-          <t>3389</t>
+      <c r="W103" t="n">
+        <v>3389</v>
+      </c>
+      <c r="X103" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y103" t="inlineStr">
+        <is>
+          <t>3433</t>
         </is>
       </c>
     </row>
@@ -8584,9 +9194,15 @@
       <c r="V104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W104" t="inlineStr">
-        <is>
-          <t>2560</t>
+      <c r="W104" t="n">
+        <v>2560</v>
+      </c>
+      <c r="X104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y104" t="inlineStr">
+        <is>
+          <t>2578</t>
         </is>
       </c>
     </row>
@@ -8663,9 +9279,15 @@
       <c r="V105" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W105" t="inlineStr">
-        <is>
-          <t>3454</t>
+      <c r="W105" t="n">
+        <v>3454</v>
+      </c>
+      <c r="X105" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y105" t="inlineStr">
+        <is>
+          <t>3704</t>
         </is>
       </c>
     </row>
@@ -8742,9 +9364,15 @@
       <c r="V106" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W106" t="inlineStr">
-        <is>
-          <t>3053</t>
+      <c r="W106" t="n">
+        <v>3053</v>
+      </c>
+      <c r="X106" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y106" t="inlineStr">
+        <is>
+          <t>3315</t>
         </is>
       </c>
     </row>
@@ -8821,9 +9449,15 @@
       <c r="V107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W107" t="inlineStr">
-        <is>
-          <t>3545</t>
+      <c r="W107" t="n">
+        <v>3545</v>
+      </c>
+      <c r="X107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y107" t="inlineStr">
+        <is>
+          <t>3603</t>
         </is>
       </c>
     </row>
@@ -8900,9 +9534,15 @@
       <c r="V108" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="W108" t="inlineStr">
-        <is>
-          <t>2667</t>
+      <c r="W108" t="n">
+        <v>2667</v>
+      </c>
+      <c r="X108" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y108" t="inlineStr">
+        <is>
+          <t>2754</t>
         </is>
       </c>
     </row>
@@ -8979,9 +9619,15 @@
       <c r="V109" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="W109" t="inlineStr">
-        <is>
-          <t>2742</t>
+      <c r="W109" t="n">
+        <v>2742</v>
+      </c>
+      <c r="X109" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y109" t="inlineStr">
+        <is>
+          <t>2767</t>
         </is>
       </c>
     </row>
@@ -9058,9 +9704,15 @@
       <c r="V110" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="W110" t="inlineStr">
-        <is>
-          <t>3345</t>
+      <c r="W110" t="n">
+        <v>3345</v>
+      </c>
+      <c r="X110" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y110" t="inlineStr">
+        <is>
+          <t>3346</t>
         </is>
       </c>
     </row>
@@ -9137,9 +9789,15 @@
       <c r="V111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W111" t="inlineStr">
-        <is>
-          <t>2864</t>
+      <c r="W111" t="n">
+        <v>2864</v>
+      </c>
+      <c r="X111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y111" t="inlineStr">
+        <is>
+          <t>3004</t>
         </is>
       </c>
     </row>
@@ -9216,9 +9874,15 @@
       <c r="V112" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="W112" t="inlineStr">
-        <is>
-          <t>3370</t>
+      <c r="W112" t="n">
+        <v>3370</v>
+      </c>
+      <c r="X112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y112" t="inlineStr">
+        <is>
+          <t>3473</t>
         </is>
       </c>
     </row>
@@ -9295,9 +9959,15 @@
       <c r="V113" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="W113" t="inlineStr">
-        <is>
-          <t>2524</t>
+      <c r="W113" t="n">
+        <v>2524</v>
+      </c>
+      <c r="X113" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y113" t="inlineStr">
+        <is>
+          <t>2702</t>
         </is>
       </c>
     </row>
@@ -9374,9 +10044,15 @@
       <c r="V114" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W114" t="inlineStr">
-        <is>
-          <t>3567</t>
+      <c r="W114" t="n">
+        <v>3567</v>
+      </c>
+      <c r="X114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y114" t="inlineStr">
+        <is>
+          <t>3635</t>
         </is>
       </c>
     </row>
@@ -9453,9 +10129,15 @@
       <c r="V115" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W115" t="inlineStr">
-        <is>
-          <t>2645</t>
+      <c r="W115" t="n">
+        <v>2645</v>
+      </c>
+      <c r="X115" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y115" t="inlineStr">
+        <is>
+          <t>2689</t>
         </is>
       </c>
     </row>
@@ -9532,9 +10214,15 @@
       <c r="V116" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="W116" t="inlineStr">
-        <is>
-          <t>3105</t>
+      <c r="W116" t="n">
+        <v>3105</v>
+      </c>
+      <c r="X116" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y116" t="inlineStr">
+        <is>
+          <t>3193</t>
         </is>
       </c>
     </row>
@@ -9611,9 +10299,15 @@
       <c r="V117" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W117" t="inlineStr">
-        <is>
-          <t>3215</t>
+      <c r="W117" t="n">
+        <v>3215</v>
+      </c>
+      <c r="X117" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y117" t="inlineStr">
+        <is>
+          <t>3169</t>
         </is>
       </c>
     </row>
@@ -9685,6 +10379,8 @@
       <c r="U118" t="inlineStr"/>
       <c r="V118" s="3" t="inlineStr"/>
       <c r="W118" t="inlineStr"/>
+      <c r="X118" s="3" t="inlineStr"/>
+      <c r="Y118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -9759,9 +10455,15 @@
       <c r="V119" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W119" t="inlineStr">
-        <is>
-          <t>3432</t>
+      <c r="W119" t="n">
+        <v>3432</v>
+      </c>
+      <c r="X119" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y119" t="inlineStr">
+        <is>
+          <t>3472</t>
         </is>
       </c>
     </row>
@@ -9838,9 +10540,15 @@
       <c r="V120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W120" t="inlineStr">
-        <is>
-          <t>3193</t>
+      <c r="W120" t="n">
+        <v>3193</v>
+      </c>
+      <c r="X120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y120" t="inlineStr">
+        <is>
+          <t>3186</t>
         </is>
       </c>
     </row>
@@ -9917,9 +10625,15 @@
       <c r="V121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W121" t="inlineStr">
-        <is>
-          <t>2173</t>
+      <c r="W121" t="n">
+        <v>2173</v>
+      </c>
+      <c r="X121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y121" t="inlineStr">
+        <is>
+          <t>2162</t>
         </is>
       </c>
     </row>
@@ -9996,9 +10710,15 @@
       <c r="V122" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="W122" t="inlineStr">
-        <is>
-          <t>2560</t>
+      <c r="W122" t="n">
+        <v>2560</v>
+      </c>
+      <c r="X122" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y122" t="inlineStr">
+        <is>
+          <t>2578</t>
         </is>
       </c>
     </row>
@@ -10075,9 +10795,15 @@
       <c r="V123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W123" t="inlineStr">
-        <is>
-          <t>2675</t>
+      <c r="W123" t="n">
+        <v>2675</v>
+      </c>
+      <c r="X123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y123" t="inlineStr">
+        <is>
+          <t>2684</t>
         </is>
       </c>
     </row>
@@ -10154,9 +10880,15 @@
       <c r="V124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W124" t="inlineStr">
-        <is>
-          <t>3498</t>
+      <c r="W124" t="n">
+        <v>3498</v>
+      </c>
+      <c r="X124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y124" t="inlineStr">
+        <is>
+          <t>3535</t>
         </is>
       </c>
     </row>
@@ -10233,7 +10965,13 @@
       <c r="V125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W125" t="inlineStr">
+      <c r="W125" t="n">
+        <v>0</v>
+      </c>
+      <c r="X125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10312,9 +11050,15 @@
       <c r="V126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W126" t="inlineStr">
-        <is>
-          <t>2892</t>
+      <c r="W126" t="n">
+        <v>2892</v>
+      </c>
+      <c r="X126" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y126" t="inlineStr">
+        <is>
+          <t>3008</t>
         </is>
       </c>
     </row>
@@ -10391,9 +11135,15 @@
       <c r="V127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W127" t="inlineStr">
-        <is>
-          <t>2566</t>
+      <c r="W127" t="n">
+        <v>2566</v>
+      </c>
+      <c r="X127" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y127" t="inlineStr">
+        <is>
+          <t>2801</t>
         </is>
       </c>
     </row>
@@ -10470,9 +11220,15 @@
       <c r="V128" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W128" t="inlineStr">
-        <is>
-          <t>2736</t>
+      <c r="W128" t="n">
+        <v>2736</v>
+      </c>
+      <c r="X128" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y128" t="inlineStr">
+        <is>
+          <t>2692</t>
         </is>
       </c>
     </row>
@@ -10549,9 +11305,15 @@
       <c r="V129" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="W129" t="inlineStr">
-        <is>
-          <t>2574</t>
+      <c r="W129" t="n">
+        <v>2574</v>
+      </c>
+      <c r="X129" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y129" t="inlineStr">
+        <is>
+          <t>2570</t>
         </is>
       </c>
     </row>
@@ -10628,9 +11390,15 @@
       <c r="V130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W130" t="inlineStr">
-        <is>
-          <t>1914</t>
+      <c r="W130" t="n">
+        <v>1914</v>
+      </c>
+      <c r="X130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y130" t="inlineStr">
+        <is>
+          <t>1927</t>
         </is>
       </c>
     </row>
@@ -10707,7 +11475,13 @@
       <c r="V131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W131" t="inlineStr">
+      <c r="W131" t="n">
+        <v>0</v>
+      </c>
+      <c r="X131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10786,9 +11560,15 @@
       <c r="V132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W132" t="inlineStr">
-        <is>
-          <t>1509</t>
+      <c r="W132" t="n">
+        <v>1509</v>
+      </c>
+      <c r="X132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y132" t="inlineStr">
+        <is>
+          <t>1508</t>
         </is>
       </c>
     </row>
@@ -10860,6 +11640,8 @@
       <c r="U133" t="inlineStr"/>
       <c r="V133" s="3" t="inlineStr"/>
       <c r="W133" t="inlineStr"/>
+      <c r="X133" s="3" t="inlineStr"/>
+      <c r="Y133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -10934,9 +11716,15 @@
       <c r="V134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W134" t="inlineStr">
-        <is>
-          <t>2035</t>
+      <c r="W134" t="n">
+        <v>2035</v>
+      </c>
+      <c r="X134" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y134" t="inlineStr">
+        <is>
+          <t>2041</t>
         </is>
       </c>
     </row>
@@ -11013,9 +11801,15 @@
       <c r="V135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W135" t="inlineStr">
-        <is>
-          <t>2218</t>
+      <c r="W135" t="n">
+        <v>2218</v>
+      </c>
+      <c r="X135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y135" t="inlineStr">
+        <is>
+          <t>2208</t>
         </is>
       </c>
     </row>
@@ -11092,9 +11886,15 @@
       <c r="V136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W136" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="W136" t="n">
+        <v>0</v>
+      </c>
+      <c r="X136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y136" t="inlineStr">
+        <is>
+          <t>1518</t>
         </is>
       </c>
     </row>
@@ -11166,6 +11966,8 @@
       <c r="U137" t="inlineStr"/>
       <c r="V137" s="3" t="inlineStr"/>
       <c r="W137" t="inlineStr"/>
+      <c r="X137" s="3" t="inlineStr"/>
+      <c r="Y137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -11240,7 +12042,13 @@
       <c r="V138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W138" t="inlineStr">
+      <c r="W138" t="n">
+        <v>0</v>
+      </c>
+      <c r="X138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11314,6 +12122,8 @@
       <c r="U139" t="inlineStr"/>
       <c r="V139" s="3" t="inlineStr"/>
       <c r="W139" t="inlineStr"/>
+      <c r="X139" s="3" t="inlineStr"/>
+      <c r="Y139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -11388,9 +12198,15 @@
       <c r="V140" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="W140" t="inlineStr">
-        <is>
-          <t>4402</t>
+      <c r="W140" t="n">
+        <v>4402</v>
+      </c>
+      <c r="X140" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y140" t="inlineStr">
+        <is>
+          <t>4802</t>
         </is>
       </c>
     </row>
@@ -11467,7 +12283,13 @@
       <c r="V141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W141" t="inlineStr">
+      <c r="W141" t="n">
+        <v>0</v>
+      </c>
+      <c r="X141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11546,7 +12368,13 @@
       <c r="V142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W142" t="inlineStr">
+      <c r="W142" t="n">
+        <v>0</v>
+      </c>
+      <c r="X142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11625,9 +12453,15 @@
       <c r="V143" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="W143" t="inlineStr">
-        <is>
-          <t>4934</t>
+      <c r="W143" t="n">
+        <v>4934</v>
+      </c>
+      <c r="X143" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y143" t="inlineStr">
+        <is>
+          <t>5149</t>
         </is>
       </c>
     </row>
@@ -11704,7 +12538,13 @@
       <c r="V144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W144" t="inlineStr">
+      <c r="W144" t="n">
+        <v>0</v>
+      </c>
+      <c r="X144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11783,9 +12623,15 @@
       <c r="V145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W145" t="inlineStr">
-        <is>
-          <t>2736</t>
+      <c r="W145" t="n">
+        <v>2736</v>
+      </c>
+      <c r="X145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y145" t="inlineStr">
+        <is>
+          <t>2746</t>
         </is>
       </c>
     </row>
@@ -11862,7 +12708,13 @@
       <c r="V146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W146" t="inlineStr">
+      <c r="W146" t="n">
+        <v>0</v>
+      </c>
+      <c r="X146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11941,9 +12793,15 @@
       <c r="V147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W147" t="inlineStr">
-        <is>
-          <t>2764</t>
+      <c r="W147" t="n">
+        <v>2764</v>
+      </c>
+      <c r="X147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y147" t="inlineStr">
+        <is>
+          <t>2825</t>
         </is>
       </c>
     </row>
@@ -11998,9 +12856,15 @@
       <c r="V148" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W148" t="inlineStr">
-        <is>
-          <t>2997</t>
+      <c r="W148" t="n">
+        <v>2997</v>
+      </c>
+      <c r="X148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y148" t="inlineStr">
+        <is>
+          <t>2887</t>
         </is>
       </c>
     </row>
@@ -12071,7 +12935,13 @@
       <c r="V149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W149" t="inlineStr">
+      <c r="W149" t="n">
+        <v>0</v>
+      </c>
+      <c r="X149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12144,7 +13014,13 @@
       <c r="V150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W150" t="inlineStr">
+      <c r="W150" t="n">
+        <v>0</v>
+      </c>
+      <c r="X150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12205,9 +13081,15 @@
       <c r="V151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W151" t="inlineStr">
-        <is>
-          <t>2249</t>
+      <c r="W151" t="n">
+        <v>2249</v>
+      </c>
+      <c r="X151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y151" t="inlineStr">
+        <is>
+          <t>2267</t>
         </is>
       </c>
     </row>
@@ -12266,7 +13148,13 @@
       <c r="V152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W152" t="inlineStr">
+      <c r="W152" t="n">
+        <v>0</v>
+      </c>
+      <c r="X152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12319,9 +13207,15 @@
       <c r="V153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W153" t="inlineStr">
-        <is>
-          <t>3750</t>
+      <c r="W153" t="n">
+        <v>3750</v>
+      </c>
+      <c r="X153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y153" t="inlineStr">
+        <is>
+          <t>3769</t>
         </is>
       </c>
     </row>
@@ -12372,9 +13266,15 @@
       <c r="V154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W154" t="inlineStr">
-        <is>
-          <t>1665</t>
+      <c r="W154" t="n">
+        <v>1665</v>
+      </c>
+      <c r="X154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y154" t="inlineStr">
+        <is>
+          <t>1658</t>
         </is>
       </c>
     </row>
@@ -12421,9 +13321,15 @@
       <c r="V155" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="W155" t="inlineStr">
-        <is>
-          <t>1538</t>
+      <c r="W155" t="n">
+        <v>1538</v>
+      </c>
+      <c r="X155" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y155" t="inlineStr">
+        <is>
+          <t>1555</t>
         </is>
       </c>
     </row>
@@ -12466,7 +13372,13 @@
       <c r="V156" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="W156" t="inlineStr">
+      <c r="W156" t="n">
+        <v>3476</v>
+      </c>
+      <c r="X156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y156" t="inlineStr">
         <is>
           <t>3476</t>
         </is>
@@ -12511,9 +13423,15 @@
       <c r="V157" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W157" t="inlineStr">
-        <is>
-          <t>5772</t>
+      <c r="W157" t="n">
+        <v>5772</v>
+      </c>
+      <c r="X157" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y157" t="inlineStr">
+        <is>
+          <t>6264</t>
         </is>
       </c>
     </row>
@@ -12555,12 +13473,12 @@
       </c>
       <c r="V158" s="3" t="inlineStr"/>
       <c r="W158" t="inlineStr"/>
+      <c r="X158" s="3" t="inlineStr"/>
+      <c r="Y158" t="inlineStr"/>
     </row>
     <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>7857221</t>
-        </is>
+      <c r="A159" t="n">
+        <v>7857221</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
@@ -12593,17 +13511,21 @@
       <c r="V159" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W159" t="inlineStr">
-        <is>
-          <t>4733</t>
+      <c r="W159" t="n">
+        <v>4733</v>
+      </c>
+      <c r="X159" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y159" t="inlineStr">
+        <is>
+          <t>5042</t>
         </is>
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>57038133</t>
-        </is>
+      <c r="A160" t="n">
+        <v>57038133</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -12636,17 +13558,21 @@
       <c r="V160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W160" t="inlineStr">
-        <is>
-          <t>2628</t>
+      <c r="W160" t="n">
+        <v>2628</v>
+      </c>
+      <c r="X160" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y160" t="inlineStr">
+        <is>
+          <t>2648</t>
         </is>
       </c>
     </row>
     <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>58463042</t>
-        </is>
+      <c r="A161" t="n">
+        <v>58463042</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -12679,17 +13605,21 @@
       <c r="V161" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="W161" t="inlineStr">
-        <is>
-          <t>1848</t>
+      <c r="W161" t="n">
+        <v>1848</v>
+      </c>
+      <c r="X161" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y161" t="inlineStr">
+        <is>
+          <t>1885</t>
         </is>
       </c>
     </row>
     <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>58526469</t>
-        </is>
+      <c r="A162" t="n">
+        <v>58526469</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
@@ -12722,9 +13652,60 @@
       <c r="V162" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W162" t="inlineStr">
-        <is>
-          <t>1371</t>
+      <c r="W162" t="n">
+        <v>1371</v>
+      </c>
+      <c r="X162" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y162" t="inlineStr">
+        <is>
+          <t>1650</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>58380905</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Player-58380905</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr"/>
+      <c r="D163" t="inlineStr"/>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F163" s="3" t="inlineStr"/>
+      <c r="G163" t="inlineStr"/>
+      <c r="H163" s="3" t="inlineStr"/>
+      <c r="I163" t="inlineStr"/>
+      <c r="J163" s="3" t="inlineStr"/>
+      <c r="K163" t="inlineStr"/>
+      <c r="L163" s="3" t="inlineStr"/>
+      <c r="M163" t="inlineStr"/>
+      <c r="N163" s="3" t="inlineStr"/>
+      <c r="O163" t="inlineStr"/>
+      <c r="P163" s="3" t="inlineStr"/>
+      <c r="Q163" t="inlineStr"/>
+      <c r="R163" s="3" t="inlineStr"/>
+      <c r="S163" t="inlineStr"/>
+      <c r="T163" s="3" t="inlineStr"/>
+      <c r="U163" t="inlineStr"/>
+      <c r="V163" s="3" t="inlineStr"/>
+      <c r="W163" t="inlineStr"/>
+      <c r="X163" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y163" t="inlineStr">
+        <is>
+          <t>1654</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-11 18:52:28
</commit_message>
<xml_diff>
--- a/Season_Attack/81.xlsx
+++ b/Season_Attack/81.xlsx
@@ -13665,10 +13665,8 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>58380905</t>
-        </is>
+      <c r="A163" t="n">
+        <v>58380905</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-01-12 11:30:33
</commit_message>
<xml_diff>
--- a/Season_Attack/81.xlsx
+++ b/Season_Attack/81.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y163"/>
+  <dimension ref="A1:AA166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,6 +516,16 @@
           <t>01-10_0</t>
         </is>
       </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>01-11_A</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>01-11_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -596,9 +606,15 @@
       <c r="X2" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>4248</t>
+      <c r="Y2" t="n">
+        <v>4248</v>
+      </c>
+      <c r="Z2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>4241</t>
         </is>
       </c>
     </row>
@@ -681,9 +697,15 @@
       <c r="X3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>4753</t>
+      <c r="Y3" t="n">
+        <v>4753</v>
+      </c>
+      <c r="Z3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>5004</t>
         </is>
       </c>
     </row>
@@ -766,9 +788,15 @@
       <c r="X4" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>5415</t>
+      <c r="Y4" t="n">
+        <v>5415</v>
+      </c>
+      <c r="Z4" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>5606</t>
         </is>
       </c>
     </row>
@@ -851,9 +879,15 @@
       <c r="X5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>5724</t>
+      <c r="Y5" t="n">
+        <v>5724</v>
+      </c>
+      <c r="Z5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>5933</t>
         </is>
       </c>
     </row>
@@ -936,9 +970,15 @@
       <c r="X6" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>5616</t>
+      <c r="Y6" t="n">
+        <v>5616</v>
+      </c>
+      <c r="Z6" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>5800</t>
         </is>
       </c>
     </row>
@@ -1021,9 +1061,15 @@
       <c r="X7" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>5746</t>
+      <c r="Y7" t="n">
+        <v>5746</v>
+      </c>
+      <c r="Z7" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>5985</t>
         </is>
       </c>
     </row>
@@ -1106,9 +1152,15 @@
       <c r="X8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>4930</t>
+      <c r="Y8" t="n">
+        <v>4930</v>
+      </c>
+      <c r="Z8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>5176</t>
         </is>
       </c>
     </row>
@@ -1191,9 +1243,15 @@
       <c r="X9" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>5073</t>
+      <c r="Y9" t="n">
+        <v>5073</v>
+      </c>
+      <c r="Z9" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>5256</t>
         </is>
       </c>
     </row>
@@ -1276,9 +1334,15 @@
       <c r="X10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>4529</t>
+      <c r="Y10" t="n">
+        <v>4529</v>
+      </c>
+      <c r="Z10" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>4582</t>
         </is>
       </c>
     </row>
@@ -1361,9 +1425,15 @@
       <c r="X11" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y11" t="inlineStr">
-        <is>
-          <t>5704</t>
+      <c r="Y11" t="n">
+        <v>5704</v>
+      </c>
+      <c r="Z11" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>6172</t>
         </is>
       </c>
     </row>
@@ -1446,9 +1516,15 @@
       <c r="X12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y12" t="inlineStr">
-        <is>
-          <t>4998</t>
+      <c r="Y12" t="n">
+        <v>4998</v>
+      </c>
+      <c r="Z12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>5460</t>
         </is>
       </c>
     </row>
@@ -1531,9 +1607,15 @@
       <c r="X13" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>2863</t>
+      <c r="Y13" t="n">
+        <v>2863</v>
+      </c>
+      <c r="Z13" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>2927</t>
         </is>
       </c>
     </row>
@@ -1616,9 +1698,15 @@
       <c r="X14" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="Y14" t="inlineStr">
-        <is>
-          <t>6065</t>
+      <c r="Y14" t="n">
+        <v>6065</v>
+      </c>
+      <c r="Z14" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>6408</t>
         </is>
       </c>
     </row>
@@ -1701,9 +1789,15 @@
       <c r="X15" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="Y15" t="inlineStr">
-        <is>
-          <t>5254</t>
+      <c r="Y15" t="n">
+        <v>5254</v>
+      </c>
+      <c r="Z15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>5481</t>
         </is>
       </c>
     </row>
@@ -1786,9 +1880,15 @@
       <c r="X16" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y16" t="inlineStr">
-        <is>
-          <t>5710</t>
+      <c r="Y16" t="n">
+        <v>5710</v>
+      </c>
+      <c r="Z16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>5913</t>
         </is>
       </c>
     </row>
@@ -1871,9 +1971,15 @@
       <c r="X17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y17" t="inlineStr">
-        <is>
-          <t>5066</t>
+      <c r="Y17" t="n">
+        <v>5066</v>
+      </c>
+      <c r="Z17" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>5123</t>
         </is>
       </c>
     </row>
@@ -1956,9 +2062,15 @@
       <c r="X18" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="Y18" t="inlineStr">
-        <is>
-          <t>4964</t>
+      <c r="Y18" t="n">
+        <v>4964</v>
+      </c>
+      <c r="Z18" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>5177</t>
         </is>
       </c>
     </row>
@@ -2041,9 +2153,15 @@
       <c r="X19" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="Y19" t="inlineStr">
-        <is>
-          <t>5523</t>
+      <c r="Y19" t="n">
+        <v>5523</v>
+      </c>
+      <c r="Z19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>5775</t>
         </is>
       </c>
     </row>
@@ -2126,9 +2244,15 @@
       <c r="X20" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="Y20" t="inlineStr">
-        <is>
-          <t>5941</t>
+      <c r="Y20" t="n">
+        <v>5941</v>
+      </c>
+      <c r="Z20" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>6197</t>
         </is>
       </c>
     </row>
@@ -2211,9 +2335,15 @@
       <c r="X21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y21" t="inlineStr">
-        <is>
-          <t>4818</t>
+      <c r="Y21" t="n">
+        <v>4818</v>
+      </c>
+      <c r="Z21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>5076</t>
         </is>
       </c>
     </row>
@@ -2296,9 +2426,15 @@
       <c r="X22" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Y22" t="inlineStr">
-        <is>
-          <t>5560</t>
+      <c r="Y22" t="n">
+        <v>5560</v>
+      </c>
+      <c r="Z22" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>5752</t>
         </is>
       </c>
     </row>
@@ -2381,9 +2517,15 @@
       <c r="X23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y23" t="inlineStr">
-        <is>
-          <t>5419</t>
+      <c r="Y23" t="n">
+        <v>5419</v>
+      </c>
+      <c r="Z23" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>5468</t>
         </is>
       </c>
     </row>
@@ -2466,9 +2608,15 @@
       <c r="X24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y24" t="inlineStr">
-        <is>
-          <t>5211</t>
+      <c r="Y24" t="n">
+        <v>5211</v>
+      </c>
+      <c r="Z24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA24" t="inlineStr">
+        <is>
+          <t>5098</t>
         </is>
       </c>
     </row>
@@ -2551,7 +2699,13 @@
       <c r="X25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y25" t="inlineStr">
+      <c r="Y25" t="n">
+        <v>2500</v>
+      </c>
+      <c r="Z25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA25" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2636,9 +2790,15 @@
       <c r="X26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Y26" t="inlineStr">
-        <is>
-          <t>5419</t>
+      <c r="Y26" t="n">
+        <v>5419</v>
+      </c>
+      <c r="Z26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA26" t="inlineStr">
+        <is>
+          <t>5659</t>
         </is>
       </c>
     </row>
@@ -2721,9 +2881,15 @@
       <c r="X27" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Y27" t="inlineStr">
-        <is>
-          <t>5705</t>
+      <c r="Y27" t="n">
+        <v>5705</v>
+      </c>
+      <c r="Z27" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA27" t="inlineStr">
+        <is>
+          <t>6052</t>
         </is>
       </c>
     </row>
@@ -2806,9 +2972,15 @@
       <c r="X28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y28" t="inlineStr">
-        <is>
-          <t>4267</t>
+      <c r="Y28" t="n">
+        <v>4267</v>
+      </c>
+      <c r="Z28" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>4399</t>
         </is>
       </c>
     </row>
@@ -2891,9 +3063,15 @@
       <c r="X29" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y29" t="inlineStr">
-        <is>
-          <t>4714</t>
+      <c r="Y29" t="n">
+        <v>4714</v>
+      </c>
+      <c r="Z29" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA29" t="inlineStr">
+        <is>
+          <t>5164</t>
         </is>
       </c>
     </row>
@@ -2976,9 +3154,15 @@
       <c r="X30" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Y30" t="inlineStr">
-        <is>
-          <t>5768</t>
+      <c r="Y30" t="n">
+        <v>5768</v>
+      </c>
+      <c r="Z30" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA30" t="inlineStr">
+        <is>
+          <t>6014</t>
         </is>
       </c>
     </row>
@@ -3061,9 +3245,15 @@
       <c r="X31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y31" t="inlineStr">
-        <is>
-          <t>5367</t>
+      <c r="Y31" t="n">
+        <v>5367</v>
+      </c>
+      <c r="Z31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>5630</t>
         </is>
       </c>
     </row>
@@ -3146,9 +3336,15 @@
       <c r="X32" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Y32" t="inlineStr">
-        <is>
-          <t>5737</t>
+      <c r="Y32" t="n">
+        <v>5737</v>
+      </c>
+      <c r="Z32" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA32" t="inlineStr">
+        <is>
+          <t>5969</t>
         </is>
       </c>
     </row>
@@ -3231,9 +3427,15 @@
       <c r="X33" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Y33" t="inlineStr">
-        <is>
-          <t>5880</t>
+      <c r="Y33" t="n">
+        <v>5880</v>
+      </c>
+      <c r="Z33" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="AA33" t="inlineStr">
+        <is>
+          <t>6311</t>
         </is>
       </c>
     </row>
@@ -3316,7 +3518,13 @@
       <c r="X34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y34" t="inlineStr">
+      <c r="Y34" t="n">
+        <v>3476</v>
+      </c>
+      <c r="Z34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA34" t="inlineStr">
         <is>
           <t>3476</t>
         </is>
@@ -3401,9 +3609,15 @@
       <c r="X35" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="Y35" t="inlineStr">
-        <is>
-          <t>5760</t>
+      <c r="Y35" t="n">
+        <v>5760</v>
+      </c>
+      <c r="Z35" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="AA35" t="inlineStr">
+        <is>
+          <t>6028</t>
         </is>
       </c>
     </row>
@@ -3486,9 +3700,15 @@
       <c r="X36" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y36" t="inlineStr">
-        <is>
-          <t>4816</t>
+      <c r="Y36" t="n">
+        <v>4816</v>
+      </c>
+      <c r="Z36" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA36" t="inlineStr">
+        <is>
+          <t>5141</t>
         </is>
       </c>
     </row>
@@ -3571,9 +3791,15 @@
       <c r="X37" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="Y37" t="inlineStr">
-        <is>
-          <t>4767</t>
+      <c r="Y37" t="n">
+        <v>4767</v>
+      </c>
+      <c r="Z37" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA37" t="inlineStr">
+        <is>
+          <t>4749</t>
         </is>
       </c>
     </row>
@@ -3656,9 +3882,15 @@
       <c r="X38" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Y38" t="inlineStr">
-        <is>
-          <t>5307</t>
+      <c r="Y38" t="n">
+        <v>5307</v>
+      </c>
+      <c r="Z38" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA38" t="inlineStr">
+        <is>
+          <t>5475</t>
         </is>
       </c>
     </row>
@@ -3741,9 +3973,15 @@
       <c r="X39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Y39" t="inlineStr">
-        <is>
-          <t>5113</t>
+      <c r="Y39" t="n">
+        <v>5113</v>
+      </c>
+      <c r="Z39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA39" t="inlineStr">
+        <is>
+          <t>5216</t>
         </is>
       </c>
     </row>
@@ -3826,9 +4064,15 @@
       <c r="X40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y40" t="inlineStr">
-        <is>
-          <t>5817</t>
+      <c r="Y40" t="n">
+        <v>5817</v>
+      </c>
+      <c r="Z40" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="AA40" t="inlineStr">
+        <is>
+          <t>6227</t>
         </is>
       </c>
     </row>
@@ -3911,9 +4155,15 @@
       <c r="X41" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y41" t="inlineStr">
-        <is>
-          <t>5556</t>
+      <c r="Y41" t="n">
+        <v>5556</v>
+      </c>
+      <c r="Z41" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA41" t="inlineStr">
+        <is>
+          <t>5599</t>
         </is>
       </c>
     </row>
@@ -3996,9 +4246,15 @@
       <c r="X42" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Y42" t="inlineStr">
-        <is>
-          <t>5921</t>
+      <c r="Y42" t="n">
+        <v>5921</v>
+      </c>
+      <c r="Z42" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="AA42" t="inlineStr">
+        <is>
+          <t>6263</t>
         </is>
       </c>
     </row>
@@ -4081,9 +4337,15 @@
       <c r="X43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y43" t="inlineStr">
-        <is>
-          <t>5298</t>
+      <c r="Y43" t="n">
+        <v>5298</v>
+      </c>
+      <c r="Z43" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA43" t="inlineStr">
+        <is>
+          <t>5481</t>
         </is>
       </c>
     </row>
@@ -4166,9 +4428,15 @@
       <c r="X44" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="Y44" t="inlineStr">
-        <is>
-          <t>4428</t>
+      <c r="Y44" t="n">
+        <v>4428</v>
+      </c>
+      <c r="Z44" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA44" t="inlineStr">
+        <is>
+          <t>4501</t>
         </is>
       </c>
     </row>
@@ -4251,9 +4519,15 @@
       <c r="X45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y45" t="inlineStr">
-        <is>
-          <t>4995</t>
+      <c r="Y45" t="n">
+        <v>4995</v>
+      </c>
+      <c r="Z45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA45" t="inlineStr">
+        <is>
+          <t>5295</t>
         </is>
       </c>
     </row>
@@ -4336,9 +4610,15 @@
       <c r="X46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y46" t="inlineStr">
-        <is>
-          <t>5019</t>
+      <c r="Y46" t="n">
+        <v>5019</v>
+      </c>
+      <c r="Z46" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA46" t="inlineStr">
+        <is>
+          <t>5352</t>
         </is>
       </c>
     </row>
@@ -4421,9 +4701,15 @@
       <c r="X47" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="Y47" t="inlineStr">
-        <is>
-          <t>4702</t>
+      <c r="Y47" t="n">
+        <v>4702</v>
+      </c>
+      <c r="Z47" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="AA47" t="inlineStr">
+        <is>
+          <t>4910</t>
         </is>
       </c>
     </row>
@@ -4506,9 +4792,15 @@
       <c r="X48" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="Y48" t="inlineStr">
-        <is>
-          <t>5300</t>
+      <c r="Y48" t="n">
+        <v>5300</v>
+      </c>
+      <c r="Z48" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="AA48" t="inlineStr">
+        <is>
+          <t>5618</t>
         </is>
       </c>
     </row>
@@ -4591,9 +4883,15 @@
       <c r="X49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y49" t="inlineStr">
-        <is>
-          <t>3676</t>
+      <c r="Y49" t="n">
+        <v>3676</v>
+      </c>
+      <c r="Z49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA49" t="inlineStr">
+        <is>
+          <t>3637</t>
         </is>
       </c>
     </row>
@@ -4676,9 +4974,15 @@
       <c r="X50" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="Y50" t="inlineStr">
-        <is>
-          <t>5112</t>
+      <c r="Y50" t="n">
+        <v>5112</v>
+      </c>
+      <c r="Z50" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="AA50" t="inlineStr">
+        <is>
+          <t>5287</t>
         </is>
       </c>
     </row>
@@ -4761,9 +5065,15 @@
       <c r="X51" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Y51" t="inlineStr">
-        <is>
-          <t>5256</t>
+      <c r="Y51" t="n">
+        <v>5256</v>
+      </c>
+      <c r="Z51" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA51" t="inlineStr">
+        <is>
+          <t>5477</t>
         </is>
       </c>
     </row>
@@ -4846,9 +5156,15 @@
       <c r="X52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y52" t="inlineStr">
-        <is>
-          <t>2647</t>
+      <c r="Y52" t="n">
+        <v>2647</v>
+      </c>
+      <c r="Z52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA52" t="inlineStr">
+        <is>
+          <t>2672</t>
         </is>
       </c>
     </row>
@@ -4931,9 +5247,15 @@
       <c r="X53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y53" t="inlineStr">
-        <is>
-          <t>3175</t>
+      <c r="Y53" t="n">
+        <v>3175</v>
+      </c>
+      <c r="Z53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA53" t="inlineStr">
+        <is>
+          <t>3232</t>
         </is>
       </c>
     </row>
@@ -5016,9 +5338,15 @@
       <c r="X54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y54" t="inlineStr">
-        <is>
-          <t>3079</t>
+      <c r="Y54" t="n">
+        <v>3079</v>
+      </c>
+      <c r="Z54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA54" t="inlineStr">
+        <is>
+          <t>3117</t>
         </is>
       </c>
     </row>
@@ -5101,9 +5429,15 @@
       <c r="X55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Y55" t="inlineStr">
-        <is>
-          <t>4111</t>
+      <c r="Y55" t="n">
+        <v>4111</v>
+      </c>
+      <c r="Z55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA55" t="inlineStr">
+        <is>
+          <t>4167</t>
         </is>
       </c>
     </row>
@@ -5186,9 +5520,15 @@
       <c r="X56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y56" t="inlineStr">
-        <is>
-          <t>4263</t>
+      <c r="Y56" t="n">
+        <v>4263</v>
+      </c>
+      <c r="Z56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA56" t="inlineStr">
+        <is>
+          <t>4327</t>
         </is>
       </c>
     </row>
@@ -5271,9 +5611,15 @@
       <c r="X57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y57" t="inlineStr">
-        <is>
-          <t>4778</t>
+      <c r="Y57" t="n">
+        <v>4778</v>
+      </c>
+      <c r="Z57" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA57" t="inlineStr">
+        <is>
+          <t>4907</t>
         </is>
       </c>
     </row>
@@ -5356,9 +5702,15 @@
       <c r="X58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y58" t="inlineStr">
-        <is>
-          <t>4155</t>
+      <c r="Y58" t="n">
+        <v>4155</v>
+      </c>
+      <c r="Z58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA58" t="inlineStr">
+        <is>
+          <t>4349</t>
         </is>
       </c>
     </row>
@@ -5441,9 +5793,15 @@
       <c r="X59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y59" t="inlineStr">
-        <is>
-          <t>4689</t>
+      <c r="Y59" t="n">
+        <v>4689</v>
+      </c>
+      <c r="Z59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA59" t="inlineStr">
+        <is>
+          <t>4849</t>
         </is>
       </c>
     </row>
@@ -5526,9 +5884,15 @@
       <c r="X60" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Y60" t="inlineStr">
-        <is>
-          <t>4990</t>
+      <c r="Y60" t="n">
+        <v>4990</v>
+      </c>
+      <c r="Z60" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA60" t="inlineStr">
+        <is>
+          <t>5181</t>
         </is>
       </c>
     </row>
@@ -5611,9 +5975,15 @@
       <c r="X61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y61" t="inlineStr">
-        <is>
-          <t>4785</t>
+      <c r="Y61" t="n">
+        <v>4785</v>
+      </c>
+      <c r="Z61" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA61" t="inlineStr">
+        <is>
+          <t>4818</t>
         </is>
       </c>
     </row>
@@ -5696,9 +6066,15 @@
       <c r="X62" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="Y62" t="inlineStr">
-        <is>
-          <t>4870</t>
+      <c r="Y62" t="n">
+        <v>4870</v>
+      </c>
+      <c r="Z62" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA62" t="inlineStr">
+        <is>
+          <t>5215</t>
         </is>
       </c>
     </row>
@@ -5781,9 +6157,15 @@
       <c r="X63" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y63" t="inlineStr">
-        <is>
-          <t>4166</t>
+      <c r="Y63" t="n">
+        <v>4166</v>
+      </c>
+      <c r="Z63" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA63" t="inlineStr">
+        <is>
+          <t>4320</t>
         </is>
       </c>
     </row>
@@ -5866,9 +6248,15 @@
       <c r="X64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y64" t="inlineStr">
-        <is>
-          <t>2605</t>
+      <c r="Y64" t="n">
+        <v>2605</v>
+      </c>
+      <c r="Z64" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA64" t="inlineStr">
+        <is>
+          <t>3094</t>
         </is>
       </c>
     </row>
@@ -5951,9 +6339,15 @@
       <c r="X65" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y65" t="inlineStr">
-        <is>
-          <t>4019</t>
+      <c r="Y65" t="n">
+        <v>4019</v>
+      </c>
+      <c r="Z65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA65" t="inlineStr">
+        <is>
+          <t>4117</t>
         </is>
       </c>
     </row>
@@ -6036,9 +6430,15 @@
       <c r="X66" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="Y66" t="inlineStr">
-        <is>
-          <t>3976</t>
+      <c r="Y66" t="n">
+        <v>3976</v>
+      </c>
+      <c r="Z66" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA66" t="inlineStr">
+        <is>
+          <t>4058</t>
         </is>
       </c>
     </row>
@@ -6121,9 +6521,15 @@
       <c r="X67" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Y67" t="inlineStr">
-        <is>
-          <t>5037</t>
+      <c r="Y67" t="n">
+        <v>5037</v>
+      </c>
+      <c r="Z67" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="AA67" t="inlineStr">
+        <is>
+          <t>5262</t>
         </is>
       </c>
     </row>
@@ -6206,9 +6612,15 @@
       <c r="X68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y68" t="inlineStr">
-        <is>
-          <t>4153</t>
+      <c r="Y68" t="n">
+        <v>4153</v>
+      </c>
+      <c r="Z68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA68" t="inlineStr">
+        <is>
+          <t>4271</t>
         </is>
       </c>
     </row>
@@ -6291,9 +6703,15 @@
       <c r="X69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y69" t="inlineStr">
-        <is>
-          <t>2741</t>
+      <c r="Y69" t="n">
+        <v>2741</v>
+      </c>
+      <c r="Z69" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA69" t="inlineStr">
+        <is>
+          <t>3264</t>
         </is>
       </c>
     </row>
@@ -6376,9 +6794,15 @@
       <c r="X70" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="Y70" t="inlineStr">
-        <is>
-          <t>3727</t>
+      <c r="Y70" t="n">
+        <v>3727</v>
+      </c>
+      <c r="Z70" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA70" t="inlineStr">
+        <is>
+          <t>3776</t>
         </is>
       </c>
     </row>
@@ -6461,9 +6885,15 @@
       <c r="X71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y71" t="inlineStr">
-        <is>
-          <t>5126</t>
+      <c r="Y71" t="n">
+        <v>5126</v>
+      </c>
+      <c r="Z71" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA71" t="inlineStr">
+        <is>
+          <t>5340</t>
         </is>
       </c>
     </row>
@@ -6546,9 +6976,15 @@
       <c r="X72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y72" t="inlineStr">
-        <is>
-          <t>3573</t>
+      <c r="Y72" t="n">
+        <v>3573</v>
+      </c>
+      <c r="Z72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA72" t="inlineStr">
+        <is>
+          <t>3561</t>
         </is>
       </c>
     </row>
@@ -6631,9 +7067,15 @@
       <c r="X73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y73" t="inlineStr">
-        <is>
-          <t>4828</t>
+      <c r="Y73" t="n">
+        <v>4828</v>
+      </c>
+      <c r="Z73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA73" t="inlineStr">
+        <is>
+          <t>5019</t>
         </is>
       </c>
     </row>
@@ -6716,9 +7158,15 @@
       <c r="X74" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Y74" t="inlineStr">
-        <is>
-          <t>4560</t>
+      <c r="Y74" t="n">
+        <v>4560</v>
+      </c>
+      <c r="Z74" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA74" t="inlineStr">
+        <is>
+          <t>4592</t>
         </is>
       </c>
     </row>
@@ -6801,9 +7249,15 @@
       <c r="X75" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Y75" t="inlineStr">
-        <is>
-          <t>4706</t>
+      <c r="Y75" t="n">
+        <v>4706</v>
+      </c>
+      <c r="Z75" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA75" t="inlineStr">
+        <is>
+          <t>4750</t>
         </is>
       </c>
     </row>
@@ -6886,9 +7340,15 @@
       <c r="X76" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y76" t="inlineStr">
-        <is>
-          <t>4497</t>
+      <c r="Y76" t="n">
+        <v>4497</v>
+      </c>
+      <c r="Z76" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA76" t="inlineStr">
+        <is>
+          <t>4714</t>
         </is>
       </c>
     </row>
@@ -6962,6 +7422,8 @@
       <c r="W77" t="inlineStr"/>
       <c r="X77" s="3" t="inlineStr"/>
       <c r="Y77" t="inlineStr"/>
+      <c r="Z77" s="3" t="inlineStr"/>
+      <c r="AA77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -7042,9 +7504,15 @@
       <c r="X78" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="Y78" t="inlineStr">
-        <is>
-          <t>4400</t>
+      <c r="Y78" t="n">
+        <v>4400</v>
+      </c>
+      <c r="Z78" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA78" t="inlineStr">
+        <is>
+          <t>4493</t>
         </is>
       </c>
     </row>
@@ -7127,9 +7595,15 @@
       <c r="X79" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y79" t="inlineStr">
-        <is>
-          <t>4267</t>
+      <c r="Y79" t="n">
+        <v>4267</v>
+      </c>
+      <c r="Z79" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA79" t="inlineStr">
+        <is>
+          <t>4498</t>
         </is>
       </c>
     </row>
@@ -7212,9 +7686,15 @@
       <c r="X80" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y80" t="inlineStr">
-        <is>
-          <t>3600</t>
+      <c r="Y80" t="n">
+        <v>3600</v>
+      </c>
+      <c r="Z80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA80" t="inlineStr">
+        <is>
+          <t>3587</t>
         </is>
       </c>
     </row>
@@ -7297,9 +7777,15 @@
       <c r="X81" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y81" t="inlineStr">
-        <is>
-          <t>3196</t>
+      <c r="Y81" t="n">
+        <v>3196</v>
+      </c>
+      <c r="Z81" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA81" t="inlineStr">
+        <is>
+          <t>3487</t>
         </is>
       </c>
     </row>
@@ -7382,9 +7868,15 @@
       <c r="X82" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y82" t="inlineStr">
-        <is>
-          <t>4398</t>
+      <c r="Y82" t="n">
+        <v>4398</v>
+      </c>
+      <c r="Z82" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA82" t="inlineStr">
+        <is>
+          <t>4746</t>
         </is>
       </c>
     </row>
@@ -7467,9 +7959,15 @@
       <c r="X83" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y83" t="inlineStr">
-        <is>
-          <t>2913</t>
+      <c r="Y83" t="n">
+        <v>2913</v>
+      </c>
+      <c r="Z83" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA83" t="inlineStr">
+        <is>
+          <t>2972</t>
         </is>
       </c>
     </row>
@@ -7552,9 +8050,15 @@
       <c r="X84" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Y84" t="inlineStr">
-        <is>
-          <t>3314</t>
+      <c r="Y84" t="n">
+        <v>3314</v>
+      </c>
+      <c r="Z84" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA84" t="inlineStr">
+        <is>
+          <t>3382</t>
         </is>
       </c>
     </row>
@@ -7637,9 +8141,15 @@
       <c r="X85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y85" t="inlineStr">
-        <is>
-          <t>2116</t>
+      <c r="Y85" t="n">
+        <v>2116</v>
+      </c>
+      <c r="Z85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA85" t="inlineStr">
+        <is>
+          <t>2085</t>
         </is>
       </c>
     </row>
@@ -7722,9 +8232,15 @@
       <c r="X86" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y86" t="inlineStr">
-        <is>
-          <t>2832</t>
+      <c r="Y86" t="n">
+        <v>2832</v>
+      </c>
+      <c r="Z86" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA86" t="inlineStr">
+        <is>
+          <t>2840</t>
         </is>
       </c>
     </row>
@@ -7807,9 +8323,15 @@
       <c r="X87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y87" t="inlineStr">
-        <is>
-          <t>3084</t>
+      <c r="Y87" t="n">
+        <v>3084</v>
+      </c>
+      <c r="Z87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA87" t="inlineStr">
+        <is>
+          <t>3155</t>
         </is>
       </c>
     </row>
@@ -7892,9 +8414,15 @@
       <c r="X88" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="Y88" t="inlineStr">
-        <is>
-          <t>2436</t>
+      <c r="Y88" t="n">
+        <v>2436</v>
+      </c>
+      <c r="Z88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA88" t="inlineStr">
+        <is>
+          <t>2419</t>
         </is>
       </c>
     </row>
@@ -7956,6 +8484,8 @@
       <c r="W89" t="inlineStr"/>
       <c r="X89" s="3" t="inlineStr"/>
       <c r="Y89" t="inlineStr"/>
+      <c r="Z89" s="3" t="inlineStr"/>
+      <c r="AA89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -8015,6 +8545,8 @@
       <c r="W90" t="inlineStr"/>
       <c r="X90" s="3" t="inlineStr"/>
       <c r="Y90" t="inlineStr"/>
+      <c r="Z90" s="3" t="inlineStr"/>
+      <c r="AA90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -8095,9 +8627,15 @@
       <c r="X91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y91" t="inlineStr">
-        <is>
-          <t>2701</t>
+      <c r="Y91" t="n">
+        <v>2701</v>
+      </c>
+      <c r="Z91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA91" t="inlineStr">
+        <is>
+          <t>2698</t>
         </is>
       </c>
     </row>
@@ -8180,9 +8718,15 @@
       <c r="X92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y92" t="inlineStr">
-        <is>
-          <t>3307</t>
+      <c r="Y92" t="n">
+        <v>3307</v>
+      </c>
+      <c r="Z92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA92" t="inlineStr">
+        <is>
+          <t>3305</t>
         </is>
       </c>
     </row>
@@ -8265,9 +8809,15 @@
       <c r="X93" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="Y93" t="inlineStr">
-        <is>
-          <t>3086</t>
+      <c r="Y93" t="n">
+        <v>3086</v>
+      </c>
+      <c r="Z93" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA93" t="inlineStr">
+        <is>
+          <t>3243</t>
         </is>
       </c>
     </row>
@@ -8350,9 +8900,15 @@
       <c r="X94" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y94" t="inlineStr">
-        <is>
-          <t>4235</t>
+      <c r="Y94" t="n">
+        <v>4235</v>
+      </c>
+      <c r="Z94" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA94" t="inlineStr">
+        <is>
+          <t>4379</t>
         </is>
       </c>
     </row>
@@ -8435,9 +8991,15 @@
       <c r="X95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y95" t="inlineStr">
-        <is>
-          <t>3932</t>
+      <c r="Y95" t="n">
+        <v>3932</v>
+      </c>
+      <c r="Z95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA95" t="inlineStr">
+        <is>
+          <t>4017</t>
         </is>
       </c>
     </row>
@@ -8520,9 +9082,15 @@
       <c r="X96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y96" t="inlineStr">
-        <is>
-          <t>3649</t>
+      <c r="Y96" t="n">
+        <v>3649</v>
+      </c>
+      <c r="Z96" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA96" t="inlineStr">
+        <is>
+          <t>3853</t>
         </is>
       </c>
     </row>
@@ -8605,9 +9173,15 @@
       <c r="X97" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="Y97" t="inlineStr">
-        <is>
-          <t>4288</t>
+      <c r="Y97" t="n">
+        <v>4288</v>
+      </c>
+      <c r="Z97" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA97" t="inlineStr">
+        <is>
+          <t>4451</t>
         </is>
       </c>
     </row>
@@ -8690,9 +9264,15 @@
       <c r="X98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y98" t="inlineStr">
-        <is>
-          <t>3430</t>
+      <c r="Y98" t="n">
+        <v>3430</v>
+      </c>
+      <c r="Z98" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA98" t="inlineStr">
+        <is>
+          <t>3795</t>
         </is>
       </c>
     </row>
@@ -8775,9 +9355,15 @@
       <c r="X99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y99" t="inlineStr">
-        <is>
-          <t>2855</t>
+      <c r="Y99" t="n">
+        <v>2855</v>
+      </c>
+      <c r="Z99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA99" t="inlineStr">
+        <is>
+          <t>2829</t>
         </is>
       </c>
     </row>
@@ -8860,9 +9446,15 @@
       <c r="X100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y100" t="inlineStr">
-        <is>
-          <t>2628</t>
+      <c r="Y100" t="n">
+        <v>2628</v>
+      </c>
+      <c r="Z100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA100" t="inlineStr">
+        <is>
+          <t>2623</t>
         </is>
       </c>
     </row>
@@ -8945,9 +9537,15 @@
       <c r="X101" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y101" t="inlineStr">
-        <is>
-          <t>4377</t>
+      <c r="Y101" t="n">
+        <v>4377</v>
+      </c>
+      <c r="Z101" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA101" t="inlineStr">
+        <is>
+          <t>4510</t>
         </is>
       </c>
     </row>
@@ -9030,9 +9628,15 @@
       <c r="X102" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="Y102" t="inlineStr">
-        <is>
-          <t>3831</t>
+      <c r="Y102" t="n">
+        <v>3831</v>
+      </c>
+      <c r="Z102" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA102" t="inlineStr">
+        <is>
+          <t>3905</t>
         </is>
       </c>
     </row>
@@ -9115,9 +9719,15 @@
       <c r="X103" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y103" t="inlineStr">
-        <is>
-          <t>3433</t>
+      <c r="Y103" t="n">
+        <v>3433</v>
+      </c>
+      <c r="Z103" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA103" t="inlineStr">
+        <is>
+          <t>3522</t>
         </is>
       </c>
     </row>
@@ -9200,9 +9810,15 @@
       <c r="X104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y104" t="inlineStr">
-        <is>
-          <t>2578</t>
+      <c r="Y104" t="n">
+        <v>2578</v>
+      </c>
+      <c r="Z104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA104" t="inlineStr">
+        <is>
+          <t>2606</t>
         </is>
       </c>
     </row>
@@ -9285,9 +9901,15 @@
       <c r="X105" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y105" t="inlineStr">
-        <is>
-          <t>3704</t>
+      <c r="Y105" t="n">
+        <v>3704</v>
+      </c>
+      <c r="Z105" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA105" t="inlineStr">
+        <is>
+          <t>3935</t>
         </is>
       </c>
     </row>
@@ -9370,9 +9992,15 @@
       <c r="X106" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Y106" t="inlineStr">
-        <is>
-          <t>3315</t>
+      <c r="Y106" t="n">
+        <v>3315</v>
+      </c>
+      <c r="Z106" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA106" t="inlineStr">
+        <is>
+          <t>3504</t>
         </is>
       </c>
     </row>
@@ -9455,9 +10083,15 @@
       <c r="X107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y107" t="inlineStr">
-        <is>
-          <t>3603</t>
+      <c r="Y107" t="n">
+        <v>3603</v>
+      </c>
+      <c r="Z107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA107" t="inlineStr">
+        <is>
+          <t>3680</t>
         </is>
       </c>
     </row>
@@ -9540,9 +10174,15 @@
       <c r="X108" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="Y108" t="inlineStr">
-        <is>
-          <t>2754</t>
+      <c r="Y108" t="n">
+        <v>2754</v>
+      </c>
+      <c r="Z108" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA108" t="inlineStr">
+        <is>
+          <t>2751</t>
         </is>
       </c>
     </row>
@@ -9625,9 +10265,15 @@
       <c r="X109" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Y109" t="inlineStr">
-        <is>
-          <t>2767</t>
+      <c r="Y109" t="n">
+        <v>2767</v>
+      </c>
+      <c r="Z109" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA109" t="inlineStr">
+        <is>
+          <t>2819</t>
         </is>
       </c>
     </row>
@@ -9710,9 +10356,15 @@
       <c r="X110" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="Y110" t="inlineStr">
-        <is>
-          <t>3346</t>
+      <c r="Y110" t="n">
+        <v>3346</v>
+      </c>
+      <c r="Z110" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA110" t="inlineStr">
+        <is>
+          <t>3505</t>
         </is>
       </c>
     </row>
@@ -9795,9 +10447,15 @@
       <c r="X111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y111" t="inlineStr">
-        <is>
-          <t>3004</t>
+      <c r="Y111" t="n">
+        <v>3004</v>
+      </c>
+      <c r="Z111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA111" t="inlineStr">
+        <is>
+          <t>3100</t>
         </is>
       </c>
     </row>
@@ -9880,9 +10538,15 @@
       <c r="X112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y112" t="inlineStr">
-        <is>
-          <t>3473</t>
+      <c r="Y112" t="n">
+        <v>3473</v>
+      </c>
+      <c r="Z112" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA112" t="inlineStr">
+        <is>
+          <t>3520</t>
         </is>
       </c>
     </row>
@@ -9965,9 +10629,15 @@
       <c r="X113" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y113" t="inlineStr">
-        <is>
-          <t>2702</t>
+      <c r="Y113" t="n">
+        <v>2702</v>
+      </c>
+      <c r="Z113" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA113" t="inlineStr">
+        <is>
+          <t>2870</t>
         </is>
       </c>
     </row>
@@ -10050,9 +10720,15 @@
       <c r="X114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y114" t="inlineStr">
-        <is>
-          <t>3635</t>
+      <c r="Y114" t="n">
+        <v>3635</v>
+      </c>
+      <c r="Z114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA114" t="inlineStr">
+        <is>
+          <t>3690</t>
         </is>
       </c>
     </row>
@@ -10135,9 +10811,15 @@
       <c r="X115" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y115" t="inlineStr">
-        <is>
-          <t>2689</t>
+      <c r="Y115" t="n">
+        <v>2689</v>
+      </c>
+      <c r="Z115" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA115" t="inlineStr">
+        <is>
+          <t>2666</t>
         </is>
       </c>
     </row>
@@ -10220,9 +10902,15 @@
       <c r="X116" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y116" t="inlineStr">
-        <is>
-          <t>3193</t>
+      <c r="Y116" t="n">
+        <v>3193</v>
+      </c>
+      <c r="Z116" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA116" t="inlineStr">
+        <is>
+          <t>3272</t>
         </is>
       </c>
     </row>
@@ -10305,9 +10993,15 @@
       <c r="X117" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y117" t="inlineStr">
-        <is>
-          <t>3169</t>
+      <c r="Y117" t="n">
+        <v>3169</v>
+      </c>
+      <c r="Z117" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="AA117" t="inlineStr">
+        <is>
+          <t>3261</t>
         </is>
       </c>
     </row>
@@ -10381,6 +11075,8 @@
       <c r="W118" t="inlineStr"/>
       <c r="X118" s="3" t="inlineStr"/>
       <c r="Y118" t="inlineStr"/>
+      <c r="Z118" s="3" t="inlineStr"/>
+      <c r="AA118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -10461,9 +11157,15 @@
       <c r="X119" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y119" t="inlineStr">
-        <is>
-          <t>3472</t>
+      <c r="Y119" t="n">
+        <v>3472</v>
+      </c>
+      <c r="Z119" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA119" t="inlineStr">
+        <is>
+          <t>3596</t>
         </is>
       </c>
     </row>
@@ -10546,9 +11248,15 @@
       <c r="X120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y120" t="inlineStr">
-        <is>
-          <t>3186</t>
+      <c r="Y120" t="n">
+        <v>3186</v>
+      </c>
+      <c r="Z120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA120" t="inlineStr">
+        <is>
+          <t>3258</t>
         </is>
       </c>
     </row>
@@ -10631,9 +11339,15 @@
       <c r="X121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y121" t="inlineStr">
-        <is>
-          <t>2162</t>
+      <c r="Y121" t="n">
+        <v>2162</v>
+      </c>
+      <c r="Z121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA121" t="inlineStr">
+        <is>
+          <t>2161</t>
         </is>
       </c>
     </row>
@@ -10716,9 +11430,15 @@
       <c r="X122" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="Y122" t="inlineStr">
-        <is>
-          <t>2578</t>
+      <c r="Y122" t="n">
+        <v>2578</v>
+      </c>
+      <c r="Z122" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA122" t="inlineStr">
+        <is>
+          <t>2641</t>
         </is>
       </c>
     </row>
@@ -10801,9 +11521,15 @@
       <c r="X123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y123" t="inlineStr">
-        <is>
-          <t>2684</t>
+      <c r="Y123" t="n">
+        <v>2684</v>
+      </c>
+      <c r="Z123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA123" t="inlineStr">
+        <is>
+          <t>2723</t>
         </is>
       </c>
     </row>
@@ -10886,9 +11612,15 @@
       <c r="X124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y124" t="inlineStr">
-        <is>
-          <t>3535</t>
+      <c r="Y124" t="n">
+        <v>3535</v>
+      </c>
+      <c r="Z124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA124" t="inlineStr">
+        <is>
+          <t>3677</t>
         </is>
       </c>
     </row>
@@ -10971,7 +11703,13 @@
       <c r="X125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y125" t="inlineStr">
+      <c r="Y125" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11056,9 +11794,15 @@
       <c r="X126" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="Y126" t="inlineStr">
-        <is>
-          <t>3008</t>
+      <c r="Y126" t="n">
+        <v>3008</v>
+      </c>
+      <c r="Z126" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA126" t="inlineStr">
+        <is>
+          <t>3106</t>
         </is>
       </c>
     </row>
@@ -11141,9 +11885,15 @@
       <c r="X127" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y127" t="inlineStr">
-        <is>
-          <t>2801</t>
+      <c r="Y127" t="n">
+        <v>2801</v>
+      </c>
+      <c r="Z127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA127" t="inlineStr">
+        <is>
+          <t>2758</t>
         </is>
       </c>
     </row>
@@ -11226,9 +11976,15 @@
       <c r="X128" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Y128" t="inlineStr">
-        <is>
-          <t>2692</t>
+      <c r="Y128" t="n">
+        <v>2692</v>
+      </c>
+      <c r="Z128" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA128" t="inlineStr">
+        <is>
+          <t>2681</t>
         </is>
       </c>
     </row>
@@ -11311,9 +12067,15 @@
       <c r="X129" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="Y129" t="inlineStr">
-        <is>
-          <t>2570</t>
+      <c r="Y129" t="n">
+        <v>2570</v>
+      </c>
+      <c r="Z129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA129" t="inlineStr">
+        <is>
+          <t>2542</t>
         </is>
       </c>
     </row>
@@ -11396,9 +12158,15 @@
       <c r="X130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y130" t="inlineStr">
-        <is>
-          <t>1927</t>
+      <c r="Y130" t="n">
+        <v>1927</v>
+      </c>
+      <c r="Z130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA130" t="inlineStr">
+        <is>
+          <t>1912</t>
         </is>
       </c>
     </row>
@@ -11481,7 +12249,13 @@
       <c r="X131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y131" t="inlineStr">
+      <c r="Y131" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11566,9 +12340,15 @@
       <c r="X132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y132" t="inlineStr">
-        <is>
-          <t>1508</t>
+      <c r="Y132" t="n">
+        <v>1508</v>
+      </c>
+      <c r="Z132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA132" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -11642,6 +12422,8 @@
       <c r="W133" t="inlineStr"/>
       <c r="X133" s="3" t="inlineStr"/>
       <c r="Y133" t="inlineStr"/>
+      <c r="Z133" s="3" t="inlineStr"/>
+      <c r="AA133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -11722,9 +12504,15 @@
       <c r="X134" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Y134" t="inlineStr">
-        <is>
-          <t>2041</t>
+      <c r="Y134" t="n">
+        <v>2041</v>
+      </c>
+      <c r="Z134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA134" t="inlineStr">
+        <is>
+          <t>2063</t>
         </is>
       </c>
     </row>
@@ -11807,9 +12595,15 @@
       <c r="X135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y135" t="inlineStr">
-        <is>
-          <t>2208</t>
+      <c r="Y135" t="n">
+        <v>2208</v>
+      </c>
+      <c r="Z135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA135" t="inlineStr">
+        <is>
+          <t>2198</t>
         </is>
       </c>
     </row>
@@ -11892,9 +12686,15 @@
       <c r="X136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y136" t="inlineStr">
-        <is>
-          <t>1518</t>
+      <c r="Y136" t="n">
+        <v>1518</v>
+      </c>
+      <c r="Z136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA136" t="inlineStr">
+        <is>
+          <t>1517</t>
         </is>
       </c>
     </row>
@@ -11968,6 +12768,8 @@
       <c r="W137" t="inlineStr"/>
       <c r="X137" s="3" t="inlineStr"/>
       <c r="Y137" t="inlineStr"/>
+      <c r="Z137" s="3" t="inlineStr"/>
+      <c r="AA137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -12048,7 +12850,13 @@
       <c r="X138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y138" t="inlineStr">
+      <c r="Y138" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12124,6 +12932,8 @@
       <c r="W139" t="inlineStr"/>
       <c r="X139" s="3" t="inlineStr"/>
       <c r="Y139" t="inlineStr"/>
+      <c r="Z139" s="3" t="inlineStr"/>
+      <c r="AA139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -12204,9 +13014,15 @@
       <c r="X140" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y140" t="inlineStr">
-        <is>
-          <t>4802</t>
+      <c r="Y140" t="n">
+        <v>4802</v>
+      </c>
+      <c r="Z140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA140" t="inlineStr">
+        <is>
+          <t>4804</t>
         </is>
       </c>
     </row>
@@ -12289,7 +13105,13 @@
       <c r="X141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y141" t="inlineStr">
+      <c r="Y141" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12374,7 +13196,13 @@
       <c r="X142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y142" t="inlineStr">
+      <c r="Y142" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12459,9 +13287,15 @@
       <c r="X143" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y143" t="inlineStr">
-        <is>
-          <t>5149</t>
+      <c r="Y143" t="n">
+        <v>5149</v>
+      </c>
+      <c r="Z143" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA143" t="inlineStr">
+        <is>
+          <t>5437</t>
         </is>
       </c>
     </row>
@@ -12544,7 +13378,13 @@
       <c r="X144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y144" t="inlineStr">
+      <c r="Y144" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12629,9 +13469,15 @@
       <c r="X145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y145" t="inlineStr">
-        <is>
-          <t>2746</t>
+      <c r="Y145" t="n">
+        <v>2746</v>
+      </c>
+      <c r="Z145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA145" t="inlineStr">
+        <is>
+          <t>2745</t>
         </is>
       </c>
     </row>
@@ -12714,7 +13560,13 @@
       <c r="X146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y146" t="inlineStr">
+      <c r="Y146" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12799,9 +13651,15 @@
       <c r="X147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y147" t="inlineStr">
-        <is>
-          <t>2825</t>
+      <c r="Y147" t="n">
+        <v>2825</v>
+      </c>
+      <c r="Z147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA147" t="inlineStr">
+        <is>
+          <t>2871</t>
         </is>
       </c>
     </row>
@@ -12862,9 +13720,15 @@
       <c r="X148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y148" t="inlineStr">
-        <is>
-          <t>2887</t>
+      <c r="Y148" t="n">
+        <v>2887</v>
+      </c>
+      <c r="Z148" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA148" t="inlineStr">
+        <is>
+          <t>3052</t>
         </is>
       </c>
     </row>
@@ -12941,7 +13805,13 @@
       <c r="X149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y149" t="inlineStr">
+      <c r="Y149" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13020,7 +13890,13 @@
       <c r="X150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y150" t="inlineStr">
+      <c r="Y150" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13087,9 +13963,15 @@
       <c r="X151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y151" t="inlineStr">
-        <is>
-          <t>2267</t>
+      <c r="Y151" t="n">
+        <v>2267</v>
+      </c>
+      <c r="Z151" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA151" t="inlineStr">
+        <is>
+          <t>2485</t>
         </is>
       </c>
     </row>
@@ -13154,7 +14036,13 @@
       <c r="X152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y152" t="inlineStr">
+      <c r="Y152" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13213,9 +14101,15 @@
       <c r="X153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y153" t="inlineStr">
-        <is>
-          <t>3769</t>
+      <c r="Y153" t="n">
+        <v>3769</v>
+      </c>
+      <c r="Z153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA153" t="inlineStr">
+        <is>
+          <t>3761</t>
         </is>
       </c>
     </row>
@@ -13272,9 +14166,15 @@
       <c r="X154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y154" t="inlineStr">
-        <is>
-          <t>1658</t>
+      <c r="Y154" t="n">
+        <v>1658</v>
+      </c>
+      <c r="Z154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA154" t="inlineStr">
+        <is>
+          <t>1654</t>
         </is>
       </c>
     </row>
@@ -13327,9 +14227,15 @@
       <c r="X155" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="Y155" t="inlineStr">
-        <is>
-          <t>1555</t>
+      <c r="Y155" t="n">
+        <v>1555</v>
+      </c>
+      <c r="Z155" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA155" t="inlineStr">
+        <is>
+          <t>1692</t>
         </is>
       </c>
     </row>
@@ -13378,9 +14284,15 @@
       <c r="X156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y156" t="inlineStr">
-        <is>
-          <t>3476</t>
+      <c r="Y156" t="n">
+        <v>3476</v>
+      </c>
+      <c r="Z156" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA156" t="inlineStr">
+        <is>
+          <t>3497</t>
         </is>
       </c>
     </row>
@@ -13429,11 +14341,11 @@
       <c r="X157" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Y157" t="inlineStr">
-        <is>
-          <t>6264</t>
-        </is>
-      </c>
+      <c r="Y157" t="n">
+        <v>6264</v>
+      </c>
+      <c r="Z157" s="3" t="inlineStr"/>
+      <c r="AA157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -13475,6 +14387,8 @@
       <c r="W158" t="inlineStr"/>
       <c r="X158" s="3" t="inlineStr"/>
       <c r="Y158" t="inlineStr"/>
+      <c r="Z158" s="3" t="inlineStr"/>
+      <c r="AA158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -13517,9 +14431,15 @@
       <c r="X159" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y159" t="inlineStr">
-        <is>
-          <t>5042</t>
+      <c r="Y159" t="n">
+        <v>5042</v>
+      </c>
+      <c r="Z159" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA159" t="inlineStr">
+        <is>
+          <t>5297</t>
         </is>
       </c>
     </row>
@@ -13564,9 +14484,15 @@
       <c r="X160" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Y160" t="inlineStr">
-        <is>
-          <t>2648</t>
+      <c r="Y160" t="n">
+        <v>2648</v>
+      </c>
+      <c r="Z160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA160" t="inlineStr">
+        <is>
+          <t>2591</t>
         </is>
       </c>
     </row>
@@ -13611,9 +14537,15 @@
       <c r="X161" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="Y161" t="inlineStr">
-        <is>
-          <t>1885</t>
+      <c r="Y161" t="n">
+        <v>1885</v>
+      </c>
+      <c r="Z161" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA161" t="inlineStr">
+        <is>
+          <t>1906</t>
         </is>
       </c>
     </row>
@@ -13658,9 +14590,15 @@
       <c r="X162" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y162" t="inlineStr">
-        <is>
-          <t>1650</t>
+      <c r="Y162" t="n">
+        <v>1650</v>
+      </c>
+      <c r="Z162" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA162" t="inlineStr">
+        <is>
+          <t>1822</t>
         </is>
       </c>
     </row>
@@ -13701,9 +14639,156 @@
       <c r="X163" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Y163" t="inlineStr">
-        <is>
-          <t>1654</t>
+      <c r="Y163" t="n">
+        <v>1654</v>
+      </c>
+      <c r="Z163" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA163" t="inlineStr">
+        <is>
+          <t>1657</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>6510348</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Bonpoisson</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr"/>
+      <c r="D164" t="inlineStr"/>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F164" s="3" t="inlineStr"/>
+      <c r="G164" t="inlineStr"/>
+      <c r="H164" s="3" t="inlineStr"/>
+      <c r="I164" t="inlineStr"/>
+      <c r="J164" s="3" t="inlineStr"/>
+      <c r="K164" t="inlineStr"/>
+      <c r="L164" s="3" t="inlineStr"/>
+      <c r="M164" t="inlineStr"/>
+      <c r="N164" s="3" t="inlineStr"/>
+      <c r="O164" t="inlineStr"/>
+      <c r="P164" s="3" t="inlineStr"/>
+      <c r="Q164" t="inlineStr"/>
+      <c r="R164" s="3" t="inlineStr"/>
+      <c r="S164" t="inlineStr"/>
+      <c r="T164" s="3" t="inlineStr"/>
+      <c r="U164" t="inlineStr"/>
+      <c r="V164" s="3" t="inlineStr"/>
+      <c r="W164" t="inlineStr"/>
+      <c r="X164" s="3" t="inlineStr"/>
+      <c r="Y164" t="inlineStr"/>
+      <c r="Z164" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA164" t="inlineStr">
+        <is>
+          <t>5048</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>41463618</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>qi ye</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F165" s="3" t="inlineStr"/>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" s="3" t="inlineStr"/>
+      <c r="I165" t="inlineStr"/>
+      <c r="J165" s="3" t="inlineStr"/>
+      <c r="K165" t="inlineStr"/>
+      <c r="L165" s="3" t="inlineStr"/>
+      <c r="M165" t="inlineStr"/>
+      <c r="N165" s="3" t="inlineStr"/>
+      <c r="O165" t="inlineStr"/>
+      <c r="P165" s="3" t="inlineStr"/>
+      <c r="Q165" t="inlineStr"/>
+      <c r="R165" s="3" t="inlineStr"/>
+      <c r="S165" t="inlineStr"/>
+      <c r="T165" s="3" t="inlineStr"/>
+      <c r="U165" t="inlineStr"/>
+      <c r="V165" s="3" t="inlineStr"/>
+      <c r="W165" t="inlineStr"/>
+      <c r="X165" s="3" t="inlineStr"/>
+      <c r="Y165" t="inlineStr"/>
+      <c r="Z165" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA165" t="inlineStr">
+        <is>
+          <t>2608</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>58494374</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Kirinfire</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F166" s="3" t="inlineStr"/>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" s="3" t="inlineStr"/>
+      <c r="I166" t="inlineStr"/>
+      <c r="J166" s="3" t="inlineStr"/>
+      <c r="K166" t="inlineStr"/>
+      <c r="L166" s="3" t="inlineStr"/>
+      <c r="M166" t="inlineStr"/>
+      <c r="N166" s="3" t="inlineStr"/>
+      <c r="O166" t="inlineStr"/>
+      <c r="P166" s="3" t="inlineStr"/>
+      <c r="Q166" t="inlineStr"/>
+      <c r="R166" s="3" t="inlineStr"/>
+      <c r="S166" t="inlineStr"/>
+      <c r="T166" s="3" t="inlineStr"/>
+      <c r="U166" t="inlineStr"/>
+      <c r="V166" s="3" t="inlineStr"/>
+      <c r="W166" t="inlineStr"/>
+      <c r="X166" s="3" t="inlineStr"/>
+      <c r="Y166" t="inlineStr"/>
+      <c r="Z166" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA166" t="inlineStr">
+        <is>
+          <t>1242</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-13 11:30:34
</commit_message>
<xml_diff>
--- a/Season_Attack/81.xlsx
+++ b/Season_Attack/81.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA166"/>
+  <dimension ref="A1:AC170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,6 +526,16 @@
           <t>01-11_0</t>
         </is>
       </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>01-12_A</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>01-12_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -612,9 +622,15 @@
       <c r="Z2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>4241</t>
+      <c r="AA2" t="n">
+        <v>4241</v>
+      </c>
+      <c r="AB2" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>4556</t>
         </is>
       </c>
     </row>
@@ -703,9 +719,15 @@
       <c r="Z3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>5004</t>
+      <c r="AA3" t="n">
+        <v>5004</v>
+      </c>
+      <c r="AB3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>5312</t>
         </is>
       </c>
     </row>
@@ -794,9 +816,15 @@
       <c r="Z4" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>5606</t>
+      <c r="AA4" t="n">
+        <v>5606</v>
+      </c>
+      <c r="AB4" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>5829</t>
         </is>
       </c>
     </row>
@@ -819,7 +847,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F5" s="3" t="n">
@@ -885,9 +913,15 @@
       <c r="Z5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>5933</t>
+      <c r="AA5" t="n">
+        <v>5933</v>
+      </c>
+      <c r="AB5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>6203</t>
         </is>
       </c>
     </row>
@@ -910,7 +944,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F6" s="3" t="n">
@@ -976,9 +1010,15 @@
       <c r="Z6" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>5800</t>
+      <c r="AA6" t="n">
+        <v>5800</v>
+      </c>
+      <c r="AB6" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>5924</t>
         </is>
       </c>
     </row>
@@ -1067,9 +1107,15 @@
       <c r="Z7" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>5985</t>
+      <c r="AA7" t="n">
+        <v>5985</v>
+      </c>
+      <c r="AB7" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>6229</t>
         </is>
       </c>
     </row>
@@ -1158,9 +1204,15 @@
       <c r="Z8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>5176</t>
+      <c r="AA8" t="n">
+        <v>5176</v>
+      </c>
+      <c r="AB8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>5315</t>
         </is>
       </c>
     </row>
@@ -1249,9 +1301,15 @@
       <c r="Z9" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>5256</t>
+      <c r="AA9" t="n">
+        <v>5256</v>
+      </c>
+      <c r="AB9" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>5419</t>
         </is>
       </c>
     </row>
@@ -1274,7 +1332,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F10" s="3" t="n">
@@ -1340,9 +1398,15 @@
       <c r="Z10" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="AA10" t="inlineStr">
-        <is>
-          <t>4582</t>
+      <c r="AA10" t="n">
+        <v>4582</v>
+      </c>
+      <c r="AB10" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>5272</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1429,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F11" s="3" t="n">
@@ -1431,9 +1495,15 @@
       <c r="Z11" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="AA11" t="inlineStr">
-        <is>
-          <t>6172</t>
+      <c r="AA11" t="n">
+        <v>6172</v>
+      </c>
+      <c r="AB11" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>6774</t>
         </is>
       </c>
     </row>
@@ -1456,7 +1526,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F12" s="3" t="n">
@@ -1522,9 +1592,15 @@
       <c r="Z12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA12" t="inlineStr">
-        <is>
-          <t>5460</t>
+      <c r="AA12" t="n">
+        <v>5460</v>
+      </c>
+      <c r="AB12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>5732</t>
         </is>
       </c>
     </row>
@@ -1613,7 +1689,13 @@
       <c r="Z13" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="AA13" t="inlineStr">
+      <c r="AA13" t="n">
+        <v>2927</v>
+      </c>
+      <c r="AB13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="inlineStr">
         <is>
           <t>2927</t>
         </is>
@@ -1704,9 +1786,15 @@
       <c r="Z14" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="AA14" t="inlineStr">
-        <is>
-          <t>6408</t>
+      <c r="AA14" t="n">
+        <v>6408</v>
+      </c>
+      <c r="AB14" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>6736</t>
         </is>
       </c>
     </row>
@@ -1795,9 +1883,15 @@
       <c r="Z15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA15" t="inlineStr">
-        <is>
-          <t>5481</t>
+      <c r="AA15" t="n">
+        <v>5481</v>
+      </c>
+      <c r="AB15" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>5614</t>
         </is>
       </c>
     </row>
@@ -1886,9 +1980,15 @@
       <c r="Z16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA16" t="inlineStr">
-        <is>
-          <t>5913</t>
+      <c r="AA16" t="n">
+        <v>5913</v>
+      </c>
+      <c r="AB16" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>6195</t>
         </is>
       </c>
     </row>
@@ -1977,9 +2077,15 @@
       <c r="Z17" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="AA17" t="inlineStr">
-        <is>
-          <t>5123</t>
+      <c r="AA17" t="n">
+        <v>5123</v>
+      </c>
+      <c r="AB17" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>5318</t>
         </is>
       </c>
     </row>
@@ -2002,7 +2108,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F18" s="3" t="n">
@@ -2068,9 +2174,15 @@
       <c r="Z18" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AA18" t="inlineStr">
-        <is>
-          <t>5177</t>
+      <c r="AA18" t="n">
+        <v>5177</v>
+      </c>
+      <c r="AB18" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>5313</t>
         </is>
       </c>
     </row>
@@ -2159,9 +2271,15 @@
       <c r="Z19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA19" t="inlineStr">
-        <is>
-          <t>5775</t>
+      <c r="AA19" t="n">
+        <v>5775</v>
+      </c>
+      <c r="AB19" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>5925</t>
         </is>
       </c>
     </row>
@@ -2250,9 +2368,15 @@
       <c r="Z20" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="AA20" t="inlineStr">
-        <is>
-          <t>6197</t>
+      <c r="AA20" t="n">
+        <v>6197</v>
+      </c>
+      <c r="AB20" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>6580</t>
         </is>
       </c>
     </row>
@@ -2341,9 +2465,15 @@
       <c r="Z21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA21" t="inlineStr">
-        <is>
-          <t>5076</t>
+      <c r="AA21" t="n">
+        <v>5076</v>
+      </c>
+      <c r="AB21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>5370</t>
         </is>
       </c>
     </row>
@@ -2432,9 +2562,15 @@
       <c r="Z22" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="AA22" t="inlineStr">
-        <is>
-          <t>5752</t>
+      <c r="AA22" t="n">
+        <v>5752</v>
+      </c>
+      <c r="AB22" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>6077</t>
         </is>
       </c>
     </row>
@@ -2457,7 +2593,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F23" s="4" t="n">
@@ -2523,9 +2659,15 @@
       <c r="Z23" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="AA23" t="inlineStr">
-        <is>
-          <t>5468</t>
+      <c r="AA23" t="n">
+        <v>5468</v>
+      </c>
+      <c r="AB23" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>5549</t>
         </is>
       </c>
     </row>
@@ -2614,9 +2756,15 @@
       <c r="Z24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AA24" t="inlineStr">
-        <is>
-          <t>5098</t>
+      <c r="AA24" t="n">
+        <v>5098</v>
+      </c>
+      <c r="AB24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC24" t="inlineStr">
+        <is>
+          <t>5342</t>
         </is>
       </c>
     </row>
@@ -2705,7 +2853,13 @@
       <c r="Z25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA25" t="inlineStr">
+      <c r="AA25" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AB25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC25" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2796,9 +2950,15 @@
       <c r="Z26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="AA26" t="inlineStr">
-        <is>
-          <t>5659</t>
+      <c r="AA26" t="n">
+        <v>5659</v>
+      </c>
+      <c r="AB26" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="AC26" t="inlineStr">
+        <is>
+          <t>5770</t>
         </is>
       </c>
     </row>
@@ -2887,9 +3047,15 @@
       <c r="Z27" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="AA27" t="inlineStr">
-        <is>
-          <t>6052</t>
+      <c r="AA27" t="n">
+        <v>6052</v>
+      </c>
+      <c r="AB27" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC27" t="inlineStr">
+        <is>
+          <t>5848</t>
         </is>
       </c>
     </row>
@@ -2978,9 +3144,15 @@
       <c r="Z28" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="AA28" t="inlineStr">
-        <is>
-          <t>4399</t>
+      <c r="AA28" t="n">
+        <v>4399</v>
+      </c>
+      <c r="AB28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC28" t="inlineStr">
+        <is>
+          <t>4440</t>
         </is>
       </c>
     </row>
@@ -3069,9 +3241,15 @@
       <c r="Z29" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AA29" t="inlineStr">
-        <is>
-          <t>5164</t>
+      <c r="AA29" t="n">
+        <v>5164</v>
+      </c>
+      <c r="AB29" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC29" t="inlineStr">
+        <is>
+          <t>5625</t>
         </is>
       </c>
     </row>
@@ -3160,9 +3338,15 @@
       <c r="Z30" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="AA30" t="inlineStr">
-        <is>
-          <t>6014</t>
+      <c r="AA30" t="n">
+        <v>6014</v>
+      </c>
+      <c r="AB30" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC30" t="inlineStr">
+        <is>
+          <t>6383</t>
         </is>
       </c>
     </row>
@@ -3251,9 +3435,15 @@
       <c r="Z31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AA31" t="inlineStr">
-        <is>
-          <t>5630</t>
+      <c r="AA31" t="n">
+        <v>5630</v>
+      </c>
+      <c r="AB31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC31" t="inlineStr">
+        <is>
+          <t>5935</t>
         </is>
       </c>
     </row>
@@ -3342,9 +3532,15 @@
       <c r="Z32" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AA32" t="inlineStr">
-        <is>
-          <t>5969</t>
+      <c r="AA32" t="n">
+        <v>5969</v>
+      </c>
+      <c r="AB32" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC32" t="inlineStr">
+        <is>
+          <t>6135</t>
         </is>
       </c>
     </row>
@@ -3433,9 +3629,15 @@
       <c r="Z33" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="AA33" t="inlineStr">
-        <is>
-          <t>6311</t>
+      <c r="AA33" t="n">
+        <v>6311</v>
+      </c>
+      <c r="AB33" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC33" t="inlineStr">
+        <is>
+          <t>6461</t>
         </is>
       </c>
     </row>
@@ -3524,9 +3726,15 @@
       <c r="Z34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA34" t="inlineStr">
-        <is>
-          <t>3476</t>
+      <c r="AA34" t="n">
+        <v>3476</v>
+      </c>
+      <c r="AB34" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC34" t="inlineStr">
+        <is>
+          <t>3632</t>
         </is>
       </c>
     </row>
@@ -3549,7 +3757,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F35" s="3" t="n">
@@ -3615,9 +3823,15 @@
       <c r="Z35" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="AA35" t="inlineStr">
-        <is>
-          <t>6028</t>
+      <c r="AA35" t="n">
+        <v>6028</v>
+      </c>
+      <c r="AB35" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="AC35" t="inlineStr">
+        <is>
+          <t>6238</t>
         </is>
       </c>
     </row>
@@ -3706,9 +3920,15 @@
       <c r="Z36" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AA36" t="inlineStr">
-        <is>
-          <t>5141</t>
+      <c r="AA36" t="n">
+        <v>5141</v>
+      </c>
+      <c r="AB36" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC36" t="inlineStr">
+        <is>
+          <t>5354</t>
         </is>
       </c>
     </row>
@@ -3797,9 +4017,15 @@
       <c r="Z37" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AA37" t="inlineStr">
-        <is>
-          <t>4749</t>
+      <c r="AA37" t="n">
+        <v>4749</v>
+      </c>
+      <c r="AB37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC37" t="inlineStr">
+        <is>
+          <t>4946</t>
         </is>
       </c>
     </row>
@@ -3888,9 +4114,15 @@
       <c r="Z38" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="AA38" t="inlineStr">
-        <is>
-          <t>5475</t>
+      <c r="AA38" t="n">
+        <v>5475</v>
+      </c>
+      <c r="AB38" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC38" t="inlineStr">
+        <is>
+          <t>5687</t>
         </is>
       </c>
     </row>
@@ -3979,9 +4211,15 @@
       <c r="Z39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="AA39" t="inlineStr">
-        <is>
-          <t>5216</t>
+      <c r="AA39" t="n">
+        <v>5216</v>
+      </c>
+      <c r="AB39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="AC39" t="inlineStr">
+        <is>
+          <t>5356</t>
         </is>
       </c>
     </row>
@@ -4004,7 +4242,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F40" s="3" t="n">
@@ -4070,9 +4308,15 @@
       <c r="Z40" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="AA40" t="inlineStr">
-        <is>
-          <t>6227</t>
+      <c r="AA40" t="n">
+        <v>6227</v>
+      </c>
+      <c r="AB40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC40" t="inlineStr">
+        <is>
+          <t>6579</t>
         </is>
       </c>
     </row>
@@ -4161,9 +4405,15 @@
       <c r="Z41" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA41" t="inlineStr">
-        <is>
-          <t>5599</t>
+      <c r="AA41" t="n">
+        <v>5599</v>
+      </c>
+      <c r="AB41" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC41" t="inlineStr">
+        <is>
+          <t>5816</t>
         </is>
       </c>
     </row>
@@ -4252,9 +4502,15 @@
       <c r="Z42" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="AA42" t="inlineStr">
-        <is>
-          <t>6263</t>
+      <c r="AA42" t="n">
+        <v>6263</v>
+      </c>
+      <c r="AB42" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC42" t="inlineStr">
+        <is>
+          <t>6536</t>
         </is>
       </c>
     </row>
@@ -4343,9 +4599,15 @@
       <c r="Z43" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="AA43" t="inlineStr">
-        <is>
-          <t>5481</t>
+      <c r="AA43" t="n">
+        <v>5481</v>
+      </c>
+      <c r="AB43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC43" t="inlineStr">
+        <is>
+          <t>5718</t>
         </is>
       </c>
     </row>
@@ -4434,9 +4696,15 @@
       <c r="Z44" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="AA44" t="inlineStr">
-        <is>
-          <t>4501</t>
+      <c r="AA44" t="n">
+        <v>4501</v>
+      </c>
+      <c r="AB44" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC44" t="inlineStr">
+        <is>
+          <t>4817</t>
         </is>
       </c>
     </row>
@@ -4459,7 +4727,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F45" s="4" t="n">
@@ -4525,9 +4793,15 @@
       <c r="Z45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AA45" t="inlineStr">
-        <is>
-          <t>5295</t>
+      <c r="AA45" t="n">
+        <v>5295</v>
+      </c>
+      <c r="AB45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC45" t="inlineStr">
+        <is>
+          <t>5452</t>
         </is>
       </c>
     </row>
@@ -4550,7 +4824,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F46" s="3" t="n">
@@ -4616,9 +4890,15 @@
       <c r="Z46" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="AA46" t="inlineStr">
-        <is>
-          <t>5352</t>
+      <c r="AA46" t="n">
+        <v>5352</v>
+      </c>
+      <c r="AB46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC46" t="inlineStr">
+        <is>
+          <t>5559</t>
         </is>
       </c>
     </row>
@@ -4707,9 +4987,15 @@
       <c r="Z47" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="AA47" t="inlineStr">
-        <is>
-          <t>4910</t>
+      <c r="AA47" t="n">
+        <v>4910</v>
+      </c>
+      <c r="AB47" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC47" t="inlineStr">
+        <is>
+          <t>5040</t>
         </is>
       </c>
     </row>
@@ -4732,7 +5018,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F48" s="4" t="n">
@@ -4798,9 +5084,15 @@
       <c r="Z48" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="AA48" t="inlineStr">
-        <is>
-          <t>5618</t>
+      <c r="AA48" t="n">
+        <v>5618</v>
+      </c>
+      <c r="AB48" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="AC48" t="inlineStr">
+        <is>
+          <t>5924</t>
         </is>
       </c>
     </row>
@@ -4889,9 +5181,15 @@
       <c r="Z49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA49" t="inlineStr">
-        <is>
-          <t>3637</t>
+      <c r="AA49" t="n">
+        <v>3637</v>
+      </c>
+      <c r="AB49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC49" t="inlineStr">
+        <is>
+          <t>3696</t>
         </is>
       </c>
     </row>
@@ -4980,9 +5278,15 @@
       <c r="Z50" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="AA50" t="inlineStr">
-        <is>
-          <t>5287</t>
+      <c r="AA50" t="n">
+        <v>5287</v>
+      </c>
+      <c r="AB50" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC50" t="inlineStr">
+        <is>
+          <t>5632</t>
         </is>
       </c>
     </row>
@@ -5071,9 +5375,15 @@
       <c r="Z51" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="AA51" t="inlineStr">
-        <is>
-          <t>5477</t>
+      <c r="AA51" t="n">
+        <v>5477</v>
+      </c>
+      <c r="AB51" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC51" t="inlineStr">
+        <is>
+          <t>5809</t>
         </is>
       </c>
     </row>
@@ -5162,9 +5472,15 @@
       <c r="Z52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA52" t="inlineStr">
-        <is>
-          <t>2672</t>
+      <c r="AA52" t="n">
+        <v>2672</v>
+      </c>
+      <c r="AB52" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC52" t="inlineStr">
+        <is>
+          <t>2942</t>
         </is>
       </c>
     </row>
@@ -5253,9 +5569,15 @@
       <c r="Z53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA53" t="inlineStr">
-        <is>
-          <t>3232</t>
+      <c r="AA53" t="n">
+        <v>3232</v>
+      </c>
+      <c r="AB53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC53" t="inlineStr">
+        <is>
+          <t>3291</t>
         </is>
       </c>
     </row>
@@ -5344,9 +5666,15 @@
       <c r="Z54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA54" t="inlineStr">
-        <is>
-          <t>3117</t>
+      <c r="AA54" t="n">
+        <v>3117</v>
+      </c>
+      <c r="AB54" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC54" t="inlineStr">
+        <is>
+          <t>3616</t>
         </is>
       </c>
     </row>
@@ -5435,9 +5763,15 @@
       <c r="Z55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="AA55" t="inlineStr">
-        <is>
-          <t>4167</t>
+      <c r="AA55" t="n">
+        <v>4167</v>
+      </c>
+      <c r="AB55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC55" t="inlineStr">
+        <is>
+          <t>4262</t>
         </is>
       </c>
     </row>
@@ -5526,9 +5860,15 @@
       <c r="Z56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA56" t="inlineStr">
-        <is>
-          <t>4327</t>
+      <c r="AA56" t="n">
+        <v>4327</v>
+      </c>
+      <c r="AB56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC56" t="inlineStr">
+        <is>
+          <t>4506</t>
         </is>
       </c>
     </row>
@@ -5617,9 +5957,15 @@
       <c r="Z57" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AA57" t="inlineStr">
-        <is>
-          <t>4907</t>
+      <c r="AA57" t="n">
+        <v>4907</v>
+      </c>
+      <c r="AB57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC57" t="inlineStr">
+        <is>
+          <t>5053</t>
         </is>
       </c>
     </row>
@@ -5708,9 +6054,15 @@
       <c r="Z58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AA58" t="inlineStr">
-        <is>
-          <t>4349</t>
+      <c r="AA58" t="n">
+        <v>4349</v>
+      </c>
+      <c r="AB58" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC58" t="inlineStr">
+        <is>
+          <t>4436</t>
         </is>
       </c>
     </row>
@@ -5799,9 +6151,15 @@
       <c r="Z59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA59" t="inlineStr">
-        <is>
-          <t>4849</t>
+      <c r="AA59" t="n">
+        <v>4849</v>
+      </c>
+      <c r="AB59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC59" t="inlineStr">
+        <is>
+          <t>5066</t>
         </is>
       </c>
     </row>
@@ -5890,9 +6248,15 @@
       <c r="Z60" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AA60" t="inlineStr">
-        <is>
-          <t>5181</t>
+      <c r="AA60" t="n">
+        <v>5181</v>
+      </c>
+      <c r="AB60" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC60" t="inlineStr">
+        <is>
+          <t>5314</t>
         </is>
       </c>
     </row>
@@ -5981,9 +6345,15 @@
       <c r="Z61" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="AA61" t="inlineStr">
-        <is>
-          <t>4818</t>
+      <c r="AA61" t="n">
+        <v>4818</v>
+      </c>
+      <c r="AB61" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC61" t="inlineStr">
+        <is>
+          <t>5022</t>
         </is>
       </c>
     </row>
@@ -6072,9 +6442,15 @@
       <c r="Z62" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA62" t="inlineStr">
-        <is>
-          <t>5215</t>
+      <c r="AA62" t="n">
+        <v>5215</v>
+      </c>
+      <c r="AB62" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC62" t="inlineStr">
+        <is>
+          <t>5334</t>
         </is>
       </c>
     </row>
@@ -6163,9 +6539,15 @@
       <c r="Z63" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="AA63" t="inlineStr">
-        <is>
-          <t>4320</t>
+      <c r="AA63" t="n">
+        <v>4320</v>
+      </c>
+      <c r="AB63" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC63" t="inlineStr">
+        <is>
+          <t>4369</t>
         </is>
       </c>
     </row>
@@ -6254,9 +6636,15 @@
       <c r="Z64" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA64" t="inlineStr">
-        <is>
-          <t>3094</t>
+      <c r="AA64" t="n">
+        <v>3094</v>
+      </c>
+      <c r="AB64" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC64" t="inlineStr">
+        <is>
+          <t>3661</t>
         </is>
       </c>
     </row>
@@ -6345,9 +6733,15 @@
       <c r="Z65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA65" t="inlineStr">
-        <is>
-          <t>4117</t>
+      <c r="AA65" t="n">
+        <v>4117</v>
+      </c>
+      <c r="AB65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC65" t="inlineStr">
+        <is>
+          <t>4220</t>
         </is>
       </c>
     </row>
@@ -6436,9 +6830,15 @@
       <c r="Z66" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="AA66" t="inlineStr">
-        <is>
-          <t>4058</t>
+      <c r="AA66" t="n">
+        <v>4058</v>
+      </c>
+      <c r="AB66" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC66" t="inlineStr">
+        <is>
+          <t>4201</t>
         </is>
       </c>
     </row>
@@ -6527,9 +6927,15 @@
       <c r="Z67" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="AA67" t="inlineStr">
-        <is>
-          <t>5262</t>
+      <c r="AA67" t="n">
+        <v>5262</v>
+      </c>
+      <c r="AB67" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC67" t="inlineStr">
+        <is>
+          <t>5398</t>
         </is>
       </c>
     </row>
@@ -6618,9 +7024,15 @@
       <c r="Z68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA68" t="inlineStr">
-        <is>
-          <t>4271</t>
+      <c r="AA68" t="n">
+        <v>4271</v>
+      </c>
+      <c r="AB68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC68" t="inlineStr">
+        <is>
+          <t>4444</t>
         </is>
       </c>
     </row>
@@ -6709,9 +7121,15 @@
       <c r="Z69" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA69" t="inlineStr">
-        <is>
-          <t>3264</t>
+      <c r="AA69" t="n">
+        <v>3264</v>
+      </c>
+      <c r="AB69" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC69" t="inlineStr">
+        <is>
+          <t>3551</t>
         </is>
       </c>
     </row>
@@ -6800,9 +7218,15 @@
       <c r="Z70" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="AA70" t="inlineStr">
-        <is>
-          <t>3776</t>
+      <c r="AA70" t="n">
+        <v>3776</v>
+      </c>
+      <c r="AB70" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC70" t="inlineStr">
+        <is>
+          <t>3845</t>
         </is>
       </c>
     </row>
@@ -6891,9 +7315,15 @@
       <c r="Z71" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AA71" t="inlineStr">
-        <is>
-          <t>5340</t>
+      <c r="AA71" t="n">
+        <v>5340</v>
+      </c>
+      <c r="AB71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC71" t="inlineStr">
+        <is>
+          <t>5508</t>
         </is>
       </c>
     </row>
@@ -6982,9 +7412,15 @@
       <c r="Z72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA72" t="inlineStr">
-        <is>
-          <t>3561</t>
+      <c r="AA72" t="n">
+        <v>3561</v>
+      </c>
+      <c r="AB72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC72" t="inlineStr">
+        <is>
+          <t>3591</t>
         </is>
       </c>
     </row>
@@ -7073,9 +7509,15 @@
       <c r="Z73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA73" t="inlineStr">
-        <is>
-          <t>5019</t>
+      <c r="AA73" t="n">
+        <v>5019</v>
+      </c>
+      <c r="AB73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC73" t="inlineStr">
+        <is>
+          <t>5092</t>
         </is>
       </c>
     </row>
@@ -7164,9 +7606,15 @@
       <c r="Z74" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AA74" t="inlineStr">
-        <is>
-          <t>4592</t>
+      <c r="AA74" t="n">
+        <v>4592</v>
+      </c>
+      <c r="AB74" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC74" t="inlineStr">
+        <is>
+          <t>4731</t>
         </is>
       </c>
     </row>
@@ -7255,9 +7703,15 @@
       <c r="Z75" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AA75" t="inlineStr">
-        <is>
-          <t>4750</t>
+      <c r="AA75" t="n">
+        <v>4750</v>
+      </c>
+      <c r="AB75" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC75" t="inlineStr">
+        <is>
+          <t>4943</t>
         </is>
       </c>
     </row>
@@ -7346,9 +7800,15 @@
       <c r="Z76" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA76" t="inlineStr">
-        <is>
-          <t>4714</t>
+      <c r="AA76" t="n">
+        <v>4714</v>
+      </c>
+      <c r="AB76" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC76" t="inlineStr">
+        <is>
+          <t>4809</t>
         </is>
       </c>
     </row>
@@ -7424,6 +7884,8 @@
       <c r="Y77" t="inlineStr"/>
       <c r="Z77" s="3" t="inlineStr"/>
       <c r="AA77" t="inlineStr"/>
+      <c r="AB77" s="3" t="inlineStr"/>
+      <c r="AC77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -7510,9 +7972,15 @@
       <c r="Z78" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA78" t="inlineStr">
-        <is>
-          <t>4493</t>
+      <c r="AA78" t="n">
+        <v>4493</v>
+      </c>
+      <c r="AB78" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC78" t="inlineStr">
+        <is>
+          <t>4656</t>
         </is>
       </c>
     </row>
@@ -7601,9 +8069,15 @@
       <c r="Z79" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA79" t="inlineStr">
-        <is>
-          <t>4498</t>
+      <c r="AA79" t="n">
+        <v>4498</v>
+      </c>
+      <c r="AB79" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC79" t="inlineStr">
+        <is>
+          <t>4525</t>
         </is>
       </c>
     </row>
@@ -7692,9 +8166,15 @@
       <c r="Z80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA80" t="inlineStr">
-        <is>
-          <t>3587</t>
+      <c r="AA80" t="n">
+        <v>3587</v>
+      </c>
+      <c r="AB80" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC80" t="inlineStr">
+        <is>
+          <t>3689</t>
         </is>
       </c>
     </row>
@@ -7783,9 +8263,15 @@
       <c r="Z81" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA81" t="inlineStr">
-        <is>
-          <t>3487</t>
+      <c r="AA81" t="n">
+        <v>3487</v>
+      </c>
+      <c r="AB81" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC81" t="inlineStr">
+        <is>
+          <t>3521</t>
         </is>
       </c>
     </row>
@@ -7874,9 +8360,15 @@
       <c r="Z82" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AA82" t="inlineStr">
-        <is>
-          <t>4746</t>
+      <c r="AA82" t="n">
+        <v>4746</v>
+      </c>
+      <c r="AB82" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC82" t="inlineStr">
+        <is>
+          <t>4922</t>
         </is>
       </c>
     </row>
@@ -7965,9 +8457,15 @@
       <c r="Z83" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA83" t="inlineStr">
-        <is>
-          <t>2972</t>
+      <c r="AA83" t="n">
+        <v>2972</v>
+      </c>
+      <c r="AB83" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC83" t="inlineStr">
+        <is>
+          <t>3049</t>
         </is>
       </c>
     </row>
@@ -8056,9 +8554,15 @@
       <c r="Z84" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA84" t="inlineStr">
-        <is>
-          <t>3382</t>
+      <c r="AA84" t="n">
+        <v>3382</v>
+      </c>
+      <c r="AB84" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC84" t="inlineStr">
+        <is>
+          <t>3480</t>
         </is>
       </c>
     </row>
@@ -8147,7 +8651,13 @@
       <c r="Z85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA85" t="inlineStr">
+      <c r="AA85" t="n">
+        <v>2085</v>
+      </c>
+      <c r="AB85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC85" t="inlineStr">
         <is>
           <t>2085</t>
         </is>
@@ -8238,9 +8748,15 @@
       <c r="Z86" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA86" t="inlineStr">
-        <is>
-          <t>2840</t>
+      <c r="AA86" t="n">
+        <v>2840</v>
+      </c>
+      <c r="AB86" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC86" t="inlineStr">
+        <is>
+          <t>2821</t>
         </is>
       </c>
     </row>
@@ -8329,9 +8845,15 @@
       <c r="Z87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA87" t="inlineStr">
-        <is>
-          <t>3155</t>
+      <c r="AA87" t="n">
+        <v>3155</v>
+      </c>
+      <c r="AB87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC87" t="inlineStr">
+        <is>
+          <t>3145</t>
         </is>
       </c>
     </row>
@@ -8420,9 +8942,15 @@
       <c r="Z88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA88" t="inlineStr">
-        <is>
-          <t>2419</t>
+      <c r="AA88" t="n">
+        <v>2419</v>
+      </c>
+      <c r="AB88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC88" t="inlineStr">
+        <is>
+          <t>2409</t>
         </is>
       </c>
     </row>
@@ -8486,6 +9014,8 @@
       <c r="Y89" t="inlineStr"/>
       <c r="Z89" s="3" t="inlineStr"/>
       <c r="AA89" t="inlineStr"/>
+      <c r="AB89" s="3" t="inlineStr"/>
+      <c r="AC89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -8547,6 +9077,8 @@
       <c r="Y90" t="inlineStr"/>
       <c r="Z90" s="3" t="inlineStr"/>
       <c r="AA90" t="inlineStr"/>
+      <c r="AB90" s="3" t="inlineStr"/>
+      <c r="AC90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -8633,9 +9165,15 @@
       <c r="Z91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA91" t="inlineStr">
-        <is>
-          <t>2698</t>
+      <c r="AA91" t="n">
+        <v>2698</v>
+      </c>
+      <c r="AB91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC91" t="inlineStr">
+        <is>
+          <t>2689</t>
         </is>
       </c>
     </row>
@@ -8724,7 +9262,13 @@
       <c r="Z92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA92" t="inlineStr">
+      <c r="AA92" t="n">
+        <v>3305</v>
+      </c>
+      <c r="AB92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC92" t="inlineStr">
         <is>
           <t>3305</t>
         </is>
@@ -8815,9 +9359,15 @@
       <c r="Z93" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="AA93" t="inlineStr">
-        <is>
-          <t>3243</t>
+      <c r="AA93" t="n">
+        <v>3243</v>
+      </c>
+      <c r="AB93" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC93" t="inlineStr">
+        <is>
+          <t>3339</t>
         </is>
       </c>
     </row>
@@ -8906,9 +9456,15 @@
       <c r="Z94" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA94" t="inlineStr">
-        <is>
-          <t>4379</t>
+      <c r="AA94" t="n">
+        <v>4379</v>
+      </c>
+      <c r="AB94" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC94" t="inlineStr">
+        <is>
+          <t>4484</t>
         </is>
       </c>
     </row>
@@ -8997,9 +9553,15 @@
       <c r="Z95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA95" t="inlineStr">
-        <is>
-          <t>4017</t>
+      <c r="AA95" t="n">
+        <v>4017</v>
+      </c>
+      <c r="AB95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC95" t="inlineStr">
+        <is>
+          <t>4093</t>
         </is>
       </c>
     </row>
@@ -9088,9 +9650,15 @@
       <c r="Z96" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="AA96" t="inlineStr">
-        <is>
-          <t>3853</t>
+      <c r="AA96" t="n">
+        <v>3853</v>
+      </c>
+      <c r="AB96" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC96" t="inlineStr">
+        <is>
+          <t>3944</t>
         </is>
       </c>
     </row>
@@ -9179,9 +9747,15 @@
       <c r="Z97" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AA97" t="inlineStr">
-        <is>
-          <t>4451</t>
+      <c r="AA97" t="n">
+        <v>4451</v>
+      </c>
+      <c r="AB97" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC97" t="inlineStr">
+        <is>
+          <t>4540</t>
         </is>
       </c>
     </row>
@@ -9270,9 +9844,15 @@
       <c r="Z98" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AA98" t="inlineStr">
-        <is>
-          <t>3795</t>
+      <c r="AA98" t="n">
+        <v>3795</v>
+      </c>
+      <c r="AB98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC98" t="inlineStr">
+        <is>
+          <t>3887</t>
         </is>
       </c>
     </row>
@@ -9361,9 +9941,15 @@
       <c r="Z99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA99" t="inlineStr">
-        <is>
-          <t>2829</t>
+      <c r="AA99" t="n">
+        <v>2829</v>
+      </c>
+      <c r="AB99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC99" t="inlineStr">
+        <is>
+          <t>2808</t>
         </is>
       </c>
     </row>
@@ -9452,9 +10038,15 @@
       <c r="Z100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA100" t="inlineStr">
-        <is>
-          <t>2623</t>
+      <c r="AA100" t="n">
+        <v>2623</v>
+      </c>
+      <c r="AB100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC100" t="inlineStr">
+        <is>
+          <t>2610</t>
         </is>
       </c>
     </row>
@@ -9543,9 +10135,15 @@
       <c r="Z101" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA101" t="inlineStr">
-        <is>
-          <t>4510</t>
+      <c r="AA101" t="n">
+        <v>4510</v>
+      </c>
+      <c r="AB101" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC101" t="inlineStr">
+        <is>
+          <t>4861</t>
         </is>
       </c>
     </row>
@@ -9634,9 +10232,15 @@
       <c r="Z102" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="AA102" t="inlineStr">
-        <is>
-          <t>3905</t>
+      <c r="AA102" t="n">
+        <v>3905</v>
+      </c>
+      <c r="AB102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC102" t="inlineStr">
+        <is>
+          <t>3987</t>
         </is>
       </c>
     </row>
@@ -9725,9 +10329,15 @@
       <c r="Z103" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA103" t="inlineStr">
-        <is>
-          <t>3522</t>
+      <c r="AA103" t="n">
+        <v>3522</v>
+      </c>
+      <c r="AB103" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC103" t="inlineStr">
+        <is>
+          <t>3559</t>
         </is>
       </c>
     </row>
@@ -9816,9 +10426,15 @@
       <c r="Z104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA104" t="inlineStr">
-        <is>
-          <t>2606</t>
+      <c r="AA104" t="n">
+        <v>2606</v>
+      </c>
+      <c r="AB104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC104" t="inlineStr">
+        <is>
+          <t>2625</t>
         </is>
       </c>
     </row>
@@ -9907,9 +10523,15 @@
       <c r="Z105" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA105" t="inlineStr">
-        <is>
-          <t>3935</t>
+      <c r="AA105" t="n">
+        <v>3935</v>
+      </c>
+      <c r="AB105" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC105" t="inlineStr">
+        <is>
+          <t>4034</t>
         </is>
       </c>
     </row>
@@ -9998,9 +10620,15 @@
       <c r="Z106" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA106" t="inlineStr">
-        <is>
-          <t>3504</t>
+      <c r="AA106" t="n">
+        <v>3504</v>
+      </c>
+      <c r="AB106" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC106" t="inlineStr">
+        <is>
+          <t>3621</t>
         </is>
       </c>
     </row>
@@ -10089,9 +10717,15 @@
       <c r="Z107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA107" t="inlineStr">
-        <is>
-          <t>3680</t>
+      <c r="AA107" t="n">
+        <v>3680</v>
+      </c>
+      <c r="AB107" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC107" t="inlineStr">
+        <is>
+          <t>3903</t>
         </is>
       </c>
     </row>
@@ -10180,9 +10814,15 @@
       <c r="Z108" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="AA108" t="inlineStr">
-        <is>
-          <t>2751</t>
+      <c r="AA108" t="n">
+        <v>2751</v>
+      </c>
+      <c r="AB108" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC108" t="inlineStr">
+        <is>
+          <t>2745</t>
         </is>
       </c>
     </row>
@@ -10271,9 +10911,15 @@
       <c r="Z109" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="AA109" t="inlineStr">
-        <is>
-          <t>2819</t>
+      <c r="AA109" t="n">
+        <v>2819</v>
+      </c>
+      <c r="AB109" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC109" t="inlineStr">
+        <is>
+          <t>2856</t>
         </is>
       </c>
     </row>
@@ -10362,9 +11008,15 @@
       <c r="Z110" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="AA110" t="inlineStr">
-        <is>
-          <t>3505</t>
+      <c r="AA110" t="n">
+        <v>3505</v>
+      </c>
+      <c r="AB110" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC110" t="inlineStr">
+        <is>
+          <t>3486</t>
         </is>
       </c>
     </row>
@@ -10453,9 +11105,15 @@
       <c r="Z111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA111" t="inlineStr">
-        <is>
-          <t>3100</t>
+      <c r="AA111" t="n">
+        <v>3100</v>
+      </c>
+      <c r="AB111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC111" t="inlineStr">
+        <is>
+          <t>3102</t>
         </is>
       </c>
     </row>
@@ -10544,9 +11202,15 @@
       <c r="Z112" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="AA112" t="inlineStr">
-        <is>
-          <t>3520</t>
+      <c r="AA112" t="n">
+        <v>3520</v>
+      </c>
+      <c r="AB112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC112" t="inlineStr">
+        <is>
+          <t>3654</t>
         </is>
       </c>
     </row>
@@ -10635,9 +11299,15 @@
       <c r="Z113" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA113" t="inlineStr">
-        <is>
-          <t>2870</t>
+      <c r="AA113" t="n">
+        <v>2870</v>
+      </c>
+      <c r="AB113" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC113" t="inlineStr">
+        <is>
+          <t>3047</t>
         </is>
       </c>
     </row>
@@ -10726,9 +11396,15 @@
       <c r="Z114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA114" t="inlineStr">
-        <is>
-          <t>3690</t>
+      <c r="AA114" t="n">
+        <v>3690</v>
+      </c>
+      <c r="AB114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC114" t="inlineStr">
+        <is>
+          <t>3698</t>
         </is>
       </c>
     </row>
@@ -10817,9 +11493,15 @@
       <c r="Z115" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="AA115" t="inlineStr">
-        <is>
-          <t>2666</t>
+      <c r="AA115" t="n">
+        <v>2666</v>
+      </c>
+      <c r="AB115" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC115" t="inlineStr">
+        <is>
+          <t>2737</t>
         </is>
       </c>
     </row>
@@ -10908,9 +11590,15 @@
       <c r="Z116" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA116" t="inlineStr">
-        <is>
-          <t>3272</t>
+      <c r="AA116" t="n">
+        <v>3272</v>
+      </c>
+      <c r="AB116" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC116" t="inlineStr">
+        <is>
+          <t>3280</t>
         </is>
       </c>
     </row>
@@ -10999,9 +11687,15 @@
       <c r="Z117" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="AA117" t="inlineStr">
-        <is>
-          <t>3261</t>
+      <c r="AA117" t="n">
+        <v>3261</v>
+      </c>
+      <c r="AB117" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC117" t="inlineStr">
+        <is>
+          <t>3257</t>
         </is>
       </c>
     </row>
@@ -11077,6 +11771,8 @@
       <c r="Y118" t="inlineStr"/>
       <c r="Z118" s="3" t="inlineStr"/>
       <c r="AA118" t="inlineStr"/>
+      <c r="AB118" s="3" t="inlineStr"/>
+      <c r="AC118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -11163,9 +11859,15 @@
       <c r="Z119" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA119" t="inlineStr">
-        <is>
-          <t>3596</t>
+      <c r="AA119" t="n">
+        <v>3596</v>
+      </c>
+      <c r="AB119" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC119" t="inlineStr">
+        <is>
+          <t>3621</t>
         </is>
       </c>
     </row>
@@ -11254,9 +11956,15 @@
       <c r="Z120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA120" t="inlineStr">
-        <is>
-          <t>3258</t>
+      <c r="AA120" t="n">
+        <v>3258</v>
+      </c>
+      <c r="AB120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC120" t="inlineStr">
+        <is>
+          <t>3330</t>
         </is>
       </c>
     </row>
@@ -11345,9 +12053,15 @@
       <c r="Z121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA121" t="inlineStr">
-        <is>
-          <t>2161</t>
+      <c r="AA121" t="n">
+        <v>2161</v>
+      </c>
+      <c r="AB121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC121" t="inlineStr">
+        <is>
+          <t>2158</t>
         </is>
       </c>
     </row>
@@ -11436,9 +12150,15 @@
       <c r="Z122" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="AA122" t="inlineStr">
-        <is>
-          <t>2641</t>
+      <c r="AA122" t="n">
+        <v>2641</v>
+      </c>
+      <c r="AB122" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="AC122" t="inlineStr">
+        <is>
+          <t>2730</t>
         </is>
       </c>
     </row>
@@ -11527,9 +12247,15 @@
       <c r="Z123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA123" t="inlineStr">
-        <is>
-          <t>2723</t>
+      <c r="AA123" t="n">
+        <v>2723</v>
+      </c>
+      <c r="AB123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC123" t="inlineStr">
+        <is>
+          <t>2761</t>
         </is>
       </c>
     </row>
@@ -11618,9 +12344,15 @@
       <c r="Z124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA124" t="inlineStr">
-        <is>
-          <t>3677</t>
+      <c r="AA124" t="n">
+        <v>3677</v>
+      </c>
+      <c r="AB124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC124" t="inlineStr">
+        <is>
+          <t>3705</t>
         </is>
       </c>
     </row>
@@ -11709,7 +12441,13 @@
       <c r="Z125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA125" t="inlineStr">
+      <c r="AA125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11800,9 +12538,15 @@
       <c r="Z126" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="AA126" t="inlineStr">
-        <is>
-          <t>3106</t>
+      <c r="AA126" t="n">
+        <v>3106</v>
+      </c>
+      <c r="AB126" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC126" t="inlineStr">
+        <is>
+          <t>3097</t>
         </is>
       </c>
     </row>
@@ -11891,9 +12635,15 @@
       <c r="Z127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA127" t="inlineStr">
-        <is>
-          <t>2758</t>
+      <c r="AA127" t="n">
+        <v>2758</v>
+      </c>
+      <c r="AB127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC127" t="inlineStr">
+        <is>
+          <t>2702</t>
         </is>
       </c>
     </row>
@@ -11982,9 +12732,15 @@
       <c r="Z128" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="AA128" t="inlineStr">
-        <is>
-          <t>2681</t>
+      <c r="AA128" t="n">
+        <v>2681</v>
+      </c>
+      <c r="AB128" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC128" t="inlineStr">
+        <is>
+          <t>2725</t>
         </is>
       </c>
     </row>
@@ -12073,9 +12829,15 @@
       <c r="Z129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA129" t="inlineStr">
-        <is>
-          <t>2542</t>
+      <c r="AA129" t="n">
+        <v>2542</v>
+      </c>
+      <c r="AB129" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC129" t="inlineStr">
+        <is>
+          <t>2495</t>
         </is>
       </c>
     </row>
@@ -12164,9 +12926,15 @@
       <c r="Z130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA130" t="inlineStr">
-        <is>
-          <t>1912</t>
+      <c r="AA130" t="n">
+        <v>1912</v>
+      </c>
+      <c r="AB130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC130" t="inlineStr">
+        <is>
+          <t>1929</t>
         </is>
       </c>
     </row>
@@ -12255,7 +13023,13 @@
       <c r="Z131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA131" t="inlineStr">
+      <c r="AA131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12346,7 +13120,13 @@
       <c r="Z132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA132" t="inlineStr">
+      <c r="AA132" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12424,6 +13204,8 @@
       <c r="Y133" t="inlineStr"/>
       <c r="Z133" s="3" t="inlineStr"/>
       <c r="AA133" t="inlineStr"/>
+      <c r="AB133" s="3" t="inlineStr"/>
+      <c r="AC133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -12510,9 +13292,15 @@
       <c r="Z134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA134" t="inlineStr">
-        <is>
-          <t>2063</t>
+      <c r="AA134" t="n">
+        <v>2063</v>
+      </c>
+      <c r="AB134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC134" t="inlineStr">
+        <is>
+          <t>2088</t>
         </is>
       </c>
     </row>
@@ -12601,7 +13389,13 @@
       <c r="Z135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA135" t="inlineStr">
+      <c r="AA135" t="n">
+        <v>2198</v>
+      </c>
+      <c r="AB135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC135" t="inlineStr">
         <is>
           <t>2198</t>
         </is>
@@ -12692,9 +13486,15 @@
       <c r="Z136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA136" t="inlineStr">
-        <is>
-          <t>1517</t>
+      <c r="AA136" t="n">
+        <v>1517</v>
+      </c>
+      <c r="AB136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC136" t="inlineStr">
+        <is>
+          <t>1532</t>
         </is>
       </c>
     </row>
@@ -12770,6 +13570,8 @@
       <c r="Y137" t="inlineStr"/>
       <c r="Z137" s="3" t="inlineStr"/>
       <c r="AA137" t="inlineStr"/>
+      <c r="AB137" s="3" t="inlineStr"/>
+      <c r="AC137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -12856,7 +13658,13 @@
       <c r="Z138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA138" t="inlineStr">
+      <c r="AA138" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12934,6 +13742,8 @@
       <c r="Y139" t="inlineStr"/>
       <c r="Z139" s="3" t="inlineStr"/>
       <c r="AA139" t="inlineStr"/>
+      <c r="AB139" s="3" t="inlineStr"/>
+      <c r="AC139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -13020,9 +13830,15 @@
       <c r="Z140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA140" t="inlineStr">
-        <is>
-          <t>4804</t>
+      <c r="AA140" t="n">
+        <v>4804</v>
+      </c>
+      <c r="AB140" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC140" t="inlineStr">
+        <is>
+          <t>5083</t>
         </is>
       </c>
     </row>
@@ -13111,7 +13927,13 @@
       <c r="Z141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA141" t="inlineStr">
+      <c r="AA141" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13202,7 +14024,13 @@
       <c r="Z142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA142" t="inlineStr">
+      <c r="AA142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13293,9 +14121,15 @@
       <c r="Z143" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA143" t="inlineStr">
-        <is>
-          <t>5437</t>
+      <c r="AA143" t="n">
+        <v>5437</v>
+      </c>
+      <c r="AB143" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC143" t="inlineStr">
+        <is>
+          <t>5805</t>
         </is>
       </c>
     </row>
@@ -13384,7 +14218,13 @@
       <c r="Z144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA144" t="inlineStr">
+      <c r="AA144" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13475,9 +14315,15 @@
       <c r="Z145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA145" t="inlineStr">
-        <is>
-          <t>2745</t>
+      <c r="AA145" t="n">
+        <v>2745</v>
+      </c>
+      <c r="AB145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC145" t="inlineStr">
+        <is>
+          <t>2765</t>
         </is>
       </c>
     </row>
@@ -13566,7 +14412,13 @@
       <c r="Z146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA146" t="inlineStr">
+      <c r="AA146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13657,9 +14509,15 @@
       <c r="Z147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA147" t="inlineStr">
-        <is>
-          <t>2871</t>
+      <c r="AA147" t="n">
+        <v>2871</v>
+      </c>
+      <c r="AB147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC147" t="inlineStr">
+        <is>
+          <t>2897</t>
         </is>
       </c>
     </row>
@@ -13726,9 +14584,15 @@
       <c r="Z148" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA148" t="inlineStr">
-        <is>
-          <t>3052</t>
+      <c r="AA148" t="n">
+        <v>3052</v>
+      </c>
+      <c r="AB148" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="AC148" t="inlineStr">
+        <is>
+          <t>3001</t>
         </is>
       </c>
     </row>
@@ -13811,7 +14675,13 @@
       <c r="Z149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA149" t="inlineStr">
+      <c r="AA149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13896,7 +14766,13 @@
       <c r="Z150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA150" t="inlineStr">
+      <c r="AA150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13969,9 +14845,15 @@
       <c r="Z151" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AA151" t="inlineStr">
-        <is>
-          <t>2485</t>
+      <c r="AA151" t="n">
+        <v>2485</v>
+      </c>
+      <c r="AB151" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC151" t="inlineStr">
+        <is>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -14042,7 +14924,13 @@
       <c r="Z152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA152" t="inlineStr">
+      <c r="AA152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14107,9 +14995,15 @@
       <c r="Z153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA153" t="inlineStr">
-        <is>
-          <t>3761</t>
+      <c r="AA153" t="n">
+        <v>3761</v>
+      </c>
+      <c r="AB153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC153" t="inlineStr">
+        <is>
+          <t>3795</t>
         </is>
       </c>
     </row>
@@ -14172,9 +15066,15 @@
       <c r="Z154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA154" t="inlineStr">
-        <is>
-          <t>1654</t>
+      <c r="AA154" t="n">
+        <v>1654</v>
+      </c>
+      <c r="AB154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC154" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -14233,9 +15133,15 @@
       <c r="Z155" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="AA155" t="inlineStr">
-        <is>
-          <t>1692</t>
+      <c r="AA155" t="n">
+        <v>1692</v>
+      </c>
+      <c r="AB155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC155" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -14290,9 +15196,15 @@
       <c r="Z156" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="AA156" t="inlineStr">
-        <is>
-          <t>3497</t>
+      <c r="AA156" t="n">
+        <v>3497</v>
+      </c>
+      <c r="AB156" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC156" t="inlineStr">
+        <is>
+          <t>3910</t>
         </is>
       </c>
     </row>
@@ -14346,6 +15258,8 @@
       </c>
       <c r="Z157" s="3" t="inlineStr"/>
       <c r="AA157" t="inlineStr"/>
+      <c r="AB157" s="3" t="inlineStr"/>
+      <c r="AC157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -14389,6 +15303,8 @@
       <c r="Y158" t="inlineStr"/>
       <c r="Z158" s="3" t="inlineStr"/>
       <c r="AA158" t="inlineStr"/>
+      <c r="AB158" s="3" t="inlineStr"/>
+      <c r="AC158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -14437,9 +15353,15 @@
       <c r="Z159" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA159" t="inlineStr">
-        <is>
-          <t>5297</t>
+      <c r="AA159" t="n">
+        <v>5297</v>
+      </c>
+      <c r="AB159" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC159" t="inlineStr">
+        <is>
+          <t>5488</t>
         </is>
       </c>
     </row>
@@ -14490,9 +15412,15 @@
       <c r="Z160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA160" t="inlineStr">
-        <is>
-          <t>2591</t>
+      <c r="AA160" t="n">
+        <v>2591</v>
+      </c>
+      <c r="AB160" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC160" t="inlineStr">
+        <is>
+          <t>2743</t>
         </is>
       </c>
     </row>
@@ -14543,9 +15471,15 @@
       <c r="Z161" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="AA161" t="inlineStr">
-        <is>
-          <t>1906</t>
+      <c r="AA161" t="n">
+        <v>1906</v>
+      </c>
+      <c r="AB161" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC161" t="inlineStr">
+        <is>
+          <t>2117</t>
         </is>
       </c>
     </row>
@@ -14596,9 +15530,15 @@
       <c r="Z162" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA162" t="inlineStr">
-        <is>
-          <t>1822</t>
+      <c r="AA162" t="n">
+        <v>1822</v>
+      </c>
+      <c r="AB162" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC162" t="inlineStr">
+        <is>
+          <t>1827</t>
         </is>
       </c>
     </row>
@@ -14645,17 +15585,21 @@
       <c r="Z163" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="AA163" t="inlineStr">
-        <is>
-          <t>1657</t>
+      <c r="AA163" t="n">
+        <v>1657</v>
+      </c>
+      <c r="AB163" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC163" t="inlineStr">
+        <is>
+          <t>1627</t>
         </is>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>6510348</t>
-        </is>
+      <c r="A164" t="n">
+        <v>6510348</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -14666,7 +15610,7 @@
       <c r="D164" t="inlineStr"/>
       <c r="E164" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F164" s="3" t="inlineStr"/>
@@ -14692,17 +15636,21 @@
       <c r="Z164" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="AA164" t="inlineStr">
-        <is>
-          <t>5048</t>
+      <c r="AA164" t="n">
+        <v>5048</v>
+      </c>
+      <c r="AB164" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC164" t="inlineStr">
+        <is>
+          <t>5284</t>
         </is>
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>41463618</t>
-        </is>
+      <c r="A165" t="n">
+        <v>41463618</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -14739,17 +15687,21 @@
       <c r="Z165" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA165" t="inlineStr">
-        <is>
-          <t>2608</t>
+      <c r="AA165" t="n">
+        <v>2608</v>
+      </c>
+      <c r="AB165" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC165" t="inlineStr">
+        <is>
+          <t>2576</t>
         </is>
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>58494374</t>
-        </is>
+      <c r="A166" t="n">
+        <v>58494374</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -14786,9 +15738,211 @@
       <c r="Z166" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="AA166" t="inlineStr">
-        <is>
-          <t>1242</t>
+      <c r="AA166" t="n">
+        <v>1242</v>
+      </c>
+      <c r="AB166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC166" t="inlineStr">
+        <is>
+          <t>1259</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>22161051</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Botz5</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr"/>
+      <c r="D167" t="inlineStr"/>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F167" s="3" t="inlineStr"/>
+      <c r="G167" t="inlineStr"/>
+      <c r="H167" s="3" t="inlineStr"/>
+      <c r="I167" t="inlineStr"/>
+      <c r="J167" s="3" t="inlineStr"/>
+      <c r="K167" t="inlineStr"/>
+      <c r="L167" s="3" t="inlineStr"/>
+      <c r="M167" t="inlineStr"/>
+      <c r="N167" s="3" t="inlineStr"/>
+      <c r="O167" t="inlineStr"/>
+      <c r="P167" s="3" t="inlineStr"/>
+      <c r="Q167" t="inlineStr"/>
+      <c r="R167" s="3" t="inlineStr"/>
+      <c r="S167" t="inlineStr"/>
+      <c r="T167" s="3" t="inlineStr"/>
+      <c r="U167" t="inlineStr"/>
+      <c r="V167" s="3" t="inlineStr"/>
+      <c r="W167" t="inlineStr"/>
+      <c r="X167" s="3" t="inlineStr"/>
+      <c r="Y167" t="inlineStr"/>
+      <c r="Z167" s="3" t="inlineStr"/>
+      <c r="AA167" t="inlineStr"/>
+      <c r="AB167" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC167" t="inlineStr">
+        <is>
+          <t>3179</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>53090046</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Naransolongo</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr"/>
+      <c r="D168" t="inlineStr"/>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F168" s="3" t="inlineStr"/>
+      <c r="G168" t="inlineStr"/>
+      <c r="H168" s="3" t="inlineStr"/>
+      <c r="I168" t="inlineStr"/>
+      <c r="J168" s="3" t="inlineStr"/>
+      <c r="K168" t="inlineStr"/>
+      <c r="L168" s="3" t="inlineStr"/>
+      <c r="M168" t="inlineStr"/>
+      <c r="N168" s="3" t="inlineStr"/>
+      <c r="O168" t="inlineStr"/>
+      <c r="P168" s="3" t="inlineStr"/>
+      <c r="Q168" t="inlineStr"/>
+      <c r="R168" s="3" t="inlineStr"/>
+      <c r="S168" t="inlineStr"/>
+      <c r="T168" s="3" t="inlineStr"/>
+      <c r="U168" t="inlineStr"/>
+      <c r="V168" s="3" t="inlineStr"/>
+      <c r="W168" t="inlineStr"/>
+      <c r="X168" s="3" t="inlineStr"/>
+      <c r="Y168" t="inlineStr"/>
+      <c r="Z168" s="3" t="inlineStr"/>
+      <c r="AA168" t="inlineStr"/>
+      <c r="AB168" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC168" t="inlineStr">
+        <is>
+          <t>2669</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>57605565</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>"Leonel Messi"</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr"/>
+      <c r="D169" t="inlineStr"/>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F169" s="3" t="inlineStr"/>
+      <c r="G169" t="inlineStr"/>
+      <c r="H169" s="3" t="inlineStr"/>
+      <c r="I169" t="inlineStr"/>
+      <c r="J169" s="3" t="inlineStr"/>
+      <c r="K169" t="inlineStr"/>
+      <c r="L169" s="3" t="inlineStr"/>
+      <c r="M169" t="inlineStr"/>
+      <c r="N169" s="3" t="inlineStr"/>
+      <c r="O169" t="inlineStr"/>
+      <c r="P169" s="3" t="inlineStr"/>
+      <c r="Q169" t="inlineStr"/>
+      <c r="R169" s="3" t="inlineStr"/>
+      <c r="S169" t="inlineStr"/>
+      <c r="T169" s="3" t="inlineStr"/>
+      <c r="U169" t="inlineStr"/>
+      <c r="V169" s="3" t="inlineStr"/>
+      <c r="W169" t="inlineStr"/>
+      <c r="X169" s="3" t="inlineStr"/>
+      <c r="Y169" t="inlineStr"/>
+      <c r="Z169" s="3" t="inlineStr"/>
+      <c r="AA169" t="inlineStr"/>
+      <c r="AB169" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC169" t="inlineStr">
+        <is>
+          <t>1932</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>58479166</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>ريانRedSomebody264</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr"/>
+      <c r="D170" t="inlineStr"/>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F170" s="3" t="inlineStr"/>
+      <c r="G170" t="inlineStr"/>
+      <c r="H170" s="3" t="inlineStr"/>
+      <c r="I170" t="inlineStr"/>
+      <c r="J170" s="3" t="inlineStr"/>
+      <c r="K170" t="inlineStr"/>
+      <c r="L170" s="3" t="inlineStr"/>
+      <c r="M170" t="inlineStr"/>
+      <c r="N170" s="3" t="inlineStr"/>
+      <c r="O170" t="inlineStr"/>
+      <c r="P170" s="3" t="inlineStr"/>
+      <c r="Q170" t="inlineStr"/>
+      <c r="R170" s="3" t="inlineStr"/>
+      <c r="S170" t="inlineStr"/>
+      <c r="T170" s="3" t="inlineStr"/>
+      <c r="U170" t="inlineStr"/>
+      <c r="V170" s="3" t="inlineStr"/>
+      <c r="W170" t="inlineStr"/>
+      <c r="X170" s="3" t="inlineStr"/>
+      <c r="Y170" t="inlineStr"/>
+      <c r="Z170" s="3" t="inlineStr"/>
+      <c r="AA170" t="inlineStr"/>
+      <c r="AB170" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC170" t="inlineStr">
+        <is>
+          <t>1140</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-14 11:30:33
</commit_message>
<xml_diff>
--- a/Season_Attack/81.xlsx
+++ b/Season_Attack/81.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC170"/>
+  <dimension ref="A1:AE173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,6 +536,16 @@
           <t>01-12_0</t>
         </is>
       </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>01-13_A</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>01-13_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -628,9 +638,15 @@
       <c r="AB2" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>4556</t>
+      <c r="AC2" t="n">
+        <v>4556</v>
+      </c>
+      <c r="AD2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>4591</t>
         </is>
       </c>
     </row>
@@ -725,9 +741,15 @@
       <c r="AB3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>5312</t>
+      <c r="AC3" t="n">
+        <v>5312</v>
+      </c>
+      <c r="AD3" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>5662</t>
         </is>
       </c>
     </row>
@@ -822,9 +844,15 @@
       <c r="AB4" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>5829</t>
+      <c r="AC4" t="n">
+        <v>5829</v>
+      </c>
+      <c r="AD4" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>5988</t>
         </is>
       </c>
     </row>
@@ -919,9 +947,15 @@
       <c r="AB5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>6203</t>
+      <c r="AC5" t="n">
+        <v>6203</v>
+      </c>
+      <c r="AD5" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>6423</t>
         </is>
       </c>
     </row>
@@ -1016,9 +1050,15 @@
       <c r="AB6" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>5924</t>
+      <c r="AC6" t="n">
+        <v>5924</v>
+      </c>
+      <c r="AD6" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>6179</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1081,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F7" s="3" t="n">
@@ -1113,9 +1153,15 @@
       <c r="AB7" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>6229</t>
+      <c r="AC7" t="n">
+        <v>6229</v>
+      </c>
+      <c r="AD7" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>6306</t>
         </is>
       </c>
     </row>
@@ -1210,9 +1256,15 @@
       <c r="AB8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC8" t="inlineStr">
-        <is>
-          <t>5315</t>
+      <c r="AC8" t="n">
+        <v>5315</v>
+      </c>
+      <c r="AD8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>5441</t>
         </is>
       </c>
     </row>
@@ -1307,9 +1359,15 @@
       <c r="AB9" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AC9" t="inlineStr">
-        <is>
-          <t>5419</t>
+      <c r="AC9" t="n">
+        <v>5419</v>
+      </c>
+      <c r="AD9" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>5501</t>
         </is>
       </c>
     </row>
@@ -1404,9 +1462,15 @@
       <c r="AB10" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AC10" t="inlineStr">
-        <is>
-          <t>5272</t>
+      <c r="AC10" t="n">
+        <v>5272</v>
+      </c>
+      <c r="AD10" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>5729</t>
         </is>
       </c>
     </row>
@@ -1501,9 +1565,15 @@
       <c r="AB11" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="AC11" t="inlineStr">
-        <is>
-          <t>6774</t>
+      <c r="AC11" t="n">
+        <v>6774</v>
+      </c>
+      <c r="AD11" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>6993</t>
         </is>
       </c>
     </row>
@@ -1598,9 +1668,15 @@
       <c r="AB12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC12" t="inlineStr">
-        <is>
-          <t>5732</t>
+      <c r="AC12" t="n">
+        <v>5732</v>
+      </c>
+      <c r="AD12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>6071</t>
         </is>
       </c>
     </row>
@@ -1695,9 +1771,15 @@
       <c r="AB13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC13" t="inlineStr">
-        <is>
-          <t>2927</t>
+      <c r="AC13" t="n">
+        <v>2927</v>
+      </c>
+      <c r="AD13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>2970</t>
         </is>
       </c>
     </row>
@@ -1720,7 +1802,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F14" s="4" t="n">
@@ -1792,9 +1874,15 @@
       <c r="AB14" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="AC14" t="inlineStr">
-        <is>
-          <t>6736</t>
+      <c r="AC14" t="n">
+        <v>6736</v>
+      </c>
+      <c r="AD14" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>6898</t>
         </is>
       </c>
     </row>
@@ -1817,7 +1905,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F15" s="3" t="n">
@@ -1889,9 +1977,15 @@
       <c r="AB15" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AC15" t="inlineStr">
-        <is>
-          <t>5614</t>
+      <c r="AC15" t="n">
+        <v>5614</v>
+      </c>
+      <c r="AD15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>5905</t>
         </is>
       </c>
     </row>
@@ -1914,7 +2008,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F16" s="3" t="n">
@@ -1986,9 +2080,15 @@
       <c r="AB16" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="AC16" t="inlineStr">
-        <is>
-          <t>6195</t>
+      <c r="AC16" t="n">
+        <v>6195</v>
+      </c>
+      <c r="AD16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>6515</t>
         </is>
       </c>
     </row>
@@ -2083,9 +2183,15 @@
       <c r="AB17" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AC17" t="inlineStr">
-        <is>
-          <t>5318</t>
+      <c r="AC17" t="n">
+        <v>5318</v>
+      </c>
+      <c r="AD17" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>5525</t>
         </is>
       </c>
     </row>
@@ -2180,9 +2286,15 @@
       <c r="AB18" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC18" t="inlineStr">
-        <is>
-          <t>5313</t>
+      <c r="AC18" t="n">
+        <v>5313</v>
+      </c>
+      <c r="AD18" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>5382</t>
         </is>
       </c>
     </row>
@@ -2205,7 +2317,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F19" s="4" t="n">
@@ -2277,9 +2389,15 @@
       <c r="AB19" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AC19" t="inlineStr">
-        <is>
-          <t>5925</t>
+      <c r="AC19" t="n">
+        <v>5925</v>
+      </c>
+      <c r="AD19" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>6148</t>
         </is>
       </c>
     </row>
@@ -2302,7 +2420,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F20" s="4" t="n">
@@ -2374,9 +2492,15 @@
       <c r="AB20" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="AC20" t="inlineStr">
-        <is>
-          <t>6580</t>
+      <c r="AC20" t="n">
+        <v>6580</v>
+      </c>
+      <c r="AD20" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>6855</t>
         </is>
       </c>
     </row>
@@ -2471,9 +2595,15 @@
       <c r="AB21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC21" t="inlineStr">
-        <is>
-          <t>5370</t>
+      <c r="AC21" t="n">
+        <v>5370</v>
+      </c>
+      <c r="AD21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE21" t="inlineStr">
+        <is>
+          <t>5656</t>
         </is>
       </c>
     </row>
@@ -2496,7 +2626,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F22" s="4" t="n">
@@ -2568,9 +2698,15 @@
       <c r="AB22" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="AC22" t="inlineStr">
-        <is>
-          <t>6077</t>
+      <c r="AC22" t="n">
+        <v>6077</v>
+      </c>
+      <c r="AD22" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="AE22" t="inlineStr">
+        <is>
+          <t>6241</t>
         </is>
       </c>
     </row>
@@ -2665,9 +2801,15 @@
       <c r="AB23" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="AC23" t="inlineStr">
-        <is>
-          <t>5549</t>
+      <c r="AC23" t="n">
+        <v>5549</v>
+      </c>
+      <c r="AD23" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="AE23" t="inlineStr">
+        <is>
+          <t>6075</t>
         </is>
       </c>
     </row>
@@ -2690,7 +2832,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F24" s="4" t="n">
@@ -2762,9 +2904,15 @@
       <c r="AB24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AC24" t="inlineStr">
-        <is>
-          <t>5342</t>
+      <c r="AC24" t="n">
+        <v>5342</v>
+      </c>
+      <c r="AD24" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="AE24" t="inlineStr">
+        <is>
+          <t>5685</t>
         </is>
       </c>
     </row>
@@ -2859,7 +3007,13 @@
       <c r="AB25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC25" t="inlineStr">
+      <c r="AC25" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AD25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE25" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2884,7 +3038,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F26" s="3" t="n">
@@ -2956,9 +3110,15 @@
       <c r="AB26" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="AC26" t="inlineStr">
-        <is>
-          <t>5770</t>
+      <c r="AC26" t="n">
+        <v>5770</v>
+      </c>
+      <c r="AD26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE26" t="inlineStr">
+        <is>
+          <t>6027</t>
         </is>
       </c>
     </row>
@@ -2981,7 +3141,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F27" s="4" t="n">
@@ -3053,9 +3213,15 @@
       <c r="AB27" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="AC27" t="inlineStr">
-        <is>
-          <t>5848</t>
+      <c r="AC27" t="n">
+        <v>5848</v>
+      </c>
+      <c r="AD27" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE27" t="inlineStr">
+        <is>
+          <t>6307</t>
         </is>
       </c>
     </row>
@@ -3150,9 +3316,15 @@
       <c r="AB28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC28" t="inlineStr">
-        <is>
-          <t>4440</t>
+      <c r="AC28" t="n">
+        <v>4440</v>
+      </c>
+      <c r="AD28" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE28" t="inlineStr">
+        <is>
+          <t>4759</t>
         </is>
       </c>
     </row>
@@ -3175,7 +3347,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F29" s="3" t="n">
@@ -3247,9 +3419,15 @@
       <c r="AB29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AC29" t="inlineStr">
-        <is>
-          <t>5625</t>
+      <c r="AC29" t="n">
+        <v>5625</v>
+      </c>
+      <c r="AD29" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE29" t="inlineStr">
+        <is>
+          <t>6036</t>
         </is>
       </c>
     </row>
@@ -3272,7 +3450,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F30" s="4" t="n">
@@ -3344,9 +3522,15 @@
       <c r="AB30" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="AC30" t="inlineStr">
-        <is>
-          <t>6383</t>
+      <c r="AC30" t="n">
+        <v>6383</v>
+      </c>
+      <c r="AD30" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE30" t="inlineStr">
+        <is>
+          <t>6487</t>
         </is>
       </c>
     </row>
@@ -3369,7 +3553,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F31" s="4" t="n">
@@ -3441,9 +3625,15 @@
       <c r="AB31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC31" t="inlineStr">
-        <is>
-          <t>5935</t>
+      <c r="AC31" t="n">
+        <v>5935</v>
+      </c>
+      <c r="AD31" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="AE31" t="inlineStr">
+        <is>
+          <t>6215</t>
         </is>
       </c>
     </row>
@@ -3466,7 +3656,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F32" s="4" t="n">
@@ -3538,9 +3728,15 @@
       <c r="AB32" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="AC32" t="inlineStr">
-        <is>
-          <t>6135</t>
+      <c r="AC32" t="n">
+        <v>6135</v>
+      </c>
+      <c r="AD32" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE32" t="inlineStr">
+        <is>
+          <t>6383</t>
         </is>
       </c>
     </row>
@@ -3635,9 +3831,15 @@
       <c r="AB33" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="AC33" t="inlineStr">
-        <is>
-          <t>6461</t>
+      <c r="AC33" t="n">
+        <v>6461</v>
+      </c>
+      <c r="AD33" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="AE33" t="inlineStr">
+        <is>
+          <t>6886</t>
         </is>
       </c>
     </row>
@@ -3660,7 +3862,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F34" s="2" t="n">
@@ -3732,7 +3934,13 @@
       <c r="AB34" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="AC34" t="inlineStr">
+      <c r="AC34" t="n">
+        <v>3632</v>
+      </c>
+      <c r="AD34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE34" t="inlineStr">
         <is>
           <t>3632</t>
         </is>
@@ -3829,9 +4037,15 @@
       <c r="AB35" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="AC35" t="inlineStr">
-        <is>
-          <t>6238</t>
+      <c r="AC35" t="n">
+        <v>6238</v>
+      </c>
+      <c r="AD35" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE35" t="inlineStr">
+        <is>
+          <t>6553</t>
         </is>
       </c>
     </row>
@@ -3854,7 +4068,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F36" s="5" t="n">
@@ -3926,9 +4140,15 @@
       <c r="AB36" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC36" t="inlineStr">
-        <is>
-          <t>5354</t>
+      <c r="AC36" t="n">
+        <v>5354</v>
+      </c>
+      <c r="AD36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE36" t="inlineStr">
+        <is>
+          <t>5468</t>
         </is>
       </c>
     </row>
@@ -3951,7 +4171,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F37" s="3" t="n">
@@ -4023,9 +4243,15 @@
       <c r="AB37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AC37" t="inlineStr">
-        <is>
-          <t>4946</t>
+      <c r="AC37" t="n">
+        <v>4946</v>
+      </c>
+      <c r="AD37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE37" t="inlineStr">
+        <is>
+          <t>4985</t>
         </is>
       </c>
     </row>
@@ -4048,7 +4274,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F38" s="3" t="n">
@@ -4120,9 +4346,15 @@
       <c r="AB38" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="AC38" t="inlineStr">
-        <is>
-          <t>5687</t>
+      <c r="AC38" t="n">
+        <v>5687</v>
+      </c>
+      <c r="AD38" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="AE38" t="inlineStr">
+        <is>
+          <t>5891</t>
         </is>
       </c>
     </row>
@@ -4217,9 +4449,15 @@
       <c r="AB39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="AC39" t="inlineStr">
-        <is>
-          <t>5356</t>
+      <c r="AC39" t="n">
+        <v>5356</v>
+      </c>
+      <c r="AD39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="AE39" t="inlineStr">
+        <is>
+          <t>5508</t>
         </is>
       </c>
     </row>
@@ -4314,9 +4552,15 @@
       <c r="AB40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AC40" t="inlineStr">
-        <is>
-          <t>6579</t>
+      <c r="AC40" t="n">
+        <v>6579</v>
+      </c>
+      <c r="AD40" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="AE40" t="inlineStr">
+        <is>
+          <t>6959</t>
         </is>
       </c>
     </row>
@@ -4411,9 +4655,15 @@
       <c r="AB41" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC41" t="inlineStr">
-        <is>
-          <t>5816</t>
+      <c r="AC41" t="n">
+        <v>5816</v>
+      </c>
+      <c r="AD41" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AE41" t="inlineStr">
+        <is>
+          <t>6041</t>
         </is>
       </c>
     </row>
@@ -4436,7 +4686,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F42" s="4" t="n">
@@ -4508,9 +4758,15 @@
       <c r="AB42" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="AC42" t="inlineStr">
-        <is>
-          <t>6536</t>
+      <c r="AC42" t="n">
+        <v>6536</v>
+      </c>
+      <c r="AD42" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="AE42" t="inlineStr">
+        <is>
+          <t>6855</t>
         </is>
       </c>
     </row>
@@ -4533,7 +4789,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F43" s="4" t="n">
@@ -4605,9 +4861,15 @@
       <c r="AB43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AC43" t="inlineStr">
-        <is>
-          <t>5718</t>
+      <c r="AC43" t="n">
+        <v>5718</v>
+      </c>
+      <c r="AD43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE43" t="inlineStr">
+        <is>
+          <t>5957</t>
         </is>
       </c>
     </row>
@@ -4702,9 +4964,15 @@
       <c r="AB44" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC44" t="inlineStr">
-        <is>
-          <t>4817</t>
+      <c r="AC44" t="n">
+        <v>4817</v>
+      </c>
+      <c r="AD44" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE44" t="inlineStr">
+        <is>
+          <t>5006</t>
         </is>
       </c>
     </row>
@@ -4799,9 +5067,15 @@
       <c r="AB45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AC45" t="inlineStr">
-        <is>
-          <t>5452</t>
+      <c r="AC45" t="n">
+        <v>5452</v>
+      </c>
+      <c r="AD45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE45" t="inlineStr">
+        <is>
+          <t>5650</t>
         </is>
       </c>
     </row>
@@ -4896,9 +5170,15 @@
       <c r="AB46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC46" t="inlineStr">
-        <is>
-          <t>5559</t>
+      <c r="AC46" t="n">
+        <v>5559</v>
+      </c>
+      <c r="AD46" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE46" t="inlineStr">
+        <is>
+          <t>5814</t>
         </is>
       </c>
     </row>
@@ -4993,9 +5273,15 @@
       <c r="AB47" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="AC47" t="inlineStr">
-        <is>
-          <t>5040</t>
+      <c r="AC47" t="n">
+        <v>5040</v>
+      </c>
+      <c r="AD47" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="AE47" t="inlineStr">
+        <is>
+          <t>5236</t>
         </is>
       </c>
     </row>
@@ -5090,9 +5376,15 @@
       <c r="AB48" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="AC48" t="inlineStr">
-        <is>
-          <t>5924</t>
+      <c r="AC48" t="n">
+        <v>5924</v>
+      </c>
+      <c r="AD48" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="AE48" t="inlineStr">
+        <is>
+          <t>6201</t>
         </is>
       </c>
     </row>
@@ -5187,9 +5479,15 @@
       <c r="AB49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC49" t="inlineStr">
-        <is>
-          <t>3696</t>
+      <c r="AC49" t="n">
+        <v>3696</v>
+      </c>
+      <c r="AD49" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE49" t="inlineStr">
+        <is>
+          <t>3817</t>
         </is>
       </c>
     </row>
@@ -5284,9 +5582,15 @@
       <c r="AB50" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="AC50" t="inlineStr">
-        <is>
-          <t>5632</t>
+      <c r="AC50" t="n">
+        <v>5632</v>
+      </c>
+      <c r="AD50" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="AE50" t="inlineStr">
+        <is>
+          <t>5885</t>
         </is>
       </c>
     </row>
@@ -5309,7 +5613,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F51" s="3" t="n">
@@ -5381,9 +5685,15 @@
       <c r="AB51" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="AC51" t="inlineStr">
-        <is>
-          <t>5809</t>
+      <c r="AC51" t="n">
+        <v>5809</v>
+      </c>
+      <c r="AD51" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE51" t="inlineStr">
+        <is>
+          <t>5929</t>
         </is>
       </c>
     </row>
@@ -5478,9 +5788,15 @@
       <c r="AB52" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC52" t="inlineStr">
-        <is>
-          <t>2942</t>
+      <c r="AC52" t="n">
+        <v>2942</v>
+      </c>
+      <c r="AD52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE52" t="inlineStr">
+        <is>
+          <t>2962</t>
         </is>
       </c>
     </row>
@@ -5575,9 +5891,15 @@
       <c r="AB53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC53" t="inlineStr">
-        <is>
-          <t>3291</t>
+      <c r="AC53" t="n">
+        <v>3291</v>
+      </c>
+      <c r="AD53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE53" t="inlineStr">
+        <is>
+          <t>3322</t>
         </is>
       </c>
     </row>
@@ -5672,9 +5994,15 @@
       <c r="AB54" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC54" t="inlineStr">
-        <is>
-          <t>3616</t>
+      <c r="AC54" t="n">
+        <v>3616</v>
+      </c>
+      <c r="AD54" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE54" t="inlineStr">
+        <is>
+          <t>4042</t>
         </is>
       </c>
     </row>
@@ -5769,9 +6097,15 @@
       <c r="AB55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="AC55" t="inlineStr">
-        <is>
-          <t>4262</t>
+      <c r="AC55" t="n">
+        <v>4262</v>
+      </c>
+      <c r="AD55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE55" t="inlineStr">
+        <is>
+          <t>4431</t>
         </is>
       </c>
     </row>
@@ -5866,9 +6200,15 @@
       <c r="AB56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC56" t="inlineStr">
-        <is>
-          <t>4506</t>
+      <c r="AC56" t="n">
+        <v>4506</v>
+      </c>
+      <c r="AD56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE56" t="inlineStr">
+        <is>
+          <t>4531</t>
         </is>
       </c>
     </row>
@@ -5963,9 +6303,15 @@
       <c r="AB57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC57" t="inlineStr">
-        <is>
-          <t>5053</t>
+      <c r="AC57" t="n">
+        <v>5053</v>
+      </c>
+      <c r="AD57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE57" t="inlineStr">
+        <is>
+          <t>5100</t>
         </is>
       </c>
     </row>
@@ -6060,9 +6406,15 @@
       <c r="AB58" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="AC58" t="inlineStr">
-        <is>
-          <t>4436</t>
+      <c r="AC58" t="n">
+        <v>4436</v>
+      </c>
+      <c r="AD58" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="AE58" t="inlineStr">
+        <is>
+          <t>4573</t>
         </is>
       </c>
     </row>
@@ -6157,9 +6509,15 @@
       <c r="AB59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC59" t="inlineStr">
-        <is>
-          <t>5066</t>
+      <c r="AC59" t="n">
+        <v>5066</v>
+      </c>
+      <c r="AD59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE59" t="inlineStr">
+        <is>
+          <t>5098</t>
         </is>
       </c>
     </row>
@@ -6254,9 +6612,15 @@
       <c r="AB60" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AC60" t="inlineStr">
-        <is>
-          <t>5314</t>
+      <c r="AC60" t="n">
+        <v>5314</v>
+      </c>
+      <c r="AD60" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="AE60" t="inlineStr">
+        <is>
+          <t>5515</t>
         </is>
       </c>
     </row>
@@ -6351,9 +6715,15 @@
       <c r="AB61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC61" t="inlineStr">
-        <is>
-          <t>5022</t>
+      <c r="AC61" t="n">
+        <v>5022</v>
+      </c>
+      <c r="AD61" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE61" t="inlineStr">
+        <is>
+          <t>5208</t>
         </is>
       </c>
     </row>
@@ -6448,9 +6818,15 @@
       <c r="AB62" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AC62" t="inlineStr">
-        <is>
-          <t>5334</t>
+      <c r="AC62" t="n">
+        <v>5334</v>
+      </c>
+      <c r="AD62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE62" t="inlineStr">
+        <is>
+          <t>5713</t>
         </is>
       </c>
     </row>
@@ -6545,9 +6921,15 @@
       <c r="AB63" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="AC63" t="inlineStr">
-        <is>
-          <t>4369</t>
+      <c r="AC63" t="n">
+        <v>4369</v>
+      </c>
+      <c r="AD63" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="AE63" t="inlineStr">
+        <is>
+          <t>4577</t>
         </is>
       </c>
     </row>
@@ -6642,9 +7024,15 @@
       <c r="AB64" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC64" t="inlineStr">
-        <is>
-          <t>3661</t>
+      <c r="AC64" t="n">
+        <v>3661</v>
+      </c>
+      <c r="AD64" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE64" t="inlineStr">
+        <is>
+          <t>4161</t>
         </is>
       </c>
     </row>
@@ -6739,9 +7127,15 @@
       <c r="AB65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC65" t="inlineStr">
-        <is>
-          <t>4220</t>
+      <c r="AC65" t="n">
+        <v>4220</v>
+      </c>
+      <c r="AD65" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE65" t="inlineStr">
+        <is>
+          <t>4413</t>
         </is>
       </c>
     </row>
@@ -6836,9 +7230,15 @@
       <c r="AB66" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AC66" t="inlineStr">
-        <is>
-          <t>4201</t>
+      <c r="AC66" t="n">
+        <v>4201</v>
+      </c>
+      <c r="AD66" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE66" t="inlineStr">
+        <is>
+          <t>4238</t>
         </is>
       </c>
     </row>
@@ -6933,9 +7333,15 @@
       <c r="AB67" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="AC67" t="inlineStr">
-        <is>
-          <t>5398</t>
+      <c r="AC67" t="n">
+        <v>5398</v>
+      </c>
+      <c r="AD67" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE67" t="inlineStr">
+        <is>
+          <t>5764</t>
         </is>
       </c>
     </row>
@@ -7030,9 +7436,15 @@
       <c r="AB68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC68" t="inlineStr">
-        <is>
-          <t>4444</t>
+      <c r="AC68" t="n">
+        <v>4444</v>
+      </c>
+      <c r="AD68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE68" t="inlineStr">
+        <is>
+          <t>4548</t>
         </is>
       </c>
     </row>
@@ -7127,9 +7539,15 @@
       <c r="AB69" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="AC69" t="inlineStr">
-        <is>
-          <t>3551</t>
+      <c r="AC69" t="n">
+        <v>3551</v>
+      </c>
+      <c r="AD69" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE69" t="inlineStr">
+        <is>
+          <t>4030</t>
         </is>
       </c>
     </row>
@@ -7224,9 +7642,15 @@
       <c r="AB70" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AC70" t="inlineStr">
-        <is>
-          <t>3845</t>
+      <c r="AC70" t="n">
+        <v>3845</v>
+      </c>
+      <c r="AD70" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="AE70" t="inlineStr">
+        <is>
+          <t>3902</t>
         </is>
       </c>
     </row>
@@ -7321,9 +7745,15 @@
       <c r="AB71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC71" t="inlineStr">
-        <is>
-          <t>5508</t>
+      <c r="AC71" t="n">
+        <v>5508</v>
+      </c>
+      <c r="AD71" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE71" t="inlineStr">
+        <is>
+          <t>5645</t>
         </is>
       </c>
     </row>
@@ -7418,7 +7848,13 @@
       <c r="AB72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC72" t="inlineStr">
+      <c r="AC72" t="n">
+        <v>3591</v>
+      </c>
+      <c r="AD72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE72" t="inlineStr">
         <is>
           <t>3591</t>
         </is>
@@ -7515,9 +7951,15 @@
       <c r="AB73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC73" t="inlineStr">
-        <is>
-          <t>5092</t>
+      <c r="AC73" t="n">
+        <v>5092</v>
+      </c>
+      <c r="AD73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE73" t="inlineStr">
+        <is>
+          <t>5285</t>
         </is>
       </c>
     </row>
@@ -7612,9 +8054,15 @@
       <c r="AB74" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AC74" t="inlineStr">
-        <is>
-          <t>4731</t>
+      <c r="AC74" t="n">
+        <v>4731</v>
+      </c>
+      <c r="AD74" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE74" t="inlineStr">
+        <is>
+          <t>4893</t>
         </is>
       </c>
     </row>
@@ -7709,9 +8157,15 @@
       <c r="AB75" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="AC75" t="inlineStr">
-        <is>
-          <t>4943</t>
+      <c r="AC75" t="n">
+        <v>4943</v>
+      </c>
+      <c r="AD75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE75" t="inlineStr">
+        <is>
+          <t>4988</t>
         </is>
       </c>
     </row>
@@ -7806,9 +8260,15 @@
       <c r="AB76" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC76" t="inlineStr">
-        <is>
-          <t>4809</t>
+      <c r="AC76" t="n">
+        <v>4809</v>
+      </c>
+      <c r="AD76" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE76" t="inlineStr">
+        <is>
+          <t>4813</t>
         </is>
       </c>
     </row>
@@ -7886,6 +8346,8 @@
       <c r="AA77" t="inlineStr"/>
       <c r="AB77" s="3" t="inlineStr"/>
       <c r="AC77" t="inlineStr"/>
+      <c r="AD77" s="3" t="inlineStr"/>
+      <c r="AE77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -7978,9 +8440,15 @@
       <c r="AB78" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC78" t="inlineStr">
-        <is>
-          <t>4656</t>
+      <c r="AC78" t="n">
+        <v>4656</v>
+      </c>
+      <c r="AD78" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE78" t="inlineStr">
+        <is>
+          <t>4742</t>
         </is>
       </c>
     </row>
@@ -8075,9 +8543,15 @@
       <c r="AB79" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC79" t="inlineStr">
-        <is>
-          <t>4525</t>
+      <c r="AC79" t="n">
+        <v>4525</v>
+      </c>
+      <c r="AD79" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE79" t="inlineStr">
+        <is>
+          <t>4627</t>
         </is>
       </c>
     </row>
@@ -8172,9 +8646,15 @@
       <c r="AB80" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC80" t="inlineStr">
-        <is>
-          <t>3689</t>
+      <c r="AC80" t="n">
+        <v>3689</v>
+      </c>
+      <c r="AD80" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE80" t="inlineStr">
+        <is>
+          <t>3924</t>
         </is>
       </c>
     </row>
@@ -8269,9 +8749,15 @@
       <c r="AB81" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="AC81" t="inlineStr">
-        <is>
-          <t>3521</t>
+      <c r="AC81" t="n">
+        <v>3521</v>
+      </c>
+      <c r="AD81" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE81" t="inlineStr">
+        <is>
+          <t>3686</t>
         </is>
       </c>
     </row>
@@ -8366,9 +8852,15 @@
       <c r="AB82" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AC82" t="inlineStr">
-        <is>
-          <t>4922</t>
+      <c r="AC82" t="n">
+        <v>4922</v>
+      </c>
+      <c r="AD82" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="AE82" t="inlineStr">
+        <is>
+          <t>4971</t>
         </is>
       </c>
     </row>
@@ -8463,9 +8955,15 @@
       <c r="AB83" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC83" t="inlineStr">
-        <is>
-          <t>3049</t>
+      <c r="AC83" t="n">
+        <v>3049</v>
+      </c>
+      <c r="AD83" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE83" t="inlineStr">
+        <is>
+          <t>3067</t>
         </is>
       </c>
     </row>
@@ -8560,9 +9058,15 @@
       <c r="AB84" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC84" t="inlineStr">
-        <is>
-          <t>3480</t>
+      <c r="AC84" t="n">
+        <v>3480</v>
+      </c>
+      <c r="AD84" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE84" t="inlineStr">
+        <is>
+          <t>3561</t>
         </is>
       </c>
     </row>
@@ -8657,9 +9161,15 @@
       <c r="AB85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC85" t="inlineStr">
-        <is>
-          <t>2085</t>
+      <c r="AC85" t="n">
+        <v>2085</v>
+      </c>
+      <c r="AD85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE85" t="inlineStr">
+        <is>
+          <t>2105</t>
         </is>
       </c>
     </row>
@@ -8754,9 +9264,15 @@
       <c r="AB86" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC86" t="inlineStr">
-        <is>
-          <t>2821</t>
+      <c r="AC86" t="n">
+        <v>2821</v>
+      </c>
+      <c r="AD86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE86" t="inlineStr">
+        <is>
+          <t>2828</t>
         </is>
       </c>
     </row>
@@ -8851,9 +9367,15 @@
       <c r="AB87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC87" t="inlineStr">
-        <is>
-          <t>3145</t>
+      <c r="AC87" t="n">
+        <v>3145</v>
+      </c>
+      <c r="AD87" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE87" t="inlineStr">
+        <is>
+          <t>3198</t>
         </is>
       </c>
     </row>
@@ -8948,9 +9470,15 @@
       <c r="AB88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC88" t="inlineStr">
-        <is>
-          <t>2409</t>
+      <c r="AC88" t="n">
+        <v>2409</v>
+      </c>
+      <c r="AD88" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE88" t="inlineStr">
+        <is>
+          <t>2464</t>
         </is>
       </c>
     </row>
@@ -9016,6 +9544,8 @@
       <c r="AA89" t="inlineStr"/>
       <c r="AB89" s="3" t="inlineStr"/>
       <c r="AC89" t="inlineStr"/>
+      <c r="AD89" s="3" t="inlineStr"/>
+      <c r="AE89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -9079,6 +9609,8 @@
       <c r="AA90" t="inlineStr"/>
       <c r="AB90" s="3" t="inlineStr"/>
       <c r="AC90" t="inlineStr"/>
+      <c r="AD90" s="3" t="inlineStr"/>
+      <c r="AE90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -9171,9 +9703,15 @@
       <c r="AB91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC91" t="inlineStr">
-        <is>
-          <t>2689</t>
+      <c r="AC91" t="n">
+        <v>2689</v>
+      </c>
+      <c r="AD91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE91" t="inlineStr">
+        <is>
+          <t>2686</t>
         </is>
       </c>
     </row>
@@ -9268,9 +9806,15 @@
       <c r="AB92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC92" t="inlineStr">
-        <is>
-          <t>3305</t>
+      <c r="AC92" t="n">
+        <v>3305</v>
+      </c>
+      <c r="AD92" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE92" t="inlineStr">
+        <is>
+          <t>3384</t>
         </is>
       </c>
     </row>
@@ -9365,9 +9909,15 @@
       <c r="AB93" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="AC93" t="inlineStr">
-        <is>
-          <t>3339</t>
+      <c r="AC93" t="n">
+        <v>3339</v>
+      </c>
+      <c r="AD93" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE93" t="inlineStr">
+        <is>
+          <t>3326</t>
         </is>
       </c>
     </row>
@@ -9462,9 +10012,15 @@
       <c r="AB94" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC94" t="inlineStr">
-        <is>
-          <t>4484</t>
+      <c r="AC94" t="n">
+        <v>4484</v>
+      </c>
+      <c r="AD94" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE94" t="inlineStr">
+        <is>
+          <t>4595</t>
         </is>
       </c>
     </row>
@@ -9559,9 +10115,15 @@
       <c r="AB95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC95" t="inlineStr">
-        <is>
-          <t>4093</t>
+      <c r="AC95" t="n">
+        <v>4093</v>
+      </c>
+      <c r="AD95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE95" t="inlineStr">
+        <is>
+          <t>4185</t>
         </is>
       </c>
     </row>
@@ -9656,9 +10218,15 @@
       <c r="AB96" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="AC96" t="inlineStr">
-        <is>
-          <t>3944</t>
+      <c r="AC96" t="n">
+        <v>3944</v>
+      </c>
+      <c r="AD96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE96" t="inlineStr">
+        <is>
+          <t>3934</t>
         </is>
       </c>
     </row>
@@ -9753,9 +10321,15 @@
       <c r="AB97" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AC97" t="inlineStr">
-        <is>
-          <t>4540</t>
+      <c r="AC97" t="n">
+        <v>4540</v>
+      </c>
+      <c r="AD97" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE97" t="inlineStr">
+        <is>
+          <t>4677</t>
         </is>
       </c>
     </row>
@@ -9850,9 +10424,15 @@
       <c r="AB98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC98" t="inlineStr">
-        <is>
-          <t>3887</t>
+      <c r="AC98" t="n">
+        <v>3887</v>
+      </c>
+      <c r="AD98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE98" t="inlineStr">
+        <is>
+          <t>3974</t>
         </is>
       </c>
     </row>
@@ -9947,9 +10527,15 @@
       <c r="AB99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC99" t="inlineStr">
-        <is>
-          <t>2808</t>
+      <c r="AC99" t="n">
+        <v>2808</v>
+      </c>
+      <c r="AD99" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE99" t="inlineStr">
+        <is>
+          <t>3020</t>
         </is>
       </c>
     </row>
@@ -10044,9 +10630,15 @@
       <c r="AB100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC100" t="inlineStr">
-        <is>
-          <t>2610</t>
+      <c r="AC100" t="n">
+        <v>2610</v>
+      </c>
+      <c r="AD100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE100" t="inlineStr">
+        <is>
+          <t>2621</t>
         </is>
       </c>
     </row>
@@ -10141,9 +10733,15 @@
       <c r="AB101" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AC101" t="inlineStr">
-        <is>
-          <t>4861</t>
+      <c r="AC101" t="n">
+        <v>4861</v>
+      </c>
+      <c r="AD101" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE101" t="inlineStr">
+        <is>
+          <t>5371</t>
         </is>
       </c>
     </row>
@@ -10238,9 +10836,15 @@
       <c r="AB102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC102" t="inlineStr">
-        <is>
-          <t>3987</t>
+      <c r="AC102" t="n">
+        <v>3987</v>
+      </c>
+      <c r="AD102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE102" t="inlineStr">
+        <is>
+          <t>4049</t>
         </is>
       </c>
     </row>
@@ -10335,9 +10939,15 @@
       <c r="AB103" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC103" t="inlineStr">
-        <is>
-          <t>3559</t>
+      <c r="AC103" t="n">
+        <v>3559</v>
+      </c>
+      <c r="AD103" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE103" t="inlineStr">
+        <is>
+          <t>3611</t>
         </is>
       </c>
     </row>
@@ -10432,9 +11042,15 @@
       <c r="AB104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC104" t="inlineStr">
-        <is>
-          <t>2625</t>
+      <c r="AC104" t="n">
+        <v>2625</v>
+      </c>
+      <c r="AD104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE104" t="inlineStr">
+        <is>
+          <t>2775</t>
         </is>
       </c>
     </row>
@@ -10529,9 +11145,15 @@
       <c r="AB105" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC105" t="inlineStr">
-        <is>
-          <t>4034</t>
+      <c r="AC105" t="n">
+        <v>4034</v>
+      </c>
+      <c r="AD105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE105" t="inlineStr">
+        <is>
+          <t>4064</t>
         </is>
       </c>
     </row>
@@ -10626,9 +11248,15 @@
       <c r="AB106" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC106" t="inlineStr">
-        <is>
-          <t>3621</t>
+      <c r="AC106" t="n">
+        <v>3621</v>
+      </c>
+      <c r="AD106" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE106" t="inlineStr">
+        <is>
+          <t>3724</t>
         </is>
       </c>
     </row>
@@ -10723,9 +11351,15 @@
       <c r="AB107" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="AC107" t="inlineStr">
-        <is>
-          <t>3903</t>
+      <c r="AC107" t="n">
+        <v>3903</v>
+      </c>
+      <c r="AD107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE107" t="inlineStr">
+        <is>
+          <t>3930</t>
         </is>
       </c>
     </row>
@@ -10820,9 +11454,15 @@
       <c r="AB108" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="AC108" t="inlineStr">
-        <is>
-          <t>2745</t>
+      <c r="AC108" t="n">
+        <v>2745</v>
+      </c>
+      <c r="AD108" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE108" t="inlineStr">
+        <is>
+          <t>2804</t>
         </is>
       </c>
     </row>
@@ -10917,9 +11557,15 @@
       <c r="AB109" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="AC109" t="inlineStr">
-        <is>
-          <t>2856</t>
+      <c r="AC109" t="n">
+        <v>2856</v>
+      </c>
+      <c r="AD109" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE109" t="inlineStr">
+        <is>
+          <t>2903</t>
         </is>
       </c>
     </row>
@@ -11014,9 +11660,15 @@
       <c r="AB110" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="AC110" t="inlineStr">
-        <is>
-          <t>3486</t>
+      <c r="AC110" t="n">
+        <v>3486</v>
+      </c>
+      <c r="AD110" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AE110" t="inlineStr">
+        <is>
+          <t>3631</t>
         </is>
       </c>
     </row>
@@ -11111,9 +11763,15 @@
       <c r="AB111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC111" t="inlineStr">
-        <is>
-          <t>3102</t>
+      <c r="AC111" t="n">
+        <v>3102</v>
+      </c>
+      <c r="AD111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE111" t="inlineStr">
+        <is>
+          <t>3237</t>
         </is>
       </c>
     </row>
@@ -11208,9 +11866,15 @@
       <c r="AB112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC112" t="inlineStr">
-        <is>
-          <t>3654</t>
+      <c r="AC112" t="n">
+        <v>3654</v>
+      </c>
+      <c r="AD112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE112" t="inlineStr">
+        <is>
+          <t>3758</t>
         </is>
       </c>
     </row>
@@ -11305,9 +11969,15 @@
       <c r="AB113" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AC113" t="inlineStr">
-        <is>
-          <t>3047</t>
+      <c r="AC113" t="n">
+        <v>3047</v>
+      </c>
+      <c r="AD113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE113" t="inlineStr">
+        <is>
+          <t>3038</t>
         </is>
       </c>
     </row>
@@ -11402,9 +12072,15 @@
       <c r="AB114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC114" t="inlineStr">
-        <is>
-          <t>3698</t>
+      <c r="AC114" t="n">
+        <v>3698</v>
+      </c>
+      <c r="AD114" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE114" t="inlineStr">
+        <is>
+          <t>3809</t>
         </is>
       </c>
     </row>
@@ -11499,9 +12175,15 @@
       <c r="AB115" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AC115" t="inlineStr">
-        <is>
-          <t>2737</t>
+      <c r="AC115" t="n">
+        <v>2737</v>
+      </c>
+      <c r="AD115" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE115" t="inlineStr">
+        <is>
+          <t>2740</t>
         </is>
       </c>
     </row>
@@ -11596,9 +12278,15 @@
       <c r="AB116" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC116" t="inlineStr">
-        <is>
-          <t>3280</t>
+      <c r="AC116" t="n">
+        <v>3280</v>
+      </c>
+      <c r="AD116" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE116" t="inlineStr">
+        <is>
+          <t>3321</t>
         </is>
       </c>
     </row>
@@ -11693,9 +12381,15 @@
       <c r="AB117" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC117" t="inlineStr">
-        <is>
-          <t>3257</t>
+      <c r="AC117" t="n">
+        <v>3257</v>
+      </c>
+      <c r="AD117" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE117" t="inlineStr">
+        <is>
+          <t>3320</t>
         </is>
       </c>
     </row>
@@ -11773,6 +12467,8 @@
       <c r="AA118" t="inlineStr"/>
       <c r="AB118" s="3" t="inlineStr"/>
       <c r="AC118" t="inlineStr"/>
+      <c r="AD118" s="3" t="inlineStr"/>
+      <c r="AE118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -11865,9 +12561,15 @@
       <c r="AB119" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC119" t="inlineStr">
-        <is>
-          <t>3621</t>
+      <c r="AC119" t="n">
+        <v>3621</v>
+      </c>
+      <c r="AD119" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="AE119" t="inlineStr">
+        <is>
+          <t>3768</t>
         </is>
       </c>
     </row>
@@ -11962,9 +12664,15 @@
       <c r="AB120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC120" t="inlineStr">
-        <is>
-          <t>3330</t>
+      <c r="AC120" t="n">
+        <v>3330</v>
+      </c>
+      <c r="AD120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE120" t="inlineStr">
+        <is>
+          <t>3350</t>
         </is>
       </c>
     </row>
@@ -12059,9 +12767,15 @@
       <c r="AB121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC121" t="inlineStr">
-        <is>
-          <t>2158</t>
+      <c r="AC121" t="n">
+        <v>2158</v>
+      </c>
+      <c r="AD121" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE121" t="inlineStr">
+        <is>
+          <t>2254</t>
         </is>
       </c>
     </row>
@@ -12156,9 +12870,15 @@
       <c r="AB122" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="AC122" t="inlineStr">
-        <is>
-          <t>2730</t>
+      <c r="AC122" t="n">
+        <v>2730</v>
+      </c>
+      <c r="AD122" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE122" t="inlineStr">
+        <is>
+          <t>2725</t>
         </is>
       </c>
     </row>
@@ -12253,9 +12973,15 @@
       <c r="AB123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC123" t="inlineStr">
-        <is>
-          <t>2761</t>
+      <c r="AC123" t="n">
+        <v>2761</v>
+      </c>
+      <c r="AD123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE123" t="inlineStr">
+        <is>
+          <t>2781</t>
         </is>
       </c>
     </row>
@@ -12350,9 +13076,15 @@
       <c r="AB124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC124" t="inlineStr">
-        <is>
-          <t>3705</t>
+      <c r="AC124" t="n">
+        <v>3705</v>
+      </c>
+      <c r="AD124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE124" t="inlineStr">
+        <is>
+          <t>3863</t>
         </is>
       </c>
     </row>
@@ -12447,7 +13179,13 @@
       <c r="AB125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC125" t="inlineStr">
+      <c r="AC125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12544,9 +13282,15 @@
       <c r="AB126" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="AC126" t="inlineStr">
-        <is>
-          <t>3097</t>
+      <c r="AC126" t="n">
+        <v>3097</v>
+      </c>
+      <c r="AD126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE126" t="inlineStr">
+        <is>
+          <t>3068</t>
         </is>
       </c>
     </row>
@@ -12641,9 +13385,15 @@
       <c r="AB127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC127" t="inlineStr">
-        <is>
-          <t>2702</t>
+      <c r="AC127" t="n">
+        <v>2702</v>
+      </c>
+      <c r="AD127" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE127" t="inlineStr">
+        <is>
+          <t>2942</t>
         </is>
       </c>
     </row>
@@ -12738,7 +13488,13 @@
       <c r="AB128" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="AC128" t="inlineStr">
+      <c r="AC128" t="n">
+        <v>2725</v>
+      </c>
+      <c r="AD128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE128" t="inlineStr">
         <is>
           <t>2725</t>
         </is>
@@ -12835,9 +13591,15 @@
       <c r="AB129" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="AC129" t="inlineStr">
-        <is>
-          <t>2495</t>
+      <c r="AC129" t="n">
+        <v>2495</v>
+      </c>
+      <c r="AD129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE129" t="inlineStr">
+        <is>
+          <t>2480</t>
         </is>
       </c>
     </row>
@@ -12932,9 +13694,15 @@
       <c r="AB130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC130" t="inlineStr">
-        <is>
-          <t>1929</t>
+      <c r="AC130" t="n">
+        <v>1929</v>
+      </c>
+      <c r="AD130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE130" t="inlineStr">
+        <is>
+          <t>1907</t>
         </is>
       </c>
     </row>
@@ -13029,7 +13797,13 @@
       <c r="AB131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC131" t="inlineStr">
+      <c r="AC131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13126,7 +13900,13 @@
       <c r="AB132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC132" t="inlineStr">
+      <c r="AC132" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13206,6 +13986,8 @@
       <c r="AA133" t="inlineStr"/>
       <c r="AB133" s="3" t="inlineStr"/>
       <c r="AC133" t="inlineStr"/>
+      <c r="AD133" s="3" t="inlineStr"/>
+      <c r="AE133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -13298,7 +14080,13 @@
       <c r="AB134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC134" t="inlineStr">
+      <c r="AC134" t="n">
+        <v>2088</v>
+      </c>
+      <c r="AD134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE134" t="inlineStr">
         <is>
           <t>2088</t>
         </is>
@@ -13395,9 +14183,15 @@
       <c r="AB135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC135" t="inlineStr">
-        <is>
-          <t>2198</t>
+      <c r="AC135" t="n">
+        <v>2198</v>
+      </c>
+      <c r="AD135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE135" t="inlineStr">
+        <is>
+          <t>2193</t>
         </is>
       </c>
     </row>
@@ -13492,9 +14286,15 @@
       <c r="AB136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC136" t="inlineStr">
-        <is>
-          <t>1532</t>
+      <c r="AC136" t="n">
+        <v>1532</v>
+      </c>
+      <c r="AD136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE136" t="inlineStr">
+        <is>
+          <t>1531</t>
         </is>
       </c>
     </row>
@@ -13572,6 +14372,8 @@
       <c r="AA137" t="inlineStr"/>
       <c r="AB137" s="3" t="inlineStr"/>
       <c r="AC137" t="inlineStr"/>
+      <c r="AD137" s="3" t="inlineStr"/>
+      <c r="AE137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -13664,7 +14466,13 @@
       <c r="AB138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC138" t="inlineStr">
+      <c r="AC138" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13744,6 +14552,8 @@
       <c r="AA139" t="inlineStr"/>
       <c r="AB139" s="3" t="inlineStr"/>
       <c r="AC139" t="inlineStr"/>
+      <c r="AD139" s="3" t="inlineStr"/>
+      <c r="AE139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -13836,9 +14646,15 @@
       <c r="AB140" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC140" t="inlineStr">
-        <is>
-          <t>5083</t>
+      <c r="AC140" t="n">
+        <v>5083</v>
+      </c>
+      <c r="AD140" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="AE140" t="inlineStr">
+        <is>
+          <t>5317</t>
         </is>
       </c>
     </row>
@@ -13933,7 +14749,13 @@
       <c r="AB141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC141" t="inlineStr">
+      <c r="AC141" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14030,7 +14852,13 @@
       <c r="AB142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC142" t="inlineStr">
+      <c r="AC142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14127,9 +14955,15 @@
       <c r="AB143" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC143" t="inlineStr">
-        <is>
-          <t>5805</t>
+      <c r="AC143" t="n">
+        <v>5805</v>
+      </c>
+      <c r="AD143" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AE143" t="inlineStr">
+        <is>
+          <t>6024</t>
         </is>
       </c>
     </row>
@@ -14224,7 +15058,13 @@
       <c r="AB144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC144" t="inlineStr">
+      <c r="AC144" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14321,9 +15161,15 @@
       <c r="AB145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC145" t="inlineStr">
-        <is>
-          <t>2765</t>
+      <c r="AC145" t="n">
+        <v>2765</v>
+      </c>
+      <c r="AD145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE145" t="inlineStr">
+        <is>
+          <t>2833</t>
         </is>
       </c>
     </row>
@@ -14418,7 +15264,13 @@
       <c r="AB146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC146" t="inlineStr">
+      <c r="AC146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14515,9 +15367,15 @@
       <c r="AB147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC147" t="inlineStr">
-        <is>
-          <t>2897</t>
+      <c r="AC147" t="n">
+        <v>2897</v>
+      </c>
+      <c r="AD147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE147" t="inlineStr">
+        <is>
+          <t>2977</t>
         </is>
       </c>
     </row>
@@ -14534,7 +15392,7 @@
       <c r="D148" t="inlineStr"/>
       <c r="E148" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F148" s="3" t="n">
@@ -14590,9 +15448,15 @@
       <c r="AB148" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="AC148" t="inlineStr">
-        <is>
-          <t>3001</t>
+      <c r="AC148" t="n">
+        <v>3001</v>
+      </c>
+      <c r="AD148" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE148" t="inlineStr">
+        <is>
+          <t>2996</t>
         </is>
       </c>
     </row>
@@ -14681,7 +15545,13 @@
       <c r="AB149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC149" t="inlineStr">
+      <c r="AC149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14772,7 +15642,13 @@
       <c r="AB150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC150" t="inlineStr">
+      <c r="AC150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14851,9 +15727,15 @@
       <c r="AB151" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AC151" t="inlineStr">
-        <is>
-          <t>2528</t>
+      <c r="AC151" t="n">
+        <v>2528</v>
+      </c>
+      <c r="AD151" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="AE151" t="inlineStr">
+        <is>
+          <t>2614</t>
         </is>
       </c>
     </row>
@@ -14930,7 +15812,13 @@
       <c r="AB152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC152" t="inlineStr">
+      <c r="AC152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15001,9 +15889,15 @@
       <c r="AB153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC153" t="inlineStr">
-        <is>
-          <t>3795</t>
+      <c r="AC153" t="n">
+        <v>3795</v>
+      </c>
+      <c r="AD153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE153" t="inlineStr">
+        <is>
+          <t>3801</t>
         </is>
       </c>
     </row>
@@ -15072,7 +15966,13 @@
       <c r="AB154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC154" t="inlineStr">
+      <c r="AC154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15139,9 +16039,15 @@
       <c r="AB155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC155" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AC155" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE155" t="inlineStr">
+        <is>
+          <t>1685</t>
         </is>
       </c>
     </row>
@@ -15202,7 +16108,13 @@
       <c r="AB156" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AC156" t="inlineStr">
+      <c r="AC156" t="n">
+        <v>3910</v>
+      </c>
+      <c r="AD156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE156" t="inlineStr">
         <is>
           <t>3910</t>
         </is>
@@ -15260,6 +16172,8 @@
       <c r="AA157" t="inlineStr"/>
       <c r="AB157" s="3" t="inlineStr"/>
       <c r="AC157" t="inlineStr"/>
+      <c r="AD157" s="3" t="inlineStr"/>
+      <c r="AE157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -15305,6 +16219,8 @@
       <c r="AA158" t="inlineStr"/>
       <c r="AB158" s="3" t="inlineStr"/>
       <c r="AC158" t="inlineStr"/>
+      <c r="AD158" s="3" t="inlineStr"/>
+      <c r="AE158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -15359,9 +16275,15 @@
       <c r="AB159" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC159" t="inlineStr">
-        <is>
-          <t>5488</t>
+      <c r="AC159" t="n">
+        <v>5488</v>
+      </c>
+      <c r="AD159" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE159" t="inlineStr">
+        <is>
+          <t>5893</t>
         </is>
       </c>
     </row>
@@ -15418,9 +16340,15 @@
       <c r="AB160" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="AC160" t="inlineStr">
-        <is>
-          <t>2743</t>
+      <c r="AC160" t="n">
+        <v>2743</v>
+      </c>
+      <c r="AD160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE160" t="inlineStr">
+        <is>
+          <t>2779</t>
         </is>
       </c>
     </row>
@@ -15477,9 +16405,15 @@
       <c r="AB161" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC161" t="inlineStr">
-        <is>
-          <t>2117</t>
+      <c r="AC161" t="n">
+        <v>2117</v>
+      </c>
+      <c r="AD161" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE161" t="inlineStr">
+        <is>
+          <t>2169</t>
         </is>
       </c>
     </row>
@@ -15536,9 +16470,15 @@
       <c r="AB162" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="AC162" t="inlineStr">
-        <is>
-          <t>1827</t>
+      <c r="AC162" t="n">
+        <v>1827</v>
+      </c>
+      <c r="AD162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE162" t="inlineStr">
+        <is>
+          <t>1772</t>
         </is>
       </c>
     </row>
@@ -15591,9 +16531,15 @@
       <c r="AB163" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="AC163" t="inlineStr">
-        <is>
-          <t>1627</t>
+      <c r="AC163" t="n">
+        <v>1627</v>
+      </c>
+      <c r="AD163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE163" t="inlineStr">
+        <is>
+          <t>1622</t>
         </is>
       </c>
     </row>
@@ -15642,9 +16588,15 @@
       <c r="AB164" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="AC164" t="inlineStr">
-        <is>
-          <t>5284</t>
+      <c r="AC164" t="n">
+        <v>5284</v>
+      </c>
+      <c r="AD164" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE164" t="inlineStr">
+        <is>
+          <t>5573</t>
         </is>
       </c>
     </row>
@@ -15693,9 +16645,15 @@
       <c r="AB165" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC165" t="inlineStr">
-        <is>
-          <t>2576</t>
+      <c r="AC165" t="n">
+        <v>2576</v>
+      </c>
+      <c r="AD165" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE165" t="inlineStr">
+        <is>
+          <t>2550</t>
         </is>
       </c>
     </row>
@@ -15744,17 +16702,21 @@
       <c r="AB166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC166" t="inlineStr">
-        <is>
-          <t>1259</t>
+      <c r="AC166" t="n">
+        <v>1259</v>
+      </c>
+      <c r="AD166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE166" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>22161051</t>
-        </is>
+      <c r="A167" t="n">
+        <v>22161051</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -15793,17 +16755,21 @@
       <c r="AB167" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="AC167" t="inlineStr">
-        <is>
-          <t>3179</t>
+      <c r="AC167" t="n">
+        <v>3179</v>
+      </c>
+      <c r="AD167" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="AE167" t="inlineStr">
+        <is>
+          <t>3354</t>
         </is>
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>53090046</t>
-        </is>
+      <c r="A168" t="n">
+        <v>53090046</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -15842,17 +16808,15 @@
       <c r="AB168" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AC168" t="inlineStr">
-        <is>
-          <t>2669</t>
-        </is>
-      </c>
+      <c r="AC168" t="n">
+        <v>2669</v>
+      </c>
+      <c r="AD168" s="3" t="inlineStr"/>
+      <c r="AE168" t="inlineStr"/>
     </row>
     <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>57605565</t>
-        </is>
+      <c r="A169" t="n">
+        <v>57605565</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -15891,17 +16855,15 @@
       <c r="AB169" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="AC169" t="inlineStr">
-        <is>
-          <t>1932</t>
-        </is>
-      </c>
+      <c r="AC169" t="n">
+        <v>1932</v>
+      </c>
+      <c r="AD169" s="3" t="inlineStr"/>
+      <c r="AE169" t="inlineStr"/>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>58479166</t>
-        </is>
+      <c r="A170" t="n">
+        <v>58479166</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -15940,9 +16902,168 @@
       <c r="AB170" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="AC170" t="inlineStr">
-        <is>
-          <t>1140</t>
+      <c r="AC170" t="n">
+        <v>1140</v>
+      </c>
+      <c r="AD170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE170" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>57484853</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>"vector to islam"</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr"/>
+      <c r="D171" t="inlineStr"/>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F171" s="3" t="inlineStr"/>
+      <c r="G171" t="inlineStr"/>
+      <c r="H171" s="3" t="inlineStr"/>
+      <c r="I171" t="inlineStr"/>
+      <c r="J171" s="3" t="inlineStr"/>
+      <c r="K171" t="inlineStr"/>
+      <c r="L171" s="3" t="inlineStr"/>
+      <c r="M171" t="inlineStr"/>
+      <c r="N171" s="3" t="inlineStr"/>
+      <c r="O171" t="inlineStr"/>
+      <c r="P171" s="3" t="inlineStr"/>
+      <c r="Q171" t="inlineStr"/>
+      <c r="R171" s="3" t="inlineStr"/>
+      <c r="S171" t="inlineStr"/>
+      <c r="T171" s="3" t="inlineStr"/>
+      <c r="U171" t="inlineStr"/>
+      <c r="V171" s="3" t="inlineStr"/>
+      <c r="W171" t="inlineStr"/>
+      <c r="X171" s="3" t="inlineStr"/>
+      <c r="Y171" t="inlineStr"/>
+      <c r="Z171" s="3" t="inlineStr"/>
+      <c r="AA171" t="inlineStr"/>
+      <c r="AB171" s="3" t="inlineStr"/>
+      <c r="AC171" t="inlineStr"/>
+      <c r="AD171" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE171" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>58537218</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>"BRAWL TALK"</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr"/>
+      <c r="D172" t="inlineStr"/>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F172" s="3" t="inlineStr"/>
+      <c r="G172" t="inlineStr"/>
+      <c r="H172" s="3" t="inlineStr"/>
+      <c r="I172" t="inlineStr"/>
+      <c r="J172" s="3" t="inlineStr"/>
+      <c r="K172" t="inlineStr"/>
+      <c r="L172" s="3" t="inlineStr"/>
+      <c r="M172" t="inlineStr"/>
+      <c r="N172" s="3" t="inlineStr"/>
+      <c r="O172" t="inlineStr"/>
+      <c r="P172" s="3" t="inlineStr"/>
+      <c r="Q172" t="inlineStr"/>
+      <c r="R172" s="3" t="inlineStr"/>
+      <c r="S172" t="inlineStr"/>
+      <c r="T172" s="3" t="inlineStr"/>
+      <c r="U172" t="inlineStr"/>
+      <c r="V172" s="3" t="inlineStr"/>
+      <c r="W172" t="inlineStr"/>
+      <c r="X172" s="3" t="inlineStr"/>
+      <c r="Y172" t="inlineStr"/>
+      <c r="Z172" s="3" t="inlineStr"/>
+      <c r="AA172" t="inlineStr"/>
+      <c r="AB172" s="3" t="inlineStr"/>
+      <c r="AC172" t="inlineStr"/>
+      <c r="AD172" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="AE172" t="inlineStr">
+        <is>
+          <t>1774</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>58572199</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>你干嘛～哎呦～</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr"/>
+      <c r="D173" t="inlineStr"/>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F173" s="3" t="inlineStr"/>
+      <c r="G173" t="inlineStr"/>
+      <c r="H173" s="3" t="inlineStr"/>
+      <c r="I173" t="inlineStr"/>
+      <c r="J173" s="3" t="inlineStr"/>
+      <c r="K173" t="inlineStr"/>
+      <c r="L173" s="3" t="inlineStr"/>
+      <c r="M173" t="inlineStr"/>
+      <c r="N173" s="3" t="inlineStr"/>
+      <c r="O173" t="inlineStr"/>
+      <c r="P173" s="3" t="inlineStr"/>
+      <c r="Q173" t="inlineStr"/>
+      <c r="R173" s="3" t="inlineStr"/>
+      <c r="S173" t="inlineStr"/>
+      <c r="T173" s="3" t="inlineStr"/>
+      <c r="U173" t="inlineStr"/>
+      <c r="V173" s="3" t="inlineStr"/>
+      <c r="W173" t="inlineStr"/>
+      <c r="X173" s="3" t="inlineStr"/>
+      <c r="Y173" t="inlineStr"/>
+      <c r="Z173" s="3" t="inlineStr"/>
+      <c r="AA173" t="inlineStr"/>
+      <c r="AB173" s="3" t="inlineStr"/>
+      <c r="AC173" t="inlineStr"/>
+      <c r="AD173" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE173" t="inlineStr">
+        <is>
+          <t>1361</t>
         </is>
       </c>
     </row>

</xml_diff>